<commit_message>
More work on... everything.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="139">
   <si>
     <t>Type</t>
   </si>
@@ -123,9 +123,6 @@
     <t>The Easily-Disrupted Payoff</t>
   </si>
   <si>
-    <t>The Unexpected Payoff Card</t>
-  </si>
-  <si>
     <t>This card favors those who have this deck memorized.</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>The Early Investment Payoff</t>
   </si>
   <si>
-    <t>See! I knew that would pay off.</t>
-  </si>
-  <si>
     <t>Yes, We Harvest Now</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Wild Boar</t>
   </si>
   <si>
-    <t>But everyone just calls them pigs.</t>
-  </si>
-  <si>
     <t>May be bought by other players on their turn for one of any of the following: Wood, Stone, Silk, Gold, Cattle</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>The Unfair Deck Dive</t>
   </si>
   <si>
-    <t>You may substitute 1 Animal for 1 Wood or 1 Stone</t>
-  </si>
-  <si>
     <t>Building</t>
   </si>
   <si>
@@ -270,21 +258,12 @@
     <t>2 VP for each Military, +2 additional VP if you end the game with the most military (ties don't count).</t>
   </si>
   <si>
-    <t>Agression does have its benefits.</t>
-  </si>
-  <si>
     <t>The number of Glass you have in your hand squared plus the number of Silks you have.</t>
   </si>
   <si>
     <t>1 VP for each type of Resource.</t>
   </si>
   <si>
-    <t>This is to make you feel better about having stuff leftover.</t>
-  </si>
-  <si>
-    <t>5 VP only if you have 1 Glass, 1 Gold, and 1 Vegetable.</t>
-  </si>
-  <si>
     <t>The Clay Building Building</t>
   </si>
   <si>
@@ -330,12 +309,6 @@
     <t>The Cooking Building</t>
   </si>
   <si>
-    <t>You may substitute 2 Grain or 1 Vegetable for any Resource.</t>
-  </si>
-  <si>
-    <t>Please use this card. People just hate it so much.</t>
-  </si>
-  <si>
     <t>Upon playing this card, you may obtain any card in the discard pile and place it in your hand.</t>
   </si>
   <si>
@@ -354,12 +327,6 @@
     <t>I REALLY hope nobody notices that I played this.</t>
   </si>
   <si>
-    <t>8 VPs only if you have Starting Player at the end of the game. Once you play this card, you may not steal starting player.</t>
-  </si>
-  <si>
-    <t>Tray of Vegetables</t>
-  </si>
-  <si>
     <t>A Cattle</t>
   </si>
   <si>
@@ -382,6 +349,90 @@
   </si>
   <si>
     <t>Some Gold Coins</t>
+  </si>
+  <si>
+    <t>This is to make you feel better about having unused stuff.</t>
+  </si>
+  <si>
+    <t>See! I told you that card would pay off.</t>
+  </si>
+  <si>
+    <t>5 VP if you have 1 Glass, 1 Gold, and 1 Vegetable.</t>
+  </si>
+  <si>
+    <t>8 VPs  if you have Starting Player at the end of the game. Once you play this card, you may not steal starting player.</t>
+  </si>
+  <si>
+    <t>1 VP for each Wood, Sheep, or Grain</t>
+  </si>
+  <si>
+    <t>The Unexpected Payoff</t>
+  </si>
+  <si>
+    <t>2 VPs for each Cattle, Vegetable</t>
+  </si>
+  <si>
+    <t>Aggression does have its benefits.</t>
+  </si>
+  <si>
+    <t>Sheep Breed!</t>
+  </si>
+  <si>
+    <t>Cattle Breed!</t>
+  </si>
+  <si>
+    <t>The Building Payoff Building</t>
+  </si>
+  <si>
+    <t>Go ahead and take your next turn, this is gonna take me a moment.</t>
+  </si>
+  <si>
+    <t>2 VP for each Building you've played</t>
+  </si>
+  <si>
+    <t>You may use 2 Grain or 1 Vegetable for any 1 Resource.</t>
+  </si>
+  <si>
+    <t>The Grain Engine</t>
+  </si>
+  <si>
+    <t>Playing this has the hidden advantage of making your opponents hate you.</t>
+  </si>
+  <si>
+    <t>Instead of a Wood or Stone, you may substitute 1 Animal once per play.</t>
+  </si>
+  <si>
+    <t>Place this in front of another player. They may pay 1 Stone to move it to another player, or 2 Stone to remove it from the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do it not for the competitive advantage, but for the schadenfreude. </t>
+  </si>
+  <si>
+    <t>The Expensive Yet Efficient Engine</t>
+  </si>
+  <si>
+    <t>You may use 1 Grain for any 1 Resource, once per play.</t>
+  </si>
+  <si>
+    <t>You may use 1 Resource for other Resource, twice per play.</t>
+  </si>
+  <si>
+    <t>The Animal Engine</t>
+  </si>
+  <si>
+    <t>You may use 1 Animal for any 1 Resource.</t>
+  </si>
+  <si>
+    <t>Hunting Trip</t>
+  </si>
+  <si>
+    <t>Everyone just calls them pigs. Really they're just windfalls,</t>
+  </si>
+  <si>
+    <t>Garden!</t>
+  </si>
+  <si>
+    <t>Requires3</t>
   </si>
 </sst>
 </file>
@@ -740,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,8 +806,8 @@
     <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
     <col min="10" max="10" width="62.7109375" customWidth="1"/>
     <col min="11" max="11" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -788,6 +839,9 @@
       <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
@@ -800,22 +854,22 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
@@ -878,10 +932,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K5" s="3">
         <v>0</v>
@@ -918,7 +972,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -935,13 +989,16 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -955,7 +1012,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -964,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -978,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
@@ -995,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -1012,7 +1069,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1029,13 +1086,13 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
@@ -1052,16 +1109,16 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1072,16 +1129,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
         <v>45</v>
-      </c>
-      <c r="K15" s="3">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1092,22 +1149,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1118,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J17" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1138,19 +1195,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
         <v>42</v>
-      </c>
-      <c r="J18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="3">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1161,19 +1218,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
@@ -1187,19 +1244,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
         <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -1213,19 +1270,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
@@ -1239,13 +1296,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
         <v>11</v>
@@ -1265,13 +1322,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H23" t="s">
         <v>20</v>
@@ -1291,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
         <v>16</v>
@@ -1309,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1320,13 +1377,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H25" t="s">
         <v>20</v>
@@ -1346,13 +1403,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
@@ -1372,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H27" t="s">
         <v>11</v>
@@ -1398,16 +1455,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="K28" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1418,20 +1478,23 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
       </c>
+      <c r="K29" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1441,97 +1504,114 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>119</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" t="s">
         <v>16</v>
       </c>
-      <c r="J30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" t="s">
-        <v>41</v>
-      </c>
       <c r="J32" t="s">
-        <v>69</v>
-      </c>
-      <c r="K32" s="3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="3">
         <v>-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="J33" t="s">
-        <v>62</v>
-      </c>
-      <c r="K33" s="3">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1542,25 +1622,20 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" t="s">
-        <v>71</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E35" s="6"/>
       <c r="J35" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="K35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1571,22 +1646,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
-      </c>
-      <c r="G36" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
-      </c>
-      <c r="K36" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,213 +1663,399 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" t="s">
+        <v>97</v>
+      </c>
+      <c r="K38" s="3">
+        <v>-1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" t="s">
         <v>17</v>
       </c>
-      <c r="J37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" t="s">
-        <v>30</v>
-      </c>
-      <c r="G39" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" t="s">
-        <v>18</v>
-      </c>
       <c r="J39" t="s">
-        <v>80</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L39" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" t="s">
-        <v>81</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="J40" t="s">
+        <v>128</v>
+      </c>
+      <c r="K40" s="3">
+        <v>-2</v>
       </c>
       <c r="L40" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>125</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
       </c>
       <c r="J41" t="s">
-        <v>112</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L41" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>130</v>
+      </c>
+      <c r="G42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>88</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L42" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>39</v>
+        <v>133</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
       </c>
       <c r="J43" t="s">
-        <v>86</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L43" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
       <c r="C44" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>45</v>
-      </c>
-      <c r="K44" s="3">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>76</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="L44" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
       <c r="C45" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="G45" t="s">
+        <v>74</v>
+      </c>
+      <c r="H45" t="s">
+        <v>77</v>
+      </c>
+      <c r="J45" t="s">
+        <v>117</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L45" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
       <c r="C46" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="J46" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="L46" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
       <c r="C47" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="J47" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L47" t="s">
-        <v>84</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J48" t="s">
+        <v>81</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="3">
+        <v>5</v>
+      </c>
+      <c r="L49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>55</v>
+      </c>
+      <c r="J50" t="s">
+        <v>115</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L50" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>62</v>
+      </c>
+      <c r="J51" t="s">
+        <v>80</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="J52" t="s">
+        <v>79</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" t="s">
+        <v>121</v>
+      </c>
+      <c r="G53" t="s">
+        <v>64</v>
+      </c>
+      <c r="J53" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranging bonuses and more game development
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="146">
   <si>
     <t>Type</t>
   </si>
@@ -150,24 +150,12 @@
     <t>You may use any Animals as a replacement for Food.</t>
   </si>
   <si>
-    <t>Early Investment</t>
-  </si>
-  <si>
-    <t>Does nothing now, but I have a feeling this will pay off later.</t>
-  </si>
-  <si>
     <t>The Early Investment Payoff</t>
   </si>
   <si>
     <t>Yes, We Harvest Now</t>
   </si>
   <si>
-    <t>Starting</t>
-  </si>
-  <si>
-    <t>Starting Player</t>
-  </si>
-  <si>
     <t>Silk</t>
   </si>
   <si>
@@ -180,9 +168,6 @@
     <t>Wild Boar</t>
   </si>
   <si>
-    <t>May be bought by other players on their turn for one of any of the following: Wood, Stone, Silk, Gold, Cattle</t>
-  </si>
-  <si>
     <t>The Low-Risk Payoff</t>
   </si>
   <si>
@@ -192,9 +177,6 @@
     <t>Hey, at least you know nobody else is going for it.</t>
   </si>
   <si>
-    <t>Flexible, Yet Inefficient Trader</t>
-  </si>
-  <si>
     <t>In building, you may substitute 3 of any single resource for 1 of any resource</t>
   </si>
   <si>
@@ -243,9 +225,6 @@
     <t>Silk Market</t>
   </si>
   <si>
-    <t>The Trader for That One Strategy</t>
-  </si>
-  <si>
     <t>2 VPs for each Payoff you have placed.</t>
   </si>
   <si>
@@ -300,18 +279,9 @@
     <t>The Military Building</t>
   </si>
   <si>
-    <t>Name says it all.</t>
-  </si>
-  <si>
-    <t>Allows you to build buildings. May also be discarded any time for 1 Food.</t>
-  </si>
-  <si>
     <t>The Cooking Building</t>
   </si>
   <si>
-    <t>Upon playing this card, you may obtain any card in the discard pile and place it in your hand.</t>
-  </si>
-  <si>
     <t>Bag of Grain</t>
   </si>
   <si>
@@ -339,9 +309,6 @@
     <t>At any time, you may substitute 2 Gold for any Resource when playing a card.</t>
   </si>
   <si>
-    <t>A Free Meal</t>
-  </si>
-  <si>
     <t>Requiring food is how we keep you from making powerful moves. You're welcome.</t>
   </si>
   <si>
@@ -408,9 +375,6 @@
     <t xml:space="preserve">Do it not for the competitive advantage, but for the schadenfreude. </t>
   </si>
   <si>
-    <t>The Expensive Yet Efficient Engine</t>
-  </si>
-  <si>
     <t>You may use 1 Grain for any 1 Resource, once per play.</t>
   </si>
   <si>
@@ -429,17 +393,74 @@
     <t>Everyone just calls them pigs. Really they're just windfalls,</t>
   </si>
   <si>
-    <t>Garden!</t>
-  </si>
-  <si>
     <t>Requires3</t>
+  </si>
+  <si>
+    <t>The Expensive Engine</t>
+  </si>
+  <si>
+    <t>That One Strategy</t>
+  </si>
+  <si>
+    <t>Does nothing now, but will pay off later.</t>
+  </si>
+  <si>
+    <t>Sheep: the rabbits of farming.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows you to build buildings. </t>
+  </si>
+  <si>
+    <t>Does it provide the skill of building, or an actual building? Does that ambiguity bother you?</t>
+  </si>
+  <si>
+    <t>Just in case you needed another option to consider.</t>
+  </si>
+  <si>
+    <t>Rotating Advantage</t>
+  </si>
+  <si>
+    <t>Extra Move</t>
+  </si>
+  <si>
+    <t>Make an extra move upon playing. May be bought by other players on their turn for one of any of the following: Wood, Stone, Silk, Gold, Cattle</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Veggies!</t>
+  </si>
+  <si>
+    <t>An Early Investment</t>
+  </si>
+  <si>
+    <t>Free Food!</t>
+  </si>
+  <si>
+    <t>The Flexible Trader</t>
+  </si>
+  <si>
+    <t>Upon playing this card, you may obtain any card in the Resource pile.</t>
+  </si>
+  <si>
+    <t>Grain Breed!</t>
+  </si>
+  <si>
+    <t>You may also use this card for 1 Food</t>
+  </si>
+  <si>
+    <t>More Veggies!</t>
+  </si>
+  <si>
+    <t>You may also use this card for 2 Food</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,7 +600,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -614,7 +634,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -790,31 +809,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
     <col min="10" max="10" width="62.7109375" customWidth="1"/>
     <col min="11" max="11" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -840,7 +859,7 @@
         <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -852,35 +871,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>48</v>
+    <row r="2" spans="1:12" s="4" customFormat="1">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>54</v>
+      <c r="C2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" t="s">
+        <v>135</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -891,6 +913,9 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
       <c r="K3" s="3">
         <v>0</v>
       </c>
@@ -898,12 +923,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -921,21 +946,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K5" s="3">
         <v>0</v>
@@ -944,12 +969,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
@@ -960,59 +985,71 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -1021,10 +1058,10 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1040,76 +1077,88 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>145</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -1118,84 +1167,90 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>136</v>
       </c>
       <c r="K15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -1210,7 +1265,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1218,25 +1273,25 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1244,25 +1299,25 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H20" t="s">
         <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1270,25 +1325,25 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1296,13 +1351,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
         <v>11</v>
@@ -1314,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1322,13 +1377,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H23" t="s">
         <v>20</v>
@@ -1340,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1348,13 +1403,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s">
         <v>16</v>
@@ -1366,10 +1421,10 @@
         <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1377,13 +1432,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s">
         <v>20</v>
@@ -1395,7 +1450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1403,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
@@ -1421,7 +1476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1429,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H27" t="s">
         <v>11</v>
@@ -1447,7 +1502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="14.25" customHeight="1">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1455,22 +1510,22 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K28" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="14.25" customHeight="1">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1478,36 +1533,36 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="K29" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="14.25" customHeight="1">
       <c r="A30" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -1522,21 +1577,24 @@
         <v>17</v>
       </c>
       <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
         <v>18</v>
@@ -1548,382 +1606,400 @@
         <v>18</v>
       </c>
       <c r="K31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
         <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14.25" customHeight="1">
       <c r="A33" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
       </c>
       <c r="G34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" t="s">
         <v>40</v>
       </c>
-      <c r="J34" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="3">
+      <c r="J38" t="s">
+        <v>59</v>
+      </c>
+      <c r="K38" s="3">
         <v>-3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="J35" t="s">
-        <v>59</v>
-      </c>
-      <c r="K35" s="3">
-        <v>1</v>
-      </c>
-      <c r="L35" t="s">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="J39" t="s">
+        <v>53</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E41" t="s">
         <v>61</v>
       </c>
-      <c r="J36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="G41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J41" t="s">
+        <v>62</v>
+      </c>
+      <c r="K41" s="3">
+        <v>2</v>
+      </c>
+      <c r="L41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E37" t="s">
-        <v>67</v>
-      </c>
-      <c r="G37" t="s">
-        <v>67</v>
-      </c>
-      <c r="J37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K37" s="3">
-        <v>2</v>
-      </c>
-      <c r="L37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" t="s">
-        <v>63</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" t="s">
         <v>21</v>
       </c>
-      <c r="J38" t="s">
-        <v>97</v>
-      </c>
-      <c r="K38" s="3">
+      <c r="J42" t="s">
+        <v>141</v>
+      </c>
+      <c r="K42" s="3">
         <v>-1</v>
       </c>
-      <c r="L38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" t="s">
-        <v>75</v>
-      </c>
-      <c r="H39" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="L42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" t="s">
-        <v>128</v>
-      </c>
-      <c r="K40" s="3">
-        <v>-2</v>
-      </c>
-      <c r="L40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>125</v>
-      </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>130</v>
-      </c>
-      <c r="G42" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>133</v>
       </c>
       <c r="G43" t="s">
         <v>17</v>
       </c>
       <c r="J43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
-      </c>
-      <c r="G44" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" t="s">
+        <v>117</v>
+      </c>
+      <c r="K44" s="3">
+        <v>-2</v>
+      </c>
+      <c r="L44" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" t="s">
+        <v>119</v>
+      </c>
+      <c r="K45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s">
+        <v>121</v>
+      </c>
+      <c r="G47" t="s">
         <v>17</v>
       </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" t="s">
-        <v>76</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" t="s">
-        <v>56</v>
-      </c>
-      <c r="G45" t="s">
-        <v>74</v>
-      </c>
-      <c r="H45" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" t="s">
-        <v>117</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" t="s">
-        <v>34</v>
-      </c>
-      <c r="J46" t="s">
-        <v>114</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" t="s">
-        <v>116</v>
-      </c>
       <c r="J47" t="s">
-        <v>113</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="K47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1931,22 +2007,28 @@
         <v>1</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
       </c>
       <c r="J48" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1954,22 +2036,28 @@
         <v>1</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>44</v>
-      </c>
-      <c r="K49" s="3">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="H49" t="s">
+        <v>70</v>
+      </c>
+      <c r="J49" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="L49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1977,22 +2065,22 @@
         <v>1</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="J50" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -2000,22 +2088,22 @@
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="J51" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L51" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -2023,22 +2111,22 @@
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="J52" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L52" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -2046,16 +2134,111 @@
         <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="G53" t="s">
+        <v>136</v>
+      </c>
+      <c r="K53" s="3">
+        <v>5</v>
+      </c>
+      <c r="L53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="J54" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" t="s">
+        <v>56</v>
+      </c>
+      <c r="J55" t="s">
+        <v>73</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
         <v>64</v>
       </c>
-      <c r="J53" t="s">
-        <v>123</v>
+      <c r="J56" t="s">
+        <v>72</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G57" t="s">
+        <v>58</v>
+      </c>
+      <c r="J57" t="s">
+        <v>112</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2064,24 +2247,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More balancing and snarking.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="185">
   <si>
     <t>Type</t>
   </si>
@@ -174,21 +174,12 @@
     <t>Military</t>
   </si>
   <si>
-    <t>If you currently have the most military you may substitute any 1 Resource to build. Ties don't count.</t>
-  </si>
-  <si>
-    <t>I swear this strategy worked for me once.</t>
-  </si>
-  <si>
     <t>The Military Payoff</t>
   </si>
   <si>
     <t>You do not need to pay any required Stone for Buildings.</t>
   </si>
   <si>
-    <t>You may substitute Silk for any Resource.</t>
-  </si>
-  <si>
     <t>Silk Market</t>
   </si>
   <si>
@@ -222,12 +213,6 @@
     <t>You do not need to pay any required Clay for Buildings.</t>
   </si>
   <si>
-    <t>The Clay+Wood Building</t>
-  </si>
-  <si>
-    <t>The Clay+Stone Building</t>
-  </si>
-  <si>
     <t>The Wood Building</t>
   </si>
   <si>
@@ -237,9 +222,6 @@
     <t>The Stone Building</t>
   </si>
   <si>
-    <t>The Wood+Stone Building</t>
-  </si>
-  <si>
     <t>The Military Building</t>
   </si>
   <si>
@@ -336,21 +318,12 @@
     <t>That One Strategy</t>
   </si>
   <si>
-    <t>Does nothing now, but will pay off later.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows you to build buildings. </t>
-  </si>
-  <si>
     <t>Just in case you needed another option to consider.</t>
   </si>
   <si>
     <t>Rotating Advantage</t>
   </si>
   <si>
-    <t>Extra Move</t>
-  </si>
-  <si>
     <t>Investment</t>
   </si>
   <si>
@@ -363,9 +336,6 @@
     <t>Free Food!</t>
   </si>
   <si>
-    <t>The Flexible Trader</t>
-  </si>
-  <si>
     <t>You may also use this card for 1 Food</t>
   </si>
   <si>
@@ -399,9 +369,6 @@
     <t>The Arms Race</t>
   </si>
   <si>
-    <t>Is it the skill of building, or an actual building? Does that ambiguity bother you?</t>
-  </si>
-  <si>
     <t>Grow, Grain, Grow!</t>
   </si>
   <si>
@@ -411,9 +378,6 @@
     <t>8 VPs  if you have Rotating Advantage. at the end of the game. Once you play this card, you may not steal Rotating Advantage.</t>
   </si>
   <si>
-    <t>Make an extra play. May be bought by other players on their turn for one of any of the following: Clay, Stone, Silk, Gold, Cattle, Veggie.</t>
-  </si>
-  <si>
     <t>The Dude</t>
   </si>
   <si>
@@ -423,15 +387,9 @@
     <t>The Cheap Resources</t>
   </si>
   <si>
-    <t>A Middle-Tier Resource</t>
-  </si>
-  <si>
     <t>A Decent Combo</t>
   </si>
   <si>
-    <t>The Premium Stone Resource</t>
-  </si>
-  <si>
     <t>The Wildcard Resource</t>
   </si>
   <si>
@@ -441,12 +399,6 @@
     <t>Everyone just calls them pigs.</t>
   </si>
   <si>
-    <t>When played, pass to the player to your left. On their turn, they must trash 1 Food and may continue passing it.</t>
-  </si>
-  <si>
-    <t>Sorry, we can't just have you do whatever you want.</t>
-  </si>
-  <si>
     <t>The Middle-Tier Resource</t>
   </si>
   <si>
@@ -459,9 +411,6 @@
     <t>Wish this had come out sooner…</t>
   </si>
   <si>
-    <t>You may use 1 Cattle for 2 Food.</t>
-  </si>
-  <si>
     <t>The Artificial Need</t>
   </si>
   <si>
@@ -474,9 +423,6 @@
     <t>You may also trash this card for 2 Food.</t>
   </si>
   <si>
-    <t>You may use any Animals as a 1-1 replacement for Food.</t>
-  </si>
-  <si>
     <t>The Cattle Building</t>
   </si>
   <si>
@@ -516,17 +462,122 @@
     <t>I won't tell you how we got this cow to breed by itself.</t>
   </si>
   <si>
-    <t>And how do we feel about military right about now?</t>
-  </si>
-  <si>
     <t>You may only play this if you already have at least 1 Military.</t>
+  </si>
+  <si>
+    <t>A Better Combo</t>
+  </si>
+  <si>
+    <t>The Premium Resource</t>
+  </si>
+  <si>
+    <t>You may also trash this card for 1 Food</t>
+  </si>
+  <si>
+    <t>You may also trash this card for 2 Food</t>
+  </si>
+  <si>
+    <t>You may substitute 1 Animal for 1 Food, any number of times.</t>
+  </si>
+  <si>
+    <t>You may substitute 1 Silk for any 1 Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>The Clay, Wood Building</t>
+  </si>
+  <si>
+    <t>The Clay, Stone Building</t>
+  </si>
+  <si>
+    <t>The Wood, Stone Building</t>
+  </si>
+  <si>
+    <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
+  </si>
+  <si>
+    <t>You may now build buildings. You may take only one of these into your hand.</t>
+  </si>
+  <si>
+    <t>Plus, you don't have to think about how to make your food!</t>
+  </si>
+  <si>
+    <t>Does nothing now, but it will pay off later. The engine can wait.</t>
+  </si>
+  <si>
+    <t>When played, place in front of the player to your left. Subsequent players must trash 1 Food and to continue passing.</t>
+  </si>
+  <si>
+    <t>Each turn, take an extra Resource card. Other players may transfer this card to their playing area for one of any of the following: Stone, Silk, Gold, Cattle, Veggie.</t>
+  </si>
+  <si>
+    <t>The Obligatory 3:1 Trader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a garden, not some sort of weird patch that passively injects beta-Carotene into your skin. </t>
+  </si>
+  <si>
+    <t>Grain: the best breeder of them all.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may use 1 Cattle for 2 Food, or 1 Cattle for any other Resource. </t>
+  </si>
+  <si>
+    <t>I'm pretty sure this strategy worked for me at least once.</t>
+  </si>
+  <si>
+    <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count.</t>
+  </si>
+  <si>
+    <t>It is by pure coincidence that we actually need stone for our building.</t>
+  </si>
+  <si>
+    <t>It is by pure coincidence that we actually need Wood for our building.</t>
+  </si>
+  <si>
+    <t>It is by pure coincidence that we actually need Clay for our building.</t>
+  </si>
+  <si>
+    <t>Personally, I find grain to much more filling than vegetables.</t>
+  </si>
+  <si>
+    <t>Just don't miss your opportunity to use it.</t>
+  </si>
+  <si>
+    <t>Think of it like breeding VPs.</t>
+  </si>
+  <si>
+    <t>Be sure to take this from someone who has collected silk.</t>
+  </si>
+  <si>
+    <t>Hopefully you didn’t spend all your cattle on Food.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexible, if you invested in farming. </t>
+  </si>
+  <si>
+    <t>Don't get all your VPs too early now.</t>
+  </si>
+  <si>
+    <t>Just when you think you've pulled ahead, someone else will get a bigger building than this.</t>
+  </si>
+  <si>
+    <t>Nice! Way to get some bigger points on the board.</t>
+  </si>
+  <si>
+    <t>Nice! Way to get some points on the board.</t>
+  </si>
+  <si>
+    <t>And how do we feel about going military right about now?</t>
+  </si>
+  <si>
+    <t>Hey, VPs are VPs. Every little bit counts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,7 +717,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -701,7 +751,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -877,15 +926,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
@@ -900,7 +949,7 @@
     <col min="11" max="11" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +972,7 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -935,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -958,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -966,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -978,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -989,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1001,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1021,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1041,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
@@ -1064,7 +1113,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1084,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1104,10 +1153,10 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1115,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
@@ -1127,10 +1176,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1138,13 +1187,13 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="J11" s="3">
         <v>0</v>
@@ -1153,7 +1202,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1161,19 +1210,22 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -1193,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1201,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1209,8 +1261,11 @@
       <c r="J14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1218,19 +1273,22 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1296,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1247,10 +1305,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1258,25 +1316,25 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1284,19 +1342,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="J18" s="3">
         <v>2</v>
       </c>
       <c r="K18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1310,16 +1368,16 @@
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1333,13 +1391,13 @@
         <v>51</v>
       </c>
       <c r="I20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J20" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1347,7 +1405,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
@@ -1359,13 +1417,13 @@
         <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="J21" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1373,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -1385,13 +1443,13 @@
         <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="J22" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -1408,13 +1466,13 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J23" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1425,7 +1483,7 @@
         <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
@@ -1434,7 +1492,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1442,39 +1500,42 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="J25" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="J26" s="3">
         <v>-5</v>
       </c>
       <c r="K26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1482,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
         <v>50</v>
@@ -1491,13 +1552,16 @@
         <v>15</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
         <v>50</v>
@@ -1514,13 +1578,16 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J28" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1528,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
         <v>50</v>
@@ -1537,13 +1604,16 @@
         <v>19</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
         <v>50</v>
@@ -1565,8 +1635,11 @@
       <c r="J30" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
@@ -1588,8 +1661,11 @@
       <c r="J31" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1597,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
@@ -1612,10 +1688,10 @@
         <v>7</v>
       </c>
       <c r="K32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1623,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>155</v>
       </c>
       <c r="F33" t="s">
         <v>50</v>
@@ -1635,10 +1711,13 @@
         <v>10</v>
       </c>
       <c r="J33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1646,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
         <v>50</v>
@@ -1658,10 +1737,13 @@
         <v>15</v>
       </c>
       <c r="J34" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="K34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="F35" t="s">
         <v>50</v>
@@ -1681,10 +1763,13 @@
         <v>15</v>
       </c>
       <c r="J35" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.25" customHeight="1">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1692,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
         <v>51</v>
@@ -1704,16 +1789,16 @@
         <v>50</v>
       </c>
       <c r="I36" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="J36" s="3">
         <v>2</v>
       </c>
       <c r="K36" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="14.25" customHeight="1">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +1806,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
@@ -1739,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="14.25" customHeight="1">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1750,22 +1835,22 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="J38" s="3">
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="14.25" customHeight="1">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1773,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -1791,10 +1876,10 @@
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="14.25" customHeight="1">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1802,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F40" t="s">
         <v>50</v>
@@ -1811,13 +1896,16 @@
         <v>15</v>
       </c>
       <c r="I40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J40" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="14.25" customHeight="1">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1825,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
@@ -1836,8 +1924,11 @@
       <c r="J41" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="14.25" customHeight="1">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1845,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
         <v>29</v>
@@ -1857,13 +1948,16 @@
         <v>29</v>
       </c>
       <c r="I42" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="14.25" customHeight="1">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1871,7 +1965,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -1883,13 +1977,16 @@
         <v>18</v>
       </c>
       <c r="I43" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="J43" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1897,22 +1994,19 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="I44" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="J44" s="3">
         <v>-2</v>
       </c>
       <c r="K44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1920,11 +2014,11 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="D45" s="6"/>
       <c r="I45" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="J45" s="3">
         <v>1</v>
@@ -1933,7 +2027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1947,16 +2041,16 @@
         <v>20</v>
       </c>
       <c r="I46" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J46" s="3">
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1964,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
         <v>51</v>
@@ -1973,16 +2067,16 @@
         <v>51</v>
       </c>
       <c r="I47" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="J47" s="3">
         <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1996,16 +2090,16 @@
         <v>20</v>
       </c>
       <c r="I48" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="J48" s="3">
         <v>0</v>
       </c>
       <c r="K48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" customHeight="1">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2013,22 +2107,22 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
       </c>
       <c r="I49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J49" s="3">
         <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -2036,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -2045,16 +2139,16 @@
         <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="J50" s="3">
         <v>2</v>
       </c>
       <c r="K50" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -2062,22 +2156,22 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J51" s="3">
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2094,7 +2188,7 @@
         <v>17</v>
       </c>
       <c r="I52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>35</v>
@@ -2103,7 +2197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2114,13 +2208,13 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G53" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I53" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>35</v>
@@ -2129,7 +2223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2140,16 +2234,16 @@
         <v>30</v>
       </c>
       <c r="I54" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K54" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2157,10 +2251,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I55" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>35</v>
@@ -2169,7 +2263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2180,16 +2274,16 @@
         <v>34</v>
       </c>
       <c r="I56" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2200,16 +2294,16 @@
         <v>39</v>
       </c>
       <c r="F57" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J57" s="3">
         <v>5</v>
       </c>
       <c r="K57" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2220,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="I58" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>35</v>
@@ -2229,7 +2323,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2240,16 +2334,16 @@
         <v>48</v>
       </c>
       <c r="I59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2257,19 +2351,19 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2277,19 +2371,19 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F61" t="s">
         <v>50</v>
       </c>
       <c r="I61" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K61" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2298,24 +2392,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Game dev. Also split out the marketing
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Deck" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="179">
   <si>
     <t>Type</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Ubiquitous Wood Resource</t>
-  </si>
-  <si>
-    <t>Cheap. Abundant. Necessary. No VPs.</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Look at you, Dr. Fancy Man!</t>
   </si>
   <si>
-    <t>Soft, Cuddly Sheep</t>
-  </si>
-  <si>
     <t>The Building Building Building</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>Insta-slaughter</t>
   </si>
   <si>
-    <t>Can we go back to an abstract theme please?</t>
-  </si>
-  <si>
     <t>Silk</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
     <t>I'm sure I'll use this enough to justify its purchase.</t>
   </si>
   <si>
-    <t>Expand Your Hand</t>
-  </si>
-  <si>
     <t>The Payoff With Math</t>
   </si>
   <si>
@@ -210,54 +195,27 @@
     <t>You do not need to pay any required Clay for Buildings.</t>
   </si>
   <si>
-    <t>The Wood Building</t>
-  </si>
-  <si>
-    <t>The Clay Building</t>
-  </si>
-  <si>
-    <t>The Stone Building</t>
-  </si>
-  <si>
     <t>The Military Building</t>
   </si>
   <si>
-    <t>The Cooking Building</t>
-  </si>
-  <si>
     <t>Bag of Grain</t>
   </si>
   <si>
-    <t>If you currently have the most military you may substitute any 1 Resource for any 1 other Resource. Ties don't count.</t>
-  </si>
-  <si>
     <t>Seems like a lot now, but we have an epic endgame coming up.</t>
   </si>
   <si>
     <t>I REALLY hope nobody notices that I played this.</t>
   </si>
   <si>
-    <t>Rare, But Valuable Glass</t>
-  </si>
-  <si>
     <t>At any time, you may substitute 2 Gold for any Resource when playing a card.</t>
   </si>
   <si>
-    <t>You may hold  10 cards instead of the usual 7</t>
-  </si>
-  <si>
-    <t>Some Gold Coins</t>
-  </si>
-  <si>
     <t>This is to make you feel better about having unused stuff.</t>
   </si>
   <si>
     <t>See! I told you that card would pay off.</t>
   </si>
   <si>
-    <t>5 VP if you have 1 Glass, 1 Gold, and 1 Vegetable.</t>
-  </si>
-  <si>
     <t>1 VP for each Wood, Sheep, or Grain</t>
   </si>
   <si>
@@ -285,9 +243,6 @@
     <t>2 VP for each Building you've played</t>
   </si>
   <si>
-    <t>You may use 2 Grain or 1 Vegetable for any 1 Resource.</t>
-  </si>
-  <si>
     <t>The Grain Engine</t>
   </si>
   <si>
@@ -300,27 +255,12 @@
     <t>You may use 1 Grain for any 1 Resource, once per play.</t>
   </si>
   <si>
-    <t>The Animal Engine</t>
-  </si>
-  <si>
-    <t>You may use 1 Animal for any 1 Resource.</t>
-  </si>
-  <si>
     <t>Requires3</t>
   </si>
   <si>
     <t>The Expensive Engine</t>
   </si>
   <si>
-    <t>That One Strategy</t>
-  </si>
-  <si>
-    <t>Just in case you needed another option to consider.</t>
-  </si>
-  <si>
-    <t>Rotating Advantage</t>
-  </si>
-  <si>
     <t>Investment</t>
   </si>
   <si>
@@ -366,33 +306,18 @@
     <t>The Arms Race</t>
   </si>
   <si>
-    <t>Grow, Grain, Grow!</t>
-  </si>
-  <si>
     <t>You had to see this one coming.</t>
   </si>
   <si>
-    <t>8 VPs  if you have Rotating Advantage. at the end of the game. Once you play this card, you may not steal Rotating Advantage.</t>
-  </si>
-  <si>
     <t>The Dude</t>
   </si>
   <si>
     <t>Upon playing this card, you may obtain any card in the Resource deck.</t>
   </si>
   <si>
-    <t>The Cheap Resources</t>
-  </si>
-  <si>
-    <t>A Decent Combo</t>
-  </si>
-  <si>
     <t>The Wildcard Resource</t>
   </si>
   <si>
-    <t>Hunting Trip Windfall</t>
-  </si>
-  <si>
     <t>Everyone just calls them pigs.</t>
   </si>
   <si>
@@ -414,15 +339,9 @@
     <t>Blocker</t>
   </si>
   <si>
-    <t>You may also trash this card for 1 Food.</t>
-  </si>
-  <si>
     <t>You may also trash this card for 2 Food.</t>
   </si>
   <si>
-    <t>The Cattle Building</t>
-  </si>
-  <si>
     <t>Or is it ore? Mountains? Rock? Definitely not clay.</t>
   </si>
   <si>
@@ -441,30 +360,15 @@
     <t>Ever heard of a meat building?</t>
   </si>
   <si>
-    <t>Not sure how glass accomplishes this.</t>
-  </si>
-  <si>
     <t>One move of the dude is a four-point swing. Don't ever forget about him.</t>
   </si>
   <si>
-    <t>Veggie Patch!</t>
-  </si>
-  <si>
     <t>Sheep: the rabbits of farm animals.</t>
   </si>
   <si>
-    <t>A Cow.</t>
-  </si>
-  <si>
     <t>I won't tell you how we got this cow to breed by itself.</t>
   </si>
   <si>
-    <t>You may only play this if you already have at least 1 Military.</t>
-  </si>
-  <si>
-    <t>A Better Combo</t>
-  </si>
-  <si>
     <t>The Premium Resource</t>
   </si>
   <si>
@@ -474,21 +378,9 @@
     <t>You may also trash this card for 2 Food</t>
   </si>
   <si>
-    <t>You may substitute 1 Animal for 1 Food, any number of times.</t>
-  </si>
-  <si>
     <t>You may substitute 1 Silk for any 1 Resource, any number of times.</t>
   </si>
   <si>
-    <t>The Clay, Wood Building</t>
-  </si>
-  <si>
-    <t>The Clay, Stone Building</t>
-  </si>
-  <si>
-    <t>The Wood, Stone Building</t>
-  </si>
-  <si>
     <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
   </si>
   <si>
@@ -501,12 +393,6 @@
     <t>Does nothing now, but it will pay off later. The engine can wait.</t>
   </si>
   <si>
-    <t>When played, place in front of the player to your left. Subsequent players must trash 1 Food and to continue passing.</t>
-  </si>
-  <si>
-    <t>Each turn, take an extra Resource card. Other players may transfer this card to their playing area for one of any of the following: Stone, Silk, Gold, Cattle, Veggie.</t>
-  </si>
-  <si>
     <t>The Obligatory 3:1 Trader</t>
   </si>
   <si>
@@ -522,9 +408,6 @@
     <t>I'm pretty sure this strategy worked for me at least once.</t>
   </si>
   <si>
-    <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count.</t>
-  </si>
-  <si>
     <t>It is by pure coincidence that we actually need stone for our building.</t>
   </si>
   <si>
@@ -540,18 +423,9 @@
     <t>Just don't miss your opportunity to use it.</t>
   </si>
   <si>
-    <t>Think of it like breeding VPs.</t>
-  </si>
-  <si>
     <t>Be sure to take this from someone who has collected silk.</t>
   </si>
   <si>
-    <t>Hopefully you didn’t spend all your cattle on Food.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flexible, if you invested in farming. </t>
-  </si>
-  <si>
     <t>Don't get all your VPs too early now.</t>
   </si>
   <si>
@@ -586,6 +460,99 @@
   </si>
   <si>
     <t>Kinda like the double-wood, only clay.</t>
+  </si>
+  <si>
+    <t>The Coveted Starting Player</t>
+  </si>
+  <si>
+    <t>Go first!</t>
+  </si>
+  <si>
+    <t>Because just going around in a circle is not strategic enough.</t>
+  </si>
+  <si>
+    <t>Cheap. Abundant. Necessary.</t>
+  </si>
+  <si>
+    <t>The Cheap Resource</t>
+  </si>
+  <si>
+    <t>The Windfall Resource</t>
+  </si>
+  <si>
+    <t>Rare Yet Valuable Resource</t>
+  </si>
+  <si>
+    <t>The Inherently Valuable Resource</t>
+  </si>
+  <si>
+    <t>You gotta spend VPs to earn VPs.</t>
+  </si>
+  <si>
+    <t>8 VPs  if you have Starting Player at the end of the game. Once you play this card, you may not steal Starting Player.</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Cheap Resource Combo</t>
+  </si>
+  <si>
+    <t>Better Resource Combo</t>
+  </si>
+  <si>
+    <t>Decent Resource Combo</t>
+  </si>
+  <si>
+    <t>The Not-as-Cute Yet Expensive Animal</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>The Soft, Cuddly Resource</t>
+  </si>
+  <si>
+    <t>You may use 1 Animal for any 1 Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>If you currently have the most military you may substitute any 1 Resource for any 1 other Resource, once per turn. Ties don't count.</t>
+  </si>
+  <si>
+    <t>The Cheap Combo Building</t>
+  </si>
+  <si>
+    <t>The Better Combo Building</t>
+  </si>
+  <si>
+    <t>The Premium Building</t>
+  </si>
+  <si>
+    <t>The Okay Building</t>
+  </si>
+  <si>
+    <t>The Cheap Building</t>
+  </si>
+  <si>
+    <t>The Decent Combo Building</t>
+  </si>
+  <si>
+    <t>Even More Grain!</t>
+  </si>
+  <si>
+    <t>Even More Veggies!</t>
+  </si>
+  <si>
+    <t>When played, place in front of the player to your left. Subsequent players may trash 1 Food to continue passing, or trash 2 food to remove this card from the game.</t>
+  </si>
+  <si>
+    <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count. You may only play this if you already have at least 1 Military.</t>
+  </si>
+  <si>
+    <t>The Weird Strategy</t>
+  </si>
+  <si>
+    <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable.</t>
   </si>
 </sst>
 </file>
@@ -942,16 +909,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -969,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -981,13 +948,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -999,136 +966,148 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" s="4" customFormat="1">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>5</v>
+        <v>158</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3">
+        <v>149</v>
+      </c>
+      <c r="I2" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>122</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>166</v>
       </c>
       <c r="J4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>165</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>102</v>
       </c>
       <c r="J7" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1136,22 +1115,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1162,16 +1141,19 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
       </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
       <c r="J9" s="3">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1179,22 +1161,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1202,22 +1181,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>132</v>
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
       </c>
       <c r="J11" s="3">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1225,22 +1204,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>133</v>
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1248,22 +1227,22 @@
         <v>6</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J13" s="3">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1274,16 +1253,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1294,189 +1273,168 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>74</v>
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
       </c>
       <c r="J15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="J16" s="3">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
         <v>100</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>162</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="J18" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>160</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="J20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="J21" s="3">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="14.25" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" t="s">
-        <v>151</v>
+        <v>33</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1484,28 +1442,22 @@
         <v>7</v>
       </c>
       <c r="B23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
         <v>93</v>
       </c>
       <c r="J23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1513,16 +1465,25 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
@@ -1530,42 +1491,51 @@
         <v>7</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="J25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="B26" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
       </c>
       <c r="I26" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J26" s="3">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="K26" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1576,22 +1546,22 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J27" s="3">
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1602,22 +1572,22 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J28" s="3">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1628,22 +1598,22 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1654,10 +1624,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1669,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="K30" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1680,22 +1650,22 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J31" s="3">
         <v>4</v>
       </c>
       <c r="K31" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1706,22 +1676,22 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J32" s="3">
         <v>7</v>
       </c>
       <c r="K32" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1732,13 +1702,13 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H33" t="s">
         <v>10</v>
@@ -1747,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="K33" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1758,22 +1728,22 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J34" s="3">
         <v>6</v>
       </c>
       <c r="K34" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1784,22 +1754,22 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
         <v>10</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J35" s="3">
         <v>5</v>
       </c>
       <c r="K35" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="14.25" customHeight="1">
@@ -1810,25 +1780,28 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="G36" t="s">
+        <v>45</v>
       </c>
       <c r="I36" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="J36" s="3">
         <v>2</v>
       </c>
       <c r="K36" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.25" customHeight="1">
@@ -1839,25 +1812,25 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J37" s="3">
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.25" customHeight="1">
@@ -1868,19 +1841,19 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" t="s">
         <v>128</v>
       </c>
-      <c r="F38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" t="s">
-        <v>166</v>
-      </c>
       <c r="J38" s="3">
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.25" customHeight="1">
@@ -1891,25 +1864,25 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J39" s="3">
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.25" customHeight="1">
@@ -1917,25 +1890,28 @@
         <v>9</v>
       </c>
       <c r="B40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>173</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I40" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J40" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1">
@@ -1943,25 +1919,31 @@
         <v>9</v>
       </c>
       <c r="B41" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>174</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>87</v>
       </c>
       <c r="J41" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="14.25" customHeight="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1969,28 +1951,19 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" t="s">
-        <v>29</v>
-      </c>
-      <c r="F42" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="I42" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="J42" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="14.25" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1998,45 +1971,43 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" t="s">
-        <v>18</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D43" s="6"/>
       <c r="I43" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="J43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>45</v>
       </c>
       <c r="I44" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="J44" s="3">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="K44" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
@@ -2047,17 +2018,19 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
-      </c>
-      <c r="D45" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
       <c r="I45" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="J45" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
@@ -2068,140 +2041,146 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I46" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J46" s="3">
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F47" t="s">
-        <v>50</v>
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
       </c>
       <c r="I47" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="J47" s="3">
         <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
       <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>49</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" t="s">
         <v>48</v>
       </c>
-      <c r="F48" t="s">
-        <v>20</v>
-      </c>
-      <c r="I48" t="s">
-        <v>120</v>
-      </c>
-      <c r="J48" s="3">
-        <v>0</v>
-      </c>
-      <c r="K48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
+      <c r="G49" t="s">
+        <v>50</v>
       </c>
       <c r="I49" t="s">
-        <v>92</v>
-      </c>
-      <c r="J49" s="3">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K49" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I50" t="s">
-        <v>137</v>
-      </c>
-      <c r="J50" s="3">
-        <v>2</v>
+        <v>157</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K50" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" t="s">
         <v>16</v>
       </c>
-      <c r="I51" t="s">
-        <v>95</v>
-      </c>
       <c r="J51" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K51" t="s">
-        <v>140</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2212,22 +2191,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="I52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K52" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2238,22 +2211,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="F53" t="s">
-        <v>53</v>
-      </c>
-      <c r="G53" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" t="s">
-        <v>82</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>35</v>
+        <v>81</v>
+      </c>
+      <c r="J53" s="3">
+        <v>5</v>
       </c>
       <c r="K53" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2264,16 +2231,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I54" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K54" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2284,16 +2251,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="I55" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K55" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2304,16 +2271,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I56" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2324,103 +2291,24 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>184</v>
+        <v>72</v>
       </c>
       <c r="F57" t="s">
-        <v>101</v>
-      </c>
-      <c r="J57" s="3">
-        <v>5</v>
+        <v>44</v>
+      </c>
+      <c r="I57" t="s">
+        <v>74</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" s="3">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>42</v>
-      </c>
-      <c r="I58" t="s">
-        <v>80</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" s="3">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>47</v>
-      </c>
-      <c r="I59" t="s">
-        <v>57</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="3">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>51</v>
-      </c>
-      <c r="I60" t="s">
-        <v>56</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K60" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="3">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>86</v>
-      </c>
-      <c r="F61" t="s">
-        <v>49</v>
-      </c>
-      <c r="I61" t="s">
-        <v>88</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K61" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Balancing and shrinking the game down a bit
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Stats" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="182">
   <si>
     <t>Type</t>
   </si>
@@ -249,9 +248,6 @@
     <t>Playing this has the hidden advantage of making your opponents hate you.</t>
   </si>
   <si>
-    <t>Instead of a Wood or Stone, you may substitute 1 Animal once per play.</t>
-  </si>
-  <si>
     <t>You may use 1 Grain for any 1 Resource, once per play.</t>
   </si>
   <si>
@@ -261,9 +257,6 @@
     <t>The Expensive Engine</t>
   </si>
   <si>
-    <t>Investment</t>
-  </si>
-  <si>
     <t>Veggies!</t>
   </si>
   <si>
@@ -312,9 +305,6 @@
     <t>The Dude</t>
   </si>
   <si>
-    <t>Upon playing this card, you may obtain any card in the Resource deck.</t>
-  </si>
-  <si>
     <t>The Wildcard Resource</t>
   </si>
   <si>
@@ -354,9 +344,6 @@
     <t>Don't base your entire strategy on this card.</t>
   </si>
   <si>
-    <t>Forget the theme. We need a card that does this.</t>
-  </si>
-  <si>
     <t>Ever heard of a meat building?</t>
   </si>
   <si>
@@ -549,17 +536,38 @@
     <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count. You may only play this if you already have at least 1 Military.</t>
   </si>
   <si>
-    <t>The Weird Strategy</t>
-  </si>
-  <si>
     <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable.</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Go First!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huffle afterward. </t>
+  </si>
+  <si>
+    <t>Players</t>
+  </si>
+  <si>
+    <t>Total Rounds</t>
+  </si>
+  <si>
+    <t>Early Game Rounds</t>
+  </si>
+  <si>
+    <t>Midgame Rounds</t>
+  </si>
+  <si>
+    <t>Endgame Rounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,7 +592,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -592,11 +600,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,6 +647,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,6 +753,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -733,6 +788,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -908,15 +964,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
@@ -931,7 +987,7 @@
     <col min="11" max="11" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +1010,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -966,32 +1022,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1">
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1003,24 +1059,21 @@
         <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1032,18 +1085,18 @@
         <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1052,24 +1105,21 @@
         <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -1078,39 +1128,39 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="14.25" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J7" s="3">
         <v>-5</v>
       </c>
       <c r="K7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1118,7 +1168,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1130,10 +1180,10 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1141,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1153,10 +1203,10 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1164,7 +1214,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1173,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -1196,18 +1246,18 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1219,18 +1269,18 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1242,10 +1292,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1303,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -1265,7 +1315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1323,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -1285,18 +1335,18 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -1305,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1316,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
@@ -1328,15 +1378,15 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>60</v>
@@ -1351,7 +1401,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1359,22 +1409,22 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1382,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -1391,10 +1441,10 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
@@ -1414,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1425,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -1434,38 +1484,38 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J23" s="3">
         <v>2</v>
       </c>
       <c r="K23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1477,24 +1527,24 @@
         <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
@@ -1506,16 +1556,16 @@
         <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J25" s="3">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="14.25" customHeight="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1529,120 +1579,120 @@
         <v>44</v>
       </c>
       <c r="I26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J26" s="3">
         <v>2</v>
       </c>
       <c r="K26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
-      </c>
-      <c r="F27" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J27" s="3">
-        <v>1</v>
-      </c>
-      <c r="K27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J28" s="3">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
         <v>44</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
         <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
+        <v>58</v>
       </c>
       <c r="J30" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1650,25 +1700,25 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
         <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J31" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1676,25 +1726,25 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F32" t="s">
         <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J32" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1702,25 +1752,25 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F33" t="s">
         <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J33" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1728,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F34" t="s">
         <v>44</v>
@@ -1737,16 +1787,16 @@
         <v>17</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J34" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1754,25 +1804,25 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F35" t="s">
         <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H35" t="s">
         <v>13</v>
       </c>
       <c r="J35" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="14.25" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1780,60 +1830,57 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="F36" t="s">
         <v>44</v>
       </c>
       <c r="G36" t="s">
-        <v>45</v>
-      </c>
-      <c r="I36" t="s">
-        <v>176</v>
+        <v>10</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
       </c>
       <c r="J36" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="14.25" customHeight="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="I37" t="s">
+        <v>172</v>
       </c>
       <c r="J37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="14.25" customHeight="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1841,22 +1888,22 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="I38" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J38" s="3">
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="14.25" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1882,10 +1929,10 @@
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="14.25" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1893,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -1905,16 +1952,16 @@
         <v>26</v>
       </c>
       <c r="I40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J40" s="3">
         <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="14.25" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
@@ -1934,16 +1981,16 @@
         <v>16</v>
       </c>
       <c r="I41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J41" s="3">
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1951,19 +1998,19 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I42" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J42" s="3">
         <v>-2</v>
       </c>
       <c r="K42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1971,11 +2018,11 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D43" s="6"/>
       <c r="I43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J43" s="3">
         <v>1</v>
@@ -1984,15 +2031,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
         <v>45</v>
@@ -2001,16 +2048,16 @@
         <v>45</v>
       </c>
       <c r="I44" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J44" s="3">
         <v>2</v>
       </c>
       <c r="K44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -2024,16 +2071,16 @@
         <v>18</v>
       </c>
       <c r="I45" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="J45" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2041,48 +2088,51 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
       <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" t="s">
+        <v>107</v>
+      </c>
+      <c r="J46" s="3">
+        <v>2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" t="s">
         <v>14</v>
       </c>
-      <c r="I46" t="s">
-        <v>77</v>
-      </c>
-      <c r="J46" s="3">
-        <v>1</v>
-      </c>
-      <c r="K46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" t="s">
-        <v>13</v>
-      </c>
       <c r="G47" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I47" t="s">
-        <v>110</v>
-      </c>
-      <c r="J47" s="3">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2090,25 +2140,25 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I48" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2116,25 +2166,22 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
-      </c>
-      <c r="G49" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="I49" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2142,22 +2189,25 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="F50" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" t="s">
-        <v>157</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="3">
+        <v>6</v>
       </c>
       <c r="K50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2165,25 +2215,19 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="3">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="I51" t="s">
+        <v>53</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2191,19 +2235,19 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I52" t="s">
-        <v>53</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>32</v>
+        <v>138</v>
+      </c>
+      <c r="F52" t="s">
+        <v>91</v>
+      </c>
+      <c r="J52" s="3">
+        <v>5</v>
       </c>
       <c r="K52" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2211,19 +2255,19 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
-      </c>
-      <c r="F53" t="s">
-        <v>81</v>
-      </c>
-      <c r="J53" s="3">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="I53" t="s">
+        <v>66</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K53" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2231,19 +2275,19 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I54" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K54" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2251,19 +2295,19 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2271,39 +2315,19 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>72</v>
+      </c>
+      <c r="F56" t="s">
+        <v>44</v>
       </c>
       <c r="I56" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>72</v>
-      </c>
-      <c r="F57" t="s">
-        <v>44</v>
-      </c>
-      <c r="I57" t="s">
-        <v>74</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2313,25 +2337,318 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A2)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A2)</f>
+        <v>15</v>
+      </c>
+      <c r="C2" s="11">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A2)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A2)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A2)</f>
+        <v>9</v>
+      </c>
+      <c r="G2" s="11">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G2)</f>
+        <v>2</v>
+      </c>
+      <c r="I2" s="11">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G2)</f>
+        <v>4.75</v>
+      </c>
+      <c r="J2" s="11">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K2" s="7">
+        <f>SUM(H2:J2)</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A3)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A3)</f>
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A3)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A3)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A3)</f>
+        <v>12</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G3)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I3" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G3)</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="J3" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G3)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K4" si="0">SUM(H3:J3)</f>
+        <v>6.166666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A4)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A4)</f>
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A4)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A4)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A4)</f>
+        <v>8</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G4)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G4)</f>
+        <v>2.375</v>
+      </c>
+      <c r="J4" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G4)</f>
+        <v>1.25</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A5)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A5)</f>
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A5)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A5)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A6)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A6)</f>
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A6)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A6)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A7)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A7)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A8)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A8)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A8)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A8)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A8)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A9)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A9)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A10)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A10)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A10)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A11)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A11)</f>
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A11)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A11)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A12)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A12)</f>
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A12)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A12)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A13)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A13)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A14)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A14)</f>
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A14)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A14)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A15)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A15)</f>
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A15)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A15)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A15)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A16)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A16)</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A16)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A16)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A16)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="10">
+        <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A17)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A17)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A17)</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some game revisions, cut lines for pdf
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
   </bookViews>
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>Food</t>
   </si>
   <si>
-    <t>Insta-slaughter</t>
-  </si>
-  <si>
     <t>Silk</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>The Military Building</t>
   </si>
   <si>
-    <t>Bag of Grain</t>
-  </si>
-  <si>
     <t>Seems like a lot now, but we have an epic endgame coming up.</t>
   </si>
   <si>
@@ -257,12 +251,6 @@
     <t>The Expensive Engine</t>
   </si>
   <si>
-    <t>Veggies!</t>
-  </si>
-  <si>
-    <t>An Early Investment</t>
-  </si>
-  <si>
     <t>Free Food!</t>
   </si>
   <si>
@@ -467,9 +455,6 @@
     <t>The Windfall Resource</t>
   </si>
   <si>
-    <t>Rare Yet Valuable Resource</t>
-  </si>
-  <si>
     <t>The Inherently Valuable Resource</t>
   </si>
   <si>
@@ -482,15 +467,6 @@
     <t>Special</t>
   </si>
   <si>
-    <t>Cheap Resource Combo</t>
-  </si>
-  <si>
-    <t>Better Resource Combo</t>
-  </si>
-  <si>
-    <t>Decent Resource Combo</t>
-  </si>
-  <si>
     <t>The Not-as-Cute Yet Expensive Animal</t>
   </si>
   <si>
@@ -536,9 +512,6 @@
     <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count. You may only play this if you already have at least 1 Military.</t>
   </si>
   <si>
-    <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable.</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -561,6 +534,33 @@
   </si>
   <si>
     <t>Endgame Rounds</t>
+  </si>
+  <si>
+    <t>The Insta-slaughter</t>
+  </si>
+  <si>
+    <t>The Cheap Resource Combo</t>
+  </si>
+  <si>
+    <t>The Better Resource Combo</t>
+  </si>
+  <si>
+    <t>The Decent Resource Combo</t>
+  </si>
+  <si>
+    <t>The Growing Resource</t>
+  </si>
+  <si>
+    <t>The Other Farming Resource</t>
+  </si>
+  <si>
+    <t>The Rare yet Valuable Resource</t>
+  </si>
+  <si>
+    <t>The Early Investment</t>
+  </si>
+  <si>
+    <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
   </si>
 </sst>
 </file>
@@ -967,9 +967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1010,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -1024,30 +1024,30 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1056,24 +1056,24 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1082,82 +1082,82 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J7" s="3">
         <v>-5</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1303,10 +1303,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
@@ -1323,7 +1323,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1346,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1366,19 +1366,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="3">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1389,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1409,19 +1409,19 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1452,19 +1452,19 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J21" s="3">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1495,16 +1495,16 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J23" s="3">
         <v>2</v>
       </c>
       <c r="K23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1527,13 +1527,13 @@
         <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
@@ -1556,13 +1556,13 @@
         <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J25" s="3">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,19 +1573,19 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I26" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J26" s="3">
         <v>2</v>
       </c>
       <c r="K26" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1611,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1622,22 +1622,22 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" t="s">
         <v>13</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J28" s="3">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1648,22 +1648,22 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" t="s">
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1674,22 +1674,22 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
         <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30" s="3">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1700,10 +1700,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
@@ -1715,7 +1715,7 @@
         <v>2</v>
       </c>
       <c r="K31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1726,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G32" t="s">
         <v>17</v>
@@ -1741,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="K32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,10 +1752,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G33" t="s">
         <v>13</v>
@@ -1767,7 +1767,7 @@
         <v>7</v>
       </c>
       <c r="K33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1778,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G34" t="s">
         <v>17</v>
@@ -1793,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="K34" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1804,10 +1804,10 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G35" t="s">
         <v>17</v>
@@ -1819,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="K35" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,10 +1830,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G36" t="s">
         <v>10</v>
@@ -1845,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="K36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1856,28 +1856,28 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" t="s">
         <v>44</v>
       </c>
-      <c r="G37" t="s">
-        <v>45</v>
-      </c>
       <c r="I37" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="J37" s="3">
         <v>2</v>
       </c>
       <c r="K37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1888,19 +1888,19 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J38" s="3">
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
@@ -1929,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -1952,13 +1952,13 @@
         <v>26</v>
       </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J40" s="3">
         <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
@@ -1981,13 +1981,13 @@
         <v>16</v>
       </c>
       <c r="I41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J41" s="3">
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1998,16 +1998,16 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I42" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="J42" s="3">
         <v>-2</v>
       </c>
       <c r="K42" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,17 +2018,17 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D43" s="6"/>
       <c r="I43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J43" s="3">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,22 +2039,22 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="J44" s="3">
         <v>2</v>
       </c>
       <c r="K44" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,19 +2065,19 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F45" t="s">
         <v>18</v>
       </c>
       <c r="I45" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J45" s="3">
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
@@ -2097,13 +2097,13 @@
         <v>13</v>
       </c>
       <c r="I46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J46" s="3">
         <v>2</v>
       </c>
       <c r="K46" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
         <v>15</v>
       </c>
       <c r="I47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>32</v>
@@ -2140,16 +2140,16 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>32</v>
@@ -2172,13 +2172,13 @@
         <v>17</v>
       </c>
       <c r="I49" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F50" t="s">
         <v>18</v>
@@ -2218,13 +2218,13 @@
         <v>31</v>
       </c>
       <c r="I51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2235,16 +2235,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F52" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J52" s="3">
         <v>5</v>
       </c>
       <c r="K52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,16 +2255,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2275,16 +2275,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2295,16 +2295,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2315,19 +2315,19 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" t="s">
+        <v>43</v>
+      </c>
+      <c r="I56" t="s">
         <v>72</v>
-      </c>
-      <c r="F56" t="s">
-        <v>44</v>
-      </c>
-      <c r="I56" t="s">
-        <v>74</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2340,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,22 +2364,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A11)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A11)</f>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>

</xml_diff>

<commit_message>
Better military strategy cards, tweaking Sheep
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="184">
   <si>
     <t>Type</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Playing this has the hidden advantage of making your opponents hate you.</t>
   </si>
   <si>
-    <t>You may use 1 Grain for any 1 Resource, once per play.</t>
-  </si>
-  <si>
     <t>Requires3</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>You may use 1 Animal for any 1 Resource, any number of times.</t>
   </si>
   <si>
-    <t>If you currently have the most military you may substitute any 1 Resource for any 1 other Resource, once per turn. Ties don't count.</t>
-  </si>
-  <si>
     <t>The Cheap Combo Building</t>
   </si>
   <si>
@@ -561,6 +555,18 @@
   </si>
   <si>
     <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
+  </si>
+  <si>
+    <t>You may use 1 Grain for any 1 Resource, or 1 Grain for 2 Food, any number of times.</t>
+  </si>
+  <si>
+    <t>The Reaction to Military Strategy</t>
+  </si>
+  <si>
+    <t>If you currently have the most military you may substitute any 1 Resource for any 1 other Resource, once per turn. In the case of a tie, nobody gets the bonus. You may only own 1 Military Engine.</t>
+  </si>
+  <si>
+    <t>If this card is available, somebody better take this.</t>
   </si>
 </sst>
 </file>
@@ -965,11 +971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1016,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -1024,30 +1030,30 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1062,21 +1068,21 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1085,102 +1091,102 @@
         <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
+        <v>181</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>180</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="I7" t="s">
+        <v>152</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="3">
         <v>-5</v>
       </c>
-      <c r="K7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
       <c r="K8" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1188,22 +1194,22 @@
         <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J9" s="3">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1211,19 +1217,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1231,22 +1240,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J11" s="3">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1254,22 +1260,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,10 +1286,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1292,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1303,16 +1309,19 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1323,19 +1332,16 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J15" s="3">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1343,19 +1349,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" s="3">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1366,19 +1372,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1386,19 +1389,22 @@
         <v>6</v>
       </c>
       <c r="B18" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
       </c>
       <c r="J18" s="3">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,22 +1412,19 @@
         <v>6</v>
       </c>
       <c r="B19" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>125</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1429,19 +1432,22 @@
         <v>6</v>
       </c>
       <c r="B20" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>99</v>
       </c>
       <c r="J20" s="3">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1449,65 +1455,65 @@
         <v>6</v>
       </c>
       <c r="B21" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J23" s="3">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>180</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="3">
-        <v>2</v>
-      </c>
       <c r="K23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1515,25 +1521,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="J24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1544,25 +1541,25 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J25" s="3">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,19 +1570,25 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,48 +1599,45 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="I27" t="s">
+        <v>111</v>
       </c>
       <c r="J27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="J28" s="3">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1648,22 +1648,22 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
         <v>43</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1674,48 +1674,48 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
         <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J30" s="3">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
         <v>43</v>
       </c>
       <c r="G31" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="I31" t="s">
+        <v>57</v>
       </c>
       <c r="J31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1726,22 +1726,22 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F32" t="s">
         <v>43</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J32" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,22 +1752,22 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s">
         <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J33" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K33" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1784,16 +1784,16 @@
         <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J34" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K34" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F35" t="s">
         <v>43</v>
@@ -1813,13 +1813,13 @@
         <v>17</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J35" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,25 +1830,25 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F36" t="s">
         <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H36" t="s">
         <v>13</v>
       </c>
       <c r="J36" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1856,28 +1856,22 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="F37" t="s">
         <v>43</v>
       </c>
       <c r="G37" t="s">
-        <v>44</v>
-      </c>
-      <c r="I37" t="s">
-        <v>164</v>
+        <v>10</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
       </c>
       <c r="J37" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1888,19 +1882,28 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
       </c>
       <c r="I38" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K38" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,28 +1911,22 @@
         <v>9</v>
       </c>
       <c r="B39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" t="s">
         <v>13</v>
       </c>
+      <c r="I39" t="s">
+        <v>119</v>
+      </c>
       <c r="J39" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K39" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1940,25 +1937,22 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I40" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="J40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K40" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,19 +1963,19 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J41" s="3">
         <v>0</v>
@@ -1990,7 +1984,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1998,19 +1992,28 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>160</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
       </c>
       <c r="I42" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
       <c r="J42" s="3">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -2018,17 +2021,16 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="6"/>
+        <v>90</v>
+      </c>
       <c r="I43" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="J43" s="3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="K43" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,25 +2038,20 @@
         <v>9</v>
       </c>
       <c r="B44" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" t="s">
-        <v>44</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D44" s="6"/>
       <c r="I44" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="J44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2062,25 +2059,28 @@
         <v>9</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="I45" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="J45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2088,48 +2088,45 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I46" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="J46" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>32</v>
+        <v>102</v>
+      </c>
+      <c r="J47" s="3">
+        <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2140,22 +2137,22 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2166,19 +2163,22 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="G49" t="s">
+        <v>49</v>
       </c>
       <c r="I49" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K49" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2189,22 +2189,19 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" t="s">
-        <v>16</v>
-      </c>
-      <c r="J50" s="3">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="I50" t="s">
+        <v>147</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K50" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2215,16 +2212,22 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
-      </c>
-      <c r="I51" t="s">
-        <v>52</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="3">
+        <v>6</v>
       </c>
       <c r="K51" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2235,16 +2238,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
-      </c>
-      <c r="F52" t="s">
-        <v>87</v>
-      </c>
-      <c r="J52" s="3">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="I52" t="s">
+        <v>52</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,16 +2258,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
-      </c>
-      <c r="I53" t="s">
-        <v>64</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>32</v>
+        <v>133</v>
+      </c>
+      <c r="F53" t="s">
+        <v>86</v>
+      </c>
+      <c r="J53" s="3">
+        <v>5</v>
       </c>
       <c r="K53" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2275,16 +2278,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I54" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K54" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2295,16 +2298,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I55" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K55" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2315,19 +2318,39 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I56" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>90</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" t="s">
+        <v>72</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K57" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2364,22 +2387,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2399,11 +2422,11 @@
       </c>
       <c r="H2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G2)</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="I2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G2)</f>
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="J2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G2)</f>
@@ -2424,18 +2447,18 @@
       </c>
       <c r="C3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A3)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A3)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A3)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
       </c>
       <c r="H3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G3)</f>
-        <v>1.3333333333333333</v>
+        <v>1.5</v>
       </c>
       <c r="I3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G3)</f>
-        <v>3.1666666666666665</v>
+        <v>3</v>
       </c>
       <c r="J3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G3)</f>
@@ -2463,11 +2486,11 @@
       </c>
       <c r="H4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G4)</f>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G4)</f>
-        <v>2.375</v>
+        <v>2.25</v>
       </c>
       <c r="J4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G4)</f>
@@ -2484,11 +2507,11 @@
       </c>
       <c r="B5" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A5)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A5)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A5)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A5)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2584,7 +2607,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
@@ -2614,11 +2637,11 @@
       </c>
       <c r="B15" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A15)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A15)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A15)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A15)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A15)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2636,7 +2659,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>

</xml_diff>

<commit_message>
Game balancing from playtest, added starter cards
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="187">
   <si>
     <t>Type</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Silk</t>
   </si>
   <si>
-    <t xml:space="preserve">Or is it wheat? Or corn? </t>
-  </si>
-  <si>
     <t>Wild Boar</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>I REALLY hope nobody notices that I played this.</t>
   </si>
   <si>
-    <t>At any time, you may substitute 2 Gold for any Resource when playing a card.</t>
-  </si>
-  <si>
     <t>This is to make you feel better about having unused stuff.</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>Everyone just calls them pigs.</t>
   </si>
   <si>
-    <t>The Middle-Tier Resource</t>
-  </si>
-  <si>
     <t>Give one to each player. To trash this card, you must trash 3 Food.</t>
   </si>
   <si>
@@ -314,24 +305,15 @@
     <t>Blocker</t>
   </si>
   <si>
-    <t>You may also trash this card for 2 Food.</t>
-  </si>
-  <si>
     <t>Or is it ore? Mountains? Rock? Definitely not clay.</t>
   </si>
   <si>
     <t>Good for more narrow situations.</t>
   </si>
   <si>
-    <t>You may use 1 Resource for other Resource, once per turn.</t>
-  </si>
-  <si>
     <t>Don't base your entire strategy on this card.</t>
   </si>
   <si>
-    <t>Ever heard of a meat building?</t>
-  </si>
-  <si>
     <t>One move of the dude is a four-point swing. Don't ever forget about him.</t>
   </si>
   <si>
@@ -341,24 +323,12 @@
     <t>I won't tell you how we got this cow to breed by itself.</t>
   </si>
   <si>
-    <t>The Premium Resource</t>
-  </si>
-  <si>
-    <t>You may also trash this card for 1 Food</t>
-  </si>
-  <si>
-    <t>You may also trash this card for 2 Food</t>
-  </si>
-  <si>
     <t>You may substitute 1 Silk for any 1 Resource, any number of times.</t>
   </si>
   <si>
     <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
   </si>
   <si>
-    <t>You may now build buildings. You may take only one of these into your hand.</t>
-  </si>
-  <si>
     <t>Plus, you don't have to think about how to make your food!</t>
   </si>
   <si>
@@ -389,9 +359,6 @@
     <t>It is by pure coincidence that we actually need Clay for our building.</t>
   </si>
   <si>
-    <t>Personally, I find grain to much more filling than vegetables.</t>
-  </si>
-  <si>
     <t>Just don't miss your opportunity to use it.</t>
   </si>
   <si>
@@ -428,9 +395,6 @@
     <t>What's better than one veggie? Two veggies and a VP.</t>
   </si>
   <si>
-    <t>A solid choice.</t>
-  </si>
-  <si>
     <t>Kinda like the double-wood, only clay.</t>
   </si>
   <si>
@@ -446,18 +410,9 @@
     <t>Cheap. Abundant. Necessary.</t>
   </si>
   <si>
-    <t>The Cheap Resource</t>
-  </si>
-  <si>
-    <t>The Windfall Resource</t>
-  </si>
-  <si>
     <t>The Inherently Valuable Resource</t>
   </si>
   <si>
-    <t>You gotta spend VPs to earn VPs.</t>
-  </si>
-  <si>
     <t>8 VPs  if you have Starting Player at the end of the game. Once you play this card, you may not steal Starting Player.</t>
   </si>
   <si>
@@ -467,9 +422,6 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>The Soft, Cuddly Resource</t>
-  </si>
-  <si>
     <t>You may use 1 Animal for any 1 Resource, any number of times.</t>
   </si>
   <si>
@@ -527,15 +479,6 @@
     <t>The Insta-slaughter</t>
   </si>
   <si>
-    <t>The Cheap Resource Combo</t>
-  </si>
-  <si>
-    <t>The Better Resource Combo</t>
-  </si>
-  <si>
-    <t>The Decent Resource Combo</t>
-  </si>
-  <si>
     <t>The Growing Resource</t>
   </si>
   <si>
@@ -548,9 +491,6 @@
     <t>The Early Investment</t>
   </si>
   <si>
-    <t>Other players may transfer this card to their playing area for one of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
-  </si>
-  <si>
     <t>You may use 1 Grain for any 1 Resource, or 1 Grain for 2 Food, any number of times.</t>
   </si>
   <si>
@@ -566,7 +506,76 @@
     <t>You may retrieve any Resource, Early Game, or Midgame card in the discard pile and play it immediately without prerequisites.</t>
   </si>
   <si>
-    <t>The Not-as-Cute and Expensive Animal</t>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>You must play this card before playing an Engine.</t>
+  </si>
+  <si>
+    <t>You may trash this card for 2 Food.</t>
+  </si>
+  <si>
+    <t>Hey, you gotta spend VPs to earn VPs.</t>
+  </si>
+  <si>
+    <t>Let's just say you should be happy this card has no artwork.</t>
+  </si>
+  <si>
+    <t>A solid choice, but be sure to commit to it.</t>
+  </si>
+  <si>
+    <t>The Cheap Material</t>
+  </si>
+  <si>
+    <t>The Soft, Cuddly Animal</t>
+  </si>
+  <si>
+    <t>The Windfall Animal</t>
+  </si>
+  <si>
+    <t>The Wildcard Building</t>
+  </si>
+  <si>
+    <t>Or is it wheat? Or corn? Seeds?</t>
+  </si>
+  <si>
+    <t>Personally, I find grain to be much more filling than vegetables.</t>
+  </si>
+  <si>
+    <t>You may trash this card for 1 Food.</t>
+  </si>
+  <si>
+    <t>The Middle-Tier Material</t>
+  </si>
+  <si>
+    <t>The Premium Material</t>
+  </si>
+  <si>
+    <t>The Cheap Material Combo</t>
+  </si>
+  <si>
+    <t>The Better Material Combo</t>
+  </si>
+  <si>
+    <t>The Decent Material Combo</t>
+  </si>
+  <si>
+    <t>The Not-as-Cute Animal</t>
+  </si>
+  <si>
+    <t>Other players may transfer this card to their playing area for 1 of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
+  </si>
+  <si>
+    <t>You may now build buildings. You may only take one of these into your hand per game.</t>
+  </si>
+  <si>
+    <t>If you currently have the most military you may substitute any 1 Resource to play a card. In case of tie, nobody gets the bonus.</t>
+  </si>
+  <si>
+    <t>You may substitute 1 Gold for any 1 Resource.</t>
+  </si>
+  <si>
+    <t>You may use 1 Resource for 1 other Resource, once per turn.</t>
   </si>
 </sst>
 </file>
@@ -974,8 +983,8 @@
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1025,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -1030,30 +1039,30 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1062,24 +1071,24 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -1088,105 +1097,105 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J8" s="3">
         <v>-5</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1197,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1209,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1220,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1232,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1243,7 +1252,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1252,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1263,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1275,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1286,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -1298,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1321,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1332,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -1352,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1361,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1372,7 +1381,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1381,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1392,19 +1401,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>165</v>
       </c>
       <c r="J18" s="3">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1415,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1424,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1435,19 +1447,19 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="J20" s="3">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1458,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1467,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,19 +1490,19 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="J22" s="3">
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -1510,38 +1522,41 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="I24" t="s">
+        <v>164</v>
       </c>
       <c r="J24" s="3">
         <v>2</v>
       </c>
       <c r="K24" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -1553,24 +1568,24 @@
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="J25" s="3">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -1582,47 +1597,47 @@
         <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="J26" s="3">
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="F27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J27" s="3">
         <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B28" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1637,99 +1652,99 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J29" s="3">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J30" s="3">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
         <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J31" s="3">
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
@@ -1741,21 +1756,21 @@
         <v>2</v>
       </c>
       <c r="K32" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
         <v>17</v>
@@ -1767,59 +1782,68 @@
         <v>4</v>
       </c>
       <c r="K33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
       </c>
       <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
         <v>43</v>
       </c>
-      <c r="G34" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" t="s">
-        <v>13</v>
+      <c r="I34" t="s">
+        <v>145</v>
       </c>
       <c r="J34" s="3">
+        <v>2</v>
+      </c>
+      <c r="K34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>7</v>
       </c>
-      <c r="K34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
       <c r="B35" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>142</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
       </c>
       <c r="F35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="I35" t="s">
+        <v>76</v>
       </c>
       <c r="J35" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K35" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,22 +1854,22 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H36" t="s">
         <v>13</v>
       </c>
       <c r="J36" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K36" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1856,25 +1880,25 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
         <v>10</v>
       </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
       <c r="J37" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1882,31 +1906,25 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="F38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s">
-        <v>44</v>
-      </c>
-      <c r="I38" t="s">
-        <v>161</v>
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>13</v>
       </c>
       <c r="J38" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1914,19 +1932,22 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" t="s">
         <v>13</v>
       </c>
-      <c r="I39" t="s">
-        <v>119</v>
-      </c>
       <c r="J39" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K39" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1937,22 +1958,19 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="I40" t="s">
+        <v>109</v>
       </c>
       <c r="J40" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K40" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1960,28 +1978,25 @@
         <v>9</v>
       </c>
       <c r="B41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I41" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="J41" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K41" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,10 +2004,10 @@
         <v>9</v>
       </c>
       <c r="B42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D42" t="s">
         <v>16</v>
@@ -2004,13 +2019,13 @@
         <v>16</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J42" s="3">
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2021,16 +2036,16 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I43" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="J43" s="3">
         <v>-2</v>
       </c>
       <c r="K43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2041,17 +2056,17 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D44" s="6"/>
       <c r="I44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J44" s="3">
         <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2062,22 +2077,22 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I45" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="J45" s="3">
         <v>2</v>
       </c>
       <c r="K45" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2088,19 +2103,19 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" t="s">
         <v>18</v>
       </c>
       <c r="I46" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="J46" s="3">
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2111,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
@@ -2120,13 +2135,13 @@
         <v>13</v>
       </c>
       <c r="I47" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
       <c r="J47" s="3">
         <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2146,7 +2161,7 @@
         <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>32</v>
@@ -2163,16 +2178,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>32</v>
@@ -2195,13 +2210,13 @@
         <v>17</v>
       </c>
       <c r="I50" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2212,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F51" t="s">
         <v>18</v>
@@ -2241,13 +2256,13 @@
         <v>31</v>
       </c>
       <c r="I52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2258,16 +2273,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J53" s="3">
         <v>5</v>
       </c>
       <c r="K53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2278,16 +2293,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2298,16 +2313,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2318,16 +2333,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2338,19 +2353,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" t="s">
+        <v>42</v>
+      </c>
+      <c r="I57" t="s">
         <v>70</v>
-      </c>
-      <c r="F57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I57" t="s">
-        <v>72</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2387,22 +2402,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2422,11 +2437,11 @@
       </c>
       <c r="H2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G2)</f>
-        <v>2.25</v>
+        <v>1.25</v>
       </c>
       <c r="I2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G2)</f>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="J2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G2)</f>
@@ -2434,7 +2449,7 @@
       </c>
       <c r="K2" s="7">
         <f>SUM(H2:J2)</f>
-        <v>9.25</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2454,11 +2469,11 @@
       </c>
       <c r="H3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G3)</f>
-        <v>1.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G3)</f>
-        <v>3</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="J3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G3)</f>
@@ -2466,7 +2481,7 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K4" si="0">SUM(H3:J3)</f>
-        <v>6.166666666666667</v>
+        <v>5.166666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2486,11 +2501,11 @@
       </c>
       <c r="H4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G4)</f>
-        <v>1.125</v>
+        <v>0.625</v>
       </c>
       <c r="I4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G4)</f>
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="J4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G4)</f>
@@ -2498,7 +2513,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>4.625</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2507,11 +2522,11 @@
       </c>
       <c r="B5" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A5)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A5)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A5)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A5)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2520,16 +2535,16 @@
       </c>
       <c r="B6" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A6)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A6)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A6)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A6)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
@@ -2546,16 +2561,16 @@
       </c>
       <c r="B8" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A8)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A8)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A8)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A8)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A8)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
@@ -2568,7 +2583,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
@@ -2607,7 +2622,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
@@ -2637,11 +2652,11 @@
       </c>
       <c r="B15" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A15)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A15)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A15)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A15)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A15)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2659,7 +2674,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>

</xml_diff>

<commit_message>
Brought in trashing and split out requires
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="187">
   <si>
     <t>Type</t>
   </si>
@@ -155,24 +155,12 @@
     <t>You do not need to pay any required Stone for Buildings.</t>
   </si>
   <si>
-    <t>Silk Market</t>
-  </si>
-  <si>
     <t>2 VPs for each Payoff you have placed.</t>
   </si>
   <si>
-    <t>Clay Building</t>
-  </si>
-  <si>
     <t>2 VP for each Military, +2 additional VP if you end the game with the most military (ties don't count).</t>
   </si>
   <si>
-    <t>The number of Glass you have in your hand squared plus the number of Silks you have.</t>
-  </si>
-  <si>
-    <t>1 VP for each type of Resource.</t>
-  </si>
-  <si>
     <t>The Clay Building Building</t>
   </si>
   <si>
@@ -236,9 +224,6 @@
     <t>Playing this has the hidden advantage of making your opponents hate you.</t>
   </si>
   <si>
-    <t>Requires3</t>
-  </si>
-  <si>
     <t>The Expensive Engine</t>
   </si>
   <si>
@@ -419,24 +404,12 @@
     <t>You may use 1 Animal for any 1 Resource, any number of times.</t>
   </si>
   <si>
-    <t>The Cheap Combo Building</t>
-  </si>
-  <si>
-    <t>The Better Combo Building</t>
-  </si>
-  <si>
     <t>The Premium Building</t>
   </si>
   <si>
-    <t>The Okay Building</t>
-  </si>
-  <si>
     <t>The Cheap Building</t>
   </si>
   <si>
-    <t>The Decent Combo Building</t>
-  </si>
-  <si>
     <t>Even More Grain!</t>
   </si>
   <si>
@@ -473,15 +446,6 @@
     <t>The Insta-slaughter</t>
   </si>
   <si>
-    <t>The Growing Resource</t>
-  </si>
-  <si>
-    <t>The Other Farming Resource</t>
-  </si>
-  <si>
-    <t>The Rare yet Valuable Resource</t>
-  </si>
-  <si>
     <t>The Early Investment</t>
   </si>
   <si>
@@ -521,9 +485,6 @@
     <t>The Cheap Material</t>
   </si>
   <si>
-    <t>The Soft, Cuddly Animal</t>
-  </si>
-  <si>
     <t>The Windfall Animal</t>
   </si>
   <si>
@@ -539,24 +500,15 @@
     <t>You may trash this card for 1 Food.</t>
   </si>
   <si>
-    <t>The Middle-Tier Material</t>
-  </si>
-  <si>
     <t>The Premium Material</t>
   </si>
   <si>
-    <t>The Cheap Material Combo</t>
-  </si>
-  <si>
     <t>The Better Material Combo</t>
   </si>
   <si>
     <t>The Decent Material Combo</t>
   </si>
   <si>
-    <t>The Not-as-Cute Animal</t>
-  </si>
-  <si>
     <t>Other players may transfer this card to their playing area for 1 of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
   </si>
   <si>
@@ -576,6 +528,54 @@
   </si>
   <si>
     <t>You may substitute 3 Resources of any type(s) for 1 of any Resource.</t>
+  </si>
+  <si>
+    <t>Trash1</t>
+  </si>
+  <si>
+    <t>Trash2</t>
+  </si>
+  <si>
+    <t>The Better Building</t>
+  </si>
+  <si>
+    <t>The Decent Building</t>
+  </si>
+  <si>
+    <t>The Cuddly Animal</t>
+  </si>
+  <si>
+    <t>The Expensive Animal</t>
+  </si>
+  <si>
+    <t>1 VP for each type of Resource at the end of the game.</t>
+  </si>
+  <si>
+    <t>At game end, VPs are the number of Glass you have in your hand squared plus the number of Silks you have.</t>
+  </si>
+  <si>
+    <t>The Multiplying Plant</t>
+  </si>
+  <si>
+    <t>The Expensive Plant</t>
+  </si>
+  <si>
+    <t>The Rare Resource</t>
+  </si>
+  <si>
+    <t>The Good Material</t>
+  </si>
+  <si>
+    <t>The Good Building</t>
+  </si>
+  <si>
+    <t>The Easy Material Combo</t>
+  </si>
+  <si>
+    <t>The Easy Building</t>
+  </si>
+  <si>
+    <t>Carrot</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -679,6 +679,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,11 +983,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,15 +997,13 @@
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="62.7109375" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.140625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="62.7109375" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,51 +1019,58 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>127</v>
-      </c>
-      <c r="I2" t="s">
-        <v>180</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>132</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1073,22 +1081,19 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>181</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" s="3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -1099,106 +1104,100 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
-        <v>158</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="J5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="3">
         <v>2</v>
       </c>
-      <c r="K5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>156</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="J6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>133</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="3">
+        <v>88</v>
+      </c>
+      <c r="J8" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="3">
         <v>-5</v>
       </c>
-      <c r="K8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1214,14 +1213,14 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1229,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1237,14 +1236,14 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1252,19 +1251,19 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1280,14 +1279,14 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>0</v>
       </c>
-      <c r="K12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -1303,14 +1302,14 @@
       <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>0</v>
       </c>
-      <c r="K13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1326,14 +1325,14 @@
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>0</v>
       </c>
-      <c r="K14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1341,19 +1340,19 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1361,19 +1360,19 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1381,19 +1380,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1409,17 +1408,17 @@
       <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="I18" t="s">
-        <v>163</v>
-      </c>
-      <c r="J18" s="3">
+      <c r="J18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K18" s="3">
         <v>0</v>
       </c>
-      <c r="K18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1427,19 +1426,19 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1447,22 +1446,22 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" t="s">
-        <v>163</v>
-      </c>
-      <c r="J20" s="3">
+        <v>186</v>
+      </c>
+      <c r="J20" t="s">
+        <v>151</v>
+      </c>
+      <c r="K20" s="3">
         <v>0</v>
       </c>
-      <c r="K20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1470,19 +1469,19 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1490,22 +1489,22 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="I22" t="s">
-        <v>183</v>
-      </c>
-      <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>167</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1513,50 +1512,50 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="I24" t="s">
-        <v>162</v>
-      </c>
-      <c r="J24" s="3">
+        <v>78</v>
+      </c>
+      <c r="J24" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" s="3">
         <v>2</v>
       </c>
-      <c r="K24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -1564,80 +1563,80 @@
       <c r="E25" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I25" t="s">
-        <v>173</v>
-      </c>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" t="s">
-        <v>163</v>
-      </c>
-      <c r="J26" s="3">
-        <v>1</v>
-      </c>
-      <c r="K26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J26" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
-      </c>
-      <c r="F27" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J27" s="3">
+      <c r="J27" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="3">
         <v>2</v>
       </c>
-      <c r="K27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B28" s="3">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1645,95 +1644,95 @@
       <c r="E28" t="s">
         <v>14</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" t="s">
         <v>52</v>
       </c>
-      <c r="F31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1741,25 +1740,22 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
-      </c>
-      <c r="F32" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="3">
-        <v>2</v>
-      </c>
-      <c r="K32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>103</v>
+      </c>
+      <c r="K32" s="3">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1767,25 +1763,20 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33" s="3">
-        <v>4</v>
-      </c>
-      <c r="K33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="J33" t="s">
+        <v>170</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1793,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
         <v>43</v>
@@ -1801,23 +1792,23 @@
       <c r="E34" t="s">
         <v>43</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="I34" t="s">
-        <v>143</v>
-      </c>
-      <c r="J34" s="3">
+      <c r="J34" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" s="3">
         <v>2</v>
       </c>
-      <c r="K34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1825,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
@@ -1833,20 +1824,20 @@
       <c r="E35" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I35" t="s">
-        <v>76</v>
-      </c>
-      <c r="J35" s="3">
+      <c r="J35" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" s="3">
         <v>0</v>
       </c>
-      <c r="K35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1854,25 +1845,25 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36" s="3">
-        <v>7</v>
-      </c>
-      <c r="K36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="3">
+        <v>2</v>
+      </c>
+      <c r="L36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1880,25 +1871,25 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
-      </c>
-      <c r="F37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G37" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-      <c r="J37" s="3">
-        <v>4</v>
-      </c>
-      <c r="K37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="3">
+        <v>7</v>
+      </c>
+      <c r="L37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1906,25 +1897,25 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G38" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="3">
-        <v>6</v>
-      </c>
-      <c r="K38" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="3">
+        <v>4</v>
+      </c>
+      <c r="L38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1932,25 +1923,25 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" t="s">
+        <v>183</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39" s="3">
-        <v>5</v>
-      </c>
-      <c r="K39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="3">
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1958,48 +1949,51 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I40" t="s">
-        <v>108</v>
-      </c>
-      <c r="J40" s="3">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K40" s="3">
+        <v>6</v>
+      </c>
+      <c r="L40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
-      <c r="J41" s="3">
-        <v>3</v>
-      </c>
-      <c r="K41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="3">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2007,48 +2001,54 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>78</v>
-      </c>
-      <c r="J42" s="3">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" s="3">
+        <v>3</v>
+      </c>
+      <c r="L42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" t="s">
-        <v>142</v>
-      </c>
-      <c r="J43" s="3">
-        <v>-2</v>
-      </c>
-      <c r="K43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J43" t="s">
+        <v>73</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -2056,20 +2056,19 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="I44" t="s">
-        <v>186</v>
-      </c>
-      <c r="J44" s="3">
-        <v>1</v>
-      </c>
-      <c r="K44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="J44" t="s">
+        <v>133</v>
+      </c>
+      <c r="K44" s="3">
+        <v>-2</v>
+      </c>
+      <c r="L44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -2077,25 +2076,28 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
         <v>43</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="I45" t="s">
-        <v>182</v>
-      </c>
-      <c r="J45" s="3">
+      <c r="J45" t="s">
+        <v>166</v>
+      </c>
+      <c r="K45" s="3">
         <v>2</v>
       </c>
-      <c r="K45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2105,20 +2107,20 @@
       <c r="C46" t="s">
         <v>41</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I46" t="s">
-        <v>160</v>
-      </c>
-      <c r="J46" s="3">
-        <v>1</v>
-      </c>
-      <c r="K46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>148</v>
+      </c>
+      <c r="K46" s="3">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -2126,25 +2128,25 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I47" t="s">
-        <v>184</v>
-      </c>
-      <c r="J47" s="3">
+      <c r="J47" t="s">
+        <v>168</v>
+      </c>
+      <c r="K47" s="3">
         <v>2</v>
       </c>
-      <c r="K47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2154,23 +2156,23 @@
       <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I48" t="s">
-        <v>47</v>
-      </c>
-      <c r="J48" s="3" t="s">
+      <c r="J48" t="s">
+        <v>46</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2180,23 +2182,26 @@
       <c r="C49" t="s">
         <v>37</v>
       </c>
-      <c r="F49" t="s">
-        <v>46</v>
-      </c>
-      <c r="G49" t="s">
-        <v>48</v>
-      </c>
-      <c r="I49" t="s">
-        <v>64</v>
-      </c>
-      <c r="J49" s="3" t="s">
+      <c r="F49" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J49" t="s">
+        <v>60</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2206,20 +2211,17 @@
       <c r="C50" t="s">
         <v>27</v>
       </c>
-      <c r="F50" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" t="s">
-        <v>131</v>
-      </c>
-      <c r="J50" s="3" t="s">
+      <c r="J50" t="s">
+        <v>126</v>
+      </c>
+      <c r="K50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K50" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2227,25 +2229,22 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="3">
+      <c r="G51" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K51" s="3">
         <v>6</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2255,17 +2254,17 @@
       <c r="C52" t="s">
         <v>31</v>
       </c>
-      <c r="I52" t="s">
-        <v>51</v>
-      </c>
-      <c r="J52" s="3" t="s">
+      <c r="J52" t="s">
+        <v>177</v>
+      </c>
+      <c r="K52" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2273,19 +2272,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>121</v>
-      </c>
-      <c r="F53" t="s">
-        <v>83</v>
-      </c>
-      <c r="J53" s="3">
+        <v>116</v>
+      </c>
+      <c r="K53" s="3">
         <v>5</v>
       </c>
-      <c r="K53" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2295,17 +2291,17 @@
       <c r="C54" t="s">
         <v>36</v>
       </c>
-      <c r="I54" t="s">
-        <v>62</v>
-      </c>
-      <c r="J54" s="3" t="s">
+      <c r="J54" t="s">
+        <v>58</v>
+      </c>
+      <c r="K54" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2315,17 +2311,17 @@
       <c r="C55" t="s">
         <v>40</v>
       </c>
-      <c r="I55" t="s">
-        <v>50</v>
-      </c>
-      <c r="J55" s="3" t="s">
+      <c r="J55" t="s">
+        <v>178</v>
+      </c>
+      <c r="K55" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K55" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2335,17 +2331,17 @@
       <c r="C56" t="s">
         <v>44</v>
       </c>
-      <c r="I56" t="s">
-        <v>49</v>
-      </c>
-      <c r="J56" s="3" t="s">
+      <c r="J56" t="s">
+        <v>47</v>
+      </c>
+      <c r="K56" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K56" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2353,19 +2349,16 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F57" t="s">
-        <v>42</v>
-      </c>
-      <c r="I57" t="s">
-        <v>70</v>
-      </c>
-      <c r="J57" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J57" t="s">
+        <v>66</v>
+      </c>
+      <c r="K57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K57" t="s">
-        <v>86</v>
+      <c r="L57" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2402,22 +2395,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2428,9 +2421,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A2)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A2)</f>
         <v>15</v>
       </c>
-      <c r="C2" s="11">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A2)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A2)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A2)</f>
-        <v>9</v>
+      <c r="C2" s="11" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)</f>
+        <v>#REF!</v>
       </c>
       <c r="G2" s="11">
         <v>2</v>
@@ -2460,9 +2453,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A3)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A3)</f>
         <v>11</v>
       </c>
-      <c r="C3" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A3)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A3)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A3)</f>
-        <v>10</v>
+      <c r="C3" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)</f>
+        <v>#REF!</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -2492,9 +2485,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A4)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A4)</f>
         <v>11</v>
       </c>
-      <c r="C4" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A4)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A4)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A4)</f>
-        <v>8</v>
+      <c r="C4" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)</f>
+        <v>#REF!</v>
       </c>
       <c r="G4" s="3">
         <v>4</v>
@@ -2524,9 +2517,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A5)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A5)</f>
         <v>9</v>
       </c>
-      <c r="C5" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A5)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A5)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A5)</f>
-        <v>4</v>
+      <c r="C5" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A5)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A5)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A5)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2537,9 +2530,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A6)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A6)</f>
         <v>9</v>
       </c>
-      <c r="C6" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A6)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A6)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A6)</f>
-        <v>3</v>
+      <c r="C6" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2550,9 +2543,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
         <v>8</v>
       </c>
-      <c r="C7" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A7)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A7)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A7)</f>
-        <v>4</v>
+      <c r="C7" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2561,11 +2554,11 @@
       </c>
       <c r="B8" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A8)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A8)</f>
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A8)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A8)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A8)</f>
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A8)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A8)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A8)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2576,9 +2569,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
         <v>4</v>
       </c>
-      <c r="C9" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A9)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A9)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A9)</f>
-        <v>0</v>
+      <c r="C9" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A9)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A9)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A9)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2589,9 +2582,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
         <v>4</v>
       </c>
-      <c r="C10" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A10)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A10)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A10)</f>
-        <v>12</v>
+      <c r="C10" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A10)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A10)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A10)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2602,9 +2595,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A11)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A11)</f>
         <v>3</v>
       </c>
-      <c r="C11" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A11)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A11)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A11)</f>
-        <v>0</v>
+      <c r="C11" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A11)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A11)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A11)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2615,22 +2608,22 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A12)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A12)</f>
         <v>2</v>
       </c>
-      <c r="C12" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A12)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A12)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A12)</f>
-        <v>1</v>
+      <c r="C12" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A13)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A13)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A13)</f>
-        <v>0</v>
+      <c r="C13" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A13)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A13)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A13)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2641,9 +2634,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A14)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A14)</f>
         <v>3</v>
       </c>
-      <c r="C14" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A14)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A14)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A14)</f>
-        <v>0</v>
+      <c r="C14" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A14)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A14)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A14)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2654,9 +2647,9 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A15)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A15)</f>
         <v>6</v>
       </c>
-      <c r="C15" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A15)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A15)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A15)</f>
-        <v>3</v>
+      <c r="C15" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2667,22 +2660,22 @@
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A16)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A16)</f>
         <v>3</v>
       </c>
-      <c r="C16" s="3">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A16)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A16)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A16)</f>
-        <v>2</v>
+      <c r="C16" s="3" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A16)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A16)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A16)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>
         <v>1</v>
       </c>
-      <c r="C17" s="13">
-        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A17)+SUMIFS(Deck!B:B,Deck!G:G,Stats!A17)+SUMIFS(Deck!B:B,Deck!H:H,Stats!A17)</f>
-        <v>1</v>
+      <c r="C17" s="13" t="e">
+        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A17)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A17)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A17)</f>
+        <v>#REF!</v>
       </c>
       <c r="D17" s="12"/>
     </row>

</xml_diff>

<commit_message>
Another balance pass. More VPs overall, too!
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="186">
   <si>
     <t>Type</t>
   </si>
@@ -98,24 +98,9 @@
     <t>Grain</t>
   </si>
   <si>
-    <t>The Easily-Disrupted Payoff</t>
-  </si>
-  <si>
     <t>This card favors those who have this deck memorized.</t>
   </si>
   <si>
-    <t>The only thing better than VPs are VPs that spawned from the production of other VPs.</t>
-  </si>
-  <si>
-    <t>Was it really worth it??</t>
-  </si>
-  <si>
-    <t>The Suboptimal Strategy Payoff</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
@@ -125,12 +110,6 @@
     <t>Wild Boar</t>
   </si>
   <si>
-    <t>The Low-Risk Payoff</t>
-  </si>
-  <si>
-    <t>The High-Risk Payoff</t>
-  </si>
-  <si>
     <t>Hey, at least you know nobody else is going for it.</t>
   </si>
   <si>
@@ -155,12 +134,6 @@
     <t>You do not need to pay any required Stone for Buildings.</t>
   </si>
   <si>
-    <t>2 VPs for each Payoff you have placed.</t>
-  </si>
-  <si>
-    <t>2 VP for each Military, +2 additional VP if you end the game with the most military (ties don't count).</t>
-  </si>
-  <si>
     <t>The Clay Building Building</t>
   </si>
   <si>
@@ -182,24 +155,15 @@
     <t>Seems like a lot now, but we have an epic endgame coming up.</t>
   </si>
   <si>
-    <t>I REALLY hope nobody notices that I played this.</t>
-  </si>
-  <si>
     <t>This is to make you feel better about having unused stuff.</t>
   </si>
   <si>
     <t>See! I told you that card would pay off.</t>
   </si>
   <si>
-    <t>1 VP for each Wood, Sheep, or Grain</t>
-  </si>
-  <si>
     <t>The Unexpected Payoff</t>
   </si>
   <si>
-    <t>2 VPs for each Cattle, Vegetable</t>
-  </si>
-  <si>
     <t>Aggression does have its benefits.</t>
   </si>
   <si>
@@ -215,18 +179,12 @@
     <t>Go ahead and take your next turn, this is gonna take me a moment.</t>
   </si>
   <si>
-    <t>2 VP for each Building you've played</t>
-  </si>
-  <si>
     <t>The Grain Engine</t>
   </si>
   <si>
     <t>Playing this has the hidden advantage of making your opponents hate you.</t>
   </si>
   <si>
-    <t>The Expensive Engine</t>
-  </si>
-  <si>
     <t>Free Food!</t>
   </si>
   <si>
@@ -236,9 +194,6 @@
     <t>More Veggies!</t>
   </si>
   <si>
-    <t>You may also use this card for 2 Food</t>
-  </si>
-  <si>
     <t>More Grain!</t>
   </si>
   <si>
@@ -263,24 +218,15 @@
     <t>You had to see this one coming.</t>
   </si>
   <si>
-    <t>The Dude</t>
-  </si>
-  <si>
     <t>The Wildcard Resource</t>
   </si>
   <si>
     <t>Everyone just calls them pigs.</t>
   </si>
   <si>
-    <t>Give one to each player. To trash this card, you must trash 3 Food.</t>
-  </si>
-  <si>
     <t>The Cattle Engine</t>
   </si>
   <si>
-    <t>Wish this had come out sooner…</t>
-  </si>
-  <si>
     <t>The Artificial Need</t>
   </si>
   <si>
@@ -296,18 +242,12 @@
     <t>Don't base your entire strategy on this card.</t>
   </si>
   <si>
-    <t>One move of the dude is a four-point swing. Don't ever forget about him.</t>
-  </si>
-  <si>
     <t>Sheep: the rabbits of farm animals.</t>
   </si>
   <si>
     <t>I won't tell you how we got this cow to breed by itself.</t>
   </si>
   <si>
-    <t>You may substitute 1 Silk for any 1 Resource, any number of times.</t>
-  </si>
-  <si>
     <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
   </si>
   <si>
@@ -317,18 +257,12 @@
     <t>Does nothing now, but it will pay off later. The engine can wait.</t>
   </si>
   <si>
-    <t>The Obligatory 3:1 Trader</t>
-  </si>
-  <si>
     <t xml:space="preserve">This is a garden, not some sort of weird patch that passively injects beta-Carotene into your skin. </t>
   </si>
   <si>
     <t>Grain: the best breeder of them all.</t>
   </si>
   <si>
-    <t xml:space="preserve">You may use 1 Cattle for 2 Food, or 1 Cattle for any other Resource. </t>
-  </si>
-  <si>
     <t>I'm pretty sure this strategy worked for me at least once.</t>
   </si>
   <si>
@@ -347,15 +281,9 @@
     <t>Be sure to take this from someone who has collected silk.</t>
   </si>
   <si>
-    <t>Don't get all your VPs too early now.</t>
-  </si>
-  <si>
     <t>Just when you think you've pulled ahead, someone else will get a bigger building than this.</t>
   </si>
   <si>
-    <t>Nice! Way to get some bigger points on the board.</t>
-  </si>
-  <si>
     <t>Nice! Way to get some points on the board.</t>
   </si>
   <si>
@@ -368,9 +296,6 @@
     <t>The Investment Payoff</t>
   </si>
   <si>
-    <t>There are cards that use this. Don't worry.</t>
-  </si>
-  <si>
     <t>This strategy worked for me once. I think.</t>
   </si>
   <si>
@@ -395,9 +320,6 @@
     <t>The Inherently Valuable Resource</t>
   </si>
   <si>
-    <t>8 VPs  if you have Starting Player at the end of the game. Once you play this card, you may not steal Starting Player.</t>
-  </si>
-  <si>
     <t>Engine</t>
   </si>
   <si>
@@ -416,15 +338,9 @@
     <t>Even More Veggies!</t>
   </si>
   <si>
-    <t>When played, place in front of the player to your left. Subsequent players may trash 1 Food to continue passing, or trash 2 food to remove this card from the game.</t>
-  </si>
-  <si>
     <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count. You may only play this if you already have at least 1 Military.</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
     <t>Go First!</t>
   </si>
   <si>
@@ -449,9 +365,6 @@
     <t>The Early Investment</t>
   </si>
   <si>
-    <t>You may use 1 Grain for any 1 Resource, or 1 Grain for 2 Food, any number of times.</t>
-  </si>
-  <si>
     <t>The Reaction to Military Strategy</t>
   </si>
   <si>
@@ -461,12 +374,6 @@
     <t>If this card is available, somebody better take this.</t>
   </si>
   <si>
-    <t>You may retrieve any Resource, Early Game, or Midgame card in the discard pile and play it immediately without prerequisites.</t>
-  </si>
-  <si>
-    <t>Starter</t>
-  </si>
-  <si>
     <t>You must play this card before playing an Engine.</t>
   </si>
   <si>
@@ -503,12 +410,6 @@
     <t>The Premium Material</t>
   </si>
   <si>
-    <t>The Better Material Combo</t>
-  </si>
-  <si>
-    <t>The Decent Material Combo</t>
-  </si>
-  <si>
     <t>Other players may transfer this card to their playing area for 1 of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
   </si>
   <si>
@@ -521,39 +422,21 @@
     <t>You may substitute 1 Gold for any 1 Resource.</t>
   </si>
   <si>
-    <t>You may use 1 Resource for 1 other Resource, once per turn.</t>
-  </si>
-  <si>
     <t>First!</t>
   </si>
   <si>
-    <t>You may substitute 3 Resources of any type(s) for 1 of any Resource.</t>
-  </si>
-  <si>
     <t>Trash1</t>
   </si>
   <si>
     <t>Trash2</t>
   </si>
   <si>
-    <t>The Better Building</t>
-  </si>
-  <si>
-    <t>The Decent Building</t>
-  </si>
-  <si>
     <t>The Cuddly Animal</t>
   </si>
   <si>
     <t>The Expensive Animal</t>
   </si>
   <si>
-    <t>1 VP for each type of Resource at the end of the game.</t>
-  </si>
-  <si>
-    <t>At game end, VPs are the number of Glass you have in your hand squared plus the number of Silks you have.</t>
-  </si>
-  <si>
     <t>The Multiplying Plant</t>
   </si>
   <si>
@@ -569,13 +452,127 @@
     <t>The Good Building</t>
   </si>
   <si>
-    <t>The Easy Material Combo</t>
-  </si>
-  <si>
-    <t>The Easy Building</t>
-  </si>
-  <si>
     <t>Carrot</t>
+  </si>
+  <si>
+    <t>To trash this card, you must trash 3 Food before Endgame.</t>
+  </si>
+  <si>
+    <t>You may use 1 Grain instead of any 1 Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>The Expensive Payoff</t>
+  </si>
+  <si>
+    <t>Reconcile</t>
+  </si>
+  <si>
+    <t>All players have their last chance to get rid of their Blockers.</t>
+  </si>
+  <si>
+    <t>Even though you knew it was coming, it still comes up too soon.</t>
+  </si>
+  <si>
+    <t>Pay Up!</t>
+  </si>
+  <si>
+    <t>3 VPs for each Cattle, Vegetable</t>
+  </si>
+  <si>
+    <t>Glad you didn't have to eat these!</t>
+  </si>
+  <si>
+    <t>Trash</t>
+  </si>
+  <si>
+    <t>The Great Material Combo</t>
+  </si>
+  <si>
+    <t>The Fine Material Combo</t>
+  </si>
+  <si>
+    <t>The Amazing Material Combo</t>
+  </si>
+  <si>
+    <t>The Amazing Building</t>
+  </si>
+  <si>
+    <t>The Great Building</t>
+  </si>
+  <si>
+    <t>The Fine Building</t>
+  </si>
+  <si>
+    <t>Good move. Not Great. But Good.</t>
+  </si>
+  <si>
+    <t>Don't get all your VPs out too early now. We've got an endgame.</t>
+  </si>
+  <si>
+    <t>4 VP for each Military, +2 additional VP if you end the game with the most military (ties don't count).</t>
+  </si>
+  <si>
+    <t>At game end, VPs are the number of Glass you have in your hand squared plus the number of Silks squared.</t>
+  </si>
+  <si>
+    <t>The Unused Resources Payoff</t>
+  </si>
+  <si>
+    <t>2 VP for each Wood, Sheep, or Grain</t>
+  </si>
+  <si>
+    <t>The Diversified Strategy Payoff</t>
+  </si>
+  <si>
+    <t>3 VP for one of each of: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Veggie.</t>
+  </si>
+  <si>
+    <t>3 VP for each Building you've played</t>
+  </si>
+  <si>
+    <t>4 VPs for each Payoff you have placed.</t>
+  </si>
+  <si>
+    <t>6VP if you have Invested plus 2VP for each Gold.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>The Military Commitment</t>
+  </si>
+  <si>
+    <t>You're in it now.</t>
+  </si>
+  <si>
+    <t>You may also Trash this card for 2 Food.</t>
+  </si>
+  <si>
+    <t>You may Trash 1 Silk for any 2 Resources, any number of times.</t>
+  </si>
+  <si>
+    <t>This card is as close at this game gets to Victory Point Points.</t>
+  </si>
+  <si>
+    <t>Upon playing, you may retrieve any card in the discard piles and play it immediately without prerequisites.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may trash 1 Cattle for 2 Food, and/or 1 Cattle for any Resource. </t>
+  </si>
+  <si>
+    <t>The Obligatory Trader</t>
+  </si>
+  <si>
+    <t>You may substitute 2 different Resources for 1 of any Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>Make it count. No pressure. Are you sure you that's a good enough use for this card?? There's probably a better move.</t>
+  </si>
+  <si>
+    <t>You may trash this card for any 2 Resources.</t>
+  </si>
+  <si>
+    <t>The One-and-Done Card</t>
   </si>
 </sst>
 </file>
@@ -986,13 +983,13 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1020,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>22</v>
@@ -1043,34 +1040,34 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1079,21 +1076,24 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -1102,99 +1102,105 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>114</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="K8" s="3">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1202,10 +1208,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1217,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1225,10 +1231,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1240,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1248,10 +1254,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1260,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1271,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1283,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1294,10 +1300,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1306,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1314,22 +1320,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1340,10 +1343,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K15" s="3">
         <v>0</v>
@@ -1360,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1369,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1380,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1389,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1400,22 +1403,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1426,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1435,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1446,19 +1449,19 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="J20" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1469,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1478,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1486,22 +1489,22 @@
         <v>6</v>
       </c>
       <c r="B22" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="K22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,50 +1515,50 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K23" s="3">
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="K24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L24" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -1567,76 +1570,76 @@
         <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="K25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E26" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="J26" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="K26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>96</v>
+        <v>177</v>
       </c>
       <c r="K27" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L27" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B28" s="3">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1648,88 +1651,88 @@
         <v>14</v>
       </c>
       <c r="K28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J29" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K29" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L29" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="H30" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" t="s">
         <v>42</v>
       </c>
-      <c r="J30" t="s">
-        <v>51</v>
-      </c>
       <c r="K30" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L30" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J31" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="K31" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L31" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,19 +1743,19 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>103</v>
+        <v>180</v>
       </c>
       <c r="K32" s="3">
         <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,17 +1766,17 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="D33" s="6"/>
       <c r="J33" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="K33" s="3">
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1784,39 +1787,39 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J34" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="K34" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L34" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" s="3">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
@@ -1828,13 +1831,13 @@
         <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="K35" s="3">
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1845,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>10</v>
@@ -1854,13 +1857,13 @@
         <v>10</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K36" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L36" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1871,22 +1874,22 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K37" s="3">
         <v>7</v>
       </c>
       <c r="L37" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1897,22 +1900,22 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>17</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K38" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L38" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1923,22 +1926,22 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>17</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K39" s="3">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="L39" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1949,22 +1952,22 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K40" s="3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="L40" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -1975,22 +1978,22 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K41" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L41" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2001,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
@@ -2016,7 +2019,7 @@
         <v>3</v>
       </c>
       <c r="L42" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2027,45 +2030,54 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="E43" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="J43" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="K43" s="3">
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="J44" t="s">
         <v>133</v>
       </c>
       <c r="K44" s="3">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="L44" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2073,28 +2085,31 @@
         <v>9</v>
       </c>
       <c r="B45" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="E45" t="s">
+        <v>36</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J45" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="K45" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L45" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2105,19 +2120,19 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>18</v>
       </c>
       <c r="J46" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="K46" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2128,48 +2143,39 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>185</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>13</v>
-      </c>
       <c r="J47" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="K47" s="3">
         <v>2</v>
       </c>
       <c r="L47" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="J48" t="s">
-        <v>46</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>32</v>
+        <v>150</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2180,25 +2186,22 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="16" t="s">
-        <v>130</v>
-      </c>
       <c r="J49" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L49" t="s">
-        <v>30</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2209,16 +2212,19 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>148</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="J50" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L50" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2229,19 +2235,19 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="K51" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2252,16 +2258,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>168</v>
       </c>
       <c r="J52" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L52" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -2272,13 +2278,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
-      </c>
-      <c r="K53" s="3">
-        <v>5</v>
+        <v>92</v>
+      </c>
+      <c r="J53" t="s">
+        <v>172</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="L53" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -2289,16 +2298,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="J54" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L54" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -2309,16 +2318,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J55" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L55" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -2329,16 +2338,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J56" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="L56" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -2349,16 +2358,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>52</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="J57" t="s">
+        <v>170</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L57" t="s">
         <v>66</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L57" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +2384,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,22 +2407,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2419,10 +2431,10 @@
       </c>
       <c r="B2" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A2)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A2)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="11" t="e">
-        <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)</f>
+        <f>SUMIFS(Deck!B:B,Deck!F:F,Stats!A2)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A2)</f>
         <v>#REF!</v>
       </c>
       <c r="G2" s="11">
@@ -2430,19 +2442,19 @@
       </c>
       <c r="H2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G2)</f>
-        <v>1.25</v>
+        <v>3.25</v>
       </c>
       <c r="I2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G2)</f>
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="J2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G2)</f>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="K2" s="7">
         <f>SUM(H2:J2)</f>
-        <v>7.75</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2451,7 +2463,7 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A3)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A3)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)</f>
@@ -2462,19 +2474,19 @@
       </c>
       <c r="H3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G3)</f>
-        <v>0.83333333333333337</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="I3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G3)</f>
-        <v>2.6666666666666665</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="J3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G3)</f>
-        <v>1.6666666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K4" si="0">SUM(H3:J3)</f>
-        <v>5.166666666666667</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2483,7 +2495,7 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A4)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A4)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)</f>
@@ -2494,19 +2506,19 @@
       </c>
       <c r="H4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G4)</f>
-        <v>0.625</v>
+        <v>1.625</v>
       </c>
       <c r="I4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G4)</f>
-        <v>2</v>
+        <v>2.125</v>
       </c>
       <c r="J4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G4)</f>
-        <v>1.25</v>
+        <v>1.125</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>3.875</v>
+        <v>4.875</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2537,11 +2549,11 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A7)</f>
@@ -2563,7 +2575,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
@@ -2576,7 +2588,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
@@ -2589,7 +2601,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A11)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A11)</f>
@@ -2606,7 +2618,7 @@
       </c>
       <c r="B12" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A12)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A12)</f>
@@ -2615,7 +2627,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
@@ -2628,7 +2640,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B14" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A14)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A14)</f>
@@ -2667,7 +2679,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>

</xml_diff>

<commit_message>
Combined bonuses into PreReq for better newline usage
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="187">
   <si>
     <t>Type</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Even More Veggies!</t>
   </si>
   <si>
-    <t>If you currently have the most military you may substitute any 1 Resource to play a card. Ties don't count. You may only play this if you already have at least 1 Military.</t>
-  </si>
-  <si>
     <t>Go First!</t>
   </si>
   <si>
@@ -573,6 +570,12 @@
   </si>
   <si>
     <t>The One-and-Done Card</t>
+  </si>
+  <si>
+    <t>Highest military may substitute any 1 Resource for any 1 Resource, once per turn. Ties don't count.</t>
+  </si>
+  <si>
+    <t>You know you want this one. Figure out how to spend it later.</t>
   </si>
 </sst>
 </file>
@@ -984,7 +987,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,10 +1020,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>22</v>
@@ -1040,7 +1043,7 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1056,10 +1059,10 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K2" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
         <v>98</v>
@@ -1082,7 +1085,7 @@
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
@@ -1105,7 +1108,7 @@
         <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -1122,19 +1125,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1151,13 +1154,13 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1168,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>17</v>
@@ -1180,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1194,7 +1197,7 @@
         <v>70</v>
       </c>
       <c r="J8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" s="3">
         <v>-8</v>
@@ -1211,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1234,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1257,7 +1260,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1277,7 +1280,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1300,7 +1303,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1323,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -1333,6 +1336,9 @@
       </c>
       <c r="K14" s="3">
         <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1363,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1383,7 +1389,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1403,7 +1409,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s">
         <v>30</v>
@@ -1412,7 +1418,7 @@
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
@@ -1429,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1438,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1449,19 +1455,19 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1472,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1498,13 +1504,13 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K22" s="3">
         <v>2</v>
       </c>
       <c r="L22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1535,13 +1541,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K24" s="3">
         <v>3</v>
@@ -1570,7 +1576,7 @@
         <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K25" s="3">
         <v>0</v>
@@ -1590,16 +1596,16 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K26" s="3">
         <v>0</v>
@@ -1616,13 +1622,13 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H27" s="16" t="s">
         <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K27" s="3">
         <v>4</v>
@@ -1749,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K32" s="3">
         <v>1</v>
@@ -1766,11 +1772,11 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="6"/>
       <c r="J33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K33" s="3">
         <v>1</v>
@@ -1802,7 +1808,7 @@
         <v>36</v>
       </c>
       <c r="J34" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="K34" s="3">
         <v>3</v>
@@ -1874,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>17</v>
@@ -1900,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>17</v>
@@ -1915,7 +1921,7 @@
         <v>9</v>
       </c>
       <c r="L38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1926,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>17</v>
@@ -1941,7 +1947,7 @@
         <v>11</v>
       </c>
       <c r="L39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1952,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>10</v>
@@ -2033,16 +2039,16 @@
         <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K43" s="3">
         <v>0</v>
@@ -2071,7 +2077,7 @@
         <v>36</v>
       </c>
       <c r="J44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K44" s="3">
         <v>2</v>
@@ -2088,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -2103,13 +2109,13 @@
         <v>36</v>
       </c>
       <c r="J45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K45" s="3">
         <v>4</v>
       </c>
       <c r="L45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2126,7 +2132,7 @@
         <v>18</v>
       </c>
       <c r="J46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K46" s="3">
         <v>0</v>
@@ -2143,39 +2149,39 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K47" s="3">
         <v>2</v>
       </c>
       <c r="L47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>151</v>
+      </c>
+      <c r="J48" t="s">
         <v>149</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
-      </c>
-      <c r="J48" t="s">
-        <v>150</v>
       </c>
       <c r="K48" s="3">
         <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2195,13 +2201,13 @@
         <v>15</v>
       </c>
       <c r="J49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2212,19 +2218,19 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J50" t="s">
+        <v>152</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L50" t="s">
         <v>153</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="L50" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2241,7 +2247,7 @@
         <v>18</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K51" s="3">
         <v>8</v>
@@ -2258,13 +2264,13 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="J52" t="s">
         <v>168</v>
       </c>
-      <c r="J52" t="s">
-        <v>169</v>
-      </c>
       <c r="K52" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L52" t="s">
         <v>46</v>
@@ -2281,10 +2287,10 @@
         <v>92</v>
       </c>
       <c r="J53" t="s">
+        <v>171</v>
+      </c>
+      <c r="K53" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="L53" t="s">
         <v>47</v>
@@ -2298,13 +2304,13 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
+        <v>165</v>
+      </c>
+      <c r="J54" t="s">
         <v>166</v>
       </c>
-      <c r="J54" t="s">
-        <v>167</v>
-      </c>
       <c r="K54" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L54" t="s">
         <v>31</v>
@@ -2321,10 +2327,10 @@
         <v>33</v>
       </c>
       <c r="J55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L55" t="s">
         <v>53</v>
@@ -2341,10 +2347,10 @@
         <v>37</v>
       </c>
       <c r="J56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L56" t="s">
         <v>49</v>
@@ -2364,10 +2370,10 @@
         <v>35</v>
       </c>
       <c r="J57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L57" t="s">
         <v>66</v>
@@ -2407,22 +2413,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2627,7 +2633,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>

</xml_diff>

<commit_message>
Lots of game balancing, VP inflation
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="175">
   <si>
     <t>Type</t>
   </si>
@@ -38,15 +38,9 @@
     <t>Resource</t>
   </si>
   <si>
-    <t>Early Game</t>
-  </si>
-  <si>
     <t>Endgame</t>
   </si>
   <si>
-    <t>Midgame</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>You may also use this card for 1 Food</t>
   </si>
   <si>
-    <t>More Veggies!</t>
-  </si>
-  <si>
     <t>More Grain!</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Or is it ore? Mountains? Rock? Definitely not clay.</t>
   </si>
   <si>
-    <t>Good for more narrow situations.</t>
-  </si>
-  <si>
     <t>Don't base your entire strategy on this card.</t>
   </si>
   <si>
@@ -299,9 +287,6 @@
     <t>This strategy worked for me once. I think.</t>
   </si>
   <si>
-    <t>What's better than one veggie? Two veggies and a VP.</t>
-  </si>
-  <si>
     <t>Kinda like the double-wood, only clay.</t>
   </si>
   <si>
@@ -323,9 +308,6 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>You may use 1 Animal for any 1 Resource, any number of times.</t>
-  </si>
-  <si>
     <t>The Premium Building</t>
   </si>
   <si>
@@ -335,9 +317,6 @@
     <t>Even More Grain!</t>
   </si>
   <si>
-    <t>Even More Veggies!</t>
-  </si>
-  <si>
     <t>Go First!</t>
   </si>
   <si>
@@ -362,13 +341,7 @@
     <t>The Early Investment</t>
   </si>
   <si>
-    <t>The Reaction to Military Strategy</t>
-  </si>
-  <si>
-    <t>If you currently have the most military you may substitute any 1 Resource for any 1 other Resource, once per turn. In the case of a tie, nobody gets the bonus. You may only own 1 Military Engine.</t>
-  </si>
-  <si>
-    <t>If this card is available, somebody better take this.</t>
+    <t>Starter</t>
   </si>
   <si>
     <t>You must play this card before playing an Engine.</t>
@@ -398,27 +371,12 @@
     <t>Or is it wheat? Or corn? Seeds?</t>
   </si>
   <si>
-    <t>Personally, I find grain to be much more filling than vegetables.</t>
-  </si>
-  <si>
     <t>You may trash this card for 1 Food.</t>
   </si>
   <si>
     <t>The Premium Material</t>
   </si>
   <si>
-    <t>Other players may transfer this card to their playing area for 1 of any of the following: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Vegetable, Food.</t>
-  </si>
-  <si>
-    <t>You may now build buildings. You may only take one of these into your hand per game.</t>
-  </si>
-  <si>
-    <t>If you currently have the most military you may substitute any 1 Resource to play a card. In case of tie, nobody gets the bonus.</t>
-  </si>
-  <si>
-    <t>You may substitute 1 Gold for any 1 Resource.</t>
-  </si>
-  <si>
     <t>First!</t>
   </si>
   <si>
@@ -455,84 +413,36 @@
     <t>To trash this card, you must trash 3 Food before Endgame.</t>
   </si>
   <si>
-    <t>You may use 1 Grain instead of any 1 Resource, any number of times.</t>
-  </si>
-  <si>
     <t>The Expensive Payoff</t>
   </si>
   <si>
-    <t>Reconcile</t>
-  </si>
-  <si>
-    <t>All players have their last chance to get rid of their Blockers.</t>
-  </si>
-  <si>
-    <t>Even though you knew it was coming, it still comes up too soon.</t>
-  </si>
-  <si>
-    <t>Pay Up!</t>
-  </si>
-  <si>
-    <t>3 VPs for each Cattle, Vegetable</t>
-  </si>
-  <si>
     <t>Glad you didn't have to eat these!</t>
   </si>
   <si>
     <t>Trash</t>
   </si>
   <si>
-    <t>The Great Material Combo</t>
-  </si>
-  <si>
-    <t>The Fine Material Combo</t>
-  </si>
-  <si>
-    <t>The Amazing Material Combo</t>
-  </si>
-  <si>
     <t>The Amazing Building</t>
   </si>
   <si>
     <t>The Great Building</t>
   </si>
   <si>
-    <t>The Fine Building</t>
-  </si>
-  <si>
     <t>Good move. Not Great. But Good.</t>
   </si>
   <si>
     <t>Don't get all your VPs out too early now. We've got an endgame.</t>
   </si>
   <si>
-    <t>4 VP for each Military, +2 additional VP if you end the game with the most military (ties don't count).</t>
-  </si>
-  <si>
-    <t>At game end, VPs are the number of Glass you have in your hand squared plus the number of Silks squared.</t>
-  </si>
-  <si>
     <t>The Unused Resources Payoff</t>
   </si>
   <si>
-    <t>2 VP for each Wood, Sheep, or Grain</t>
-  </si>
-  <si>
     <t>The Diversified Strategy Payoff</t>
   </si>
   <si>
-    <t>3 VP for one of each of: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Veggie.</t>
-  </si>
-  <si>
-    <t>3 VP for each Building you've played</t>
-  </si>
-  <si>
     <t>4 VPs for each Payoff you have placed.</t>
   </si>
   <si>
-    <t>6VP if you have Invested plus 2VP for each Gold.</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -545,9 +455,6 @@
     <t>You may also Trash this card for 2 Food.</t>
   </si>
   <si>
-    <t>You may Trash 1 Silk for any 2 Resources, any number of times.</t>
-  </si>
-  <si>
     <t>This card is as close at this game gets to Victory Point Points.</t>
   </si>
   <si>
@@ -572,10 +479,67 @@
     <t>The One-and-Done Card</t>
   </si>
   <si>
-    <t>Highest military may substitute any 1 Resource for any 1 Resource, once per turn. Ties don't count.</t>
-  </si>
-  <si>
-    <t>You know you want this one. Figure out how to spend it later.</t>
+    <t>Initiate Endgame!</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>You may now build buildings.</t>
+  </si>
+  <si>
+    <t>You may trash 1 Grain for any 1 Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>The Material Combo</t>
+  </si>
+  <si>
+    <t>The Combo Building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When this card is revealed, all Blockers must be paid by the end of the turn. Initiate Endgame. </t>
+  </si>
+  <si>
+    <t>1 VP for each Building you've played</t>
+  </si>
+  <si>
+    <t>8VP if you have Invested plus 3VP for each Gold.</t>
+  </si>
+  <si>
+    <t>Players may transfer this card to their tableau for 1 of any of: Stone, Clay, Silk, Boar, Glass, Gold, Cattle, Carrot, Food.</t>
+  </si>
+  <si>
+    <t>Personally, I find grain to be much more filling than carrots</t>
+  </si>
+  <si>
+    <t>Eat More Veggies!</t>
+  </si>
+  <si>
+    <t>6 VPs for each Cattle, Vegetable</t>
+  </si>
+  <si>
+    <t>5 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
+  </si>
+  <si>
+    <t>3 VP for each Wood, Sheep, or Grain</t>
+  </si>
+  <si>
+    <t>At game end, take the number of Glass and Silk you have. Square it for VPs.</t>
+  </si>
+  <si>
+    <t>5 VP for each Military, +3 additional VP if you end the game with the most military (ties don't count).</t>
+  </si>
+  <si>
+    <t>You may trash 1 Silk for any 2 Resources, any number of times.</t>
+  </si>
+  <si>
+    <t>You may trash 1 Gold for any 1 Resource.</t>
+  </si>
+  <si>
+    <t>You may trash 1 Animal for any 1 Resource, any number of times.</t>
+  </si>
+  <si>
+    <t>Highest Military may trash any 1 Resource for any 1 other Resource, once per turn. In a tie, nobody gets the bonus.</t>
   </si>
 </sst>
 </file>
@@ -983,16 +947,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1008,10 +972,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1020,16 +984,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -1043,167 +1007,167 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="K2" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
+        <v>52</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="K5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="K7" s="3">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="L7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" t="s">
-        <v>145</v>
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="3">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1211,22 +1175,22 @@
         <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K9" s="3">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1234,22 +1198,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1257,19 +1218,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
       </c>
       <c r="K11" s="3">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1277,22 +1241,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="K12" s="3">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1303,19 +1264,16 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K13" s="3">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1323,22 +1281,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
       <c r="K14" s="3">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>186</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1346,19 +1301,25 @@
         <v>6</v>
       </c>
       <c r="B15" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>110</v>
       </c>
       <c r="K15" s="3">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1369,16 +1330,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1389,16 +1350,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>130</v>
+      </c>
+      <c r="J17" t="s">
+        <v>118</v>
       </c>
       <c r="K17" s="3">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>60</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,25 +1370,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1435,948 +1393,850 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="J19" t="s">
+        <v>172</v>
       </c>
       <c r="K19" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
-      </c>
-      <c r="J20" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" t="s">
+        <v>109</v>
+      </c>
+      <c r="K21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="3">
+      <c r="L21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" s="3">
         <v>0</v>
       </c>
-      <c r="L21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3">
+      <c r="L22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" t="s">
+        <v>171</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22" s="3">
-        <v>2</v>
-      </c>
-      <c r="L22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="3">
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="3">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" t="s">
-        <v>118</v>
-      </c>
-      <c r="K24" s="3">
+      <c r="L25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="3">
         <v>3</v>
       </c>
-      <c r="L24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" t="s">
-        <v>128</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="L26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" s="3">
+        <v>3</v>
+      </c>
+      <c r="L27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J26" t="s">
-        <v>119</v>
-      </c>
-      <c r="K26" s="3">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" t="s">
-        <v>176</v>
-      </c>
-      <c r="K27" s="3">
-        <v>4</v>
-      </c>
-      <c r="L27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B28" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>14</v>
+        <v>149</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="J28" t="s">
+        <v>150</v>
       </c>
       <c r="K28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>13</v>
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="K29" s="3">
         <v>3</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>148</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" t="s">
+        <v>55</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="3">
+        <v>8</v>
+      </c>
+      <c r="L32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="3">
         <v>10</v>
       </c>
-      <c r="H30" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K30" s="3">
-        <v>3</v>
-      </c>
-      <c r="L30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" t="s">
-        <v>43</v>
-      </c>
-      <c r="K31" s="3">
-        <v>3</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="L33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" t="s">
-        <v>179</v>
-      </c>
-      <c r="K32" s="3">
-        <v>1</v>
-      </c>
-      <c r="L32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="J33" t="s">
-        <v>181</v>
-      </c>
-      <c r="K33" s="3">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>36</v>
+        <v>129</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" t="s">
-        <v>185</v>
+        <v>33</v>
       </c>
       <c r="K34" s="3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J35" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="K35" s="3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L35" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K36" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="L36" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K37" s="3">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="L37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="3">
+        <v>3</v>
+      </c>
+      <c r="L38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" t="s">
+        <v>145</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" t="s">
+        <v>174</v>
+      </c>
+      <c r="K40" s="3">
+        <v>2</v>
+      </c>
+      <c r="L40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>143</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K38" s="3">
-        <v>9</v>
-      </c>
-      <c r="L38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>158</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="16" t="s">
+      <c r="D41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>174</v>
+      </c>
+      <c r="K41" s="3">
+        <v>4</v>
+      </c>
+      <c r="L41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" t="s">
+        <v>147</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>152</v>
+      </c>
+      <c r="K43" s="3">
+        <v>2</v>
+      </c>
+      <c r="L43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K39" s="3">
+      <c r="J44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>159</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K40" s="3">
-        <v>13</v>
-      </c>
-      <c r="L40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K41" s="3">
-        <v>15</v>
-      </c>
-      <c r="L41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K42" s="3">
-        <v>3</v>
-      </c>
-      <c r="L42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43" t="s">
-        <v>144</v>
-      </c>
-      <c r="E43" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J43" t="s">
-        <v>175</v>
-      </c>
-      <c r="K43" s="3">
-        <v>0</v>
-      </c>
-      <c r="L43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="3">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J44" t="s">
-        <v>132</v>
-      </c>
-      <c r="K44" s="3">
-        <v>2</v>
-      </c>
-      <c r="L44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="J45" t="s">
-        <v>132</v>
-      </c>
-      <c r="K45" s="3">
-        <v>4</v>
+        <v>166</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="L45" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J46" t="s">
-        <v>178</v>
+        <v>16</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="K46" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L46" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>184</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="J47" t="s">
-        <v>183</v>
-      </c>
-      <c r="K47" s="3">
-        <v>2</v>
+        <v>167</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="L47" t="s">
-        <v>182</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="J48" t="s">
-        <v>149</v>
-      </c>
-      <c r="K48" s="3">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="L48" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="J49" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L49" t="s">
-        <v>177</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="J50" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L50" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="K51" s="3">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="J51" t="s">
+        <v>170</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="L51" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>50</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L52" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="J53" t="s">
-        <v>171</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="3">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>165</v>
-      </c>
-      <c r="J54" t="s">
-        <v>166</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>8</v>
-      </c>
-      <c r="B55" s="3">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" t="s">
-        <v>164</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="3">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>37</v>
-      </c>
-      <c r="J56" t="s">
-        <v>163</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>52</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J57" t="s">
-        <v>169</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L57" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2390,7 +2250,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,30 +2270,30 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A2)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A2)</f>
@@ -2448,28 +2308,28 @@
       </c>
       <c r="H2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G2)</f>
-        <v>3.25</v>
+        <v>0</v>
       </c>
       <c r="I2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G2)</f>
-        <v>4.25</v>
+        <v>0</v>
       </c>
       <c r="J2" s="11">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G2)</f>
-        <v>2.25</v>
+        <v>0.25</v>
       </c>
       <c r="K2" s="7">
         <f>SUM(H2:J2)</f>
-        <v>9.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A3)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A3)</f>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A3)</f>
@@ -2480,28 +2340,28 @@
       </c>
       <c r="H3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G3)</f>
-        <v>2.1666666666666665</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G3)</f>
-        <v>2.8333333333333335</v>
+        <v>0</v>
       </c>
       <c r="J3" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G3)</f>
-        <v>1.5</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K4" si="0">SUM(H3:J3)</f>
-        <v>6.5</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A4)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A4)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A4)</f>
@@ -2512,24 +2372,24 @@
       </c>
       <c r="H4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Early Game")/(2*G4)</f>
-        <v>1.625</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Midgame")/(2*G4)</f>
-        <v>2.125</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!A:A,"Endgame")/(2*G4)</f>
-        <v>1.125</v>
+        <v>0.125</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>4.875</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A5)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A5)</f>
@@ -2542,11 +2402,11 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A6)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A6)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A6)</f>
@@ -2555,7 +2415,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A7)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A7)</f>
@@ -2568,7 +2428,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A8)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A8)</f>
@@ -2581,7 +2441,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A9)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A9)</f>
@@ -2594,7 +2454,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A10)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A10)</f>
@@ -2607,7 +2467,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A11)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A11)</f>
@@ -2620,7 +2480,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A12)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A12)</f>
@@ -2633,7 +2493,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B13" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A13)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A13)</f>
@@ -2646,7 +2506,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A14)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A14)</f>
@@ -2659,11 +2519,11 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A15)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A15)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="e">
         <f>SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)+SUMIFS(Deck!B:B,Deck!#REF!,Stats!A15)</f>
@@ -2672,7 +2532,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A16)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A16)</f>
@@ -2685,7 +2545,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" s="10">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Stats!A17)+SUMIFS(Deck!B:B,Deck!E:E,Stats!A17)</f>

</xml_diff>

<commit_message>
Tons more analysis and balancing
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -9,13 +9,17 @@
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
     <sheet name="Economy" sheetId="2" r:id="rId2"/>
+    <sheet name="Scenarios" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Cards" localSheetId="0">Deck!$C$2:$C$55</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="208">
   <si>
     <t>Type</t>
   </si>
@@ -134,9 +138,6 @@
     <t>The Military Building</t>
   </si>
   <si>
-    <t>Seems like a lot now, but we have an epic endgame coming up.</t>
-  </si>
-  <si>
     <t>This is to make you feel better about having unused stuff.</t>
   </si>
   <si>
@@ -179,9 +180,6 @@
     <t>Moo.</t>
   </si>
   <si>
-    <t>It's a safe bet that you'll find this useful.</t>
-  </si>
-  <si>
     <t>Food is how we keep you from making powerful moves. You're welcome.</t>
   </si>
   <si>
@@ -212,9 +210,6 @@
     <t>Blocker</t>
   </si>
   <si>
-    <t>Or is it ore? Mountains? Rock? Definitely not clay.</t>
-  </si>
-  <si>
     <t>Don't base your entire strategy on this card.</t>
   </si>
   <si>
@@ -227,9 +222,6 @@
     <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
   </si>
   <si>
-    <t>Plus, you don't have to think about how to make your food!</t>
-  </si>
-  <si>
     <t>Does nothing now, but it will pay off later. The engine can wait.</t>
   </si>
   <si>
@@ -242,9 +234,6 @@
     <t>I'm pretty sure this strategy worked for me at least once.</t>
   </si>
   <si>
-    <t>It is by pure coincidence that we actually need stone for our building.</t>
-  </si>
-  <si>
     <t>It is by pure coincidence that we actually need Wood for our building.</t>
   </si>
   <si>
@@ -275,9 +264,6 @@
     <t>This strategy worked for me once. I think.</t>
   </si>
   <si>
-    <t>Kinda like the double-wood, only clay.</t>
-  </si>
-  <si>
     <t>The Coveted Starting Player</t>
   </si>
   <si>
@@ -287,9 +273,6 @@
     <t>Because just going around in a circle is not strategic enough.</t>
   </si>
   <si>
-    <t>Cheap. Abundant. Necessary.</t>
-  </si>
-  <si>
     <t>The Inherently Valuable Resource</t>
   </si>
   <si>
@@ -476,9 +459,6 @@
     <t>Eat More Veggies!</t>
   </si>
   <si>
-    <t>6 VPs for each Cattle, Vegetable</t>
-  </si>
-  <si>
     <t>5 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
   </si>
   <si>
@@ -549,6 +529,120 @@
   </si>
   <si>
     <t>3 VP for each Military, +3 additional VP if you end the game with the most military (ties don't count).</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Action Cost</t>
+  </si>
+  <si>
+    <t>VPs</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>VPs/Action Overall</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>No cost with the chain run</t>
+  </si>
+  <si>
+    <t>Take it and play it.</t>
+  </si>
+  <si>
+    <t>Take the resource</t>
+  </si>
+  <si>
+    <t>Also no play cost. Have four grain at this point.</t>
+  </si>
+  <si>
+    <t>No cost play on the chain run</t>
+  </si>
+  <si>
+    <t>4xGrain, 4xSheep</t>
+  </si>
+  <si>
+    <t>Pay the stone</t>
+  </si>
+  <si>
+    <t>Military Strategy</t>
+  </si>
+  <si>
+    <t>Resource Collection Strategy, Lots of Chaining</t>
+  </si>
+  <si>
+    <t>No need to pay</t>
+  </si>
+  <si>
+    <t>Building Strategy, Not much chaining</t>
+  </si>
+  <si>
+    <t>Use military</t>
+  </si>
+  <si>
+    <t>The Payoff with Math</t>
+  </si>
+  <si>
+    <t>Grain, Sheep,Glass, Carrot,Silk</t>
+  </si>
+  <si>
+    <t>(2xGlass + 1xSilk)^2</t>
+  </si>
+  <si>
+    <t>Get 2xClay</t>
+  </si>
+  <si>
+    <t>Pay 2xClay</t>
+  </si>
+  <si>
+    <t>Pay 1xClay, no stone</t>
+  </si>
+  <si>
+    <t>1xMilitary</t>
+  </si>
+  <si>
+    <t>2xMilitary</t>
+  </si>
+  <si>
+    <t>This has an efficient sequence, but it's easily disrupted.</t>
+  </si>
+  <si>
+    <t>6 VPs for each Cattle, Carrot</t>
+  </si>
+  <si>
+    <t>The Strange Combo</t>
+  </si>
+  <si>
+    <t>Not to be confused with wood grain. Also, shouldn't wood be a plant? No. No it's not. Ever.</t>
+  </si>
+  <si>
+    <t>Cheap. Abundant. Necessary. Ubiquitous both in games and throughout games.</t>
+  </si>
+  <si>
+    <t>Or is it brick? Pottery? Ok fine, let's just call it the red one.</t>
+  </si>
+  <si>
+    <t>Or is it ore? Mountains? Rock? Definitely not clay, unless we allow fossilization.</t>
+  </si>
+  <si>
+    <t>It's a safe bet that you'll find this one useful.</t>
+  </si>
+  <si>
+    <t>Side benefit: easier planning! You don't have to think about how to make your food now!</t>
+  </si>
+  <si>
+    <t>It is by pure coincidence that we actually need Stone for our building.</t>
+  </si>
+  <si>
+    <t>Seems like a lot now, but this won't win you the game alone.</t>
+  </si>
+  <si>
+    <t>You didn't forget about food, did you?</t>
   </si>
 </sst>
 </file>
@@ -579,7 +673,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,8 +698,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -651,14 +751,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -732,11 +906,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
+    <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1036,11 +1260,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38:G38"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1277,7 @@
     <col min="6" max="9" width="10.140625" style="13" customWidth="1"/>
     <col min="10" max="10" width="62.7109375" customWidth="1"/>
     <col min="11" max="11" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="79.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="79.7109375" customWidth="1"/>
     <col min="13" max="13" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="3"/>
@@ -1076,10 +1300,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>19</v>
@@ -1097,40 +1321,40 @@
         <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K2" s="5">
         <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="33"/>
@@ -1138,7 +1362,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1153,18 +1377,30 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K3" s="3">
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="M3" s="35">
+        <f>IF(F3&lt;&gt;"",VLOOKUP(F3,Economy!A$2:I$13,9,FALSE),0)+IF(G3&lt;&gt;"",VLOOKUP(G3,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>1.7179619625911169</v>
+      </c>
+      <c r="N3" s="35">
+        <f>2 + M3 + IF(H3="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>3.7179619625911169</v>
+      </c>
+      <c r="O3" s="36">
+        <f t="shared" ref="O3:O5" si="0">IF(ISNUMBER(K3/N3), K3/N3,"")</f>
+        <v>0.53792911818983824</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1176,79 +1412,115 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="K4" s="3">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="M4" s="35">
+        <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:I$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="35">
+        <f>2 + M4 + IF(H4="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="O4" s="36">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="M5" s="35">
+        <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:I$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>1.5604754635042337</v>
+      </c>
+      <c r="N5" s="35">
+        <f>2 + M5 + IF(H5="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>3.5604754635042335</v>
+      </c>
+      <c r="O5" s="36">
+        <f t="shared" si="0"/>
+        <v>0.5617227307140582</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="K6" s="3">
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>102</v>
+        <v>95</v>
+      </c>
+      <c r="M6" s="35">
+        <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:I$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>1.6307255270620018</v>
+      </c>
+      <c r="N6" s="35">
+        <f>2 + M6 + IF(H6="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>3.630725527062002</v>
+      </c>
+      <c r="O6" s="36">
+        <f t="shared" ref="O6" si="1">IF(ISNUMBER(K6/N6), K6/N6,"")</f>
+        <v>0.55085408827871607</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K7" s="3">
         <v>-8</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1259,7 +1531,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>8</v>
@@ -1270,11 +1542,13 @@
       <c r="K8" s="27">
         <v>0</v>
       </c>
-      <c r="L8" s="26" t="s">
-        <v>90</v>
+      <c r="L8" s="60" t="s">
+        <v>200</v>
       </c>
       <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
+      <c r="N8" s="28">
+        <v>1</v>
+      </c>
       <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1285,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>14</v>
@@ -1296,11 +1570,13 @@
       <c r="K9" s="27">
         <v>0</v>
       </c>
-      <c r="L9" s="26" t="s">
-        <v>86</v>
+      <c r="L9" s="60" t="s">
+        <v>201</v>
       </c>
       <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="N9" s="28">
+        <v>1</v>
+      </c>
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1311,7 +1587,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>11</v>
@@ -1319,11 +1595,13 @@
       <c r="K10" s="27">
         <v>0</v>
       </c>
-      <c r="L10" s="26" t="s">
-        <v>65</v>
+      <c r="L10" s="60" t="s">
+        <v>202</v>
       </c>
       <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
+      <c r="N10" s="28">
+        <v>1</v>
+      </c>
       <c r="O10" s="27"/>
     </row>
     <row r="11" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1334,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>14</v>
@@ -1345,11 +1623,13 @@
       <c r="K11" s="27">
         <v>0</v>
       </c>
-      <c r="L11" s="26" t="s">
-        <v>54</v>
+      <c r="L11" s="60" t="s">
+        <v>203</v>
       </c>
       <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="N11" s="28">
+        <v>1</v>
+      </c>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1360,7 +1640,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>26</v>
@@ -1372,7 +1652,9 @@
         <v>17</v>
       </c>
       <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="N12" s="28">
+        <v>1</v>
+      </c>
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1383,7 +1665,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>12</v>
@@ -1392,10 +1674,12 @@
         <v>0</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="N13" s="28">
+        <v>1</v>
+      </c>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1406,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>13</v>
@@ -1414,11 +1698,13 @@
       <c r="K14" s="27">
         <v>0</v>
       </c>
-      <c r="L14" s="26" t="s">
-        <v>53</v>
+      <c r="L14" s="60" t="s">
+        <v>52</v>
       </c>
       <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="N14" s="28">
+        <v>1</v>
+      </c>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1429,7 +1715,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>27</v>
@@ -1438,16 +1724,18 @@
         <v>27</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K15" s="27">
         <v>0</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="N15" s="28">
+        <v>1</v>
+      </c>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1458,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>23</v>
@@ -1467,33 +1755,35 @@
         <v>0</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="N16" s="28">
+        <v>1</v>
+      </c>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="60" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="27">
-        <v>2</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>108</v>
+        <v>1</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>23</v>
       </c>
       <c r="K17" s="27">
         <v>0</v>
       </c>
-      <c r="L17" s="26" t="s">
-        <v>151</v>
+      <c r="L17" s="60" t="s">
+        <v>199</v>
       </c>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
@@ -1504,22 +1794,27 @@
         <v>6</v>
       </c>
       <c r="B18" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>15</v>
+        <v>113</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="K18" s="27">
         <v>0</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="N18" s="28">
+        <v>1</v>
+      </c>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1530,25 +1825,24 @@
         <v>3</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="K19" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="N19" s="28">
+        <v>1</v>
+      </c>
       <c r="O19" s="27"/>
     </row>
-    <row r="20" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>6</v>
       </c>
@@ -1556,522 +1850,514 @@
         <v>3</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="D20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="K20" s="27">
+        <v>2</v>
+      </c>
+      <c r="L20" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28">
+        <v>1</v>
+      </c>
+      <c r="O20" s="27"/>
+    </row>
+    <row r="21" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="27">
+        <v>3</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="27">
-        <v>0</v>
-      </c>
-      <c r="L20" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="27"/>
-    </row>
-    <row r="21" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="23">
-        <v>1</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="K21" s="23">
+      <c r="K21" s="27">
+        <v>0</v>
+      </c>
+      <c r="L21" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28">
+        <v>1</v>
+      </c>
+      <c r="O21" s="27"/>
+    </row>
+    <row r="22" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="23">
+        <v>1</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="23">
         <v>3</v>
       </c>
-      <c r="L21" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="24">
-        <f>IF(F21&lt;&gt;"",VLOOKUP(F21,Economy!A$2:I$13,9,FALSE),0)+IF(G21&lt;&gt;"",VLOOKUP(G21,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="31">
-        <f>2 + M21 + IF(H21="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="O21" s="23">
-        <f t="shared" ref="O21:O54" si="0">IF(ISNUMBER(K21/N21), K21/N21,"")</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="23">
-        <v>2</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="K22" s="23">
-        <v>0</v>
-      </c>
       <c r="L22" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="M22" s="24">
         <f>IF(F22&lt;&gt;"",VLOOKUP(F22,Economy!A$2:I$13,9,FALSE),0)+IF(G22&lt;&gt;"",VLOOKUP(G22,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6423591511807047</v>
-      </c>
-      <c r="N22" s="31">
+        <v>0</v>
+      </c>
+      <c r="N22" s="24">
         <f>2 + M22 + IF(H22="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.6423591511807047</v>
+        <v>2</v>
       </c>
       <c r="O22" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="O22:O55" si="2">IF(ISNUMBER(K22/N22), K22/N22,"")</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B23" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="K23" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="M23" s="24">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,Economy!A$2:I$13,9,FALSE),0)+IF(G23&lt;&gt;"",VLOOKUP(G23,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="31">
+        <v>1.6307255270620018</v>
+      </c>
+      <c r="N23" s="24">
         <f>2 + M23 + IF(H23="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>5.8132281580905927</v>
+        <v>3.630725527062002</v>
       </c>
       <c r="O23" s="23">
-        <f t="shared" si="0"/>
-        <v>0.8601073042421743</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B24" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>12</v>
+        <v>99</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>148</v>
       </c>
       <c r="K24" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M24" s="24">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:I$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6423591511807047</v>
-      </c>
-      <c r="N24" s="31">
+        <v>0</v>
+      </c>
+      <c r="N24" s="24">
         <f>2 + M24 + IF(H24="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.6423591511807047</v>
+        <v>5.8153627635310006</v>
       </c>
       <c r="O24" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.85979159053597465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B25" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>160</v>
+        <v>43</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>12</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="K25" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="M25" s="24">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:I$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.7147012989212722</v>
-      </c>
-      <c r="N25" s="31">
+        <v>1.6464466094067263</v>
+      </c>
+      <c r="N25" s="24">
         <f>2 + M25 + IF(H25="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>7.5279294570118651</v>
+        <v>3.646446609406726</v>
       </c>
       <c r="O25" s="23">
-        <f t="shared" si="0"/>
-        <v>0.66419325905648152</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B26" s="23">
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H26" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26" s="23">
         <v>5</v>
       </c>
-      <c r="L26" s="22" t="s">
-        <v>76</v>
+      <c r="L26" s="61" t="s">
+        <v>205</v>
       </c>
       <c r="M26" s="24">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:I$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.5686689071862463</v>
-      </c>
-      <c r="N26" s="31">
+        <v>1.7179619625911169</v>
+      </c>
+      <c r="N26" s="24">
         <f>2 + M26 + IF(H26="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>7.3818970652768385</v>
+        <v>7.5333247261221175</v>
       </c>
       <c r="O26" s="23">
-        <f t="shared" si="0"/>
-        <v>0.67733266337715969</v>
+        <f t="shared" si="2"/>
+        <v>0.66371757248991159</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B27" s="23">
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H27" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K27" s="23">
         <v>5</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M27" s="24">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:I$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6264563161811858</v>
-      </c>
-      <c r="N27" s="31">
+        <v>1.5604754635042337</v>
+      </c>
+      <c r="N27" s="24">
         <f>2 + M27 + IF(H27="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>7.4396844742717789</v>
+        <v>7.375838227035235</v>
       </c>
       <c r="O27" s="23">
-        <f t="shared" si="0"/>
-        <v>0.6720715128835375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.67788905424648693</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B28" s="23">
         <v>1</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="25"/>
+        <v>154</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="J28" s="22" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="K28" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="M28" s="24">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:I$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="31">
+        <v>1.6307255270620018</v>
+      </c>
+      <c r="N28" s="24">
         <f>2 + M28 + IF(H28="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>2</v>
+        <v>7.4460882905930035</v>
       </c>
       <c r="O28" s="23">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.67149351510063848</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B29" s="23">
         <v>1</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>33</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D29" s="25"/>
       <c r="J29" s="22" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="K29" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="M29" s="24">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:I$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:I$13,9,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="N29" s="31">
+      <c r="N29" s="24">
         <f>2 + M29 + IF(H29="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>5.8132281580905927</v>
+        <v>2</v>
       </c>
       <c r="O29" s="23">
-        <f t="shared" si="0"/>
-        <v>0.8601073042421743</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" s="30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="29" t="s">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="23">
+        <v>1</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K30" s="23">
+        <v>5</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="M30" s="24">
+        <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:I$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="24">
+        <f>2 + M30 + IF(H30="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>5.8153627635310006</v>
+      </c>
+      <c r="O30" s="23">
+        <f t="shared" si="2"/>
+        <v>0.85979159053597465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="30">
+        <v>1</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J30" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="K30" s="30">
+      <c r="J31" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K31" s="30">
         <v>6</v>
       </c>
-      <c r="L30" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" s="31">
-        <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:I$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.7147012989212722</v>
-      </c>
-      <c r="N30" s="31">
-        <f>2 + M30 + IF(H30="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.7147012989212724</v>
-      </c>
-      <c r="O30" s="30">
-        <f t="shared" si="0"/>
-        <v>1.6152038931750354</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="30">
-        <v>1</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="30">
-        <v>0</v>
+      <c r="L31" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="M31" s="31">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:I$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6423591511807047</v>
+        <v>1.7179619625911169</v>
       </c>
       <c r="N31" s="31">
         <f>2 + M31 + IF(H31="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.6423591511807047</v>
+        <v>3.7179619625911169</v>
       </c>
       <c r="O31" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.6137873545695149</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
-        <v>144</v>
+      <c r="A32" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="B32" s="30">
-        <v>2</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>12</v>
       </c>
       <c r="K32" s="30">
         <v>0</v>
-      </c>
-      <c r="L32" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="M32" s="31">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:I$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6423591511807047</v>
+        <v>1.6464466094067263</v>
       </c>
       <c r="N32" s="31">
         <f>2 + M32 + IF(H32="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.6423591511807047</v>
+        <v>3.646446609406726</v>
       </c>
       <c r="O32" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B33" s="30">
         <v>2</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="J33" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="K33" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L33" s="29" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="M33" s="31">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:I$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.1373378143724926</v>
+        <v>1.6307255270620018</v>
       </c>
       <c r="N33" s="31">
         <f>2 + M33 + IF(H33="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>8.9505659724630853</v>
+        <v>3.630725527062002</v>
       </c>
       <c r="O33" s="30">
-        <f t="shared" si="0"/>
-        <v>1.1172477841921458</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B34" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G34" s="29" t="s">
         <v>8</v>
@@ -2080,111 +2366,111 @@
         <v>32</v>
       </c>
       <c r="K34" s="30">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M34" s="31">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:I$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.1951252233674321</v>
+        <v>3.1209509270084674</v>
       </c>
       <c r="N34" s="31">
         <f>2 + M34 + IF(H34="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>9.0083533814580257</v>
+        <v>8.9363136905394676</v>
       </c>
       <c r="O34" s="30">
-        <f t="shared" si="0"/>
-        <v>1.3320969428996543</v>
+        <f t="shared" si="2"/>
+        <v>1.0071266868717863</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B35" s="30">
         <v>1</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H35" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K35" s="30">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="M35" s="31">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:I$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.2529126323623716</v>
+        <v>3.1912009905662355</v>
       </c>
       <c r="N35" s="31">
         <f>2 + M35 + IF(H35="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>9.0661407904529643</v>
+        <v>9.0065637540972361</v>
       </c>
       <c r="O35" s="30">
-        <f t="shared" si="0"/>
-        <v>1.433906697510098</v>
+        <f t="shared" si="2"/>
+        <v>1.1103013616542527</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B36" s="30">
         <v>1</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>32</v>
       </c>
       <c r="K36" s="30">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M36" s="31">
         <f>IF(F36&lt;&gt;"",VLOOKUP(F36,Economy!A$2:I$13,9,FALSE),0)+IF(G36&lt;&gt;"",VLOOKUP(G36,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.3411576151024578</v>
+        <v>3.2614510541240036</v>
       </c>
       <c r="N36" s="31">
         <f>2 + M36 + IF(H36="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>9.1543857731930505</v>
+        <v>9.0768138176550046</v>
       </c>
       <c r="O36" s="30">
-        <f t="shared" si="0"/>
-        <v>1.5293216111775021</v>
+        <f t="shared" si="2"/>
+        <v>1.2118789942131754</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B37" s="30">
         <v>1</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="F37" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="32" t="s">
         <v>8</v>
       </c>
       <c r="G37" s="29" t="s">
@@ -2194,36 +2480,36 @@
         <v>32</v>
       </c>
       <c r="K37" s="30">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="M37" s="31">
         <f>IF(F37&lt;&gt;"",VLOOKUP(F37,Economy!A$2:I$13,9,FALSE),0)+IF(G37&lt;&gt;"",VLOOKUP(G37,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.2833702061075183</v>
+        <v>3.2784374260953504</v>
       </c>
       <c r="N37" s="31">
         <f>2 + M37 + IF(H37="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>9.0965983641981119</v>
+        <v>9.0938001896263518</v>
       </c>
       <c r="O37" s="30">
-        <f t="shared" si="0"/>
-        <v>1.648968042717613</v>
+        <f t="shared" si="2"/>
+        <v>1.3195803459250031</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B38" s="30">
         <v>1</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>11</v>
+      <c r="C38" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>14</v>
       </c>
       <c r="G38" s="29" t="s">
         <v>11</v>
@@ -2232,476 +2518,479 @@
         <v>32</v>
       </c>
       <c r="K38" s="30">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="M38" s="31">
         <f>IF(F38&lt;&gt;"",VLOOKUP(F38,Economy!A$2:I$13,9,FALSE),0)+IF(G38&lt;&gt;"",VLOOKUP(G38,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.4294025978425444</v>
+        <v>3.3486874896531189</v>
       </c>
       <c r="N38" s="31">
         <f>2 + M38 + IF(H38="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>9.2426307559331384</v>
+        <v>9.1640502531841204</v>
       </c>
       <c r="O38" s="30">
-        <f t="shared" si="0"/>
-        <v>1.7311088609408194</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.4185867210279701</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B39" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="K39" s="30">
-        <v>4</v>
-      </c>
-      <c r="L39" s="29" t="s">
-        <v>68</v>
+        <v>14</v>
+      </c>
+      <c r="L39" s="32" t="s">
+        <v>206</v>
       </c>
       <c r="M39" s="31">
         <f>IF(F39&lt;&gt;"",VLOOKUP(F39,Economy!A$2:I$13,9,FALSE),0)+IF(G39&lt;&gt;"",VLOOKUP(G39,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.7147012989212722</v>
+        <v>3.4359239251822338</v>
       </c>
       <c r="N39" s="31">
         <f>2 + M39 + IF(H39="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.7147012989212724</v>
+        <v>9.2512866887132343</v>
       </c>
       <c r="O39" s="30">
-        <f t="shared" si="0"/>
-        <v>1.0768025954500235</v>
+        <f t="shared" si="2"/>
+        <v>1.5133030108212187</v>
       </c>
     </row>
     <row r="40" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B40" s="30">
         <v>2</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="J40" s="29" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="K40" s="30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L40" s="29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="M40" s="31">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:I$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.8132281580905929</v>
+        <v>1.7179619625911169</v>
       </c>
       <c r="N40" s="31">
         <f>2 + M40 + IF(H40="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.8132281580905927</v>
+        <v>3.7179619625911169</v>
       </c>
       <c r="O40" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.0758582363796765</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B41" s="30">
         <v>2</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>33</v>
+        <v>113</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="29" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="J41" s="29" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="K41" s="30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L41" s="29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="M41" s="31">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:I$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.5686689071862463</v>
+        <v>1.815362763531001</v>
       </c>
       <c r="N41" s="31">
         <f>2 + M41 + IF(H41="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.5686689071862463</v>
+        <v>3.815362763531001</v>
       </c>
       <c r="O41" s="30">
-        <f t="shared" si="0"/>
-        <v>1.1208660999470084</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B42" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="D42" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>33</v>
-      </c>
       <c r="F42" s="29" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H42" s="29" t="s">
         <v>33</v>
       </c>
       <c r="J42" s="29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="K42" s="30">
         <v>4</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="M42" s="31">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:I$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.6264563161811858</v>
+        <v>1.5604754635042337</v>
       </c>
       <c r="N42" s="31">
         <f>2 + M42 + IF(H42="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.6264563161811858</v>
+        <v>3.5604754635042335</v>
       </c>
       <c r="O42" s="30">
-        <f t="shared" si="0"/>
-        <v>1.1030051519308446</v>
+        <f t="shared" si="2"/>
+        <v>1.1234454614281164</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B43" s="30">
         <v>1</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>31</v>
+        <v>125</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="J43" s="29" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="K43" s="30">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="M43" s="31">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,Economy!A$2:I$13,9,FALSE),0)+IF(G43&lt;&gt;"",VLOOKUP(G43,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.8132281580905929</v>
+        <v>1.6307255270620018</v>
       </c>
       <c r="N43" s="31">
         <f>2 + M43 + IF(H43="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.8132281580905927</v>
+        <v>3.630725527062002</v>
       </c>
       <c r="O43" s="30">
-        <f t="shared" si="0"/>
-        <v>0.78673498558822075</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.9279893089755062</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B44" s="30">
         <v>1</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J44" s="29" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="K44" s="30">
         <v>3</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>140</v>
+        <v>48</v>
       </c>
       <c r="M44" s="31">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:I$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.7147012989212722</v>
+        <v>1.815362763531001</v>
       </c>
       <c r="N44" s="31">
         <f>2 + M44 + IF(H44="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.7147012989212724</v>
+        <v>3.815362763531001</v>
       </c>
       <c r="O44" s="30">
-        <f t="shared" si="0"/>
-        <v>0.80760194658751772</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" t="s">
-        <v>174</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="L45" t="s">
+        <f t="shared" si="2"/>
+        <v>0.78629482592727096</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="30">
+        <v>1</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="M45">
+      <c r="F45" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="K45" s="30">
+        <v>4</v>
+      </c>
+      <c r="L45" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="M45" s="31">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:I$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="17">
+        <v>3.1209509270084674</v>
+      </c>
+      <c r="N45" s="31">
         <f>2 + M45 + IF(H45="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="O45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>5.120950927008467</v>
+      </c>
+      <c r="O45" s="30">
+        <f t="shared" si="2"/>
+        <v>0.78110492699774825</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J46" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L46" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="M46">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,Economy!A$2:I$13,9,FALSE),0)+IF(G46&lt;&gt;"",VLOOKUP(G46,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.7147012989212722</v>
+        <v>0</v>
       </c>
       <c r="N46" s="17">
         <f>2 + M46 + IF(H46="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.7147012989212724</v>
+        <v>2</v>
       </c>
       <c r="O46" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="K47" s="3">
-        <v>12</v>
+        <v>115</v>
+      </c>
+      <c r="J47" t="s">
+        <v>197</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="L47" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="M47">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:I$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>3.6264563161811858</v>
+        <v>0</v>
       </c>
       <c r="N47" s="17">
         <f>2 + M47 + IF(H47="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>5.6264563161811854</v>
-      </c>
-      <c r="O47" s="3">
-        <f t="shared" si="0"/>
-        <v>2.1327811548965685</v>
+        <v>2</v>
+      </c>
+      <c r="O47" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" t="s">
-        <v>154</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>131</v>
+        <v>15</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="K48" s="3">
+        <v>12</v>
       </c>
       <c r="L48" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="M48">
         <f>IF(F48&lt;&gt;"",VLOOKUP(F48,Economy!A$2:I$13,9,FALSE),0)+IF(G48&lt;&gt;"",VLOOKUP(G48,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>1.5686689071862463</v>
+        <v>3.630725527062002</v>
       </c>
       <c r="N48" s="17">
         <f>2 + M48 + IF(H48="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>3.5686689071862463</v>
-      </c>
-      <c r="O48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>5.630725527062002</v>
+      </c>
+      <c r="O48" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1311640821997866</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="J49" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M49">
-        <v>2</v>
+        <f>IF(F49&lt;&gt;"",VLOOKUP(F49,Economy!A$2:I$13,9,FALSE),0)+IF(G49&lt;&gt;"",VLOOKUP(G49,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="N49" s="17">
         <f>2 + M49 + IF(H49="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O49" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="J50" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L50" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M50">
-        <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:I$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:I$13,9,FALSE),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N50" s="17">
         <f>2 + M50 + IF(H50="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="O50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="O50" s="3">
+        <f>8/N50</f>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L51" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="M51">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,Economy!A$2:I$13,9,FALSE),0)+IF(G51&lt;&gt;"",VLOOKUP(G51,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2712,28 +3001,28 @@
         <v>2</v>
       </c>
       <c r="O51" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J52" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L52" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M52">
         <f>IF(F52&lt;&gt;"",VLOOKUP(F52,Economy!A$2:I$13,9,FALSE),0)+IF(G52&lt;&gt;"",VLOOKUP(G52,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2744,31 +3033,28 @@
         <v>2</v>
       </c>
       <c r="O52" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J53" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L53" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="M53">
         <f>IF(F53&lt;&gt;"",VLOOKUP(F53,Economy!A$2:I$13,9,FALSE),0)+IF(G53&lt;&gt;"",VLOOKUP(G53,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2776,25 +3062,34 @@
       </c>
       <c r="N53" s="17">
         <f>2 + M53 + IF(H53="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>5.8132281580905927</v>
+        <v>2</v>
       </c>
       <c r="O53" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>45</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="J54" t="s">
-        <v>148</v>
+        <v>142</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="L54" t="s">
+        <v>57</v>
       </c>
       <c r="M54">
         <f>IF(F54&lt;&gt;"",VLOOKUP(F54,Economy!A$2:I$13,9,FALSE),0)+IF(G54&lt;&gt;"",VLOOKUP(G54,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2802,11 +3097,43 @@
       </c>
       <c r="N54" s="17">
         <f>2 + M54 + IF(H54="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="O54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.8153627635310006</v>
+      </c>
+      <c r="O54" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+      <c r="J55" t="s">
+        <v>141</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="L55" t="s">
+        <v>207</v>
+      </c>
+      <c r="M55">
+        <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:I$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N55" s="17">
+        <f>2 + M55 + IF(H55="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="O55" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2819,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,25 +3169,25 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2869,11 +3196,11 @@
       </c>
       <c r="B2" s="8">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Economy!A2)+SUMIFS(Deck!B:B,Deck!E:E,Economy!A2)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Economy!A2)+SUMIFS(Deck!B:B,Deck!G:G,Economy!A2)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="10">
         <f>SUMIFS(Deck!B:B,Deck!H:H,Economy!A2)+SUMIFS(Deck!B:B,Deck!I:I,Economy!A2)</f>
@@ -2881,23 +3208,23 @@
       </c>
       <c r="E2" s="16">
         <f t="shared" ref="E2:E13" si="0">IF(ISNUMBER(B2/C2),B2/C2,"")</f>
-        <v>1.3333333333333333</v>
+        <v>1.3076923076923077</v>
       </c>
       <c r="F2" s="17">
         <f t="shared" ref="F2:F13" si="1">IF(ISNUMBER(1/E2), 1/E2,"")</f>
-        <v>0.75</v>
+        <v>0.76470588235294112</v>
       </c>
       <c r="G2" s="16">
         <f t="shared" ref="G2:G13" si="2">SUM(B:B)/B2</f>
-        <v>5.375</v>
+        <v>5.1764705882352944</v>
       </c>
       <c r="H2" s="16">
         <f>1-POWER(B2/SUM(B:B),0.5)</f>
-        <v>0.5686689071862463</v>
+        <v>0.56047546350423372</v>
       </c>
       <c r="I2" s="16">
         <f>1+H2</f>
-        <v>1.5686689071862463</v>
+        <v>1.5604754635042337</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2926,15 +3253,15 @@
       </c>
       <c r="G3" s="17">
         <f t="shared" si="2"/>
-        <v>7.166666666666667</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="H3" s="21">
         <f t="shared" ref="H3:H13" si="3">1-POWER(B3/SUM(B:B),0.5)</f>
-        <v>0.6264563161811858</v>
+        <v>0.6307255270620018</v>
       </c>
       <c r="I3" s="17">
         <f t="shared" ref="I3:I13" si="4">1+H3</f>
-        <v>1.6264563161811858</v>
+        <v>1.6307255270620018</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2943,7 +3270,7 @@
       </c>
       <c r="B4" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Economy!A4)+SUMIFS(Deck!B:B,Deck!E:E,Economy!A4)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Economy!A4)+SUMIFS(Deck!B:B,Deck!G:G,Economy!A4)</f>
@@ -2955,23 +3282,23 @@
       </c>
       <c r="E4" s="17">
         <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="F4" s="17">
         <f t="shared" si="1"/>
-        <v>0.36363636363636365</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" si="2"/>
-        <v>7.8181818181818183</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="H4" s="21">
         <f t="shared" si="3"/>
-        <v>0.64235915118070475</v>
+        <v>0.6307255270620018</v>
       </c>
       <c r="I4" s="17">
         <f t="shared" si="4"/>
-        <v>1.6423591511807047</v>
+        <v>1.6307255270620018</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3000,15 +3327,15 @@
       </c>
       <c r="G5" s="17">
         <f t="shared" si="2"/>
-        <v>7.8181818181818183</v>
+        <v>8</v>
       </c>
       <c r="H5" s="21">
         <f t="shared" si="3"/>
-        <v>0.64235915118070475</v>
+        <v>0.64644660940672627</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" si="4"/>
-        <v>1.6423591511807047</v>
+        <v>1.6464466094067263</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3021,7 +3348,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUMIFS(Deck!B:B,Deck!F:F,Economy!A6)+SUMIFS(Deck!B:B,Deck!G:G,Economy!A6)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3">
         <f>SUMIFS(Deck!B:B,Deck!H:H,Economy!A6)+SUMIFS(Deck!B:B,Deck!I:I,Economy!A6)</f>
@@ -3029,23 +3356,23 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" si="0"/>
-        <v>0.58333333333333337</v>
+        <v>0.7</v>
       </c>
       <c r="F6" s="17">
         <f t="shared" si="1"/>
-        <v>1.7142857142857142</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" si="2"/>
-        <v>12.285714285714286</v>
+        <v>12.571428571428571</v>
       </c>
       <c r="H6" s="21">
         <f t="shared" si="3"/>
-        <v>0.71470129892127221</v>
+        <v>0.71796196259111689</v>
       </c>
       <c r="I6" s="17">
         <f t="shared" si="4"/>
-        <v>1.7147012989212722</v>
+        <v>1.7179619625911169</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3074,20 +3401,20 @@
       </c>
       <c r="G7" s="17">
         <f t="shared" si="2"/>
-        <v>12.285714285714286</v>
+        <v>12.571428571428571</v>
       </c>
       <c r="H7" s="21">
         <f t="shared" si="3"/>
-        <v>0.71470129892127221</v>
+        <v>0.71796196259111689</v>
       </c>
       <c r="I7" s="17">
         <f t="shared" si="4"/>
-        <v>1.7147012989212722</v>
+        <v>1.7179619625911169</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Economy!A13)+SUMIFS(Deck!B:B,Deck!E:E,Economy!A13)</f>
@@ -3111,15 +3438,15 @@
       </c>
       <c r="G8" s="17">
         <f t="shared" si="2"/>
-        <v>28.666666666666668</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="H8" s="21">
         <f t="shared" si="3"/>
-        <v>0.8132281580905929</v>
+        <v>0.8153627635310009</v>
       </c>
       <c r="I8" s="17">
         <f t="shared" si="4"/>
-        <v>1.8132281580905929</v>
+        <v>1.815362763531001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,15 +3475,15 @@
       </c>
       <c r="G9" s="17">
         <f t="shared" si="2"/>
-        <v>14.333333333333334</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" si="3"/>
-        <v>0.73586472810231285</v>
+        <v>0.73888351606645331</v>
       </c>
       <c r="I9" s="17">
         <f t="shared" si="4"/>
-        <v>1.735864728102313</v>
+        <v>1.7388835160664533</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3185,15 +3512,15 @@
       </c>
       <c r="G10" s="17">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>22</v>
       </c>
       <c r="H10" s="21">
         <f t="shared" si="3"/>
-        <v>0.78433445359312315</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="I10" s="17">
         <f t="shared" si="4"/>
-        <v>1.7843344535931231</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3222,15 +3549,15 @@
       </c>
       <c r="G11" s="17">
         <f t="shared" si="2"/>
-        <v>28.666666666666668</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="H11" s="21">
         <f t="shared" si="3"/>
-        <v>0.8132281580905929</v>
+        <v>0.8153627635310009</v>
       </c>
       <c r="I11" s="17">
         <f t="shared" si="4"/>
-        <v>1.8132281580905929</v>
+        <v>1.815362763531001</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3259,15 +3586,15 @@
       </c>
       <c r="G12" s="17">
         <f t="shared" si="2"/>
-        <v>28.666666666666668</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="H12" s="21">
         <f t="shared" si="3"/>
-        <v>0.8132281580905929</v>
+        <v>0.8153627635310009</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" si="4"/>
-        <v>1.8132281580905929</v>
+        <v>1.815362763531001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3296,15 +3623,15 @@
       </c>
       <c r="G13" s="17">
         <f t="shared" si="2"/>
-        <v>28.666666666666668</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="H13" s="21">
         <f t="shared" si="3"/>
-        <v>0.8132281580905929</v>
+        <v>0.8153627635310009</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" si="4"/>
-        <v>1.8132281580905929</v>
+        <v>1.815362763531001</v>
       </c>
     </row>
   </sheetData>
@@ -3313,4 +3640,871 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" style="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="17">
+        <f>IF(ISNA(VLOOKUP(A3,Deck!C:O,12,FALSE)),"",VLOOKUP(A3,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <f>IF(ISNA(VLOOKUP(A3,Deck!C:O,9,FALSE)),"",VLOOKUP(A3,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(E3,Deck!$C:$O,12,FALSE)),"",VLOOKUP(E3,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(E3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(E3,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="17">
+        <f>IF(ISNA(VLOOKUP(I3,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I3,Deck!$C:$O,12,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="3">
+        <f>IF(ISNA(VLOOKUP(I3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I3,Deck!$C:$O,9,FALSE))</f>
+        <v>3</v>
+      </c>
+      <c r="L3" s="53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="17">
+        <f>IF(ISNA(VLOOKUP(A4,Deck!C:O,12,FALSE)),"",VLOOKUP(A4,Deck!C:O,12,FALSE))</f>
+        <v>3.7179619625911169</v>
+      </c>
+      <c r="C4" s="3">
+        <f>IF(ISNA(VLOOKUP(A4,Deck!C:O,9,FALSE)),"",VLOOKUP(A4,Deck!C:O,9,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="17">
+        <f>IF(ISNA(VLOOKUP(E4,Deck!C:O,12,FALSE)),"",VLOOKUP(E4,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f>IF(ISNA(VLOOKUP(E4,Deck!C:O,9,FALSE)),"",VLOOKUP(E4,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="17">
+        <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="53"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="17">
+        <f>IF(ISNA(VLOOKUP(A5,Deck!C:O,12,FALSE)),"",VLOOKUP(A5,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <f>IF(ISNA(VLOOKUP(A5,Deck!C:O,9,FALSE)),"",VLOOKUP(A5,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="17">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
+        <f>IF(ISNA(VLOOKUP(E5,Deck!C:O,9,FALSE)),"",VLOOKUP(E5,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="17">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <f>IF(ISNA(VLOOKUP(I5,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I5,Deck!$C:$O,9,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <f>IF(ISNA(VLOOKUP(A6,Deck!C:O,9,FALSE)),"",VLOOKUP(A6,Deck!C:O,9,FALSE))</f>
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <f>IF(ISNA(VLOOKUP(E6,Deck!C:O,9,FALSE)),"",VLOOKUP(E6,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="17">
+        <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="53"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <f>IF(ISNA(VLOOKUP(A7,Deck!C:O,9,FALSE)),"",VLOOKUP(A7,Deck!C:O,9,FALSE))</f>
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <f>IF(ISNA(VLOOKUP(E7,Deck!C:O,9,FALSE)),"",VLOOKUP(E7,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="17">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <f>IF(ISNA(VLOOKUP(I7,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I7,Deck!$C:$O,9,FALSE))</f>
+        <v>12</v>
+      </c>
+      <c r="L7" s="53" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <f>IF(ISNA(VLOOKUP(A8,Deck!C:O,9,FALSE)),"",VLOOKUP(A8,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="17">
+        <f>IF(ISNA(VLOOKUP(E8,Deck!C:O,12,FALSE)),"",VLOOKUP(E8,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <f>IF(ISNA(VLOOKUP(E8,Deck!C:O,9,FALSE)),"",VLOOKUP(E8,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="17">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>IF(ISNA(VLOOKUP(I8,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I8,Deck!$C:$O,9,FALSE))</f>
+        <v>5</v>
+      </c>
+      <c r="L8" s="53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="17">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <f>IF(ISNA(VLOOKUP(A9,Deck!C:O,9,FALSE)),"",VLOOKUP(A9,Deck!C:O,9,FALSE))</f>
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="17">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3">
+        <f>IF(ISNA(VLOOKUP(E9,Deck!C:O,9,FALSE)),"",VLOOKUP(E9,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="17">
+        <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="53"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <f>IF(ISNA(VLOOKUP(A10,Deck!C:O,9,FALSE)),"",VLOOKUP(A10,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <f>IF(ISNA(VLOOKUP(E10,Deck!C:O,9,FALSE)),"",VLOOKUP(E10,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="17">
+        <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="53"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="17">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <f>IF(ISNA(VLOOKUP(A11,Deck!C:O,9,FALSE)),"",VLOOKUP(A11,Deck!C:O,9,FALSE))</f>
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <f>IF(ISNA(VLOOKUP(E11,Deck!C:O,9,FALSE)),"",VLOOKUP(E11,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3">
+        <f>IF(ISNA(VLOOKUP(I11,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I11,Deck!$C:$O,9,FALSE))</f>
+        <v>7</v>
+      </c>
+      <c r="L11" s="53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A13,Deck!C:O,12,FALSE)),"",VLOOKUP(A13,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A12,Deck!C:O,9,FALSE)),"",VLOOKUP(A12,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="17">
+        <f>IF(ISNA(VLOOKUP(E12,Deck!C:O,12,FALSE)),"",VLOOKUP(E12,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <f>IF(ISNA(VLOOKUP(E12,Deck!C:O,9,FALSE)),"",VLOOKUP(E12,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="17">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <f>IF(ISNA(VLOOKUP(I12,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I12,Deck!$C:$O,9,FALSE))</f>
+        <v>4</v>
+      </c>
+      <c r="L12" s="53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A14,Deck!C:O,12,FALSE)),"",VLOOKUP(A14,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A13,Deck!C:O,9,FALSE)),"",VLOOKUP(A13,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="17">
+        <f>IF(ISNA(VLOOKUP(E13,Deck!C:O,12,FALSE)),"",VLOOKUP(E13,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <f>IF(ISNA(VLOOKUP(E13,Deck!C:O,9,FALSE)),"",VLOOKUP(E13,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="17">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3">
+        <f>IF(ISNA(VLOOKUP(I13,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I13,Deck!$C:$O,9,FALSE))</f>
+        <v>4</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A15,Deck!C:O,12,FALSE)),"",VLOOKUP(A15,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A14,Deck!C:O,9,FALSE)),"",VLOOKUP(A14,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="17">
+        <f>IF(ISNA(VLOOKUP(E14,Deck!C:O,12,FALSE)),"",VLOOKUP(E14,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <f>IF(ISNA(VLOOKUP(E14,Deck!C:O,9,FALSE)),"",VLOOKUP(E14,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="38"/>
+      <c r="J14" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I14,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I14,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K14" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I14,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I14,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L14" s="53"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A16,Deck!C:O,12,FALSE)),"",VLOOKUP(A16,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A15,Deck!C:O,9,FALSE)),"",VLOOKUP(A15,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="17">
+        <f>IF(ISNA(VLOOKUP(E15,Deck!C:O,12,FALSE)),"",VLOOKUP(E15,Deck!C:O,12,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <f>IF(ISNA(VLOOKUP(E15,Deck!C:O,9,FALSE)),"",VLOOKUP(E15,Deck!C:O,9,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="38"/>
+      <c r="J15" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I15,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I15,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I15,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I15,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A17,Deck!C:O,12,FALSE)),"",VLOOKUP(A17,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A16,Deck!C:O,9,FALSE)),"",VLOOKUP(A16,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F16" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(E16,Deck!C:O,12,FALSE)),"",VLOOKUP(E16,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G16" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(E16,Deck!C:O,9,FALSE)),"",VLOOKUP(E16,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I16" s="38"/>
+      <c r="J16" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I16,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I16,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K16" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I16,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I16,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L16" s="53"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A18,Deck!C:O,12,FALSE)),"",VLOOKUP(A18,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A17,Deck!C:O,9,FALSE)),"",VLOOKUP(A17,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(E17,Deck!C:O,12,FALSE)),"",VLOOKUP(E17,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G17" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(E17,Deck!C:O,9,FALSE)),"",VLOOKUP(E17,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I17" s="38"/>
+      <c r="J17" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I17,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I17,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K17" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I17,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I17,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L17" s="53"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A18,Deck!C:O,9,FALSE)),"",VLOOKUP(A18,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(E18,Deck!C:O,12,FALSE)),"",VLOOKUP(E18,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(E18,Deck!C:O,9,FALSE)),"",VLOOKUP(E18,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I18" s="38"/>
+      <c r="J18" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I18,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I18,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K18" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I18,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I18,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L18" s="53"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,9,FALSE)),"",VLOOKUP(A19,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="17">
+        <f>IF(ISNA(VLOOKUP(E19,Deck!C:O,12,FALSE)),"",VLOOKUP(E19,Deck!C:O,12,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>9</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="I19" s="38"/>
+      <c r="J19" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I19,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I19,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K19" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I19,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I19,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L19" s="53"/>
+    </row>
+    <row r="20" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(A20,Deck!C:O,12,FALSE)),"",VLOOKUP(A20,Deck!C:O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(A20,Deck!C:O,9,FALSE)),"",VLOOKUP(A20,Deck!C:O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="17">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>25</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="I20" s="38"/>
+      <c r="J20" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(I20,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I20,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="K20" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(I20,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I20,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L20" s="53"/>
+    </row>
+    <row r="21" spans="1:12" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="17">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="17">
+        <f>IF(ISNA(VLOOKUP(E21,Deck!C:O,12,FALSE)),"",VLOOKUP(E21,Deck!C:O,12,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>24</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="17">
+        <f>IF(ISNA(VLOOKUP(I21,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I21,Deck!$C:$O,12,FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>24</v>
+      </c>
+      <c r="L21" s="53"/>
+    </row>
+    <row r="22" spans="1:12" s="45" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="52">
+        <f>SUM(B3:B21)</f>
+        <v>17.717961962591119</v>
+      </c>
+      <c r="C22" s="51">
+        <f>SUM(C3:C21)</f>
+        <v>50</v>
+      </c>
+      <c r="D22" s="51"/>
+      <c r="E22" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" s="48">
+        <f>SUM(F3:F21)</f>
+        <v>20</v>
+      </c>
+      <c r="G22" s="45">
+        <f>SUM(G3:G21)</f>
+        <v>58</v>
+      </c>
+      <c r="H22" s="54"/>
+      <c r="I22" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="J22" s="48">
+        <f>SUM(J3:J21)</f>
+        <v>20</v>
+      </c>
+      <c r="K22" s="45">
+        <f>SUM(K3:K21)</f>
+        <v>61</v>
+      </c>
+      <c r="L22" s="54"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="17">
+        <f>C22/B22</f>
+        <v>2.8219949961269628</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="49">
+        <f>G22/F22</f>
+        <v>2.9</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="49">
+        <f>K22/J22</f>
+        <v>3.05</v>
+      </c>
+      <c r="L23" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12">
+      <formula1>$C$3:$C$55</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A16:A21">
+      <formula1>$C$3:$C$55</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A10">
+      <formula1>$C$3:$C$55</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I21">
+      <formula1>$C$3:$C$55</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I9">
+      <formula1>$C$3:$C$55</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Deck!$C$3:$C$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>E14:E21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I dub thee v005
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -234,9 +234,6 @@
     <t>I'm pretty sure this strategy worked for me at least once.</t>
   </si>
   <si>
-    <t>It is by pure coincidence that we actually need Wood for our building.</t>
-  </si>
-  <si>
     <t>It is by pure coincidence that we actually need Clay for our building.</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
     <t>The Diversified Strategy Payoff</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>The Military Commitment</t>
   </si>
   <si>
@@ -636,13 +630,19 @@
     <t>Side benefit: easier planning! You don't have to think about how to make your food now!</t>
   </si>
   <si>
-    <t>It is by pure coincidence that we actually need Stone for our building.</t>
-  </si>
-  <si>
     <t>Seems like a lot now, but this won't win you the game alone.</t>
   </si>
   <si>
     <t>You didn't forget about food, did you?</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Not to be confused with the Building Wood Building, which is what we call our indoor arboretum</t>
+  </si>
+  <si>
+    <t>Technically, we're just a shack made out of fiberglass, but this game doesn't need another resource.</t>
   </si>
 </sst>
 </file>
@@ -917,12 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -940,6 +934,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,12 +946,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -1262,9 +1262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1276,7 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="10.140625" style="13" customWidth="1"/>
     <col min="10" max="10" width="62.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.7109375" customWidth="1"/>
     <col min="13" max="13" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" style="17" bestFit="1" customWidth="1"/>
@@ -1300,10 +1300,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>19</v>
@@ -1321,40 +1321,40 @@
         <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K2" s="5">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="33"/>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1377,10 +1377,10 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>138</v>
-      </c>
-      <c r="K3" s="3">
-        <v>2</v>
+        <v>136</v>
+      </c>
+      <c r="K3" s="5">
+        <v>20</v>
       </c>
       <c r="L3" t="s">
         <v>66</v>
@@ -1393,14 +1393,14 @@
         <f>2 + M3 + IF(H3="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.7179619625911169</v>
       </c>
-      <c r="O3" s="36">
-        <f t="shared" ref="O3:O5" si="0">IF(ISNUMBER(K3/N3), K3/N3,"")</f>
-        <v>0.53792911818983824</v>
+      <c r="O3" s="36" t="str">
+        <f>IF(ISNUMBER(#REF!/N3),#REF!/ N3,"")</f>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1412,13 +1412,13 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K4" s="3">
-        <v>3</v>
+        <v>149</v>
+      </c>
+      <c r="K4" s="5">
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M4" s="35">
         <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:I$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1428,14 +1428,14 @@
         <f>2 + M4 + IF(H4="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="O4" s="36">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+      <c r="O4" s="36" t="str">
+        <f>IF(ISNUMBER(#REF!/N4),#REF!/ N4,"")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1447,13 +1447,13 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
-      </c>
-      <c r="K5" s="3">
-        <v>2</v>
+        <v>137</v>
+      </c>
+      <c r="K5" s="5">
+        <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M5" s="35">
         <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:I$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1463,32 +1463,32 @@
         <f>2 + M5 + IF(H5="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.5604754635042335</v>
       </c>
-      <c r="O5" s="36">
-        <f t="shared" si="0"/>
-        <v>0.5617227307140582</v>
+      <c r="O5" s="36" t="str">
+        <f>IF(ISNUMBER(#REF!/N5),#REF!/ N5,"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>150</v>
-      </c>
-      <c r="K6" s="3">
-        <v>2</v>
+        <v>148</v>
+      </c>
+      <c r="K6" s="5">
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6" s="35">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:I$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1498,9 +1498,9 @@
         <f>2 + M6 + IF(H6="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.630725527062002</v>
       </c>
-      <c r="O6" s="36">
-        <f t="shared" ref="O6" si="1">IF(ISNUMBER(K6/N6), K6/N6,"")</f>
-        <v>0.55085408827871607</v>
+      <c r="O6" s="36" t="str">
+        <f>IF(ISNUMBER(#REF!/N6),#REF!/ N6,"")</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1514,10 +1514,10 @@
         <v>61</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
-      </c>
-      <c r="K7" s="3">
-        <v>-8</v>
+        <v>113</v>
+      </c>
+      <c r="K7" s="5">
+        <v>-80</v>
       </c>
       <c r="L7" t="s">
         <v>53</v>
@@ -1531,7 +1531,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>8</v>
@@ -1539,11 +1539,11 @@
       <c r="E8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="27">
-        <v>0</v>
-      </c>
-      <c r="L8" s="60" t="s">
-        <v>200</v>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="54" t="s">
+        <v>198</v>
       </c>
       <c r="M8" s="28"/>
       <c r="N8" s="28">
@@ -1559,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>14</v>
@@ -1567,11 +1567,11 @@
       <c r="E9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="27">
-        <v>0</v>
-      </c>
-      <c r="L9" s="60" t="s">
-        <v>201</v>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="54" t="s">
+        <v>199</v>
       </c>
       <c r="M9" s="28"/>
       <c r="N9" s="28">
@@ -1587,16 +1587,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="27">
-        <v>0</v>
-      </c>
-      <c r="L10" s="60" t="s">
-        <v>202</v>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="54" t="s">
+        <v>200</v>
       </c>
       <c r="M10" s="28"/>
       <c r="N10" s="28">
@@ -1612,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>14</v>
@@ -1620,11 +1620,11 @@
       <c r="E11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="27">
-        <v>0</v>
-      </c>
-      <c r="L11" s="60" t="s">
-        <v>203</v>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="54" t="s">
+        <v>201</v>
       </c>
       <c r="M11" s="28"/>
       <c r="N11" s="28">
@@ -1645,7 +1645,7 @@
       <c r="D12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K12" s="5">
         <v>0</v>
       </c>
       <c r="L12" s="26" t="s">
@@ -1665,12 +1665,12 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="5">
         <v>0</v>
       </c>
       <c r="L13" s="26" t="s">
@@ -1690,15 +1690,15 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="27">
-        <v>0</v>
-      </c>
-      <c r="L14" s="60" t="s">
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="54" t="s">
         <v>52</v>
       </c>
       <c r="M14" s="28"/>
@@ -1715,7 +1715,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>27</v>
@@ -1724,9 +1724,9 @@
         <v>27</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="27">
+        <v>92</v>
+      </c>
+      <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" s="26" t="s">
@@ -1746,16 +1746,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="5">
         <v>0</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="28">
@@ -1764,26 +1764,26 @@
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="27">
         <v>1</v>
       </c>
-      <c r="C17" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="D17" s="60" t="s">
+      <c r="C17" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="27">
-        <v>0</v>
-      </c>
-      <c r="L17" s="60" t="s">
-        <v>199</v>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="54" t="s">
+        <v>197</v>
       </c>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
@@ -1797,19 +1797,19 @@
         <v>2</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="27">
+        <v>100</v>
+      </c>
+      <c r="K18" s="5">
         <v>0</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M18" s="28"/>
       <c r="N18" s="28">
@@ -1825,16 +1825,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="5">
         <v>0</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M19" s="28"/>
       <c r="N19" s="28">
@@ -1850,19 +1850,19 @@
         <v>3</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>16</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="K20" s="27">
-        <v>2</v>
+        <v>147</v>
+      </c>
+      <c r="K20" s="5">
+        <v>20</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M20" s="28"/>
       <c r="N20" s="28">
@@ -1883,11 +1883,11 @@
       <c r="D21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="27">
-        <v>0</v>
-      </c>
-      <c r="L21" s="60" t="s">
-        <v>204</v>
+      <c r="K21" s="5">
+        <v>0</v>
+      </c>
+      <c r="L21" s="54" t="s">
+        <v>202</v>
       </c>
       <c r="M21" s="28"/>
       <c r="N21" s="28">
@@ -1897,22 +1897,22 @@
     </row>
     <row r="22" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="23">
         <v>1</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>54</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="K22" s="23">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="K22" s="5">
+        <v>30</v>
       </c>
       <c r="L22" s="22" t="s">
         <v>67</v>
@@ -1925,14 +1925,14 @@
         <f>2 + M22 + IF(H22="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="O22" s="23">
-        <f t="shared" ref="O22:O55" si="2">IF(ISNUMBER(K22/N22), K22/N22,"")</f>
-        <v>1.5</v>
+      <c r="O22" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N22),#REF!/ N22,"")</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="23">
         <v>2</v>
@@ -1950,9 +1950,9 @@
         <v>23</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="23">
+        <v>100</v>
+      </c>
+      <c r="K23" s="5">
         <v>0</v>
       </c>
       <c r="L23" s="22" t="s">
@@ -1966,32 +1966,32 @@
         <f>2 + M23 + IF(H23="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.630725527062002</v>
       </c>
-      <c r="O23" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O23" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N23),#REF!/ N23,"")</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="23">
         <v>1</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="K24" s="23">
-        <v>5</v>
+        <v>146</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M24" s="24">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:I$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2001,14 +2001,14 @@
         <f>2 + M24 + IF(H24="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>5.8153627635310006</v>
       </c>
-      <c r="O24" s="23">
-        <f t="shared" si="2"/>
-        <v>0.85979159053597465</v>
+      <c r="O24" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N24),#REF!/ N24,"")</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" s="23">
         <v>3</v>
@@ -2025,8 +2025,8 @@
       <c r="F25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="23">
-        <v>0</v>
+      <c r="K25" s="5">
+        <v>5</v>
       </c>
       <c r="L25" s="22" t="s">
         <v>64</v>
@@ -2039,20 +2039,20 @@
         <f>2 + M25 + IF(H25="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.646446609406726</v>
       </c>
-      <c r="O25" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O25" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N25),#REF!/ N25,"")</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="23">
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F26" s="22" t="s">
         <v>11</v>
@@ -2063,11 +2063,11 @@
       <c r="J26" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="K26" s="23">
-        <v>5</v>
-      </c>
-      <c r="L26" s="61" t="s">
-        <v>205</v>
+      <c r="K26" s="5">
+        <v>50</v>
+      </c>
+      <c r="L26" s="55" t="s">
+        <v>207</v>
       </c>
       <c r="M26" s="24">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:I$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2077,20 +2077,20 @@
         <f>2 + M26 + IF(H26="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>7.5333247261221175</v>
       </c>
-      <c r="O26" s="23">
-        <f t="shared" si="2"/>
-        <v>0.66371757248991159</v>
+      <c r="O26" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N26),#REF!/ N26,"")</f>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="23">
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>8</v>
@@ -2101,11 +2101,11 @@
       <c r="J27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="K27" s="23">
-        <v>5</v>
-      </c>
-      <c r="L27" s="22" t="s">
-        <v>71</v>
+      <c r="K27" s="5">
+        <v>50</v>
+      </c>
+      <c r="L27" s="55" t="s">
+        <v>206</v>
       </c>
       <c r="M27" s="24">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:I$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2115,20 +2115,20 @@
         <f>2 + M27 + IF(H27="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>7.375838227035235</v>
       </c>
-      <c r="O27" s="23">
-        <f t="shared" si="2"/>
-        <v>0.67788905424648693</v>
+      <c r="O27" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N27),#REF!/ N27,"")</f>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="23">
         <v>1</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>14</v>
@@ -2139,11 +2139,11 @@
       <c r="J28" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="23">
-        <v>5</v>
-      </c>
-      <c r="L28" s="22" t="s">
-        <v>72</v>
+      <c r="K28" s="5">
+        <v>50</v>
+      </c>
+      <c r="L28" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="M28" s="24">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:I$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2153,27 +2153,27 @@
         <f>2 + M28 + IF(H28="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>7.4460882905930035</v>
       </c>
-      <c r="O28" s="23">
-        <f t="shared" si="2"/>
-        <v>0.67149351510063848</v>
+      <c r="O28" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N28),#REF!/ N28,"")</f>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:15" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="23">
         <v>1</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D29" s="25"/>
       <c r="J29" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="K29" s="23">
-        <v>3</v>
+        <v>130</v>
+      </c>
+      <c r="K29" s="5">
+        <v>30</v>
       </c>
       <c r="L29" s="22" t="s">
         <v>29</v>
@@ -2186,14 +2186,14 @@
         <f>2 + M29 + IF(H29="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="O29" s="23">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+      <c r="O29" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N29),#REF!/ N29,"")</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="23">
         <v>1</v>
@@ -2214,13 +2214,13 @@
         <v>33</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="K30" s="23">
-        <v>5</v>
+        <v>149</v>
+      </c>
+      <c r="K30" s="5">
+        <v>50</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M30" s="24">
         <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:I$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2230,14 +2230,14 @@
         <f>2 + M30 + IF(H30="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>5.8153627635310006</v>
       </c>
-      <c r="O30" s="23">
-        <f t="shared" si="2"/>
-        <v>0.85979159053597465</v>
+      <c r="O30" s="23" t="str">
+        <f>IF(ISNUMBER(#REF!/N30),#REF!/ N30,"")</f>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B31" s="30">
         <v>1</v>
@@ -2249,10 +2249,10 @@
         <v>11</v>
       </c>
       <c r="J31" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="K31" s="30">
-        <v>6</v>
+        <v>128</v>
+      </c>
+      <c r="K31" s="5">
+        <v>60</v>
       </c>
       <c r="L31" s="29" t="s">
         <v>63</v>
@@ -2265,20 +2265,20 @@
         <f>2 + M31 + IF(H31="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.7179619625911169</v>
       </c>
-      <c r="O31" s="30">
-        <f t="shared" si="2"/>
-        <v>1.6137873545695149</v>
+      <c r="O31" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N31),#REF!/ N31,"")</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B32" s="30">
         <v>1</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>12</v>
@@ -2289,7 +2289,7 @@
       <c r="F32" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="30">
+      <c r="K32" s="5">
         <v>0</v>
       </c>
       <c r="M32" s="31">
@@ -2300,20 +2300,20 @@
         <f>2 + M32 + IF(H32="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.646446609406726</v>
       </c>
-      <c r="O32" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O32" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N32),#REF!/ N32,"")</f>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" s="30">
         <v>2</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>23</v>
@@ -2327,7 +2327,7 @@
       <c r="J33" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="K33" s="30">
+      <c r="K33" s="5">
         <v>0</v>
       </c>
       <c r="L33" s="29" t="s">
@@ -2341,20 +2341,20 @@
         <f>2 + M33 + IF(H33="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.630725527062002</v>
       </c>
-      <c r="O33" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O33" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N33),#REF!/ N33,"")</f>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" s="30">
         <v>2</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>8</v>
@@ -2365,11 +2365,11 @@
       <c r="H34" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="30">
-        <v>9</v>
+      <c r="K34" s="5">
+        <v>90</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M34" s="31">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:I$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2379,20 +2379,20 @@
         <f>2 + M34 + IF(H34="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>8.9363136905394676</v>
       </c>
-      <c r="O34" s="30">
-        <f t="shared" si="2"/>
-        <v>1.0071266868717863</v>
+      <c r="O34" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N34),#REF!/ N34,"")</f>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B35" s="30">
         <v>1</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>14</v>
@@ -2403,11 +2403,11 @@
       <c r="H35" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K35" s="30">
-        <v>10</v>
+      <c r="K35" s="5">
+        <v>100</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M35" s="31">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:I$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2417,20 +2417,20 @@
         <f>2 + M35 + IF(H35="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>9.0065637540972361</v>
       </c>
-      <c r="O35" s="30">
-        <f t="shared" si="2"/>
-        <v>1.1103013616542527</v>
+      <c r="O35" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N35),#REF!/ N35,"")</f>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B36" s="30">
         <v>1</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>14</v>
@@ -2441,11 +2441,11 @@
       <c r="H36" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K36" s="30">
-        <v>11</v>
+      <c r="K36" s="5">
+        <v>110</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M36" s="31">
         <f>IF(F36&lt;&gt;"",VLOOKUP(F36,Economy!A$2:I$13,9,FALSE),0)+IF(G36&lt;&gt;"",VLOOKUP(G36,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2455,20 +2455,20 @@
         <f>2 + M36 + IF(H36="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>9.0768138176550046</v>
       </c>
-      <c r="O36" s="30">
-        <f t="shared" si="2"/>
-        <v>1.2118789942131754</v>
+      <c r="O36" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N36),#REF!/ N36,"")</f>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B37" s="30">
         <v>1</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F37" s="32" t="s">
         <v>8</v>
@@ -2479,11 +2479,11 @@
       <c r="H37" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K37" s="30">
-        <v>12</v>
+      <c r="K37" s="5">
+        <v>120</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M37" s="31">
         <f>IF(F37&lt;&gt;"",VLOOKUP(F37,Economy!A$2:I$13,9,FALSE),0)+IF(G37&lt;&gt;"",VLOOKUP(G37,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2493,20 +2493,20 @@
         <f>2 + M37 + IF(H37="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>9.0938001896263518</v>
       </c>
-      <c r="O37" s="30">
-        <f t="shared" si="2"/>
-        <v>1.3195803459250031</v>
+      <c r="O37" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N37),#REF!/ N37,"")</f>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" s="30">
         <v>1</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F38" s="32" t="s">
         <v>14</v>
@@ -2517,11 +2517,11 @@
       <c r="H38" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K38" s="30">
-        <v>13</v>
+      <c r="K38" s="5">
+        <v>130</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M38" s="31">
         <f>IF(F38&lt;&gt;"",VLOOKUP(F38,Economy!A$2:I$13,9,FALSE),0)+IF(G38&lt;&gt;"",VLOOKUP(G38,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2531,20 +2531,20 @@
         <f>2 + M38 + IF(H38="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>9.1640502531841204</v>
       </c>
-      <c r="O38" s="30">
-        <f t="shared" si="2"/>
-        <v>1.4185867210279701</v>
+      <c r="O38" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N38),#REF!/ N38,"")</f>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B39" s="30">
         <v>1</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>11</v>
@@ -2555,11 +2555,11 @@
       <c r="H39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K39" s="30">
-        <v>14</v>
+      <c r="K39" s="5">
+        <v>140</v>
       </c>
       <c r="L39" s="32" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M39" s="31">
         <f>IF(F39&lt;&gt;"",VLOOKUP(F39,Economy!A$2:I$13,9,FALSE),0)+IF(G39&lt;&gt;"",VLOOKUP(G39,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2569,14 +2569,14 @@
         <f>2 + M39 + IF(H39="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>9.2512866887132343</v>
       </c>
-      <c r="O39" s="30">
-        <f t="shared" si="2"/>
-        <v>1.5133030108212187</v>
+      <c r="O39" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N39),#REF!/ N39,"")</f>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B40" s="30">
         <v>2</v>
@@ -2593,8 +2593,8 @@
       <c r="F40" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="30">
-        <v>4</v>
+      <c r="K40" s="5">
+        <v>40</v>
       </c>
       <c r="L40" s="29" t="s">
         <v>65</v>
@@ -2607,34 +2607,34 @@
         <f>2 + M40 + IF(H40="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.7179619625911169</v>
       </c>
-      <c r="O40" s="30">
-        <f t="shared" si="2"/>
-        <v>1.0758582363796765</v>
+      <c r="O40" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N40),#REF!/ N40,"")</f>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B41" s="30">
         <v>2</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J41" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="K41" s="30">
+        <v>125</v>
+      </c>
+      <c r="K41" s="5">
         <v>0</v>
       </c>
       <c r="L41" s="29" t="s">
@@ -2648,14 +2648,14 @@
         <f>2 + M41 + IF(H41="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.815362763531001</v>
       </c>
-      <c r="O41" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O41" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N41),#REF!/ N41,"")</f>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B42" s="30">
         <v>2</v>
@@ -2673,10 +2673,10 @@
         <v>33</v>
       </c>
       <c r="J42" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K42" s="30">
-        <v>4</v>
+        <v>149</v>
+      </c>
+      <c r="K42" s="5">
+        <v>40</v>
       </c>
       <c r="L42" s="29" t="s">
         <v>70</v>
@@ -2689,20 +2689,20 @@
         <f>2 + M42 + IF(H42="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.5604754635042335</v>
       </c>
-      <c r="O42" s="30">
-        <f t="shared" si="2"/>
-        <v>1.1234454614281164</v>
+      <c r="O42" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N42),#REF!/ N42,"")</f>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B43" s="30">
         <v>1</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D43" s="29" t="s">
         <v>33</v>
@@ -2717,13 +2717,13 @@
         <v>33</v>
       </c>
       <c r="J43" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K43" s="30">
-        <v>7</v>
+        <v>149</v>
+      </c>
+      <c r="K43" s="5">
+        <v>70</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M43" s="31">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,Economy!A$2:I$13,9,FALSE),0)+IF(G43&lt;&gt;"",VLOOKUP(G43,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2733,14 +2733,14 @@
         <f>2 + M43 + IF(H43="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.630725527062002</v>
       </c>
-      <c r="O43" s="30">
-        <f t="shared" si="2"/>
-        <v>1.9279893089755062</v>
+      <c r="O43" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N43),#REF!/ N43,"")</f>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B44" s="30">
         <v>1</v>
@@ -2752,10 +2752,10 @@
         <v>15</v>
       </c>
       <c r="J44" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="K44" s="30">
-        <v>3</v>
+        <v>127</v>
+      </c>
+      <c r="K44" s="5">
+        <v>30</v>
       </c>
       <c r="L44" s="29" t="s">
         <v>48</v>
@@ -2768,20 +2768,20 @@
         <f>2 + M44 + IF(H44="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>3.815362763531001</v>
       </c>
-      <c r="O44" s="30">
-        <f t="shared" si="2"/>
-        <v>0.78629482592727096</v>
+      <c r="O44" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N44),#REF!/ N44,"")</f>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B45" s="30">
         <v>1</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F45" s="32" t="s">
         <v>8</v>
@@ -2790,13 +2790,13 @@
         <v>8</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="K45" s="30">
-        <v>4</v>
+        <v>132</v>
+      </c>
+      <c r="K45" s="5">
+        <v>40</v>
       </c>
       <c r="L45" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M45" s="31">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:I$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2806,14 +2806,14 @@
         <f>2 + M45 + IF(H45="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>5.120950927008467</v>
       </c>
-      <c r="O45" s="30">
-        <f t="shared" si="2"/>
-        <v>0.78110492699774825</v>
+      <c r="O45" s="30" t="str">
+        <f>IF(ISNUMBER(#REF!/N45),#REF!/ N45,"")</f>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
@@ -2822,13 +2822,13 @@
         <v>21</v>
       </c>
       <c r="J46" t="s">
-        <v>166</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M46">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,Economy!A$2:I$13,9,FALSE),0)+IF(G46&lt;&gt;"",VLOOKUP(G46,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2839,28 +2839,28 @@
         <v>2</v>
       </c>
       <c r="O46" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N46),#REF!/ N46,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
       <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47" t="s">
+        <v>195</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L47" t="s">
         <v>115</v>
-      </c>
-      <c r="J47" t="s">
-        <v>197</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="L47" t="s">
-        <v>116</v>
       </c>
       <c r="M47">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:I$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2871,13 +2871,13 @@
         <v>2</v>
       </c>
       <c r="O47" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N47),#REF!/ N47,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
@@ -2889,10 +2889,10 @@
         <v>15</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="K48" s="3">
-        <v>12</v>
+        <v>112</v>
+      </c>
+      <c r="K48" s="5">
+        <v>120</v>
       </c>
       <c r="L48" t="s">
         <v>24</v>
@@ -2905,26 +2905,26 @@
         <f>2 + M48 + IF(H48="Building",VLOOKUP("Stone",Economy!A$2:I$13,9)+2,0)</f>
         <v>5.630725527062002</v>
       </c>
-      <c r="O48" s="3">
-        <f t="shared" si="2"/>
-        <v>2.1311640821997866</v>
+      <c r="O48" s="3" t="str">
+        <f>IF(ISNUMBER(#REF!/N48),#REF!/ N48,"")</f>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J49" t="s">
-        <v>146</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L49" t="s">
         <v>39</v>
@@ -2938,25 +2938,25 @@
         <v>2</v>
       </c>
       <c r="O49" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N49),#REF!/ N49,"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J50" t="s">
-        <v>143</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>124</v>
+        <v>141</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L50" t="s">
         <v>40</v>
@@ -2975,19 +2975,19 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J51" t="s">
-        <v>147</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>124</v>
+        <v>145</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L51" t="s">
         <v>28</v>
@@ -3001,13 +3001,13 @@
         <v>2</v>
       </c>
       <c r="O51" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N51),#REF!/ N51,"")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -3016,10 +3016,10 @@
         <v>30</v>
       </c>
       <c r="J52" t="s">
-        <v>167</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>124</v>
+        <v>165</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L52" t="s">
         <v>46</v>
@@ -3033,13 +3033,13 @@
         <v>2</v>
       </c>
       <c r="O52" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N52),#REF!/ N52,"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
@@ -3048,10 +3048,10 @@
         <v>34</v>
       </c>
       <c r="J53" t="s">
-        <v>169</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>124</v>
+        <v>167</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L53" t="s">
         <v>42</v>
@@ -3065,13 +3065,13 @@
         <v>2</v>
       </c>
       <c r="O53" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N53),#REF!/ N53,"")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
@@ -3083,10 +3083,10 @@
         <v>32</v>
       </c>
       <c r="J54" t="s">
-        <v>142</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>124</v>
+        <v>140</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L54" t="s">
         <v>57</v>
@@ -3100,7 +3100,7 @@
         <v>5.8153627635310006</v>
       </c>
       <c r="O54" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N54),#REF!/ N54,"")</f>
         <v/>
       </c>
     </row>
@@ -3112,16 +3112,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J55" t="s">
-        <v>141</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>124</v>
+        <v>139</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="L55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="M55">
         <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:I$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3132,7 +3132,7 @@
         <v>2</v>
       </c>
       <c r="O55" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(#REF!/N55),#REF!/ N55,"")</f>
         <v/>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,25 +3169,25 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>159</v>
-      </c>
       <c r="I1" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Economy!A13)+SUMIFS(Deck!B:B,Deck!E:E,Economy!A13)</f>
@@ -3647,7 +3647,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3657,9 +3657,9 @@
     <col min="3" max="3" width="11" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.85546875" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" style="51" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
@@ -3667,68 +3667,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
       <c r="I1" s="37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="50"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>172</v>
-      </c>
       <c r="H2" s="41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I2" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>172</v>
-      </c>
       <c r="L2" s="39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="17">
         <f>IF(ISNA(VLOOKUP(A3,Deck!C:O,12,FALSE)),"",VLOOKUP(A3,Deck!C:O,12,FALSE))</f>
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <f>IF(ISNA(VLOOKUP(A3,Deck!C:O,9,FALSE)),"",VLOOKUP(A3,Deck!C:O,9,FALSE))</f>
+        <f>IF(ISNA(VLOOKUP(A3,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A3,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
       <c r="F3" s="17" t="str">
@@ -3748,10 +3748,10 @@
       </c>
       <c r="K3" s="3">
         <f>IF(ISNA(VLOOKUP(I3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I3,Deck!$C:$O,9,FALSE))</f>
-        <v>3</v>
-      </c>
-      <c r="L3" s="53" t="s">
-        <v>194</v>
+        <v>30</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3763,14 +3763,14 @@
         <v>3.7179619625911169</v>
       </c>
       <c r="C4" s="3">
-        <f>IF(ISNA(VLOOKUP(A4,Deck!C:O,9,FALSE)),"",VLOOKUP(A4,Deck!C:O,9,FALSE))</f>
-        <v>2</v>
+        <f>IF(ISNA(VLOOKUP(A4,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A4,Deck!C:O,9,FALSE))</f>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="17">
         <f>IF(ISNA(VLOOKUP(E4,Deck!C:O,12,FALSE)),"",VLOOKUP(E4,Deck!C:O,12,FALSE))</f>
@@ -3780,11 +3780,11 @@
         <f>IF(ISNA(VLOOKUP(E4,Deck!C:O,9,FALSE)),"",VLOOKUP(E4,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H4" s="53" t="s">
-        <v>178</v>
+      <c r="H4" s="51" t="s">
+        <v>176</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J4" s="17">
         <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,12,FALSE))</f>
@@ -3794,18 +3794,18 @@
         <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="53"/>
+      <c r="L4" s="51"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="17">
         <f>IF(ISNA(VLOOKUP(A5,Deck!C:O,12,FALSE)),"",VLOOKUP(A5,Deck!C:O,12,FALSE))</f>
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <f>IF(ISNA(VLOOKUP(A5,Deck!C:O,9,FALSE)),"",VLOOKUP(A5,Deck!C:O,9,FALSE))</f>
+        <f>IF(ISNA(VLOOKUP(A5,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A5,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
       <c r="E5" s="38" t="s">
@@ -3818,8 +3818,8 @@
         <f>IF(ISNA(VLOOKUP(E5,Deck!C:O,9,FALSE)),"",VLOOKUP(E5,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="53" t="s">
-        <v>177</v>
+      <c r="H5" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>18</v>
@@ -3829,28 +3829,28 @@
       </c>
       <c r="K5" s="3">
         <f>IF(ISNA(VLOOKUP(I5,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I5,Deck!$C:$O,9,FALSE))</f>
-        <v>2</v>
-      </c>
-      <c r="L5" s="53" t="s">
-        <v>182</v>
+        <v>20</v>
+      </c>
+      <c r="L5" s="51" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="3">
-        <f>IF(ISNA(VLOOKUP(A6,Deck!C:O,9,FALSE)),"",VLOOKUP(A6,Deck!C:O,9,FALSE))</f>
-        <v>5</v>
+        <f>IF(ISNA(VLOOKUP(A6,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A6,Deck!C:O,9,FALSE))</f>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -3859,11 +3859,11 @@
         <f>IF(ISNA(VLOOKUP(E6,Deck!C:O,9,FALSE)),"",VLOOKUP(E6,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="53" t="s">
-        <v>176</v>
+      <c r="H6" s="51" t="s">
+        <v>174</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J6" s="17">
         <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,12,FALSE))</f>
@@ -3873,24 +3873,24 @@
         <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="L6" s="53"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="3">
-        <f>IF(ISNA(VLOOKUP(A7,Deck!C:O,9,FALSE)),"",VLOOKUP(A7,Deck!C:O,9,FALSE))</f>
-        <v>14</v>
+        <f>IF(ISNA(VLOOKUP(A7,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A7,Deck!C:O,9,FALSE))</f>
+        <v>140</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -3899,39 +3899,39 @@
         <f>IF(ISNA(VLOOKUP(E7,Deck!C:O,9,FALSE)),"",VLOOKUP(E7,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="53" t="s">
-        <v>179</v>
+      <c r="H7" s="51" t="s">
+        <v>177</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="17">
         <v>2</v>
       </c>
       <c r="K7" s="3">
         <f>IF(ISNA(VLOOKUP(I7,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I7,Deck!$C:$O,9,FALSE))</f>
-        <v>12</v>
-      </c>
-      <c r="L7" s="53" t="s">
-        <v>187</v>
+        <v>120</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <f>IF(ISNA(VLOOKUP(A8,Deck!C:O,9,FALSE)),"",VLOOKUP(A8,Deck!C:O,9,FALSE))</f>
+        <f>IF(ISNA(VLOOKUP(A8,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A8,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="17">
         <f>IF(ISNA(VLOOKUP(E8,Deck!C:O,12,FALSE)),"",VLOOKUP(E8,Deck!C:O,12,FALSE))</f>
@@ -3941,8 +3941,8 @@
         <f>IF(ISNA(VLOOKUP(E8,Deck!C:O,9,FALSE)),"",VLOOKUP(E8,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="53" t="s">
-        <v>178</v>
+      <c r="H8" s="51" t="s">
+        <v>176</v>
       </c>
       <c r="I8" s="38" t="s">
         <v>38</v>
@@ -3952,25 +3952,25 @@
       </c>
       <c r="K8" s="3">
         <f>IF(ISNA(VLOOKUP(I8,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I8,Deck!$C:$O,9,FALSE))</f>
-        <v>5</v>
-      </c>
-      <c r="L8" s="53" t="s">
-        <v>195</v>
+        <v>50</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="3">
-        <f>IF(ISNA(VLOOKUP(A9,Deck!C:O,9,FALSE)),"",VLOOKUP(A9,Deck!C:O,9,FALSE))</f>
-        <v>11</v>
+        <f>IF(ISNA(VLOOKUP(A9,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A9,Deck!C:O,9,FALSE))</f>
+        <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E9" s="38" t="s">
         <v>43</v>
@@ -3980,13 +3980,13 @@
       </c>
       <c r="G9" s="3">
         <f>IF(ISNA(VLOOKUP(E9,Deck!C:O,9,FALSE)),"",VLOOKUP(E9,Deck!C:O,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="53" t="s">
-        <v>177</v>
+        <v>5</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>175</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J9" s="17">
         <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,12,FALSE))</f>
@@ -3996,21 +3996,21 @@
         <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="L9" s="53"/>
+      <c r="L9" s="51"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <f>IF(ISNA(VLOOKUP(A10,Deck!C:O,9,FALSE)),"",VLOOKUP(A10,Deck!C:O,9,FALSE))</f>
+        <f>IF(ISNA(VLOOKUP(A10,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A10,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>43</v>
@@ -4020,13 +4020,13 @@
       </c>
       <c r="G10" s="3">
         <f>IF(ISNA(VLOOKUP(E10,Deck!C:O,9,FALSE)),"",VLOOKUP(E10,Deck!C:O,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="I10" s="59" t="s">
-        <v>97</v>
+        <v>5</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="53" t="s">
+        <v>96</v>
       </c>
       <c r="J10" s="17">
         <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,12,FALSE))</f>
@@ -4036,24 +4036,24 @@
         <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="L10" s="53"/>
+      <c r="L10" s="51"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="3">
-        <f>IF(ISNA(VLOOKUP(A11,Deck!C:O,9,FALSE)),"",VLOOKUP(A11,Deck!C:O,9,FALSE))</f>
-        <v>13</v>
+        <f>IF(ISNA(VLOOKUP(A11,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A11,Deck!C:O,9,FALSE))</f>
+        <v>130</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4062,34 +4062,36 @@
         <f>IF(ISNA(VLOOKUP(E11,Deck!C:O,9,FALSE)),"",VLOOKUP(E11,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H11" s="53" t="s">
-        <v>180</v>
+      <c r="H11" s="51" t="s">
+        <v>178</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J11" s="17">
         <v>2</v>
       </c>
       <c r="K11" s="3">
         <f>IF(ISNA(VLOOKUP(I11,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I11,Deck!$C:$O,9,FALSE))</f>
-        <v>7</v>
-      </c>
-      <c r="L11" s="53" t="s">
-        <v>195</v>
+        <v>70</v>
+      </c>
+      <c r="L11" s="51" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A13,Deck!C:O,12,FALSE)),"",VLOOKUP(A13,Deck!C:O,12,FALSE))</f>
-        <v/>
+      <c r="A12" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="17">
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A12,Deck!C:O,9,FALSE)),"",VLOOKUP(A12,Deck!C:O,9,FALSE))</f>
-        <v/>
+        <f>IF(ISNA(VLOOKUP(A12,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A12,Deck!C:O,9,FALSE))</f>
+        <v>*</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" s="17">
         <f>IF(ISNA(VLOOKUP(E12,Deck!C:O,12,FALSE)),"",VLOOKUP(E12,Deck!C:O,12,FALSE))</f>
@@ -4099,7 +4101,7 @@
         <f>IF(ISNA(VLOOKUP(E12,Deck!C:O,9,FALSE)),"",VLOOKUP(E12,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="51" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="38" t="s">
@@ -4110,10 +4112,10 @@
       </c>
       <c r="K12" s="3">
         <f>IF(ISNA(VLOOKUP(I12,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I12,Deck!$C:$O,9,FALSE))</f>
-        <v>4</v>
-      </c>
-      <c r="L12" s="53" t="s">
-        <v>194</v>
+        <v>40</v>
+      </c>
+      <c r="L12" s="51" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4121,12 +4123,8 @@
         <f>IF(ISNA(VLOOKUP(A14,Deck!C:O,12,FALSE)),"",VLOOKUP(A14,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C13" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A13,Deck!C:O,9,FALSE)),"",VLOOKUP(A13,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="E13" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" s="17">
         <f>IF(ISNA(VLOOKUP(E13,Deck!C:O,12,FALSE)),"",VLOOKUP(E13,Deck!C:O,12,FALSE))</f>
@@ -4136,8 +4134,8 @@
         <f>IF(ISNA(VLOOKUP(E13,Deck!C:O,9,FALSE)),"",VLOOKUP(E13,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H13" s="53" t="s">
-        <v>113</v>
+      <c r="H13" s="51" t="s">
+        <v>112</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>56</v>
@@ -4147,10 +4145,10 @@
       </c>
       <c r="K13" s="3">
         <f>IF(ISNA(VLOOKUP(I13,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I13,Deck!$C:$O,9,FALSE))</f>
-        <v>4</v>
-      </c>
-      <c r="L13" s="53" t="s">
-        <v>194</v>
+        <v>40</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4158,10 +4156,6 @@
         <f>IF(ISNA(VLOOKUP(A15,Deck!C:O,12,FALSE)),"",VLOOKUP(A15,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C14" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A14,Deck!C:O,9,FALSE)),"",VLOOKUP(A14,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="E14" s="38" t="s">
         <v>58</v>
       </c>
@@ -4173,7 +4167,7 @@
         <f>IF(ISNA(VLOOKUP(E14,Deck!C:O,9,FALSE)),"",VLOOKUP(E14,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="51" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="38"/>
@@ -4185,19 +4179,15 @@
         <f>IF(ISNA(VLOOKUP(I14,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I14,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L14" s="53"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A16,Deck!C:O,12,FALSE)),"",VLOOKUP(A16,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C15" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A15,Deck!C:O,9,FALSE)),"",VLOOKUP(A15,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="E15" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" s="17">
         <f>IF(ISNA(VLOOKUP(E15,Deck!C:O,12,FALSE)),"",VLOOKUP(E15,Deck!C:O,12,FALSE))</f>
@@ -4207,7 +4197,7 @@
         <f>IF(ISNA(VLOOKUP(E15,Deck!C:O,9,FALSE)),"",VLOOKUP(E15,Deck!C:O,9,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="H15" s="53" t="s">
+      <c r="H15" s="51" t="s">
         <v>15</v>
       </c>
       <c r="I15" s="38"/>
@@ -4219,8 +4209,8 @@
         <f>IF(ISNA(VLOOKUP(I15,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I15,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L15" s="53" t="s">
-        <v>196</v>
+      <c r="L15" s="51" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4228,10 +4218,6 @@
         <f>IF(ISNA(VLOOKUP(A17,Deck!C:O,12,FALSE)),"",VLOOKUP(A17,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C16" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A16,Deck!C:O,9,FALSE)),"",VLOOKUP(A16,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="F16" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E16,Deck!C:O,12,FALSE)),"",VLOOKUP(E16,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4249,17 +4235,13 @@
         <f>IF(ISNA(VLOOKUP(I16,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I16,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L16" s="53"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A18,Deck!C:O,12,FALSE)),"",VLOOKUP(A18,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C17" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A17,Deck!C:O,9,FALSE)),"",VLOOKUP(A17,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="F17" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E17,Deck!C:O,12,FALSE)),"",VLOOKUP(E17,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4277,17 +4259,13 @@
         <f>IF(ISNA(VLOOKUP(I17,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I17,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L17" s="53"/>
+      <c r="L17" s="51"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C18" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A18,Deck!C:O,9,FALSE)),"",VLOOKUP(A18,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="F18" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E18,Deck!C:O,12,FALSE)),"",VLOOKUP(E18,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4305,19 +4283,15 @@
         <f>IF(ISNA(VLOOKUP(I18,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I18,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L18" s="53"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C19" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,9,FALSE)),"",VLOOKUP(A19,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
       <c r="E19" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Deck!C:O,12,FALSE)),"",VLOOKUP(E19,Deck!C:O,12,FALSE))</f>
@@ -4326,8 +4300,8 @@
       <c r="G19" s="3">
         <v>9</v>
       </c>
-      <c r="H19" s="53" t="s">
-        <v>190</v>
+      <c r="H19" s="51" t="s">
+        <v>188</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="17" t="str">
@@ -4338,20 +4312,17 @@
         <f>IF(ISNA(VLOOKUP(I19,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I19,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L19" s="53"/>
-    </row>
-    <row r="20" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="51"/>
+    </row>
+    <row r="20" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A20,Deck!C:O,12,FALSE)),"",VLOOKUP(A20,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="C20" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A20,Deck!C:O,9,FALSE)),"",VLOOKUP(A20,Deck!C:O,9,FALSE))</f>
-        <v/>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -4359,8 +4330,8 @@
       <c r="G20" s="3">
         <v>25</v>
       </c>
-      <c r="H20" s="53" t="s">
-        <v>189</v>
+      <c r="H20" s="51" t="s">
+        <v>187</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="17" t="str">
@@ -4371,21 +4342,14 @@
         <f>IF(ISNA(VLOOKUP(I20,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I20,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L20" s="53"/>
-    </row>
-    <row r="21" spans="1:12" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="17">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3">
-        <v>5</v>
-      </c>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Deck!C:O,12,FALSE)),"",VLOOKUP(E21,Deck!C:O,12,FALSE))</f>
@@ -4394,8 +4358,8 @@
       <c r="G21" s="3">
         <v>24</v>
       </c>
-      <c r="H21" s="53" t="s">
-        <v>181</v>
+      <c r="H21" s="51" t="s">
+        <v>179</v>
       </c>
       <c r="I21" s="38" t="s">
         <v>34</v>
@@ -4407,96 +4371,84 @@
       <c r="K21" s="3">
         <v>24</v>
       </c>
-      <c r="L21" s="53"/>
-    </row>
-    <row r="22" spans="1:12" s="45" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="B22" s="52">
+      <c r="L21" s="51"/>
+    </row>
+    <row r="22" spans="1:12" s="43" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="50">
         <f>SUM(B3:B21)</f>
         <v>17.717961962591119</v>
       </c>
-      <c r="C22" s="51">
+      <c r="C22" s="49">
         <f>SUM(C3:C21)</f>
-        <v>50</v>
-      </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="F22" s="48">
+        <v>450</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="46">
         <f>SUM(F3:F21)</f>
         <v>20</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="43">
         <f>SUM(G3:G21)</f>
-        <v>58</v>
-      </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="J22" s="48">
+        <v>68</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="J22" s="46">
         <f>SUM(J3:J21)</f>
         <v>20</v>
       </c>
-      <c r="K22" s="45">
+      <c r="K22" s="43">
         <f>SUM(K3:K21)</f>
-        <v>61</v>
-      </c>
-      <c r="L22" s="54"/>
+        <v>394</v>
+      </c>
+      <c r="L22" s="52"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" s="17">
         <f>C22/B22</f>
-        <v>2.8219949961269628</v>
+        <v>25.397954965142667</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="F23" s="49">
+        <v>172</v>
+      </c>
+      <c r="F23" s="47">
         <f>G22/F22</f>
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="J23" s="49">
+        <v>172</v>
+      </c>
+      <c r="J23" s="47">
         <f>K22/J22</f>
-        <v>3.05</v>
-      </c>
-      <c r="L23" s="53"/>
+        <v>19.7</v>
+      </c>
+      <c r="L23" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12">
-      <formula1>$C$3:$C$55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A16:A21">
-      <formula1>$C$3:$C$55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A10">
-      <formula1>$C$3:$C$55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I21">
-      <formula1>$C$3:$C$55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I9">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12 A12 A16:A20 I3:I9 I11:I21 A3:A10">
       <formula1>$C$3:$C$55</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Deck!$C$3:$C$55</xm:f>

</xml_diff>

<commit_message>
shorten descriptions, general tweaking
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\victory-point-salad\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\code\victory-point-salad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,9 +408,6 @@
     <t>This card is as close at this game gets to Victory Point Points.</t>
   </si>
   <si>
-    <t>Upon playing, you may retrieve any card in the discard piles and play it immediately without prerequisites.</t>
-  </si>
-  <si>
     <t xml:space="preserve">You may trash 1 Cattle for 2 Food, and/or 1 Cattle for any Resource. </t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>The Combo Building</t>
   </si>
   <si>
-    <t xml:space="preserve">When this card is revealed, all Blockers must be paid by the end of the turn. Initiate Endgame. </t>
-  </si>
-  <si>
     <t>1 VP for each Building you've played</t>
   </si>
   <si>
@@ -525,9 +519,6 @@
     <t>The Combo Materials</t>
   </si>
   <si>
-    <t>3 VP for each Military, +3 additional VP if you end the game with the most military (ties don't count).</t>
-  </si>
-  <si>
     <t>Card</t>
   </si>
   <si>
@@ -684,9 +675,6 @@
     <t>Draw 2 Extra Resources</t>
   </si>
   <si>
-    <t>Highest Military may trash any 1 Special on the tableau at the beginning of the round. Nobody gets to do this in a tie.</t>
-  </si>
-  <si>
     <t>Soldier</t>
   </si>
   <si>
@@ -724,6 +712,18 @@
   </si>
   <si>
     <t>Stone Climb!</t>
+  </si>
+  <si>
+    <t>Highest Military may trash any 1 available Special at round start.</t>
+  </si>
+  <si>
+    <t>3 VP for each Soldier, +3 additional VP if you end the game with the most soldiers.</t>
+  </si>
+  <si>
+    <t>Upon playing, retrieve any Trashed card and play it immediately without prerequisites.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Blockers must be paid by the end of this turn. Initiate Endgame. </t>
   </si>
 </sst>
 </file>
@@ -1346,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,7 @@
     <col min="4" max="5" width="8.125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.75" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.75" customWidth="1"/>
+    <col min="10" max="10" width="75.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.75" customWidth="1"/>
     <col min="13" max="13" width="11" style="17" bestFit="1" customWidth="1"/>
@@ -1405,13 +1405,13 @@
         <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K2" s="5">
         <v>40</v>
@@ -1461,7 +1461,7 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K3" s="5">
         <v>20</v>
@@ -1493,10 +1493,10 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J4" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K4" s="5">
         <v>30</v>
@@ -1531,7 +1531,7 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K5" s="5">
         <v>20</v>
@@ -1566,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K6" s="5">
         <v>20</v>
@@ -1595,10 +1595,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" t="s">
         <v>207</v>
-      </c>
-      <c r="J7" t="s">
-        <v>210</v>
       </c>
       <c r="K7" s="5">
         <v>20</v>
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M9" s="28"/>
       <c r="N9" s="28">
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="54" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M10" s="28"/>
       <c r="N10" s="28">
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="54" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M11" s="28"/>
       <c r="N11" s="28">
@@ -1716,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>14</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="54" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="M12" s="28"/>
       <c r="N12" s="28">
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D18" s="54" t="s">
         <v>8</v>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M18" s="28"/>
       <c r="N18" s="28">
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M19" s="28"/>
       <c r="N19" s="28">
@@ -1962,7 +1962,7 @@
         <v>16</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K21" s="5">
         <v>20</v>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="54" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="M22" s="28"/>
       <c r="N22" s="28">
@@ -2091,7 +2091,7 @@
         <v>32</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K25" s="5">
         <v>50</v>
@@ -2158,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>11</v>
@@ -2173,7 +2173,7 @@
         <v>50</v>
       </c>
       <c r="L27" s="55" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M27" s="24">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:I$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2196,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>8</v>
@@ -2211,7 +2211,7 @@
         <v>50</v>
       </c>
       <c r="L28" s="55" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M28" s="24">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:I$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>14</v>
@@ -2272,11 +2272,11 @@
         <v>1</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="25"/>
       <c r="J30" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K30" s="5">
         <v>30</v>
@@ -2308,19 +2308,19 @@
         <v>38</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="55" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K31" s="5">
         <v>50</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="32" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="30">
         <v>1</v>
@@ -2355,7 +2355,7 @@
         <v>11</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K32" s="5">
         <v>60</v>
@@ -2378,13 +2378,13 @@
     </row>
     <row r="33" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" s="30">
         <v>1</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D33" s="32" t="s">
         <v>12</v>
@@ -2399,7 +2399,7 @@
         <v>10</v>
       </c>
       <c r="L33" s="32" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M33" s="31">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:I$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="34" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" s="30">
         <v>2</v>
@@ -2440,7 +2440,7 @@
         <v>10</v>
       </c>
       <c r="L34" s="32" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M34" s="31">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:I$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="35" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" s="30">
         <v>2</v>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="36" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B36" s="30">
         <v>1</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>14</v>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="37" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B37" s="30">
         <v>1</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="38" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" s="30">
         <v>1</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="39" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B39" s="30">
         <v>1</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="40" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40" s="30">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>140</v>
       </c>
       <c r="L40" s="32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M40" s="31">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:I$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="41" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="30">
         <v>2</v>
@@ -2723,13 +2723,13 @@
     </row>
     <row r="42" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="30">
         <v>2</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D42" s="29" t="s">
         <v>112</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="43" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="30">
         <v>2</v>
@@ -2782,7 +2782,7 @@
         <v>33</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K43" s="5">
         <v>40</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="44" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="30">
         <v>1</v>
@@ -2826,7 +2826,7 @@
         <v>33</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K44" s="5">
         <v>70</v>
@@ -2849,25 +2849,25 @@
     </row>
     <row r="45" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="30">
         <v>1</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F45" s="32" t="s">
         <v>12</v>
       </c>
       <c r="J45" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K45" s="5">
         <v>10</v>
       </c>
       <c r="L45" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="M45" s="31">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:I$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2884,25 +2884,25 @@
     </row>
     <row r="46" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" s="30">
         <v>1</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F46" s="32" t="s">
         <v>23</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K46" s="5">
         <v>10</v>
       </c>
       <c r="L46" s="32" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="M46" s="31">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,Economy!A$2:I$13,9,FALSE),0)+IF(G46&lt;&gt;"",VLOOKUP(G46,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2919,25 +2919,25 @@
     </row>
     <row r="47" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B47" s="30">
         <v>1</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K47" s="5">
         <v>10</v>
       </c>
       <c r="L47" s="32" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="M47" s="31">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:I$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2958,13 +2958,13 @@
         <v>1</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F48" s="32" t="s">
         <v>11</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K48" s="5">
         <v>20</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="49" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B49" s="30">
         <v>1</v>
@@ -2987,8 +2987,8 @@
       <c r="F49" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J49" s="29" t="s">
-        <v>127</v>
+      <c r="J49" s="32" t="s">
+        <v>231</v>
       </c>
       <c r="K49" s="5">
         <v>30</v>
@@ -3011,22 +3011,22 @@
     </row>
     <row r="50" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B50" s="30">
         <v>1</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J50" s="32" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K50" s="5">
         <v>20</v>
       </c>
       <c r="L50" s="32" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M50" s="31">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:I$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3043,13 +3043,13 @@
     </row>
     <row r="51" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" s="30">
         <v>1</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F51" s="32" t="s">
         <v>8</v>
@@ -3058,13 +3058,13 @@
         <v>8</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K51" s="5">
         <v>40</v>
       </c>
       <c r="L51" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M51" s="31">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,Economy!A$2:I$13,9,FALSE),0)+IF(G51&lt;&gt;"",VLOOKUP(G51,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -3090,10 +3090,10 @@
         <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L52" t="s">
         <v>126</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
@@ -3122,10 +3122,10 @@
         <v>114</v>
       </c>
       <c r="J53" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L53" t="s">
         <v>115</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
@@ -3189,10 +3189,10 @@
         <v>122</v>
       </c>
       <c r="J55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L55" t="s">
         <v>39</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
@@ -3221,10 +3221,10 @@
         <v>78</v>
       </c>
       <c r="J56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L56" t="s">
         <v>40</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
@@ -3252,10 +3252,10 @@
         <v>121</v>
       </c>
       <c r="J57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L57" t="s">
         <v>28</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B58" s="3">
         <v>1</v>
@@ -3284,10 +3284,10 @@
         <v>30</v>
       </c>
       <c r="J58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L58" t="s">
         <v>46</v>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B59" s="3">
         <v>1</v>
@@ -3316,10 +3316,10 @@
         <v>34</v>
       </c>
       <c r="J59" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L59" t="s">
         <v>42</v>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B60" s="3">
         <v>1</v>
@@ -3351,10 +3351,10 @@
         <v>32</v>
       </c>
       <c r="J60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L60" t="s">
         <v>57</v>
@@ -3380,16 +3380,16 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J61" t="s">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L61" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M61">
         <f>IF(F61&lt;&gt;"",VLOOKUP(F61,Economy!A$2:I$13,9,FALSE),0)+IF(G61&lt;&gt;"",VLOOKUP(G61,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3440,22 +3440,22 @@
         <v>116</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>156</v>
-      </c>
       <c r="I1" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3936,55 +3936,55 @@
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
       <c r="D1" s="61"/>
       <c r="E1" s="56" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F1" s="57"/>
       <c r="G1" s="57"/>
       <c r="H1" s="58"/>
       <c r="I1" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="40" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G2" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="41" t="s">
-        <v>172</v>
-      </c>
       <c r="I2" s="39" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K2" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>169</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4019,7 +4019,7 @@
         <v>30</v>
       </c>
       <c r="L3" s="51" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4035,7 +4035,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>107</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I4" s="38" t="s">
         <v>101</v>
@@ -4087,7 +4087,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>18</v>
@@ -4100,12 +4100,12 @@
         <v>20</v>
       </c>
       <c r="L5" s="51" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4115,7 +4115,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>87</v>
@@ -4128,7 +4128,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I6" s="38" t="s">
         <v>96</v>
@@ -4155,7 +4155,7 @@
         <v>140</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>87</v>
@@ -4168,7 +4168,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>118</v>
@@ -4181,7 +4181,7 @@
         <v>120</v>
       </c>
       <c r="L7" s="51" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>105</v>
@@ -4210,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="51" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I8" s="38" t="s">
         <v>38</v>
@@ -4223,7 +4223,7 @@
         <v>50</v>
       </c>
       <c r="L8" s="51" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4238,7 +4238,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E9" s="38" t="s">
         <v>43</v>
@@ -4251,7 +4251,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="51" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I9" s="38" t="s">
         <v>96</v>
@@ -4278,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>43</v>
@@ -4291,7 +4291,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="51" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I10" s="53" t="s">
         <v>96</v>
@@ -4318,10 +4318,10 @@
         <v>130</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4331,7 +4331,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="51" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I11" s="38" t="s">
         <v>123</v>
@@ -4344,7 +4344,7 @@
         <v>70</v>
       </c>
       <c r="L11" s="51" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
         <v>40</v>
       </c>
       <c r="L12" s="51" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>40</v>
       </c>
       <c r="L13" s="51" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4478,7 +4478,7 @@
         <v/>
       </c>
       <c r="L15" s="51" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4559,7 +4559,7 @@
         <v/>
       </c>
       <c r="E19" s="38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Deck!C:O,12,FALSE)),"",VLOOKUP(E19,Deck!C:O,12,FALSE))</f>
@@ -4569,7 +4569,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="17" t="str">
@@ -4599,7 +4599,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="51" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="17" t="str">
@@ -4627,7 +4627,7 @@
         <v>24</v>
       </c>
       <c r="H21" s="51" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I21" s="38" t="s">
         <v>34</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="22" spans="1:12" s="43" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B22" s="50">
         <f>SUM(B3:B21)</f>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F22" s="46">
         <f>SUM(F3:F21)</f>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J22" s="46">
         <f>SUM(J3:J21)</f>
@@ -4681,21 +4681,21 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B23" s="17">
         <f>C22/B22</f>
         <v>25.397954965142667</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F23" s="47">
         <f>G22/F22</f>
         <v>4.9000000000000004</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J23" s="47">
         <f>K22/J22</f>
@@ -4746,21 +4746,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4790,7 +4790,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,7 +4805,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4820,7 +4820,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,7 +4835,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding in point ladder - printing out
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="232">
   <si>
     <t>Type</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Building</t>
   </si>
   <si>
-    <t>Military</t>
-  </si>
-  <si>
     <t>The Military Payoff</t>
   </si>
   <si>
@@ -441,24 +438,12 @@
     <t>The Combo Building</t>
   </si>
   <si>
-    <t>1 VP for each Building you've played</t>
-  </si>
-  <si>
-    <t>8VP if you have Invested plus 3VP for each Gold.</t>
-  </si>
-  <si>
     <t>Personally, I find grain to be much more filling than carrots</t>
   </si>
   <si>
     <t>Eat More Veggies!</t>
   </si>
   <si>
-    <t>5 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
-  </si>
-  <si>
-    <t>3 VP for each Wood, Sheep, or Grain</t>
-  </si>
-  <si>
     <t>You may trash 1 Silk for any 2 Resources, any number of times.</t>
   </si>
   <si>
@@ -510,12 +495,6 @@
     <t>Trash1 Cost</t>
   </si>
   <si>
-    <t>3 VPs for each Payoff you have placed.</t>
-  </si>
-  <si>
-    <t>At game end, take the number of Glass and Silk you have. Square that for VPs.</t>
-  </si>
-  <si>
     <t>The Combo Materials</t>
   </si>
   <si>
@@ -570,9 +549,6 @@
     <t>Building Strategy, Not much chaining</t>
   </si>
   <si>
-    <t>Use military</t>
-  </si>
-  <si>
     <t>The Payoff with Math</t>
   </si>
   <si>
@@ -591,18 +567,6 @@
     <t>Pay 1xClay, no stone</t>
   </si>
   <si>
-    <t>1xMilitary</t>
-  </si>
-  <si>
-    <t>2xMilitary</t>
-  </si>
-  <si>
-    <t>This has an efficient sequence, but it's easily disrupted.</t>
-  </si>
-  <si>
-    <t>6 VPs for each Cattle, Carrot</t>
-  </si>
-  <si>
     <t>The Strange Combo</t>
   </si>
   <si>
@@ -717,13 +681,46 @@
     <t>Highest Military may trash any 1 available Special at round start.</t>
   </si>
   <si>
-    <t>3 VP for each Soldier, +3 additional VP if you end the game with the most soldiers.</t>
-  </si>
-  <si>
     <t>Upon playing, retrieve any Trashed card and play it immediately without prerequisites.</t>
   </si>
   <si>
     <t xml:space="preserve">All Blockers must be paid by the end of this turn. Initiate Endgame. </t>
+  </si>
+  <si>
+    <t>Stone ladders: also known as "steps"</t>
+  </si>
+  <si>
+    <t>See you at the top!</t>
+  </si>
+  <si>
+    <t>Take the total number of Glass and Silk you have. Square then multiply by 10 for VPs.</t>
+  </si>
+  <si>
+    <t>10 VP for each Building you've played</t>
+  </si>
+  <si>
+    <t>30 VP for each Soldier, +30 additional VP if you end the game with the most soldiers.</t>
+  </si>
+  <si>
+    <t>30 VP for each Wood, Sheep, or Grain</t>
+  </si>
+  <si>
+    <t>50 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
+  </si>
+  <si>
+    <t>60 VPs for each Cattle, Carrot</t>
+  </si>
+  <si>
+    <t>30 VPs for each Payoff you have placed.</t>
+  </si>
+  <si>
+    <t>80 VP if you have Invested plus 30 VP for each Gold.</t>
+  </si>
+  <si>
+    <t>Ladder Strategy</t>
+  </si>
+  <si>
+    <t>Figure this out with the new rule</t>
   </si>
 </sst>
 </file>
@@ -1346,9 +1343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1357,7 @@
     <col min="6" max="7" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.75" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="75.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.75" customWidth="1"/>
     <col min="13" max="13" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.875" style="17" bestFit="1" customWidth="1"/>
@@ -1384,10 +1381,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>104</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>19</v>
@@ -1405,40 +1402,40 @@
         <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K2" s="5">
         <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="33"/>
@@ -1446,7 +1443,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1461,13 +1458,13 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" s="5">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M3" s="35">
         <f>IF(F3&lt;&gt;"",VLOOKUP(F3,Economy!A$2:I$13,9,FALSE),0)+IF(G3&lt;&gt;"",VLOOKUP(G3,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1484,7 +1481,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1493,16 +1490,16 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="J4" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="K4" s="5">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M4" s="35">
         <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:I$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1519,25 +1516,25 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K5" s="5">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M5" s="35">
         <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:I$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1554,25 +1551,25 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="K6" s="5">
         <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M6" s="35">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:I$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -1589,19 +1586,22 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="J7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="K7" s="5">
         <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>221</v>
       </c>
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
@@ -1609,22 +1609,22 @@
     </row>
     <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K8" s="5">
-        <v>-80</v>
+        <v>-100</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>8</v>
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="M9" s="28"/>
       <c r="N9" s="28">
@@ -1663,7 +1663,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>14</v>
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="54" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="M10" s="28"/>
       <c r="N10" s="28">
@@ -1691,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>11</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="54" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="M11" s="28"/>
       <c r="N11" s="28">
@@ -1716,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>14</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="54" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="M12" s="28"/>
       <c r="N12" s="28">
@@ -1744,7 +1744,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>26</v>
@@ -1769,7 +1769,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>12</v>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M14" s="28"/>
       <c r="N14" s="28">
@@ -1794,7 +1794,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>13</v>
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M15" s="28"/>
       <c r="N15" s="28">
@@ -1819,7 +1819,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>27</v>
@@ -1828,13 +1828,13 @@
         <v>27</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="28">
@@ -1850,7 +1850,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>23</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M17" s="28"/>
       <c r="N17" s="28">
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D18" s="54" t="s">
         <v>8</v>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="M18" s="28"/>
       <c r="N18" s="28">
@@ -1903,19 +1903,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M19" s="28"/>
       <c r="N19" s="28">
@@ -1931,7 +1931,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>15</v>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M20" s="28"/>
       <c r="N20" s="28">
@@ -1956,19 +1956,19 @@
         <v>3</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>16</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="K21" s="5">
         <v>20</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M21" s="28"/>
       <c r="N21" s="28">
@@ -1984,7 +1984,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>25</v>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="54" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="M22" s="28"/>
       <c r="N22" s="28">
@@ -2003,25 +2003,25 @@
     </row>
     <row r="23" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="B23" s="23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>91</v>
       </c>
       <c r="K23" s="5">
         <v>30</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M23" s="24">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,Economy!A$2:I$13,9,FALSE),0)+IF(G23&lt;&gt;"",VLOOKUP(G23,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2038,13 +2038,13 @@
     </row>
     <row r="24" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="23">
         <v>2</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>23</v>
@@ -2056,13 +2056,13 @@
         <v>23</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M24" s="24">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:I$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2079,25 +2079,25 @@
     </row>
     <row r="25" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="23">
         <v>1</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H25" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K25" s="5">
         <v>50</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M25" s="24">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:I$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2114,13 +2114,13 @@
     </row>
     <row r="26" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" s="23">
         <v>3</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>12</v>
@@ -2135,7 +2135,7 @@
         <v>5</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M26" s="24">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:I$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2152,13 +2152,13 @@
     </row>
     <row r="27" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="23">
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>11</v>
@@ -2167,13 +2167,13 @@
         <v>32</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" s="5">
         <v>50</v>
       </c>
       <c r="L27" s="55" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="M27" s="24">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:I$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="28" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="23">
         <v>1</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>8</v>
@@ -2205,13 +2205,13 @@
         <v>32</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K28" s="5">
         <v>50</v>
       </c>
       <c r="L28" s="55" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="M28" s="24">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:I$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="29" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="23">
         <v>1</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>14</v>
@@ -2243,13 +2243,13 @@
         <v>32</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K29" s="5">
         <v>50</v>
       </c>
       <c r="L29" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M29" s="24">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:I$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2266,17 +2266,17 @@
     </row>
     <row r="30" spans="1:15" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="23">
         <v>1</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D30" s="25"/>
       <c r="J30" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K30" s="5">
         <v>30</v>
@@ -2299,34 +2299,34 @@
     </row>
     <row r="31" spans="1:15" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="23">
         <v>1</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="55" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="K31" s="5">
         <v>50</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M31" s="24">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:I$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2343,25 +2343,25 @@
     </row>
     <row r="32" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="30">
         <v>1</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>11</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K32" s="5">
         <v>60</v>
       </c>
       <c r="L32" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M32" s="31">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:I$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2378,13 +2378,13 @@
     </row>
     <row r="33" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="30">
         <v>1</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D33" s="32" t="s">
         <v>12</v>
@@ -2399,7 +2399,7 @@
         <v>10</v>
       </c>
       <c r="L33" s="32" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="M33" s="31">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:I$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2416,13 +2416,13 @@
     </row>
     <row r="34" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="30">
         <v>2</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>23</v>
@@ -2434,13 +2434,13 @@
         <v>23</v>
       </c>
       <c r="J34" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K34" s="5">
         <v>10</v>
       </c>
       <c r="L34" s="32" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="M34" s="31">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:I$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2457,13 +2457,13 @@
     </row>
     <row r="35" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="30">
         <v>2</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>8</v>
@@ -2478,7 +2478,7 @@
         <v>90</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M35" s="31">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:I$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="36" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="30">
         <v>1</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>14</v>
@@ -2516,7 +2516,7 @@
         <v>100</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M36" s="31">
         <f>IF(F36&lt;&gt;"",VLOOKUP(F36,Economy!A$2:I$13,9,FALSE),0)+IF(G36&lt;&gt;"",VLOOKUP(G36,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2533,13 +2533,13 @@
     </row>
     <row r="37" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="30">
         <v>1</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>14</v>
@@ -2554,7 +2554,7 @@
         <v>110</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M37" s="31">
         <f>IF(F37&lt;&gt;"",VLOOKUP(F37,Economy!A$2:I$13,9,FALSE),0)+IF(G37&lt;&gt;"",VLOOKUP(G37,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2571,13 +2571,13 @@
     </row>
     <row r="38" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B38" s="30">
         <v>1</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F38" s="32" t="s">
         <v>8</v>
@@ -2592,7 +2592,7 @@
         <v>120</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M38" s="31">
         <f>IF(F38&lt;&gt;"",VLOOKUP(F38,Economy!A$2:I$13,9,FALSE),0)+IF(G38&lt;&gt;"",VLOOKUP(G38,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2609,13 +2609,13 @@
     </row>
     <row r="39" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="30">
         <v>1</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39" s="32" t="s">
         <v>14</v>
@@ -2630,7 +2630,7 @@
         <v>130</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M39" s="31">
         <f>IF(F39&lt;&gt;"",VLOOKUP(F39,Economy!A$2:I$13,9,FALSE),0)+IF(G39&lt;&gt;"",VLOOKUP(G39,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="40" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="30">
         <v>1</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F40" s="29" t="s">
         <v>11</v>
@@ -2668,7 +2668,7 @@
         <v>140</v>
       </c>
       <c r="L40" s="32" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="M40" s="31">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:I$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2685,13 +2685,13 @@
     </row>
     <row r="41" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="30">
         <v>2</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="29" t="s">
         <v>13</v>
@@ -2706,7 +2706,7 @@
         <v>40</v>
       </c>
       <c r="L41" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M41" s="31">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:I$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2723,31 +2723,31 @@
     </row>
     <row r="42" spans="1:15" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" s="30">
         <v>2</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J42" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K42" s="5">
         <v>10</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M42" s="31">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:I$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2764,31 +2764,31 @@
     </row>
     <row r="43" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="30">
         <v>2</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="F43" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="29" t="s">
-        <v>33</v>
+      <c r="H43" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="K43" s="5">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M43" s="31">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,Economy!A$2:I$13,9,FALSE),0)+IF(G43&lt;&gt;"",VLOOKUP(G43,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2800,39 +2800,39 @@
       </c>
       <c r="O43" s="23">
         <f t="shared" si="0"/>
-        <v>11.234454614281164</v>
+        <v>22.468909228562328</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="30">
         <v>1</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>33</v>
+        <v>122</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="F44" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="29" t="s">
-        <v>33</v>
+      <c r="H44" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="K44" s="5">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M44" s="31">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:I$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2844,30 +2844,30 @@
       </c>
       <c r="O44" s="23">
         <f t="shared" si="0"/>
-        <v>19.279893089755063</v>
+        <v>27.542704413935805</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="30">
         <v>1</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F45" s="32" t="s">
         <v>12</v>
       </c>
       <c r="J45" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K45" s="5">
         <v>10</v>
       </c>
       <c r="L45" s="32" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="M45" s="31">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:I$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2884,25 +2884,25 @@
     </row>
     <row r="46" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="30">
         <v>1</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F46" s="32" t="s">
         <v>23</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K46" s="5">
         <v>10</v>
       </c>
       <c r="L46" s="32" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="M46" s="31">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,Economy!A$2:I$13,9,FALSE),0)+IF(G46&lt;&gt;"",VLOOKUP(G46,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2919,25 +2919,25 @@
     </row>
     <row r="47" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="30">
         <v>1</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K47" s="5">
         <v>10</v>
       </c>
       <c r="L47" s="32" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="M47" s="31">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:I$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -2953,30 +2953,37 @@
       </c>
     </row>
     <row r="48" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="32" t="s">
+        <v>133</v>
+      </c>
       <c r="B48" s="30">
         <v>1</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F48" s="32" t="s">
         <v>11</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K48" s="5">
         <v>20</v>
       </c>
-      <c r="L48" s="32"/>
-      <c r="M48" s="31"/>
+      <c r="L48" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="M48" s="31">
+        <f>IF(F48&lt;&gt;"",VLOOKUP(F48,Economy!A$2:I$13,9,FALSE),0)+IF(G48&lt;&gt;"",VLOOKUP(G48,Economy!A$2:I$13,9,FALSE),0)</f>
+        <v>1.7179619625911169</v>
+      </c>
       <c r="N48" s="31"/>
       <c r="O48" s="23"/>
     </row>
     <row r="49" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="30">
         <v>1</v>
@@ -2988,13 +2995,13 @@
         <v>15</v>
       </c>
       <c r="J49" s="32" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K49" s="5">
         <v>30</v>
       </c>
       <c r="L49" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M49" s="31">
         <f>IF(F49&lt;&gt;"",VLOOKUP(F49,Economy!A$2:I$13,9,FALSE),0)+IF(G49&lt;&gt;"",VLOOKUP(G49,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3011,22 +3018,22 @@
     </row>
     <row r="50" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="30">
         <v>1</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="J50" s="32" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="K50" s="5">
         <v>20</v>
       </c>
       <c r="L50" s="32" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="M50" s="31">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:I$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3043,13 +3050,13 @@
     </row>
     <row r="51" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="30">
         <v>1</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F51" s="32" t="s">
         <v>8</v>
@@ -3058,13 +3065,13 @@
         <v>8</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K51" s="5">
         <v>40</v>
       </c>
       <c r="L51" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M51" s="31">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,Economy!A$2:I$13,9,FALSE),0)+IF(G51&lt;&gt;"",VLOOKUP(G51,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3081,7 +3088,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -3090,13 +3097,13 @@
         <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M52">
         <f>IF(F52&lt;&gt;"",VLOOKUP(F52,Economy!A$2:I$13,9,FALSE),0)+IF(G52&lt;&gt;"",VLOOKUP(G52,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3113,22 +3120,22 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="J53" t="s">
+        <v>227</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L53" t="s">
         <v>114</v>
-      </c>
-      <c r="J53" t="s">
-        <v>191</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="L53" t="s">
-        <v>115</v>
       </c>
       <c r="M53">
         <f>IF(F53&lt;&gt;"",VLOOKUP(F53,Economy!A$2:I$13,9,FALSE),0)+IF(G53&lt;&gt;"",VLOOKUP(G53,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3145,19 +3152,19 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K54" s="5">
         <v>120</v>
@@ -3180,22 +3187,22 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J55" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M55">
         <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:I$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3212,22 +3219,22 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J56" t="s">
-        <v>139</v>
+        <v>229</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M56">
         <v>2</v>
@@ -3243,19 +3250,19 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J57" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L57" t="s">
         <v>28</v>
@@ -3275,7 +3282,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B58" s="3">
         <v>1</v>
@@ -3284,13 +3291,13 @@
         <v>30</v>
       </c>
       <c r="J58" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M58">
         <f>IF(F58&lt;&gt;"",VLOOKUP(F58,Economy!A$2:I$13,9,FALSE),0)+IF(G58&lt;&gt;"",VLOOKUP(G58,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3307,22 +3314,22 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="3">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J59" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M59">
         <f>IF(F59&lt;&gt;"",VLOOKUP(F59,Economy!A$2:I$13,9,FALSE),0)+IF(G59&lt;&gt;"",VLOOKUP(G59,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3339,25 +3346,25 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="3">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H60" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J60" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M60">
         <f>IF(F60&lt;&gt;"",VLOOKUP(F60,Economy!A$2:I$13,9,FALSE),0)+IF(G60&lt;&gt;"",VLOOKUP(G60,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3380,16 +3387,16 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J61" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="L61" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M61">
         <f>IF(F61&lt;&gt;"",VLOOKUP(F61,Economy!A$2:I$13,9,FALSE),0)+IF(G61&lt;&gt;"",VLOOKUP(G61,Economy!A$2:I$13,9,FALSE),0)</f>
@@ -3437,25 +3444,25 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3682,7 +3689,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Deck!B:B,Deck!D:D,Economy!A13)+SUMIFS(Deck!B:B,Deck!E:E,Economy!A13)</f>
@@ -3912,84 +3919,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.875" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.25" style="38" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.875" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
       <c r="D1" s="61"/>
       <c r="E1" s="56" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F1" s="57"/>
       <c r="G1" s="57"/>
       <c r="H1" s="58"/>
       <c r="I1" s="37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="40" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="17">
         <f>IF(ISNA(VLOOKUP(A3,Deck!C:O,12,FALSE)),"",VLOOKUP(A3,Deck!C:O,12,FALSE))</f>
@@ -4007,22 +4033,30 @@
         <f>IF(ISNA(VLOOKUP(E3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(E3,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="I3" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="I3" s="38"/>
+      <c r="J3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(I3,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I3,Deck!$C:$O,12,FALSE))</f>
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
+        <v/>
+      </c>
+      <c r="K3" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I3,Deck!$C:$O,9,FALSE))</f>
-        <v>30</v>
+        <v/>
       </c>
       <c r="L3" s="51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="M3" s="38"/>
+      <c r="N3" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M3,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M3,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O3" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M3,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M3,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -4035,10 +4069,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="17">
         <f>IF(ISNA(VLOOKUP(E4,Deck!C:O,12,FALSE)),"",VLOOKUP(E4,Deck!C:O,12,FALSE))</f>
@@ -4049,24 +4083,32 @@
         <v>0</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="17">
+        <v>165</v>
+      </c>
+      <c r="I4" s="38"/>
+      <c r="J4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,12,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
+        <v/>
+      </c>
+      <c r="K4" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I4,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I4,Deck!$C:$O,9,FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L4" s="51"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="38"/>
+      <c r="N4" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M4,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M4,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O4" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M4,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M4,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P4" s="51"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="17">
         <f>IF(ISNA(VLOOKUP(A5,Deck!C:O,12,FALSE)),"",VLOOKUP(A5,Deck!C:O,12,FALSE))</f>
@@ -4077,7 +4119,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="17">
         <v>2</v>
@@ -4087,25 +4129,31 @@
         <v>0</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>171</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>18</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="I5" s="38"/>
       <c r="J5" s="17">
         <v>2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I5,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I5,Deck!$C:$O,9,FALSE))</f>
-        <v>20</v>
-      </c>
-      <c r="L5" s="51" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L5" s="51"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M5,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M5,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M5,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M5,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P5" s="51"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4115,10 +4163,10 @@
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4128,24 +4176,32 @@
         <v>10</v>
       </c>
       <c r="H6" s="51" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="17">
+        <v>163</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,12,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="3">
+        <v/>
+      </c>
+      <c r="K6" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I6,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I6,Deck!$C:$O,9,FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L6" s="51"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="38"/>
+      <c r="N6" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M6,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M6,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O6" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M6,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M6,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P6" s="51"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4155,10 +4211,10 @@
         <v>140</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4168,25 +4224,31 @@
         <v>10</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" s="38" t="s">
-        <v>118</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="I7" s="38"/>
       <c r="J7" s="17">
         <v>2</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I7,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I7,Deck!$C:$O,9,FALSE))</f>
-        <v>120</v>
-      </c>
-      <c r="L7" s="51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L7" s="51"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M7,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M7,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M7,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M7,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P7" s="51"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4196,10 +4258,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="17">
         <f>IF(ISNA(VLOOKUP(E8,Deck!C:O,12,FALSE)),"",VLOOKUP(E8,Deck!C:O,12,FALSE))</f>
@@ -4210,25 +4272,31 @@
         <v>0</v>
       </c>
       <c r="H8" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>38</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="I8" s="38"/>
       <c r="J8" s="17">
         <v>2</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I8,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I8,Deck!$C:$O,9,FALSE))</f>
-        <v>50</v>
-      </c>
-      <c r="L8" s="51" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L8" s="51"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M8,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M8,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O8" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M8,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M8,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P8" s="51"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
@@ -4238,10 +4306,10 @@
         <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="17">
         <v>2</v>
@@ -4251,24 +4319,32 @@
         <v>5</v>
       </c>
       <c r="H9" s="51" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="17">
+        <v>164</v>
+      </c>
+      <c r="I9" s="38"/>
+      <c r="J9" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,12,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
+        <v/>
+      </c>
+      <c r="K9" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I9,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I9,Deck!$C:$O,9,FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L9" s="51"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="38"/>
+      <c r="N9" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M9,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M9,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O9" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M9,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M9,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P9" s="51"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4278,10 +4354,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="17">
         <v>1</v>
@@ -4291,24 +4367,32 @@
         <v>5</v>
       </c>
       <c r="H10" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="I10" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="17">
+        <v>167</v>
+      </c>
+      <c r="I10" s="53"/>
+      <c r="J10" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,12,FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="3">
+        <v/>
+      </c>
+      <c r="K10" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I10,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I10,Deck!$C:$O,9,FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L10" s="51"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="53"/>
+      <c r="N10" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M10,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M10,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O10" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M10,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M10,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P10" s="51"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4318,10 +4402,10 @@
         <v>130</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4331,35 +4415,40 @@
         <v>10</v>
       </c>
       <c r="H11" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>123</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="I11" s="38"/>
       <c r="J11" s="17">
         <v>2</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I11,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I11,Deck!$C:$O,9,FALSE))</f>
-        <v>70</v>
-      </c>
-      <c r="L11" s="51" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L11" s="51"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M11,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M11,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O11" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M11,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M11,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P11" s="51"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A12,Deck!'C':Economy!O,8,FALSE)),"",VLOOKUP(A12,Deck!C:O,9,FALSE))</f>
-        <v>*</v>
+      <c r="C12" s="3">
+        <v>40</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="17">
         <f>IF(ISNA(VLOOKUP(E12,Deck!C:O,12,FALSE)),"",VLOOKUP(E12,Deck!C:O,12,FALSE))</f>
@@ -4372,27 +4461,33 @@
       <c r="H12" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="I12" s="38"/>
       <c r="J12" s="17">
         <v>2</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I12,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I12,Deck!$C:$O,9,FALSE))</f>
-        <v>40</v>
-      </c>
-      <c r="L12" s="51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L12" s="51"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M12,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M12,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O12" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M12,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M12,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P12" s="51"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A14,Deck!C:O,12,FALSE)),"",VLOOKUP(A14,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
       <c r="E13" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="17">
         <f>IF(ISNA(VLOOKUP(E13,Deck!C:O,12,FALSE)),"",VLOOKUP(E13,Deck!C:O,12,FALSE))</f>
@@ -4403,29 +4498,35 @@
         <v>0</v>
       </c>
       <c r="H13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="38" t="s">
-        <v>56</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I13" s="38"/>
       <c r="J13" s="17">
         <v>2</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(I13,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I13,Deck!$C:$O,9,FALSE))</f>
-        <v>40</v>
-      </c>
-      <c r="L13" s="51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L13" s="51"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M13,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M13,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O13" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M13,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M13,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P13" s="51"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A15,Deck!C:O,12,FALSE)),"",VLOOKUP(A15,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
       <c r="E14" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="17">
         <f>IF(ISNA(VLOOKUP(E14,Deck!C:O,12,FALSE)),"",VLOOKUP(E14,Deck!C:O,12,FALSE))</f>
@@ -4448,14 +4549,24 @@
         <v/>
       </c>
       <c r="L14" s="51"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="38"/>
+      <c r="N14" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M14,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M14,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O14" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M14,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M14,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P14" s="51"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A16,Deck!C:O,12,FALSE)),"",VLOOKUP(A16,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
       <c r="E15" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F15" s="17">
         <f>IF(ISNA(VLOOKUP(E15,Deck!C:O,12,FALSE)),"",VLOOKUP(E15,Deck!C:O,12,FALSE))</f>
@@ -4477,11 +4588,19 @@
         <f>IF(ISNA(VLOOKUP(I15,Deck!$C:$O,9,FALSE)),"",VLOOKUP(I15,Deck!$C:$O,9,FALSE))</f>
         <v/>
       </c>
-      <c r="L15" s="51" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="51"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M15,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M15,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O15" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M15,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M15,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P15" s="51"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A17,Deck!C:O,12,FALSE)),"",VLOOKUP(A17,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4504,8 +4623,18 @@
         <v/>
       </c>
       <c r="L16" s="51"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="38"/>
+      <c r="N16" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M16,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M16,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O16" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M16,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M16,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P16" s="51"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A18,Deck!C:O,12,FALSE)),"",VLOOKUP(A18,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4528,8 +4657,18 @@
         <v/>
       </c>
       <c r="L17" s="51"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="38"/>
+      <c r="N17" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M17,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M17,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O17" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M17,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M17,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P17" s="51"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4552,24 +4691,34 @@
         <v/>
       </c>
       <c r="L18" s="51"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="38"/>
+      <c r="N18" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M18,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M18,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O18" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M18,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M18,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P18" s="51"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A19,Deck!C:O,12,FALSE)),"",VLOOKUP(A19,Deck!C:O,12,FALSE))</f>
         <v/>
       </c>
       <c r="E19" s="38" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Deck!C:O,12,FALSE)),"",VLOOKUP(E19,Deck!C:O,12,FALSE))</f>
         <v>2</v>
       </c>
       <c r="G19" s="3">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="17" t="str">
@@ -4581,8 +4730,18 @@
         <v/>
       </c>
       <c r="L19" s="51"/>
-    </row>
-    <row r="20" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="38"/>
+      <c r="N19" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M19,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M19,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O19" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M19,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M19,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P19" s="51"/>
+    </row>
+    <row r="20" spans="1:16" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A20,Deck!C:O,12,FALSE)),"",VLOOKUP(A20,Deck!C:O,12,FALSE))</f>
         <v/>
@@ -4590,16 +4749,16 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
       </c>
       <c r="G20" s="3">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="H20" s="51" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="17" t="str">
@@ -4611,39 +4770,59 @@
         <v/>
       </c>
       <c r="L20" s="51"/>
-    </row>
-    <row r="21" spans="1:12" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="38"/>
+      <c r="N20" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M20,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M20,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O20" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M20,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M20,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P20" s="51"/>
+    </row>
+    <row r="21" spans="1:16" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="17"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Deck!C:O,12,FALSE)),"",VLOOKUP(E21,Deck!C:O,12,FALSE))</f>
         <v>2</v>
       </c>
       <c r="G21" s="3">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="H21" s="51" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J21" s="17">
         <f>IF(ISNA(VLOOKUP(I21,Deck!$C:$O,12,FALSE)),"",VLOOKUP(I21,Deck!$C:$O,12,FALSE))</f>
         <v>2</v>
       </c>
       <c r="K21" s="3">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="L21" s="51"/>
-    </row>
-    <row r="22" spans="1:12" s="43" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="38"/>
+      <c r="N21" s="17" t="str">
+        <f>IF(ISNA(VLOOKUP(M21,Deck!$C:$O,12,FALSE)),"",VLOOKUP(M21,Deck!$C:$O,12,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O21" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(M21,Deck!$C:$O,9,FALSE)),"",VLOOKUP(M21,Deck!$C:$O,9,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P21" s="51"/>
+    </row>
+    <row r="22" spans="1:16" s="43" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B22" s="50">
         <f>SUM(B3:B21)</f>
@@ -4651,11 +4830,11 @@
       </c>
       <c r="C22" s="49">
         <f>SUM(C3:C21)</f>
-        <v>450</v>
+        <v>490</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="44" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F22" s="46">
         <f>SUM(F3:F21)</f>
@@ -4663,43 +4842,43 @@
       </c>
       <c r="G22" s="43">
         <f>SUM(G3:G21)</f>
-        <v>98</v>
+        <v>620</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="44" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J22" s="46">
         <f>SUM(J3:J21)</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K22" s="43">
         <f>SUM(K3:K21)</f>
-        <v>394</v>
+        <v>240</v>
       </c>
       <c r="L22" s="52"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B23" s="17">
         <f>C22/B22</f>
-        <v>25.397954965142667</v>
+        <v>27.655550962044238</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F23" s="47">
         <f>G22/F22</f>
-        <v>4.9000000000000004</v>
+        <v>31</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="J23" s="47">
         <f>K22/J22</f>
-        <v>19.7</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="L23" s="51"/>
     </row>
@@ -4708,15 +4887,15 @@
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12 A12 A16:A20 I3:I9 I11:I21 A3:A10">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12 A12 A16:A20 I3:I9 I11:I21 A3:A10 M3:M9 M11:M21">
       <formula1>$C$3:$C$55</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Deck!$C$3:$C$61</xm:f>
@@ -4734,7 +4913,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4746,21 +4925,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4775,7 +4954,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4790,7 +4969,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,7 +4984,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4820,7 +4999,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,7 +5014,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of work toward the wood-grain look
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Specials" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="244">
   <si>
     <t>Type</t>
   </si>
@@ -753,6 +753,12 @@
   </si>
   <si>
     <t>Upon playing, climb 1 rung on a Ladder</t>
+  </si>
+  <si>
+    <t>Resource1</t>
+  </si>
+  <si>
+    <t>Resource2</t>
   </si>
 </sst>
 </file>
@@ -1372,9 +1378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,9 +3153,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3157,7 +3163,7 @@
     <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
@@ -3174,10 +3180,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>242</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>243</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3565,11 +3571,11 @@
         <v>0.58823529411764708</v>
       </c>
       <c r="F2" s="16">
-        <f>SUM(B:B)/B2</f>
+        <f t="shared" ref="F2:F13" si="1">SUM(B:B)/B2</f>
         <v>3.7647058823529411</v>
       </c>
       <c r="G2" s="16">
-        <f>1-POWER(B2/SUM(B:B),0.5)</f>
+        <f t="shared" ref="G2:G13" si="2">1-POWER(B2/SUM(B:B),0.5)</f>
         <v>0.48461179679779243</v>
       </c>
       <c r="H2" s="16">
@@ -3590,7 +3596,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="17">
-        <f t="shared" ref="D3:D13" si="1">IF(ISNUMBER(B3/C3),B3/C3,"")</f>
+        <f t="shared" ref="D3:D13" si="3">IF(ISNUMBER(B3/C3),B3/C3,"")</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="E3" s="17">
@@ -3598,15 +3604,15 @@
         <v>0.75</v>
       </c>
       <c r="F3" s="17">
-        <f>SUM(B:B)/B3</f>
+        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="G3" s="21">
-        <f>1-POWER(B3/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.5669872981077807</v>
       </c>
       <c r="H3" s="17">
-        <f t="shared" ref="H3:H13" si="2">1+G3</f>
+        <f t="shared" ref="H3:H13" si="4">1+G3</f>
         <v>1.5669872981077808</v>
       </c>
     </row>
@@ -3623,7 +3629,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E4" s="17">
@@ -3631,15 +3637,15 @@
         <v>1.5</v>
       </c>
       <c r="F4" s="17">
-        <f>SUM(B:B)/B4</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G4" s="21">
-        <f>1-POWER(B4/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="H4" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
@@ -3656,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="E5" s="17">
@@ -3664,15 +3670,15 @@
         <v>2</v>
       </c>
       <c r="F5" s="17">
-        <f>SUM(B:B)/B5</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G5" s="21">
-        <f>1-POWER(B5/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H5" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>
@@ -3689,7 +3695,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="E6" s="17">
@@ -3697,15 +3703,15 @@
         <v>1.4285714285714286</v>
       </c>
       <c r="F6" s="17">
-        <f>SUM(B:B)/B6</f>
+        <f t="shared" si="1"/>
         <v>9.1428571428571423</v>
       </c>
       <c r="G6" s="21">
-        <f>1-POWER(B6/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.66928108611692616</v>
       </c>
       <c r="H6" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6692810861169263</v>
       </c>
     </row>
@@ -3722,7 +3728,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="E7" s="17">
@@ -3730,15 +3736,15 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F7" s="17">
-        <f>SUM(B:B)/B7</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G7" s="21">
-        <f>1-POWER(B7/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H7" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>
@@ -3755,7 +3761,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E8" s="17">
@@ -3763,15 +3769,15 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="17">
-        <f>SUM(B:B)/B8</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="G8" s="21">
-        <f>1-POWER(B8/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.82322330470336313</v>
       </c>
       <c r="H8" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.823223304703363</v>
       </c>
     </row>
@@ -3788,7 +3794,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E9" s="17">
@@ -3796,15 +3802,15 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="17">
-        <f>SUM(B:B)/B9</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G9" s="21">
-        <f>1-POWER(B9/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="H9" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
@@ -3821,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E10" s="17" t="str">
@@ -3829,15 +3835,15 @@
         <v/>
       </c>
       <c r="F10" s="17">
-        <f>SUM(B:B)/B10</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G10" s="21">
-        <f>1-POWER(B10/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H10" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>
@@ -3854,7 +3860,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E11" s="17" t="str">
@@ -3862,15 +3868,15 @@
         <v/>
       </c>
       <c r="F11" s="17">
-        <f>SUM(B:B)/B11</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G11" s="21">
-        <f>1-POWER(B11/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H11" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>
@@ -3887,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E12" s="17" t="str">
@@ -3895,15 +3901,15 @@
         <v/>
       </c>
       <c r="F12" s="17">
-        <f>SUM(B:B)/B12</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G12" s="21">
-        <f>1-POWER(B12/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>
@@ -3920,7 +3926,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E13" s="17" t="str">
@@ -3928,15 +3934,15 @@
         <v/>
       </c>
       <c r="F13" s="17">
-        <f>SUM(B:B)/B13</f>
+        <f t="shared" si="1"/>
         <v>21.333333333333332</v>
       </c>
       <c r="G13" s="21">
-        <f>1-POWER(B13/SUM(B:B),0.5)</f>
+        <f t="shared" si="2"/>
         <v>0.78349364905389041</v>
       </c>
       <c r="H13" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7834936490538904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
specials: getting there on the layout
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="258">
   <si>
     <t>Type</t>
   </si>
@@ -795,6 +795,12 @@
   </si>
   <si>
     <t>Cow Power!</t>
+  </si>
+  <si>
+    <t>Silk Trade</t>
+  </si>
+  <si>
+    <t>2:1 Trade</t>
   </si>
 </sst>
 </file>
@@ -1415,8 +1421,8 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,6 +1810,9 @@
       <c r="H11" s="22" t="s">
         <v>32</v>
       </c>
+      <c r="J11" s="54" t="s">
+        <v>256</v>
+      </c>
       <c r="K11" s="22" t="s">
         <v>132</v>
       </c>
@@ -2024,6 +2033,9 @@
         <v>120</v>
       </c>
       <c r="D17" s="25"/>
+      <c r="J17" s="54" t="s">
+        <v>257</v>
+      </c>
       <c r="K17" s="22" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
data: some wording tweaks
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="257">
   <si>
     <t>Type</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Does nothing now, but it will pay off later. The engine can wait.</t>
   </si>
   <si>
-    <t>Grain: the best breeder of them all.</t>
-  </si>
-  <si>
     <t>I'm pretty sure this strategy worked for me at least once.</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>The Coveted Starting Player</t>
   </si>
   <si>
-    <t>Go first!</t>
-  </si>
-  <si>
     <t>Because just going around in a circle is not strategic enough.</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t>The Premium Material</t>
   </si>
   <si>
-    <t>First!</t>
-  </si>
-  <si>
     <t>Trash1</t>
   </si>
   <si>
@@ -801,6 +792,12 @@
   </si>
   <si>
     <t>2:1 Trade</t>
+  </si>
+  <si>
+    <t>Grain Breed!</t>
+  </si>
+  <si>
+    <t>Setup</t>
   </si>
 </sst>
 </file>
@@ -1422,25 +1419,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.75" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="67.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="79.75" customWidth="1"/>
+    <col min="8" max="9" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="79.7109375" customWidth="1"/>
     <col min="14" max="14" width="11" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.125" style="3"/>
+    <col min="15" max="15" width="11.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1460,10 +1457,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>19</v>
@@ -1472,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1484,43 +1481,41 @@
         <v>1</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>256</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D2"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1528,7 +1523,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1543,7 +1538,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
@@ -1566,7 +1561,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1575,19 +1570,19 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L4" s="5">
         <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N4" s="34">
         <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:H$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1604,7 +1599,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1616,16 +1611,16 @@
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N5" s="34" t="e">
         <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:H$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1642,28 +1637,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="K6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N6" s="34" t="e">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:H$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1680,22 +1675,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" t="s">
         <v>182</v>
-      </c>
-      <c r="K7" t="s">
-        <v>185</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1712,7 +1707,7 @@
         <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
@@ -1723,19 +1718,19 @@
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J9" s="54" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
@@ -1758,13 +1753,13 @@
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>48</v>
+      <c r="C10" s="54" t="s">
+        <v>255</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>23</v>
@@ -1776,13 +1771,13 @@
         <v>23</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L10" s="5">
         <v>0</v>
       </c>
-      <c r="M10" s="22" t="s">
-        <v>65</v>
+      <c r="M10" s="54" t="s">
+        <v>197</v>
       </c>
       <c r="N10" s="24" t="e">
         <f>IF(F10&lt;&gt;"",VLOOKUP(F10,Economy!A$2:H$13,9,FALSE),0)+IF(G10&lt;&gt;"",VLOOKUP(G10,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1799,28 +1794,28 @@
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N11" s="24">
         <f>IF(F11&lt;&gt;"",VLOOKUP(F11,Economy!A$2:H$13,9,FALSE),0)+IF(G11&lt;&gt;"",VLOOKUP(G11,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1837,7 +1832,7 @@
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
@@ -1875,25 +1870,25 @@
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1901,13 +1896,13 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>11</v>
@@ -1916,7 +1911,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>34</v>
@@ -1925,7 +1920,7 @@
         <v>50</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="N14" s="24" t="e">
         <f>IF(F14&lt;&gt;"",VLOOKUP(F14,Economy!A$2:H$13,9,FALSE),0)+IF(G14&lt;&gt;"",VLOOKUP(G14,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1942,13 +1937,13 @@
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
@@ -1957,7 +1952,7 @@
         <v>32</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>35</v>
@@ -1966,7 +1961,7 @@
         <v>50</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N15" s="24" t="e">
         <f>IF(F15&lt;&gt;"",VLOOKUP(F15,Economy!A$2:H$13,9,FALSE),0)+IF(G15&lt;&gt;"",VLOOKUP(G15,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1983,13 +1978,13 @@
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>14</v>
@@ -1998,7 +1993,7 @@
         <v>32</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>36</v>
@@ -2007,7 +2002,7 @@
         <v>50</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N16" s="24" t="e">
         <f>IF(F16&lt;&gt;"",VLOOKUP(F16,Economy!A$2:H$13,9,FALSE),0)+IF(G16&lt;&gt;"",VLOOKUP(G16,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2024,20 +2019,20 @@
     </row>
     <row r="17" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D17" s="25"/>
       <c r="J17" s="54" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L17" s="5">
         <v>30</v>
@@ -2060,7 +2055,7 @@
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
@@ -2069,26 +2064,26 @@
         <v>37</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L18" s="5">
         <v>50</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N18" s="24">
         <f>IF(F18&lt;&gt;"",VLOOKUP(F18,Economy!A$2:H$13,9,FALSE),0)+IF(G18&lt;&gt;"",VLOOKUP(G18,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2105,7 +2100,7 @@
     </row>
     <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B19" s="29">
         <v>1</v>
@@ -2117,10 +2112,10 @@
         <v>8</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
@@ -2143,13 +2138,13 @@
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>12</v>
@@ -2164,7 +2159,7 @@
         <v>20</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N20" s="30" t="e">
         <f>IF(F20&lt;&gt;"",VLOOKUP(F20,Economy!A$2:H$13,9,FALSE),0)+IF(G20&lt;&gt;"",VLOOKUP(G20,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2181,13 +2176,13 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>23</v>
@@ -2199,13 +2194,13 @@
         <v>23</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L21" s="5">
         <v>20</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N21" s="30" t="e">
         <f>IF(F21&lt;&gt;"",VLOOKUP(F21,Economy!A$2:H$13,9,FALSE),0)+IF(G21&lt;&gt;"",VLOOKUP(G21,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2222,13 +2217,13 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>8</v>
@@ -2243,7 +2238,7 @@
         <v>80</v>
       </c>
       <c r="M22" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N22" s="30" t="e">
         <f>IF(F22&lt;&gt;"",VLOOKUP(F22,Economy!A$2:H$13,9,FALSE),0)+IF(G22&lt;&gt;"",VLOOKUP(G22,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2260,13 +2255,13 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>14</v>
@@ -2281,7 +2276,7 @@
         <v>90</v>
       </c>
       <c r="M23" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N23" s="30" t="e">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,Economy!A$2:H$13,9,FALSE),0)+IF(G23&lt;&gt;"",VLOOKUP(G23,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2298,13 +2293,13 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
@@ -2319,7 +2314,7 @@
         <v>100</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N24" s="30" t="e">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:H$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2336,13 +2331,13 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>8</v>
@@ -2357,7 +2352,7 @@
         <v>110</v>
       </c>
       <c r="M25" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="N25" s="30" t="e">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:H$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2374,13 +2369,13 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>14</v>
@@ -2395,7 +2390,7 @@
         <v>120</v>
       </c>
       <c r="M26" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N26" s="30" t="e">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:H$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2412,13 +2407,13 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>11</v>
@@ -2433,7 +2428,7 @@
         <v>130</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="N27" s="30" t="e">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:H$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2450,7 +2445,7 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
@@ -2488,13 +2483,13 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>25</v>
@@ -2503,13 +2498,13 @@
         <v>25</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L29" s="5">
         <v>10</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N29" s="30" t="e">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:H$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2526,7 +2521,7 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B30" s="29">
         <v>2</v>
@@ -2535,22 +2530,22 @@
         <v>53</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L30" s="5">
         <v>40</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N30" s="30" t="e">
         <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:H$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2567,34 +2562,34 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L31" s="5">
         <v>50</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N31" s="30" t="e">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:H$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2611,25 +2606,25 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L32" s="5">
         <v>20</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N32" s="30" t="e">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:H$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2646,25 +2641,25 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B33" s="29">
         <v>2</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L33" s="5">
         <v>20</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="N33" s="30" t="e">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:H$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2681,25 +2676,25 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L34" s="5">
         <v>30</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N34" s="30" t="e">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:H$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2716,25 +2711,25 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L35" s="5">
         <v>30</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N35" s="30" t="e">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:H$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2745,23 +2740,23 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F36" s="31"/>
       <c r="K36" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L36" s="5">
         <v>10</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2769,13 +2764,13 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" s="29">
+        <v>1</v>
+      </c>
+      <c r="C37" s="31" t="s">
         <v>234</v>
-      </c>
-      <c r="B37" s="29">
-        <v>1</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>237</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>8</v>
@@ -2788,7 +2783,7 @@
         <v>30</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2796,13 +2791,13 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>27</v>
@@ -2815,7 +2810,7 @@
         <v>40</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2823,13 +2818,13 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>11</v>
@@ -2842,7 +2837,7 @@
         <v>50</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2850,7 +2845,7 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
@@ -2862,13 +2857,13 @@
         <v>15</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L40" s="5">
         <v>-20</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N40" s="30" t="e">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:H$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2885,25 +2880,25 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L41" s="5">
         <v>20</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N41" s="30">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:H$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2920,24 +2915,24 @@
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
       <c r="K42" s="28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L42" s="5">
         <v>30</v>
       </c>
       <c r="M42" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N42" s="30">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:H$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2963,13 +2958,13 @@
         <v>21</v>
       </c>
       <c r="K43" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M43" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N43">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,Economy!A$2:H$13,9,FALSE),0)+IF(G43&lt;&gt;"",VLOOKUP(G43,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2992,16 +2987,16 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K44" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N44">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:H$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3030,10 +3025,10 @@
         <v>15</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K45" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L45" s="5">
         <v>100</v>
@@ -3062,13 +3057,13 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K46" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M46" t="s">
         <v>38</v>
@@ -3094,13 +3089,13 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M47" t="s">
         <v>39</v>
@@ -3125,13 +3120,13 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K48" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M48" t="s">
         <v>28</v>
@@ -3160,10 +3155,10 @@
         <v>30</v>
       </c>
       <c r="K49" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M49" t="s">
         <v>45</v>
@@ -3192,10 +3187,10 @@
         <v>33</v>
       </c>
       <c r="K50" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M50" t="s">
         <v>41</v>
@@ -3227,10 +3222,10 @@
         <v>32</v>
       </c>
       <c r="K51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M51" t="s">
         <v>54</v>
@@ -3256,37 +3251,37 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
+        <v>239</v>
+      </c>
+      <c r="K52" t="s">
+        <v>241</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="M52" t="s">
         <v>242</v>
-      </c>
-      <c r="K52" t="s">
-        <v>244</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="M52" t="s">
-        <v>245</v>
       </c>
       <c r="N52"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K53" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L53" s="5">
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N53">
         <f>IF(F53&lt;&gt;"",VLOOKUP(F53,Economy!A$2:H$13,9,FALSE),0)+IF(G53&lt;&gt;"",VLOOKUP(G53,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3313,18 +3308,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79.75" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3338,10 +3333,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3361,7 +3356,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3373,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3384,7 +3379,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3396,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3407,7 +3402,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>11</v>
@@ -3416,7 +3411,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3427,7 +3422,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>14</v>
@@ -3439,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3470,7 +3465,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>12</v>
@@ -3490,7 +3485,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>13</v>
@@ -3510,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>27</v>
@@ -3519,7 +3514,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -3536,7 +3531,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>23</v>
@@ -3545,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3556,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
@@ -3568,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3579,19 +3574,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3602,7 +3597,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>15</v>
@@ -3611,7 +3606,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3622,19 +3617,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3654,7 +3649,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3667,19 +3662,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3687,25 +3682,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3908,7 +3903,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -4123,94 +4118,94 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.25" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5" style="50" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="H2" s="40" t="s">
-        <v>153</v>
-      </c>
       <c r="I2" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K2" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="L2" s="38" t="s">
-        <v>153</v>
-      </c>
       <c r="M2" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="O2" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="P2" s="38" t="s">
         <v>150</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
@@ -4238,7 +4233,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -4264,10 +4259,10 @@
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
@@ -4278,7 +4273,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -4303,7 +4298,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
@@ -4321,10 +4316,10 @@
       </c>
       <c r="G5" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(E5,Specials!C:P,9,FALSE)),"",VLOOKUP(E5,Specials!C:P,9,FALSE))</f>
-        <v>You may trash this card for 1 Food.</v>
+        <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4348,7 +4343,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4358,10 +4353,10 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4371,7 +4366,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4396,7 +4391,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4406,10 +4401,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4419,7 +4414,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4443,7 +4438,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4453,10 +4448,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
@@ -4467,7 +4462,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4491,7 +4486,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
@@ -4501,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>42</v>
@@ -4514,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4539,7 +4534,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4549,7 +4544,7 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>42</v>
@@ -4562,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4587,7 +4582,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4597,10 +4592,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4610,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -4643,7 +4638,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
@@ -4682,7 +4677,7 @@
         <v/>
       </c>
       <c r="E13" s="37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
@@ -4693,7 +4688,7 @@
         <v/>
       </c>
       <c r="H13" s="50" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="17">
@@ -4761,7 +4756,7 @@
         <v/>
       </c>
       <c r="E15" s="37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
@@ -4903,7 +4898,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -4913,7 +4908,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -4944,7 +4939,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -4953,7 +4948,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -4981,7 +4976,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -4991,7 +4986,7 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>33</v>
@@ -5017,7 +5012,7 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="49" t="e">
         <f>SUM(B3:B21)</f>
@@ -5029,7 +5024,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -5041,7 +5036,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -5055,21 +5050,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -5113,28 +5108,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,7 +5144,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5164,7 +5159,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5179,7 +5174,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5194,7 +5189,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5209,7 +5204,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tons of revision from playtesting
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$15</definedName>
-    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$53</definedName>
+    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$55</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="273">
   <si>
     <t>Type</t>
   </si>
@@ -164,9 +164,6 @@
     <t>The Building Payoff Building</t>
   </si>
   <si>
-    <t>Go ahead and take your next turn, this is gonna take me a moment.</t>
-  </si>
-  <si>
     <t>The Grain Engine</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Be sure to take this from someone who has collected silk.</t>
   </si>
   <si>
-    <t>Just when you think you've pulled ahead, someone else will get a bigger building than this.</t>
-  </si>
-  <si>
     <t>Nice! Way to get some points on the board.</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
     <t>Starter</t>
   </si>
   <si>
-    <t>You must play this card before playing an Engine.</t>
-  </si>
-  <si>
     <t>You may trash this card for 2 Food.</t>
   </si>
   <si>
@@ -302,9 +293,6 @@
     <t>The Wildcard Building</t>
   </si>
   <si>
-    <t>Or is it wheat? Or corn? Seeds?</t>
-  </si>
-  <si>
     <t>You may trash this card for 1 Food.</t>
   </si>
   <si>
@@ -353,15 +341,9 @@
     <t>The Amazing Building</t>
   </si>
   <si>
-    <t>The Great Building</t>
-  </si>
-  <si>
     <t>Good move. Not Great. But Good.</t>
   </si>
   <si>
-    <t>Don't get all your VPs out too early now. We've got an endgame.</t>
-  </si>
-  <si>
     <t>The Unused Resources Payoff</t>
   </si>
   <si>
@@ -389,9 +371,6 @@
     <t>Make it count. No pressure. Are you sure you that's a good enough use for this card?? There's probably a better move.</t>
   </si>
   <si>
-    <t>You may trash this card for any 2 Resources.</t>
-  </si>
-  <si>
     <t>The One-and-Done Card</t>
   </si>
   <si>
@@ -410,9 +389,6 @@
     <t>The Combo Building</t>
   </si>
   <si>
-    <t>Personally, I find grain to be much more filling than carrots</t>
-  </si>
-  <si>
     <t>Eat More Veggies!</t>
   </si>
   <si>
@@ -638,27 +614,15 @@
     <t>See you at the top!</t>
   </si>
   <si>
-    <t>Take the total number of Glass and Silk you have. Square then multiply by 10 for VPs.</t>
-  </si>
-  <si>
     <t>10 VP for each Building you've played</t>
   </si>
   <si>
     <t>30 VP for each Soldier, +30 additional VP if you end the game with the most soldiers.</t>
   </si>
   <si>
-    <t>30 VP for each Wood, Sheep, or Grain</t>
-  </si>
-  <si>
-    <t>50 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
-  </si>
-  <si>
     <t>60 VPs for each Cattle, Carrot</t>
   </si>
   <si>
-    <t>30 VPs for each Payoff you have placed.</t>
-  </si>
-  <si>
     <t>Ladder Strategy</t>
   </si>
   <si>
@@ -677,15 +641,9 @@
     <t>Military</t>
   </si>
   <si>
-    <t>Cook</t>
-  </si>
-  <si>
     <t>Go First!</t>
   </si>
   <si>
-    <t>Can be bought for 1 of any Resource.</t>
-  </si>
-  <si>
     <t>Military Endgame Tactics</t>
   </si>
   <si>
@@ -782,9 +740,6 @@
     <t>Stone ladders: also known as "stairs".</t>
   </si>
   <si>
-    <t>Thematically this card makes no sense. We needed it for game balancing reasons.</t>
-  </si>
-  <si>
     <t>Cow Power!</t>
   </si>
   <si>
@@ -798,6 +753,99 @@
   </si>
   <si>
     <t>Setup</t>
+  </si>
+  <si>
+    <t>The Red Material</t>
+  </si>
+  <si>
+    <t>Grain: the rabbits of plants.</t>
+  </si>
+  <si>
+    <t>Thematically this card makes no sense. We needed it for game reasons.</t>
+  </si>
+  <si>
+    <t>The Breeding Plant</t>
+  </si>
+  <si>
+    <t>Or is it wheat? Or corn? Seeds? Reed?</t>
+  </si>
+  <si>
+    <t>Think of carrots like a self-insta-slaughtering animal.</t>
+  </si>
+  <si>
+    <t>Take the total number of Glass and Silk you have. Square that number, then multiply it by 10 for VPs.</t>
+  </si>
+  <si>
+    <t>"Go ahead and take your next turn, this is gonna take me a moment."</t>
+  </si>
+  <si>
+    <t>Can be bought by trashing 1 of any Resource.</t>
+  </si>
+  <si>
+    <t>30 VP for each Wood, Sheep, and Grain</t>
+  </si>
+  <si>
+    <t>40 VP for each type: Sheep, Wild Boar, Cattle, Glass, Silk, Grain, Carrot.</t>
+  </si>
+  <si>
+    <t>40 VPs for each Payoff you have played by endgame scoring.</t>
+  </si>
+  <si>
+    <t>The Unfulfilled Promises Payoff</t>
+  </si>
+  <si>
+    <t>40 VP for each Clay, Stone, Silk, Glass, Cattle, Carrot</t>
+  </si>
+  <si>
+    <t>This card makes your leftover Stones look intentional. You're secret's safe with us.</t>
+  </si>
+  <si>
+    <t>The Red Building</t>
+  </si>
+  <si>
+    <t>The Red Stone Building</t>
+  </si>
+  <si>
+    <t>The Cheap Stone Building</t>
+  </si>
+  <si>
+    <t>Just when you think you've pulled ahead, someone else will play a bigger building than this.</t>
+  </si>
+  <si>
+    <t>The stones aren't red. Wait… aren't bricks stones? I don't know. You're not supposed to think of theme in these games.</t>
+  </si>
+  <si>
+    <t>No, they won't breed. (Hm, this card mysteriously looks like it's part of a set. I wonder if that will pay off...)</t>
+  </si>
+  <si>
+    <t>Ordinarily these two things don't mix. (Hm, this card mysteriously looks like it's part of a set. I wonder if that will pay off…)</t>
+  </si>
+  <si>
+    <t>The Payoff Gambit</t>
+  </si>
+  <si>
+    <t>Payoff Spoiler</t>
+  </si>
+  <si>
+    <t>Trash Me!</t>
+  </si>
+  <si>
+    <t>On your first turn in Endgame, you get 2 extra Actions.</t>
+  </si>
+  <si>
+    <t>Ok everyone, this player is officially procrastinating on getting VPs.</t>
+  </si>
+  <si>
+    <t>You may trash this card from your tableau for any 2 Resources.</t>
+  </si>
+  <si>
+    <t>You may only play this card before playing an Engine.</t>
+  </si>
+  <si>
+    <t>Bake Bread</t>
+  </si>
+  <si>
+    <t>Trash-n-Climb</t>
   </si>
 </sst>
 </file>
@@ -1415,11 +1463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1479,7 @@
     <col min="6" max="6" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="79.7109375" customWidth="1"/>
@@ -1457,10 +1505,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>19</v>
@@ -1469,7 +1517,7 @@
         <v>20</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1481,24 +1529,24 @@
         <v>1</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="12"/>
@@ -1506,16 +1554,16 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="K2" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1523,7 +1571,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1538,13 +1586,13 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" s="34" t="e">
         <f>IF(F3&lt;&gt;"",VLOOKUP(F3,Economy!A$2:H$13,9,FALSE),0)+IF(G3&lt;&gt;"",VLOOKUP(G3,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1561,7 +1609,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1570,19 +1618,19 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="K4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="L4" s="5">
         <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N4" s="34">
         <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:H$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1599,28 +1647,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>216</v>
+        <v>271</v>
       </c>
       <c r="K5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N5" s="34" t="e">
         <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:H$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1637,28 +1685,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N6" s="34" t="e">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:H$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1675,22 +1723,25 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>171</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1698,45 +1749,45 @@
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>83</v>
+        <v>50</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>270</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N9" s="24">
         <f>IF(F9&lt;&gt;"",VLOOKUP(F9,Economy!A$2:H$13,9,FALSE),0)+IF(G9&lt;&gt;"",VLOOKUP(G9,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1753,13 +1804,13 @@
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>23</v>
@@ -1771,13 +1822,13 @@
         <v>23</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L10" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M10" s="54" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="N10" s="24" t="e">
         <f>IF(F10&lt;&gt;"",VLOOKUP(F10,Economy!A$2:H$13,9,FALSE),0)+IF(G10&lt;&gt;"",VLOOKUP(G10,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1794,28 +1845,28 @@
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N11" s="24">
         <f>IF(F11&lt;&gt;"",VLOOKUP(F11,Economy!A$2:H$13,9,FALSE),0)+IF(G11&lt;&gt;"",VLOOKUP(G11,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1832,7 +1883,7 @@
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
@@ -1850,10 +1901,10 @@
         <v>12</v>
       </c>
       <c r="L12" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N12" s="24" t="e">
         <f>IF(F12&lt;&gt;"",VLOOKUP(F12,Economy!A$2:H$13,9,FALSE),0)+IF(G12&lt;&gt;"",VLOOKUP(G12,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1870,25 +1921,25 @@
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1896,13 +1947,13 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>11</v>
@@ -1911,16 +1962,16 @@
         <v>32</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>34</v>
       </c>
       <c r="L14" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="N14" s="24" t="e">
         <f>IF(F14&lt;&gt;"",VLOOKUP(F14,Economy!A$2:H$13,9,FALSE),0)+IF(G14&lt;&gt;"",VLOOKUP(G14,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1937,13 +1988,13 @@
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
@@ -1952,16 +2003,16 @@
         <v>32</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>35</v>
       </c>
       <c r="L15" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="N15" s="24" t="e">
         <f>IF(F15&lt;&gt;"",VLOOKUP(F15,Economy!A$2:H$13,9,FALSE),0)+IF(G15&lt;&gt;"",VLOOKUP(G15,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1978,13 +2029,13 @@
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>14</v>
@@ -1993,16 +2044,16 @@
         <v>32</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="L16" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="N16" s="24" t="e">
         <f>IF(F16&lt;&gt;"",VLOOKUP(F16,Economy!A$2:H$13,9,FALSE),0)+IF(G16&lt;&gt;"",VLOOKUP(G16,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2019,20 +2070,20 @@
     </row>
     <row r="17" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D17" s="25"/>
       <c r="J17" s="54" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="L17" s="5">
         <v>30</v>
@@ -2055,7 +2106,7 @@
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
@@ -2064,26 +2115,26 @@
         <v>37</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="L18" s="5">
         <v>50</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N18" s="24">
         <f>IF(F18&lt;&gt;"",VLOOKUP(F18,Economy!A$2:H$13,9,FALSE),0)+IF(G18&lt;&gt;"",VLOOKUP(G18,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2100,28 +2151,28 @@
     </row>
     <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B19" s="29">
         <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>8</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N19" s="30" t="e">
         <f>IF(F19&lt;&gt;"",VLOOKUP(F19,Economy!A$2:H$13,9,FALSE),0)+IF(G19&lt;&gt;"",VLOOKUP(G19,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2138,13 +2189,13 @@
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>12</v>
@@ -2156,10 +2207,10 @@
         <v>12</v>
       </c>
       <c r="L20" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="N20" s="30" t="e">
         <f>IF(F20&lt;&gt;"",VLOOKUP(F20,Economy!A$2:H$13,9,FALSE),0)+IF(G20&lt;&gt;"",VLOOKUP(G20,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2176,13 +2227,13 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>23</v>
@@ -2194,13 +2245,13 @@
         <v>23</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="L21" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>197</v>
+        <v>243</v>
       </c>
       <c r="N21" s="30" t="e">
         <f>IF(F21&lt;&gt;"",VLOOKUP(F21,Economy!A$2:H$13,9,FALSE),0)+IF(G21&lt;&gt;"",VLOOKUP(G21,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2217,13 +2268,13 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>8</v>
@@ -2235,10 +2286,10 @@
         <v>32</v>
       </c>
       <c r="L22" s="5">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="M22" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N22" s="30" t="e">
         <f>IF(F22&lt;&gt;"",VLOOKUP(F22,Economy!A$2:H$13,9,FALSE),0)+IF(G22&lt;&gt;"",VLOOKUP(G22,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2255,13 +2306,13 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>14</v>
@@ -2273,10 +2324,10 @@
         <v>32</v>
       </c>
       <c r="L23" s="5">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="M23" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N23" s="30" t="e">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,Economy!A$2:H$13,9,FALSE),0)+IF(G23&lt;&gt;"",VLOOKUP(G23,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2293,13 +2344,13 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>102</v>
+      <c r="C24" s="31" t="s">
+        <v>257</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
@@ -2311,10 +2362,10 @@
         <v>32</v>
       </c>
       <c r="L24" s="5">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N24" s="30" t="e">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:H$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2331,13 +2382,13 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
-      <c r="C25" s="28" t="s">
-        <v>108</v>
+      <c r="C25" s="31" t="s">
+        <v>259</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>8</v>
@@ -2349,10 +2400,10 @@
         <v>32</v>
       </c>
       <c r="L25" s="5">
-        <v>110</v>
-      </c>
-      <c r="M25" s="28" t="s">
-        <v>110</v>
+        <v>80</v>
+      </c>
+      <c r="M25" s="31" t="s">
+        <v>260</v>
       </c>
       <c r="N25" s="30" t="e">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:H$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2369,13 +2420,13 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>107</v>
+        <v>258</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>14</v>
@@ -2387,10 +2438,10 @@
         <v>32</v>
       </c>
       <c r="L26" s="5">
-        <v>120</v>
-      </c>
-      <c r="M26" s="28" t="s">
-        <v>68</v>
+        <v>90</v>
+      </c>
+      <c r="M26" s="31" t="s">
+        <v>261</v>
       </c>
       <c r="N26" s="30" t="e">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:H$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2407,13 +2458,13 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>11</v>
@@ -2425,10 +2476,10 @@
         <v>32</v>
       </c>
       <c r="L27" s="5">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N27" s="30" t="e">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:H$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2445,7 +2496,7 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
@@ -2466,7 +2517,7 @@
         <v>40</v>
       </c>
       <c r="M28" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N28" s="30" t="e">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:H$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2483,13 +2534,13 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>25</v>
@@ -2498,13 +2549,13 @@
         <v>25</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L29" s="5">
         <v>10</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="N29" s="30" t="e">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:H$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2521,31 +2572,31 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B30" s="29">
         <v>2</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="L30" s="5">
         <v>40</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N30" s="30" t="e">
         <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:H$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2562,34 +2613,34 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="L31" s="5">
         <v>50</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="N31" s="30" t="e">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:H$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2606,25 +2657,25 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L32" s="5">
         <v>20</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="N32" s="30" t="e">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:H$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2641,25 +2692,25 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B33" s="29">
         <v>2</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L33" s="5">
         <v>20</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="N33" s="30" t="e">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:H$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2676,25 +2727,25 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L34" s="5">
         <v>30</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="N34" s="30" t="e">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:H$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2711,25 +2762,25 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L35" s="5">
         <v>30</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="N35" s="30" t="e">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:H$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2740,23 +2791,23 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="F36" s="31"/>
       <c r="K36" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="L36" s="5">
         <v>10</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2764,13 +2815,13 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>8</v>
@@ -2780,10 +2831,10 @@
       </c>
       <c r="K37" s="31"/>
       <c r="L37" s="5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2791,13 +2842,13 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>27</v>
@@ -2807,10 +2858,10 @@
       </c>
       <c r="K38" s="31"/>
       <c r="L38" s="5">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2818,13 +2869,13 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>11</v>
@@ -2834,10 +2885,10 @@
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2845,7 +2896,7 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
@@ -2857,13 +2908,13 @@
         <v>15</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L40" s="5">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="N40" s="30" t="e">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:H$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2880,25 +2931,28 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>265</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="L41" s="5">
         <v>20</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="N41" s="30">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:H$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2914,25 +2968,26 @@
       </c>
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>231</v>
+      <c r="A42" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="K42" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="L42" s="5">
+        <v>114</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="K42" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="L42" s="29">
         <v>30</v>
       </c>
       <c r="M42" s="28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="N42" s="30">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:H$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2942,71 +2997,65 @@
         <f>2 + N42 + IF(H42="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="P42" s="23">
+      <c r="P42" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="29">
+        <v>1</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="K43" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="L43" s="29">
+        <v>40</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="29"/>
+    </row>
+    <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B44" s="29">
+        <v>1</v>
+      </c>
+      <c r="C44" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="K43" t="s">
-        <v>209</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="M43" t="s">
-        <v>115</v>
-      </c>
-      <c r="N43">
-        <f>IF(F43&lt;&gt;"",VLOOKUP(F43,Economy!A$2:H$13,9,FALSE),0)+IF(G43&lt;&gt;"",VLOOKUP(G43,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O43" s="17">
-        <f>2 + N43 + IF(H43="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P43" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O43),#REF!/ O43,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>104</v>
-      </c>
-      <c r="K44" t="s">
-        <v>208</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="M44" t="s">
-        <v>105</v>
-      </c>
-      <c r="N44">
+      <c r="K44" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="L44" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="M44" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="N44" s="28">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:H$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:H$13,9,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="O44" s="17">
+      <c r="O44" s="30">
         <f>2 + N44 + IF(H44="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="P44" s="3" t="str">
+      <c r="P44" s="29" t="str">
         <f>IF(ISNUMBER(#REF!/O44),#REF!/ O44,"")</f>
         <v/>
       </c>
@@ -3019,22 +3068,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K45" t="s">
-        <v>213</v>
-      </c>
-      <c r="L45" s="5">
-        <v>100</v>
+        <v>197</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="M45" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="N45">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:H$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3057,24 +3100,30 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>40</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="K46" t="s">
-        <v>207</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>243</v>
+        <v>201</v>
+      </c>
+      <c r="L46" s="5">
+        <v>100</v>
       </c>
       <c r="M46" t="s">
-        <v>38</v>
-      </c>
-      <c r="N46">
-        <f>IF(F46&lt;&gt;"",VLOOKUP(F46,Economy!A$2:H$13,9,FALSE),0)+IF(G46&lt;&gt;"",VLOOKUP(G46,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O46" s="17">
-        <f>2 + N46 + IF(H46="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="N46" t="e">
+        <f>IF(#REF!&lt;&gt;"",VLOOKUP(#REF!,Economy!A$2:H$13,9,FALSE),0)+IF(#REF!&lt;&gt;"",VLOOKUP(#REF!,Economy!A$2:H$13,9,FALSE),0)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O46" s="17" t="e">
+        <f>2 + N46 + IF(F46="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
+        <v>#REF!</v>
       </c>
       <c r="P46" s="3" t="str">
         <f>IF(ISNUMBER(#REF!/O46),#REF!/ O46,"")</f>
@@ -3089,27 +3138,28 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="K47" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N47">
-        <v>2</v>
+        <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:H$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:H$13,9,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="O47" s="17">
         <f>2 + N47 + IF(H47="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>4</v>
-      </c>
-      <c r="P47" s="3">
-        <f>8/O47</f>
         <v>2</v>
+      </c>
+      <c r="P47" s="3" t="str">
+        <f>IF(ISNUMBER(#REF!/O47),#REF!/ O47,"")</f>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3120,28 +3170,27 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="K48" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M48" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="N48">
-        <f>IF(F48&lt;&gt;"",VLOOKUP(F48,Economy!A$2:H$13,9,FALSE),0)+IF(G48&lt;&gt;"",VLOOKUP(G48,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O48" s="17">
         <f>2 + N48 + IF(H48="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="P48" s="3">
+        <f>8/O48</f>
         <v>2</v>
-      </c>
-      <c r="P48" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O48),#REF!/ O48,"")</f>
-        <v/>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3152,16 +3201,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="K49" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M49" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="N49">
         <f>IF(F49&lt;&gt;"",VLOOKUP(F49,Economy!A$2:H$13,9,FALSE),0)+IF(G49&lt;&gt;"",VLOOKUP(G49,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3184,16 +3233,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K50" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M50" t="s">
-        <v>41</v>
+        <v>249</v>
       </c>
       <c r="N50">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:H$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3216,27 +3265,27 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="K51" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M51" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="N51">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,Economy!A$2:H$13,9,FALSE),0)+IF(G51&lt;&gt;"",VLOOKUP(G51,Economy!A$2:H$13,9,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="O51" s="17" t="e">
+      <c r="O51" s="17">
         <f>2 + N51 + IF(H51="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
+        <v>2</v>
       </c>
       <c r="P51" s="3" t="str">
         <f>IF(ISNUMBER(#REF!/O51),#REF!/ O51,"")</f>
@@ -3251,48 +3300,104 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>239</v>
+        <v>44</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="K52" t="s">
-        <v>241</v>
+        <v>195</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="M52" t="s">
-        <v>242</v>
-      </c>
-      <c r="N52"/>
+        <v>53</v>
+      </c>
+      <c r="N52">
+        <f>IF(F52&lt;&gt;"",VLOOKUP(F52,Economy!A$2:H$13,9,FALSE),0)+IF(G52&lt;&gt;"",VLOOKUP(G52,Economy!A$2:H$13,9,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O52" s="17" t="e">
+        <f>2 + N52 + IF(H52="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P52" s="3" t="str">
+        <f>IF(ISNUMBER(#REF!/O52),#REF!/ O52,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="K53" t="s">
-        <v>201</v>
-      </c>
-      <c r="L53" s="5">
+        <v>227</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M53" t="s">
+        <v>228</v>
+      </c>
+      <c r="N53"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>254</v>
+      </c>
+      <c r="K54" t="s">
+        <v>255</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M54" t="s">
+        <v>256</v>
+      </c>
+      <c r="N54"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>218</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="K55" t="s">
+        <v>193</v>
+      </c>
+      <c r="L55" s="5">
         <v>0</v>
       </c>
-      <c r="M53" t="s">
-        <v>176</v>
-      </c>
-      <c r="N53">
-        <f>IF(F53&lt;&gt;"",VLOOKUP(F53,Economy!A$2:H$13,9,FALSE),0)+IF(G53&lt;&gt;"",VLOOKUP(G53,Economy!A$2:H$13,9,FALSE),0)</f>
+      <c r="M55" t="s">
+        <v>168</v>
+      </c>
+      <c r="N55">
+        <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:H$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:H$13,9,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="O53" s="17">
-        <f>2 + N53 + IF(H53="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
+      <c r="O55" s="17">
+        <f>2 + N55 + IF(H55="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
         <v>2</v>
       </c>
-      <c r="P53" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O53),#REF!/ O53,"")</f>
+      <c r="P55" s="3" t="str">
+        <f>IF(ISNUMBER(#REF!/O55),#REF!/ O55,"")</f>
         <v/>
       </c>
     </row>
@@ -3308,7 +3413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3333,10 +3438,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3356,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3368,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3378,8 +3483,8 @@
       <c r="B3" s="27">
         <v>4</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>101</v>
+      <c r="C3" s="53" t="s">
+        <v>242</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3391,7 +3496,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3402,7 +3507,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>11</v>
@@ -3411,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3422,7 +3527,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>14</v>
@@ -3434,7 +3539,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3445,7 +3550,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>26</v>
@@ -3465,7 +3570,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>12</v>
@@ -3474,7 +3579,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3485,7 +3590,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>13</v>
@@ -3494,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3505,7 +3610,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>27</v>
@@ -3514,13 +3619,13 @@
         <v>27</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3530,8 +3635,8 @@
       <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>98</v>
+      <c r="C10" s="53" t="s">
+        <v>245</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>23</v>
@@ -3539,8 +3644,8 @@
       <c r="G10" s="5">
         <v>1</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>91</v>
+      <c r="H10" s="53" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3551,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
@@ -3563,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3574,19 +3679,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>103</v>
-      </c>
       <c r="F12" s="26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
-      <c r="H12" s="26" t="s">
-        <v>127</v>
+      <c r="H12" s="53" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3597,7 +3702,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>15</v>
@@ -3606,7 +3711,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3617,19 +3722,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3640,7 +3745,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>25</v>
@@ -3649,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3663,7 +3768,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,25 +3787,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3903,7 +4008,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -3911,15 +4016,15 @@
       </c>
       <c r="C8" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A13)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="17">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="17">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="17">
         <f t="shared" si="1"/>
@@ -3944,15 +4049,15 @@
       </c>
       <c r="C9" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A8)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="17">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="17">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="17">
         <f t="shared" si="1"/>
@@ -4010,15 +4115,15 @@
       </c>
       <c r="C11" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A10)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="17">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="17">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="1"/>
@@ -4137,75 +4242,75 @@
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="P2" s="38" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
@@ -4233,7 +4338,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -4259,10 +4364,10 @@
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
@@ -4273,7 +4378,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -4298,7 +4403,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
@@ -4309,7 +4414,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="17">
         <v>2</v>
@@ -4319,7 +4424,7 @@
         <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4343,7 +4448,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4353,10 +4458,10 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4366,7 +4471,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4391,7 +4496,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4401,10 +4506,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4414,7 +4519,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4438,7 +4543,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4448,10 +4553,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
@@ -4462,7 +4567,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4486,17 +4591,17 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="e">
         <f>IF(ISNA(VLOOKUP(A9,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A9,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>42</v>
@@ -4509,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4534,7 +4639,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4544,7 +4649,7 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>42</v>
@@ -4557,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4582,20 +4687,20 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="3" t="e">
         <f>IF(ISNA(VLOOKUP(A11,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A11,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4605,7 +4710,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -4638,7 +4743,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
@@ -4677,7 +4782,7 @@
         <v/>
       </c>
       <c r="E13" s="37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
@@ -4688,7 +4793,7 @@
         <v/>
       </c>
       <c r="H13" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="17">
@@ -4716,7 +4821,7 @@
         <v/>
       </c>
       <c r="E14" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,12,FALSE)),"",VLOOKUP(E14,Specials!C:P,12,FALSE))</f>
@@ -4756,7 +4861,7 @@
         <v/>
       </c>
       <c r="E15" s="37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
@@ -4898,7 +5003,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -4908,7 +5013,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -4939,7 +5044,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -4948,7 +5053,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -4976,7 +5081,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -4986,7 +5091,7 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>33</v>
@@ -5012,7 +5117,7 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B22" s="49" t="e">
         <f>SUM(B3:B21)</f>
@@ -5024,7 +5129,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -5036,7 +5141,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -5050,21 +5155,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -5088,7 +5193,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Specials!$C$3:$C$53</xm:f>
+            <xm:f>Specials!$C$3:$C$55</xm:f>
           </x14:formula1>
           <xm:sqref>E14:E21</xm:sqref>
         </x14:dataValidation>
@@ -5115,21 +5220,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5144,7 +5249,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5159,7 +5264,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5174,7 +5279,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,7 +5294,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5204,7 +5309,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just tweaking. ok i need to quit now.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -329,9 +329,6 @@
     <t>Carrot</t>
   </si>
   <si>
-    <t>The Expensive Payoff</t>
-  </si>
-  <si>
     <t>Glad you didn't have to eat these!</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>Technically, we're just a shack made out of fiberglass, but this game doesn't need another resource.</t>
   </si>
   <si>
-    <t>The Point Ladder Engine</t>
-  </si>
-  <si>
     <t>Point Ladder</t>
   </si>
   <si>
@@ -845,13 +839,19 @@
     <t>Draw 2 Take 1</t>
   </si>
   <si>
-    <t>As an action, once per turn, you may trash 1 Special in your hand to Climb a Ladder 1 space.</t>
-  </si>
-  <si>
     <t>The Combo Thing-in-a-Set</t>
   </si>
   <si>
     <t>"Which is more fun… scoring more points for myself, or denying points from my opponents?"</t>
+  </si>
+  <si>
+    <t>The Foodie Payoff</t>
+  </si>
+  <si>
+    <t>The Ladder Engine</t>
+  </si>
+  <si>
+    <t>As an action, once per turn, you may trash 1 Special in your hand or 1 Resource card on your tableau to Climb a Ladder 1 space.</t>
   </si>
 </sst>
 </file>
@@ -1472,8 +1472,8 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1523,7 @@
         <v>20</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1535,18 +1535,18 @@
         <v>1</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1560,10 +1560,10 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
@@ -1592,7 +1592,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
@@ -1624,13 +1624,13 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L4" s="5">
         <v>30</v>
@@ -1665,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
@@ -1697,16 +1697,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
@@ -1735,19 +1735,19 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>273</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1764,7 +1764,7 @@
         <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
@@ -1787,7 +1787,7 @@
         <v>50</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
@@ -1816,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>23</v>
@@ -1834,7 +1834,7 @@
         <v>20</v>
       </c>
       <c r="M10" s="54" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N10" s="24" t="e">
         <f>IF(F10&lt;&gt;"",VLOOKUP(F10,Economy!A$2:H$13,9,FALSE),0)+IF(G10&lt;&gt;"",VLOOKUP(G10,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -1863,10 +1863,10 @@
         <v>32</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
@@ -1927,25 +1927,25 @@
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>11</v>
@@ -1968,7 +1968,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>34</v>
@@ -1977,7 +1977,7 @@
         <v>20</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N14" s="24" t="e">
         <f>IF(F14&lt;&gt;"",VLOOKUP(F14,Economy!A$2:H$13,9,FALSE),0)+IF(G14&lt;&gt;"",VLOOKUP(G14,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
@@ -2009,7 +2009,7 @@
         <v>32</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>35</v>
@@ -2018,7 +2018,7 @@
         <v>10</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N15" s="24" t="e">
         <f>IF(F15&lt;&gt;"",VLOOKUP(F15,Economy!A$2:H$13,9,FALSE),0)+IF(G15&lt;&gt;"",VLOOKUP(G15,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2041,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>14</v>
@@ -2050,7 +2050,7 @@
         <v>32</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>36</v>
@@ -2059,7 +2059,7 @@
         <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N16" s="24" t="e">
         <f>IF(F16&lt;&gt;"",VLOOKUP(F16,Economy!A$2:H$13,9,FALSE),0)+IF(G16&lt;&gt;"",VLOOKUP(G16,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2082,14 +2082,14 @@
         <v>1</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" s="25"/>
       <c r="J17" s="54" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L17" s="5">
         <v>30</v>
@@ -2121,20 +2121,20 @@
         <v>37</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L18" s="5">
         <v>50</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B19" s="29">
         <v>1</v>
@@ -2169,10 +2169,10 @@
         <v>8</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
@@ -2195,13 +2195,13 @@
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>12</v>
@@ -2216,7 +2216,7 @@
         <v>30</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N20" s="30" t="e">
         <f>IF(F20&lt;&gt;"",VLOOKUP(F20,Economy!A$2:H$13,9,FALSE),0)+IF(G20&lt;&gt;"",VLOOKUP(G20,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
@@ -2251,13 +2251,13 @@
         <v>23</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L21" s="5">
         <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N21" s="30" t="e">
         <f>IF(F21&lt;&gt;"",VLOOKUP(F21,Economy!A$2:H$13,9,FALSE),0)+IF(G21&lt;&gt;"",VLOOKUP(G21,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
@@ -2312,13 +2312,13 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>14</v>
@@ -2350,13 +2350,13 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
@@ -2371,7 +2371,7 @@
         <v>70</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N24" s="30" t="e">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:H$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>8</v>
@@ -2409,7 +2409,7 @@
         <v>80</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N25" s="30" t="e">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:H$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>14</v>
@@ -2447,7 +2447,7 @@
         <v>90</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N26" s="30" t="e">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:H$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
@@ -2485,7 +2485,7 @@
         <v>100</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N27" s="30" t="e">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:H$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>25</v>
@@ -2561,7 +2561,7 @@
         <v>10</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N29" s="30" t="e">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:H$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B30" s="29">
         <v>2</v>
@@ -2587,16 +2587,16 @@
         <v>52</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L30" s="5">
         <v>40</v>
@@ -2619,34 +2619,34 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L31" s="5">
         <v>50</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N31" s="30" t="e">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:H$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2663,25 +2663,25 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L32" s="5">
         <v>20</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N32" s="30" t="e">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:H$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2698,25 +2698,25 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B33" s="29">
         <v>2</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L33" s="5">
         <v>20</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N33" s="30" t="e">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:H$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2733,25 +2733,25 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L34" s="5">
         <v>30</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N34" s="30" t="e">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:H$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2768,25 +2768,25 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L35" s="5">
         <v>30</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N35" s="30" t="e">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:H$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2797,23 +2797,23 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F36" s="31"/>
       <c r="K36" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L36" s="5">
         <v>10</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2821,13 +2821,13 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>8</v>
@@ -2840,7 +2840,7 @@
         <v>60</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>27</v>
@@ -2867,7 +2867,7 @@
         <v>70</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2875,13 +2875,13 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>11</v>
@@ -2894,7 +2894,7 @@
         <v>80</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
@@ -2914,13 +2914,13 @@
         <v>15</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L40" s="5">
         <v>-30</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N40" s="30" t="e">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:H$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2937,28 +2937,28 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L41" s="5">
         <v>20</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="N41" s="30">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:H$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -2975,25 +2975,25 @@
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L42" s="29">
         <v>30</v>
       </c>
       <c r="M42" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N42" s="30">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:H$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>26</v>
@@ -3022,13 +3022,13 @@
         <v>7</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L43" s="29">
         <v>40</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
@@ -3045,13 +3045,13 @@
         <v>21</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M44" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N44" s="28">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:H$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3074,16 +3074,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
+        <v>272</v>
+      </c>
+      <c r="K45" t="s">
+        <v>188</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="M45" t="s">
         <v>100</v>
-      </c>
-      <c r="K45" t="s">
-        <v>190</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M45" t="s">
-        <v>101</v>
       </c>
       <c r="N45">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:H$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3115,7 +3115,7 @@
         <v>99</v>
       </c>
       <c r="K46" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L46" s="5">
         <v>100</v>
@@ -3144,13 +3144,13 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K47" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M47" t="s">
         <v>38</v>
@@ -3179,10 +3179,10 @@
         <v>70</v>
       </c>
       <c r="K48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M48" t="s">
         <v>39</v>
@@ -3207,13 +3207,13 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M49" t="s">
         <v>28</v>
@@ -3242,13 +3242,13 @@
         <v>30</v>
       </c>
       <c r="K50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N50">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:H$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3274,13 +3274,13 @@
         <v>33</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M51" t="s">
         <v>41</v>
@@ -3312,10 +3312,10 @@
         <v>32</v>
       </c>
       <c r="K52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M52" t="s">
         <v>53</v>
@@ -3341,16 +3341,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
+        <v>215</v>
+      </c>
+      <c r="K53" t="s">
         <v>217</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="M53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N53"/>
     </row>
@@ -3362,37 +3362,37 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
+        <v>244</v>
+      </c>
+      <c r="K54" t="s">
+        <v>245</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="M54" t="s">
         <v>246</v>
-      </c>
-      <c r="K54" t="s">
-        <v>247</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" t="s">
-        <v>248</v>
       </c>
       <c r="N54"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K55" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L55" s="5">
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N55">
         <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:H$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:H$13,9,FALSE),0)</f>
@@ -3444,10 +3444,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3479,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3502,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3533,7 +3533,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>14</v>
@@ -3545,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>23</v>
@@ -3651,7 +3651,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3662,7 +3662,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3697,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3734,7 +3734,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
@@ -3760,7 +3760,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3793,25 +3793,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>129</v>
-      </c>
       <c r="H1" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4248,70 +4248,70 @@
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="47" t="s">
         <v>138</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>139</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="38" t="s">
-        <v>139</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I2" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="K2" s="38" t="s">
-        <v>139</v>
-      </c>
       <c r="L2" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M2" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="38" t="s">
-        <v>139</v>
-      </c>
       <c r="P2" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -4344,7 +4344,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -4370,7 +4370,7 @@
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>94</v>
@@ -4384,7 +4384,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -4430,7 +4430,7 @@
         <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4454,7 +4454,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4464,7 +4464,7 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>78</v>
@@ -4477,7 +4477,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4512,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>78</v>
@@ -4525,7 +4525,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4559,7 +4559,7 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E8" s="37" t="s">
         <v>92</v>
@@ -4573,7 +4573,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4607,7 +4607,7 @@
         <v>#N/A</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>42</v>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4655,7 +4655,7 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>42</v>
@@ -4668,7 +4668,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4693,7 +4693,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4703,10 +4703,10 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4716,7 +4716,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -5009,7 +5009,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -5019,7 +5019,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -5050,7 +5050,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -5059,7 +5059,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -5087,7 +5087,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -5097,7 +5097,7 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>33</v>
@@ -5123,7 +5123,7 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" s="49" t="e">
         <f>SUM(B3:B21)</f>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -5161,21 +5161,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -5229,30 +5229,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,7 +5267,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -5292,7 +5292,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -5317,7 +5317,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5342,7 +5342,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5367,7 +5367,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
more work on layout, icons, and snarks. some vp.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="272">
   <si>
     <t>Type</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Look at you, Dr. Fancy Man!</t>
-  </si>
-  <si>
     <t>The Building Building Building</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>The Amazing Building</t>
   </si>
   <si>
-    <t>Good move. Not Great. But Good.</t>
-  </si>
-  <si>
     <t>The Unused Resources Payoff</t>
   </si>
   <si>
@@ -419,21 +413,12 @@
     <t>Rarity Cost</t>
   </si>
   <si>
-    <t>VP/Action</t>
-  </si>
-  <si>
-    <t>Actions Cost</t>
-  </si>
-  <si>
     <t>Est. Action Cost</t>
   </si>
   <si>
     <t>Even More Sheep!</t>
   </si>
   <si>
-    <t>Trash1 Cost</t>
-  </si>
-  <si>
     <t>The Combo Materials</t>
   </si>
   <si>
@@ -563,9 +548,6 @@
     <t>VP/Climb</t>
   </si>
   <si>
-    <t xml:space="preserve">Are we climbing a sheep, or are is the sheep doing the climbing? </t>
-  </si>
-  <si>
     <t>Always make sure your clay ladders are kiln-dried before embarking.</t>
   </si>
   <si>
@@ -593,9 +575,6 @@
     <t>30 VP for each Soldier, +30 additional VP if you end the game with the most soldiers.</t>
   </si>
   <si>
-    <t>60 VPs for each Cattle, Carrot</t>
-  </si>
-  <si>
     <t>Ladder Strategy</t>
   </si>
   <si>
@@ -623,9 +602,6 @@
     <t>Player with most soldiers may trash any 1 available Special at round start in Midgame.</t>
   </si>
   <si>
-    <t>80 VP if you have Invested plus 10 VP for each Gold.</t>
-  </si>
-  <si>
     <t>Early Sheep Climb!</t>
   </si>
   <si>
@@ -680,9 +656,6 @@
     <t>Upon Endgame initiation, you may trash 1 available Payoff card of your choosing.</t>
   </si>
   <si>
-    <t>10/30/60 VP if you have 1/2/3 Thing-in-a-Set cards.</t>
-  </si>
-  <si>
     <t>Yay! Another point ladder.</t>
   </si>
   <si>
@@ -737,9 +710,6 @@
     <t>The Breeding Plant</t>
   </si>
   <si>
-    <t>Or is it wheat? Or corn? Seeds? Reed?</t>
-  </si>
-  <si>
     <t>Think of carrots like a self-insta-slaughtering animal.</t>
   </si>
   <si>
@@ -852,6 +822,27 @@
   </si>
   <si>
     <t>As an action, once per turn, you may trash 1 Special in your hand or 1 Resource card on your tableau to Climb a Ladder 1 space.</t>
+  </si>
+  <si>
+    <t>Or is it wheat? Reeds? Seeds? Corn? Did you know that corn is a type of grain? Be sure to bring up this fact in your next Euro game. Everyone will appreciate the rules ambiguity it creates.</t>
+  </si>
+  <si>
+    <t>Cue the sexual innuendo jokes.</t>
+  </si>
+  <si>
+    <t>Good move. Not Great. What else are you going to do to get points? No pressure. But you should think of something. Now.</t>
+  </si>
+  <si>
+    <t>Are we climbing a sheep, or is the sheep doing the climbing? Because they're not goats. Should we be worried?</t>
+  </si>
+  <si>
+    <t>50 VPs for each Cattle, Carrot</t>
+  </si>
+  <si>
+    <t>60 VP if you have Invested plus 10 VP for each Gold.</t>
+  </si>
+  <si>
+    <t>20/40/70 VP if you have 1/2/3 Thing-in-a-Set cards.</t>
   </si>
 </sst>
 </file>
@@ -1471,9 +1462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,19 +1502,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="J1" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1534,25 +1525,19 @@
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="12"/>
@@ -1560,16 +1545,16 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="K2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1577,177 +1562,141 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="34" t="e">
-        <f>IF(F3&lt;&gt;"",VLOOKUP(F3,Economy!A$2:H$13,9,FALSE),0)+IF(G3&lt;&gt;"",VLOOKUP(G3,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O3" s="34" t="e">
-        <f>2 + N3 + IF(H3="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P3" s="35" t="str">
-        <f>IF(ISNUMBER(#REF!/O3),#REF!/ O3,"")</f>
-        <v/>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L4" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="34">
-        <f>IF(F4&lt;&gt;"",VLOOKUP(F4,Economy!A$2:H$13,9,FALSE),0)+IF(G4&lt;&gt;"",VLOOKUP(G4,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="34">
-        <f>2 + N4 + IF(H4="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P4" s="35" t="str">
-        <f>IF(ISNUMBER(#REF!/O4),#REF!/ O4,"")</f>
-        <v/>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="35"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N5" s="34" t="e">
-        <f>IF(F5&lt;&gt;"",VLOOKUP(F5,Economy!A$2:H$13,9,FALSE),0)+IF(G5&lt;&gt;"",VLOOKUP(G5,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O5" s="34" t="e">
-        <f>2 + N5 + IF(H5="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P5" s="35" t="str">
-        <f>IF(ISNUMBER(#REF!/O5),#REF!/ O5,"")</f>
-        <v/>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="35"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="K6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="34" t="e">
-        <f>IF(F6&lt;&gt;"",VLOOKUP(F6,Economy!A$2:H$13,9,FALSE),0)+IF(G6&lt;&gt;"",VLOOKUP(G6,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O6" s="34" t="e">
-        <f>2 + N6 + IF(H6="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P6" s="35" t="str">
-        <f>IF(ISNUMBER(#REF!/O6),#REF!/ O6,"")</f>
-        <v/>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="35"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="K7" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1755,147 +1704,120 @@
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="N9" s="24">
-        <f>IF(F9&lt;&gt;"",VLOOKUP(F9,Economy!A$2:H$13,9,FALSE),0)+IF(G9&lt;&gt;"",VLOOKUP(G9,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="24">
-        <f>2 + N9 + IF(H9="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P9" s="23">
-        <f>L9/O9</f>
-        <v>15</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L10" s="5">
         <v>20</v>
       </c>
       <c r="M10" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="N10" s="24" t="e">
-        <f>IF(F10&lt;&gt;"",VLOOKUP(F10,Economy!A$2:H$13,9,FALSE),0)+IF(G10&lt;&gt;"",VLOOKUP(G10,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O10" s="24" t="e">
-        <f>2 + N10 + IF(H10="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P10" s="23" t="e">
-        <f t="shared" ref="P10:P42" si="0">L10/O10</f>
-        <v>#REF!</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" s="24">
-        <f>IF(F11&lt;&gt;"",VLOOKUP(F11,Economy!A$2:H$13,9,FALSE),0)+IF(G11&lt;&gt;"",VLOOKUP(G11,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="24" t="e">
-        <f>2 + N11 + IF(H11="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P11" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>12</v>
@@ -1910,42 +1832,33 @@
         <v>30</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" s="24" t="e">
-        <f>IF(F12&lt;&gt;"",VLOOKUP(F12,Economy!A$2:H$13,9,FALSE),0)+IF(G12&lt;&gt;"",VLOOKUP(G12,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O12" s="24" t="e">
-        <f>2 + N12 + IF(H12="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P12" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1953,255 +1866,201 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" s="5">
         <v>20</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="N14" s="24" t="e">
-        <f>IF(F14&lt;&gt;"",VLOOKUP(F14,Economy!A$2:H$13,9,FALSE),0)+IF(G14&lt;&gt;"",VLOOKUP(G14,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O14" s="24" t="e">
-        <f>2 + N14 + IF(H14="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P14" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L15" s="5">
         <v>10</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="N15" s="24" t="e">
-        <f>IF(F15&lt;&gt;"",VLOOKUP(F15,Economy!A$2:H$13,9,FALSE),0)+IF(G15&lt;&gt;"",VLOOKUP(G15,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O15" s="24" t="e">
-        <f>2 + N15 + IF(H15="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P15" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="23"/>
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L16" s="5">
         <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>223</v>
-      </c>
-      <c r="N16" s="24" t="e">
-        <f>IF(F16&lt;&gt;"",VLOOKUP(F16,Economy!A$2:H$13,9,FALSE),0)+IF(G16&lt;&gt;"",VLOOKUP(G16,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O16" s="24" t="e">
-        <f>2 + N16 + IF(H16="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P16" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="23"/>
     </row>
     <row r="17" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D17" s="25"/>
       <c r="J17" s="54" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L17" s="5">
         <v>30</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="24">
-        <f>IF(F17&lt;&gt;"",VLOOKUP(F17,Economy!A$2:H$13,9,FALSE),0)+IF(G17&lt;&gt;"",VLOOKUP(G17,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="24">
-        <f>2 + N17 + IF(H17="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P17" s="23">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L18" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="24">
-        <f>IF(F18&lt;&gt;"",VLOOKUP(F18,Economy!A$2:H$13,9,FALSE),0)+IF(G18&lt;&gt;"",VLOOKUP(G18,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="24" t="e">
-        <f>2 + N18 + IF(H18="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P18" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B19" s="29">
         <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>8</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="N19" s="30" t="e">
-        <f>IF(F19&lt;&gt;"",VLOOKUP(F19,Economy!A$2:H$13,9,FALSE),0)+IF(G19&lt;&gt;"",VLOOKUP(G19,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O19" s="30" t="e">
-        <f>2 + N19 + IF(H19="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P19" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>12</v>
@@ -2216,71 +2075,53 @@
         <v>30</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="N20" s="30" t="e">
-        <f>IF(F20&lt;&gt;"",VLOOKUP(F20,Economy!A$2:H$13,9,FALSE),0)+IF(G20&lt;&gt;"",VLOOKUP(G20,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O20" s="30" t="e">
-        <f>2 + N20 + IF(H20="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P20" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="23"/>
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="L21" s="5">
         <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="N21" s="30" t="e">
-        <f>IF(F21&lt;&gt;"",VLOOKUP(F21,Economy!A$2:H$13,9,FALSE),0)+IF(G21&lt;&gt;"",VLOOKUP(G21,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O21" s="30" t="e">
-        <f>2 + N21 + IF(H21="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P21" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="23"/>
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>8</v>
@@ -2289,36 +2130,27 @@
         <v>8</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L22" s="5">
         <v>60</v>
       </c>
       <c r="M22" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="N22" s="30" t="e">
-        <f>IF(F22&lt;&gt;"",VLOOKUP(F22,Economy!A$2:H$13,9,FALSE),0)+IF(G22&lt;&gt;"",VLOOKUP(G22,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O22" s="30" t="e">
-        <f>2 + N22 + IF(H22="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P22" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="23"/>
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>14</v>
@@ -2327,36 +2159,27 @@
         <v>8</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L23" s="5">
         <v>70</v>
       </c>
       <c r="M23" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="N23" s="30" t="e">
-        <f>IF(F23&lt;&gt;"",VLOOKUP(F23,Economy!A$2:H$13,9,FALSE),0)+IF(G23&lt;&gt;"",VLOOKUP(G23,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O23" s="30" t="e">
-        <f>2 + N23 + IF(H23="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P23" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="23"/>
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
@@ -2365,36 +2188,27 @@
         <v>14</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L24" s="5">
         <v>70</v>
       </c>
-      <c r="M24" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="N24" s="30" t="e">
-        <f>IF(F24&lt;&gt;"",VLOOKUP(F24,Economy!A$2:H$13,9,FALSE),0)+IF(G24&lt;&gt;"",VLOOKUP(G24,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O24" s="30" t="e">
-        <f>2 + N24 + IF(H24="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P24" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+      <c r="M24" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>8</v>
@@ -2403,36 +2217,27 @@
         <v>11</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L25" s="5">
         <v>80</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="N25" s="30" t="e">
-        <f>IF(F25&lt;&gt;"",VLOOKUP(F25,Economy!A$2:H$13,9,FALSE),0)+IF(G25&lt;&gt;"",VLOOKUP(G25,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O25" s="30" t="e">
-        <f>2 + N25 + IF(H25="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P25" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="23"/>
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>14</v>
@@ -2441,36 +2246,27 @@
         <v>11</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L26" s="5">
         <v>90</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="N26" s="30" t="e">
-        <f>IF(F26&lt;&gt;"",VLOOKUP(F26,Economy!A$2:H$13,9,FALSE),0)+IF(G26&lt;&gt;"",VLOOKUP(G26,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O26" s="30" t="e">
-        <f>2 + N26 + IF(H26="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P26" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>11</v>
@@ -2479,36 +2275,27 @@
         <v>11</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L27" s="5">
         <v>100</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="N27" s="30" t="e">
-        <f>IF(F27&lt;&gt;"",VLOOKUP(F27,Economy!A$2:H$13,9,FALSE),0)+IF(G27&lt;&gt;"",VLOOKUP(G27,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O27" s="30" t="e">
-        <f>2 + N27 + IF(H27="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P27" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="23"/>
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="28" t="s">
         <v>13</v>
@@ -2523,297 +2310,231 @@
         <v>40</v>
       </c>
       <c r="M28" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="N28" s="30" t="e">
-        <f>IF(F28&lt;&gt;"",VLOOKUP(F28,Economy!A$2:H$13,9,FALSE),0)+IF(G28&lt;&gt;"",VLOOKUP(G28,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O28" s="30" t="e">
-        <f>2 + N28 + IF(H28="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P28" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="23"/>
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L29" s="5">
         <v>10</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="N29" s="30" t="e">
-        <f>IF(F29&lt;&gt;"",VLOOKUP(F29,Economy!A$2:H$13,9,FALSE),0)+IF(G29&lt;&gt;"",VLOOKUP(G29,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O29" s="30" t="e">
-        <f>2 + N29 + IF(H29="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P29" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="23"/>
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B30" s="29">
         <v>2</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L30" s="5">
         <v>40</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="N30" s="30" t="e">
-        <f>IF(F30&lt;&gt;"",VLOOKUP(F30,Economy!A$2:H$13,9,FALSE),0)+IF(G30&lt;&gt;"",VLOOKUP(G30,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O30" s="30" t="e">
-        <f>2 + N30 + IF(H30="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P30" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="23"/>
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L31" s="5">
         <v>50</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="N31" s="30" t="e">
-        <f>IF(F31&lt;&gt;"",VLOOKUP(F31,Economy!A$2:H$13,9,FALSE),0)+IF(G31&lt;&gt;"",VLOOKUP(G31,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O31" s="30" t="e">
-        <f>2 + N31 + IF(H31="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P31" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="23"/>
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L32" s="5">
         <v>20</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="N32" s="30" t="e">
-        <f>IF(F32&lt;&gt;"",VLOOKUP(F32,Economy!A$2:H$13,9,FALSE),0)+IF(G32&lt;&gt;"",VLOOKUP(G32,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O32" s="30" t="e">
-        <f>2 + N32 + IF(H32="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P32" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="23"/>
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B33" s="29">
         <v>2</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L33" s="5">
         <v>20</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="N33" s="30" t="e">
-        <f>IF(F33&lt;&gt;"",VLOOKUP(F33,Economy!A$2:H$13,9,FALSE),0)+IF(G33&lt;&gt;"",VLOOKUP(G33,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O33" s="30" t="e">
-        <f>2 + N33 + IF(H33="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P33" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="23"/>
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L34" s="5">
         <v>30</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="N34" s="30" t="e">
-        <f>IF(F34&lt;&gt;"",VLOOKUP(F34,Economy!A$2:H$13,9,FALSE),0)+IF(G34&lt;&gt;"",VLOOKUP(G34,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O34" s="30" t="e">
-        <f>2 + N34 + IF(H34="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P34" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="23"/>
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L35" s="5">
         <v>30</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="N35" s="30" t="e">
-        <f>IF(F35&lt;&gt;"",VLOOKUP(F35,Economy!A$2:H$13,9,FALSE),0)+IF(G35&lt;&gt;"",VLOOKUP(G35,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N35" s="30"/>
       <c r="O35" s="30"/>
       <c r="P35" s="23"/>
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F36" s="31"/>
       <c r="K36" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L36" s="5">
         <v>10</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2821,26 +2542,26 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>8</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K37" s="31"/>
       <c r="L37" s="5">
         <v>60</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2848,16 +2569,16 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G38" s="31" t="s">
         <v>13</v>
@@ -2867,7 +2588,7 @@
         <v>70</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2875,26 +2596,26 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="5">
         <v>80</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2902,133 +2623,109 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="L40" s="5">
         <v>-30</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="N40" s="30" t="e">
-        <f>IF(F40&lt;&gt;"",VLOOKUP(F40,Economy!A$2:H$13,9,FALSE),0)+IF(G40&lt;&gt;"",VLOOKUP(G40,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O40" s="30" t="e">
-        <f>2 + N40 + IF(H40="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P40" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="23"/>
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="29">
+        <v>1</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="K41" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="B41" s="29">
-        <v>1</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="H41" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>216</v>
       </c>
       <c r="L41" s="5">
         <v>20</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="N41" s="30">
-        <f>IF(F41&lt;&gt;"",VLOOKUP(F41,Economy!A$2:H$13,9,FALSE),0)+IF(G41&lt;&gt;"",VLOOKUP(G41,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O41" s="30">
-        <f>2 + N41 + IF(H41="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P41" s="23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="23"/>
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="L42" s="29">
         <v>30</v>
       </c>
       <c r="M42" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="N42" s="30">
-        <f>IF(F42&lt;&gt;"",VLOOKUP(F42,Economy!A$2:H$13,9,FALSE),0)+IF(G42&lt;&gt;"",VLOOKUP(G42,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O42" s="30">
-        <f>2 + N42 + IF(H42="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P42" s="29">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="29"/>
     </row>
     <row r="43" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>200</v>
+      </c>
       <c r="B43" s="29">
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J43" s="31" t="s">
         <v>7</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="L43" s="29">
         <v>40</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -3036,35 +2733,25 @@
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M44" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="N44" s="28">
-        <f>IF(F44&lt;&gt;"",VLOOKUP(F44,Economy!A$2:H$13,9,FALSE),0)+IF(G44&lt;&gt;"",VLOOKUP(G44,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O44" s="30">
-        <f>2 + N44 + IF(H44="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P44" s="29" t="str">
-        <f>IF(ISNUMBER(#REF!/O44),#REF!/ O44,"")</f>
-        <v/>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="O44" s="30"/>
+      <c r="P44" s="29"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -3074,29 +2761,18 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="K45" t="s">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M45" t="s">
-        <v>100</v>
-      </c>
-      <c r="N45">
-        <f>IF(F45&lt;&gt;"",VLOOKUP(F45,Economy!A$2:H$13,9,FALSE),0)+IF(G45&lt;&gt;"",VLOOKUP(G45,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O45" s="17">
-        <f>2 + N45 + IF(H45="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P45" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O45),#REF!/ O45,"")</f>
-        <v/>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="N45"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -3106,35 +2782,24 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K46" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L46" s="5">
         <v>100</v>
       </c>
       <c r="M46" t="s">
-        <v>24</v>
-      </c>
-      <c r="N46" t="e">
-        <f>IF(#REF!&lt;&gt;"",VLOOKUP(#REF!,Economy!A$2:H$13,9,FALSE),0)+IF(#REF!&lt;&gt;"",VLOOKUP(#REF!,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O46" s="17" t="e">
-        <f>2 + N46 + IF(F46="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P46" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O46),#REF!/ O46,"")</f>
-        <v/>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="N46"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3144,29 +2809,18 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K47" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M47" t="s">
-        <v>38</v>
-      </c>
-      <c r="N47">
-        <f>IF(F47&lt;&gt;"",VLOOKUP(F47,Economy!A$2:H$13,9,FALSE),0)+IF(G47&lt;&gt;"",VLOOKUP(G47,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O47" s="17">
-        <f>2 + N47 + IF(H47="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P47" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O47),#REF!/ O47,"")</f>
-        <v/>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="N47"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3176,30 +2830,20 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K48" t="s">
-        <v>198</v>
+        <v>270</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M48" t="s">
-        <v>39</v>
-      </c>
-      <c r="N48">
-        <v>2</v>
-      </c>
-      <c r="O48" s="17">
-        <f>2 + N48 + IF(H48="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>4</v>
-      </c>
-      <c r="P48" s="3">
-        <f>8/O48</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="N48"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -3207,31 +2851,20 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K49" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M49" t="s">
-        <v>28</v>
-      </c>
-      <c r="N49">
-        <f>IF(F49&lt;&gt;"",VLOOKUP(F49,Economy!A$2:H$13,9,FALSE),0)+IF(G49&lt;&gt;"",VLOOKUP(G49,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O49" s="17">
-        <f>2 + N49 + IF(H49="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P49" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O49),#REF!/ O49,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="N49"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -3239,31 +2872,20 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K50" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M50" t="s">
-        <v>239</v>
-      </c>
-      <c r="N50">
-        <f>IF(F50&lt;&gt;"",VLOOKUP(F50,Economy!A$2:H$13,9,FALSE),0)+IF(G50&lt;&gt;"",VLOOKUP(G50,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O50" s="17">
-        <f>2 + N50 + IF(H50="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P50" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O50),#REF!/ O50,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="N50"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -3271,34 +2893,23 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K51" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N51">
-        <f>IF(F51&lt;&gt;"",VLOOKUP(F51,Economy!A$2:H$13,9,FALSE),0)+IF(G51&lt;&gt;"",VLOOKUP(G51,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O51" s="17">
-        <f>2 + N51 + IF(H51="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P51" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O51),#REF!/ O51,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="N51"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -3306,34 +2917,23 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K52" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M52" t="s">
-        <v>53</v>
-      </c>
-      <c r="N52">
-        <f>IF(F52&lt;&gt;"",VLOOKUP(F52,Economy!A$2:H$13,9,FALSE),0)+IF(G52&lt;&gt;"",VLOOKUP(G52,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O52" s="17" t="e">
-        <f>2 + N52 + IF(H52="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P52" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O52),#REF!/ O52,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="N52"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -3341,20 +2941,20 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="K53" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M53" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="N53"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -3362,50 +2962,39 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="K54" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="M54" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="N54"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K55" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="L55" s="5">
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>167</v>
-      </c>
-      <c r="N55">
-        <f>IF(F55&lt;&gt;"",VLOOKUP(F55,Economy!A$2:H$13,9,FALSE),0)+IF(G55&lt;&gt;"",VLOOKUP(G55,Economy!A$2:H$13,9,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O55" s="17">
-        <f>2 + N55 + IF(H55="Building",VLOOKUP("Stone",Economy!A$2:H$13,9)+2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P55" s="3" t="str">
-        <f>IF(ISNUMBER(#REF!/O55),#REF!/ O55,"")</f>
-        <v/>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="N55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3419,7 +3008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3444,10 +3033,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3467,7 +3056,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3479,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3490,7 +3079,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3502,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3513,7 +3102,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>11</v>
@@ -3522,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3533,7 +3122,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>14</v>
@@ -3545,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3556,16 +3145,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>17</v>
+      <c r="H6" s="53" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3576,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>12</v>
@@ -3585,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3596,7 +3185,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>13</v>
@@ -3605,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3616,22 +3205,22 @@
         <v>2</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3642,16 +3231,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>236</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3662,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3685,19 +3274,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3708,7 +3297,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>15</v>
@@ -3717,7 +3306,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3728,19 +3317,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3751,16 +3340,16 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3793,25 +3382,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3882,7 +3471,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A4)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A4)</f>
@@ -4014,7 +3603,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -4047,7 +3636,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A9)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A9)</f>
@@ -4080,7 +3669,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A10)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A10)</f>
@@ -4146,7 +3735,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A12)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A12)</f>
@@ -4248,75 +3837,75 @@
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>141</v>
-      </c>
       <c r="I2" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>141</v>
-      </c>
       <c r="M2" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="P2" s="38" t="s">
         <v>136</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
@@ -4344,7 +3933,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -4359,21 +3948,21 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="17" t="e">
+        <v>17</v>
+      </c>
+      <c r="B4" s="17">
         <f>IF(ISNA(VLOOKUP(A4,Specials!C:P,12,FALSE)),"",VLOOKUP(A4,Specials!C:P,12,FALSE))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(A4,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A4,Specials!C:P,9,FALSE))</f>
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
@@ -4384,7 +3973,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -4409,7 +3998,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
@@ -4420,7 +4009,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="17">
         <v>2</v>
@@ -4430,7 +4019,7 @@
         <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4454,7 +4043,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4464,10 +4053,10 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4477,7 +4066,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4502,7 +4091,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4512,10 +4101,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4525,7 +4114,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4549,7 +4138,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4559,10 +4148,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
@@ -4573,7 +4162,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4597,7 +4186,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
@@ -4607,10 +4196,10 @@
         <v>#N/A</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="17">
         <v>2</v>
@@ -4620,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4645,7 +4234,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4655,10 +4244,10 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="17">
         <v>1</v>
@@ -4668,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4693,7 +4282,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4703,10 +4292,10 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4716,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -4740,7 +4329,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
@@ -4749,7 +4338,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
@@ -4788,7 +4377,7 @@
         <v/>
       </c>
       <c r="E13" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
@@ -4799,7 +4388,7 @@
         <v/>
       </c>
       <c r="H13" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="17">
@@ -4827,7 +4416,7 @@
         <v/>
       </c>
       <c r="E14" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,12,FALSE)),"",VLOOKUP(E14,Specials!C:P,12,FALSE))</f>
@@ -4838,7 +4427,7 @@
         <v/>
       </c>
       <c r="H14" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="17" t="str">
@@ -4867,7 +4456,7 @@
         <v/>
       </c>
       <c r="E15" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
@@ -5009,7 +4598,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -5019,7 +4608,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -5050,7 +4639,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -5059,7 +4648,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -5087,7 +4676,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -5097,10 +4686,10 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J21" s="17">
         <f>IF(ISNA(VLOOKUP(I21,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I21,Specials!$C:$P,12,FALSE))</f>
@@ -5123,11 +4712,11 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="49" t="e">
+        <v>134</v>
+      </c>
+      <c r="B22" s="49">
         <f>SUM(B3:B21)</f>
-        <v>#REF!</v>
+        <v>12</v>
       </c>
       <c r="C22" s="48" t="e">
         <f>SUM(C3:C21)</f>
@@ -5135,7 +4724,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -5147,7 +4736,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -5161,21 +4750,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -5229,30 +4818,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,7 +4856,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -5292,7 +4881,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -5317,7 +4906,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5342,7 +4931,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5367,7 +4956,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
stabilizing the code a bit for newest squib
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -584,9 +584,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>No substitutions</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
@@ -776,9 +773,6 @@
     <t>Ok everyone, this player is officially procrastinating on getting VPs.</t>
   </si>
   <si>
-    <t>You may trash this card from your tableau for any 2 Resources.</t>
-  </si>
-  <si>
     <t>You may only play this card before playing an Engine.</t>
   </si>
   <si>
@@ -843,6 +837,12 @@
   </si>
   <si>
     <t>20/40/70 VP if you have 1/2/3 Thing-in-a-Set cards.</t>
+  </si>
+  <si>
+    <t>You may not do any substitutions to play this card.</t>
+  </si>
+  <si>
+    <t>You may trash this card from your tableau for any 2 available Resource cards.</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1463,8 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1514,7 @@
         <v>19</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1545,10 +1545,10 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
@@ -1603,10 +1603,10 @@
         <v>169</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
@@ -1632,7 +1632,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K5" t="s">
         <v>115</v>
@@ -1655,13 +1655,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K6" t="s">
         <v>120</v>
@@ -1684,13 +1684,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
@@ -1713,7 +1713,7 @@
         <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
@@ -1736,7 +1736,7 @@
         <v>49</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
@@ -1756,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>22</v>
@@ -1794,7 +1794,7 @@
         <v>31</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>118</v>
@@ -1846,19 +1846,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1881,7 +1881,7 @@
         <v>31</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>33</v>
@@ -1913,7 +1913,7 @@
         <v>31</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>34</v>
@@ -1945,7 +1945,7 @@
         <v>31</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>35</v>
@@ -1954,7 +1954,7 @@
         <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="D17" s="25"/>
       <c r="J17" s="54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K17" s="22" t="s">
         <v>109</v>
@@ -2007,11 +2007,11 @@
         <v>31</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L18" s="5">
         <v>40</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B19" s="29">
         <v>1</v>
@@ -2037,7 +2037,7 @@
         <v>8</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K19" s="28" t="s">
         <v>107</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
@@ -2101,13 +2101,13 @@
         <v>22</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L21" s="5">
         <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
@@ -2173,13 +2173,13 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
@@ -2194,7 +2194,7 @@
         <v>70</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
@@ -2202,13 +2202,13 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>8</v>
@@ -2223,7 +2223,7 @@
         <v>80</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>14</v>
@@ -2252,7 +2252,7 @@
         <v>90</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
@@ -2339,7 +2339,7 @@
         <v>10</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" s="29">
         <v>2</v>
@@ -2362,10 +2362,10 @@
         <v>8</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L30" s="5">
         <v>40</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
@@ -2397,10 +2397,10 @@
         <v>14</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L31" s="5">
         <v>50</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
@@ -2426,13 +2426,13 @@
         <v>12</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L32" s="5">
         <v>20</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B33" s="29">
         <v>2</v>
@@ -2452,13 +2452,13 @@
         <v>22</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L33" s="5">
         <v>20</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
@@ -2478,7 +2478,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L34" s="5">
         <v>30</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
@@ -2504,13 +2504,13 @@
         <v>11</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L35" s="5">
         <v>30</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -2518,23 +2518,23 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F36" s="31"/>
       <c r="K36" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L36" s="5">
         <v>10</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2542,13 +2542,13 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>8</v>
@@ -2561,7 +2561,7 @@
         <v>60</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2569,13 +2569,13 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>26</v>
@@ -2588,7 +2588,7 @@
         <v>70</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>11</v>
@@ -2615,7 +2615,7 @@
         <v>80</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
@@ -2641,7 +2641,7 @@
         <v>-30</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -2649,28 +2649,28 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L41" s="5">
         <v>20</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
@@ -2687,10 +2687,10 @@
         <v>111</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="L42" s="29">
         <v>30</v>
@@ -2704,13 +2704,13 @@
     </row>
     <row r="43" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B43" s="29">
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>25</v>
@@ -2719,13 +2719,13 @@
         <v>7</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L43" s="29">
         <v>40</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
@@ -2742,10 +2742,10 @@
         <v>20</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M44" s="28" t="s">
         <v>106</v>
@@ -2761,13 +2761,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M45" t="s">
         <v>99</v>
@@ -2791,7 +2791,7 @@
         <v>98</v>
       </c>
       <c r="K46" t="s">
-        <v>185</v>
+        <v>270</v>
       </c>
       <c r="L46" s="5">
         <v>100</v>
@@ -2812,10 +2812,10 @@
         <v>103</v>
       </c>
       <c r="K47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M47" t="s">
         <v>37</v>
@@ -2833,10 +2833,10 @@
         <v>69</v>
       </c>
       <c r="K48" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M48" t="s">
         <v>38</v>
@@ -2854,10 +2854,10 @@
         <v>102</v>
       </c>
       <c r="K49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M49" t="s">
         <v>27</v>
@@ -2875,13 +2875,13 @@
         <v>29</v>
       </c>
       <c r="K50" t="s">
+        <v>227</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="M50" t="s">
         <v>228</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="M50" t="s">
-        <v>229</v>
       </c>
       <c r="N50"/>
     </row>
@@ -2896,13 +2896,13 @@
         <v>32</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K51" t="s">
         <v>181</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M51" t="s">
         <v>40</v>
@@ -2926,7 +2926,7 @@
         <v>180</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M52" t="s">
         <v>52</v>
@@ -2941,16 +2941,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K53" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N53"/>
     </row>
@@ -2962,22 +2962,22 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
+        <v>233</v>
+      </c>
+      <c r="K54" t="s">
         <v>234</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="M54" t="s">
         <v>235</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="M54" t="s">
-        <v>236</v>
       </c>
       <c r="N54"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
@@ -3008,7 +3008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,10 +3033,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3079,7 +3079,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3154,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>22</v>
@@ -3240,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3286,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4835,10 +4835,10 @@
         <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>172</v>
@@ -4856,7 +4856,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4881,7 +4881,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -4906,7 +4906,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -4931,7 +4931,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -4956,7 +4956,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
specials: reworked to go back to minimalist
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$15</definedName>
-    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$55</definedName>
+    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="281">
   <si>
     <t>Type</t>
   </si>
@@ -149,9 +149,6 @@
     <t>The Unexpected Payoff</t>
   </si>
   <si>
-    <t>Aggression does have its benefits.</t>
-  </si>
-  <si>
     <t>Sheep Breed!</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>I won't tell you how we got this cow to breed by itself.</t>
   </si>
   <si>
-    <t>Really, it's just a coincidence that we happen to also be housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
-  </si>
-  <si>
     <t>Does nothing now, but it will pay off later. The engine can wait.</t>
   </si>
   <si>
@@ -752,9 +746,6 @@
     <t>The Payoff Gambit</t>
   </si>
   <si>
-    <t>Payoff Spoiler</t>
-  </si>
-  <si>
     <t>Trash Me!</t>
   </si>
   <si>
@@ -843,6 +834,42 @@
   </si>
   <si>
     <t>At round start, player with most soldiers may trash any 1 available Special from purchase row. In a tie, nobody trashes.</t>
+  </si>
+  <si>
+    <t>Take That!</t>
+  </si>
+  <si>
+    <t>There's Always a Golem</t>
+  </si>
+  <si>
+    <t>The "Free" Soldier</t>
+  </si>
+  <si>
+    <t>What's the catch?</t>
+  </si>
+  <si>
+    <t>Military Ladder</t>
+  </si>
+  <si>
+    <t>Aggression does have benefits.</t>
+  </si>
+  <si>
+    <t>Tank and spank always works.</t>
+  </si>
+  <si>
+    <t>Trash an opponent's card with exactly one soldier.</t>
+  </si>
+  <si>
+    <t>Childish Aggression</t>
+  </si>
+  <si>
+    <t>It's a total coincidence that we are housed in a building. In fact, we built our own building. We did not need a building building building building building.</t>
+  </si>
+  <si>
+    <t>At round start, player with most soldiers may also trash any 1 available Resource from purchase row. In a tie, nobody trashes.</t>
+  </si>
+  <si>
+    <t>Resource Hog</t>
   </si>
 </sst>
 </file>
@@ -1460,11 +1487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1502,7 @@
     <col min="4" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -1502,10 +1529,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>18</v>
@@ -1514,7 +1541,7 @@
         <v>19</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1531,13 +1558,13 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="12"/>
@@ -1545,16 +1572,16 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1562,7 +1589,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1577,13 +1604,13 @@
         <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>278</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
@@ -1591,7 +1618,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1600,19 +1627,19 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>186</v>
+        <v>277</v>
       </c>
       <c r="K4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
@@ -1620,28 +1647,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
@@ -1649,28 +1676,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34"/>
@@ -1678,25 +1705,25 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1704,45 +1731,45 @@
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
@@ -1750,13 +1777,13 @@
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>22</v>
@@ -1768,13 +1795,13 @@
         <v>22</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L10" s="5">
         <v>20</v>
       </c>
       <c r="M10" s="54" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N10" s="24"/>
       <c r="O10" s="24"/>
@@ -1782,28 +1809,28 @@
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
@@ -1811,13 +1838,13 @@
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>12</v>
@@ -1832,7 +1859,7 @@
         <v>30</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
@@ -1840,25 +1867,25 @@
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1866,13 +1893,13 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>11</v>
@@ -1881,7 +1908,7 @@
         <v>31</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>33</v>
@@ -1890,7 +1917,7 @@
         <v>20</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
@@ -1898,13 +1925,13 @@
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
@@ -1913,7 +1940,7 @@
         <v>31</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>34</v>
@@ -1922,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
@@ -1930,13 +1957,13 @@
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>14</v>
@@ -1945,7 +1972,7 @@
         <v>31</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>35</v>
@@ -1954,128 +1981,126 @@
         <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
       <c r="P16" s="23"/>
     </row>
-    <row r="17" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="J17" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>109</v>
-      </c>
+      <c r="C17" s="54" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>277</v>
+      </c>
+      <c r="J17" s="54"/>
       <c r="L17" s="5">
-        <v>30</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="M17" s="54" t="s">
+        <v>272</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
       <c r="P17" s="23"/>
     </row>
-    <row r="18" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="54" t="s">
-        <v>186</v>
-      </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54" t="s">
-        <v>271</v>
+        <v>106</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="J18" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="L18" s="5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
       <c r="P18" s="23"/>
     </row>
-    <row r="19" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="29">
-        <v>1</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="K19" s="28" t="s">
-        <v>107</v>
+    <row r="19" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="23">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>277</v>
+      </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54" t="s">
+        <v>268</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
       </c>
-      <c r="M19" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
+      <c r="M19" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
       <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
-      <c r="C20" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>12</v>
+      <c r="C20" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="K20" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="L20" s="5">
-        <v>30</v>
-      </c>
-      <c r="M20" s="31" t="s">
-        <v>175</v>
+        <v>40</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
@@ -2083,60 +2108,60 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B21" s="29">
-        <v>2</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="31" t="s">
-        <v>199</v>
+        <v>1</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>12</v>
       </c>
       <c r="L21" s="5">
         <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
       <c r="P21" s="23"/>
     </row>
-    <row r="22" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="29">
+        <v>2</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="29">
-        <v>1</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>31</v>
-      </c>
       <c r="L22" s="5">
-        <v>60</v>
-      </c>
-      <c r="M22" s="28" t="s">
-        <v>68</v>
+        <v>30</v>
+      </c>
+      <c r="M22" s="31" t="s">
+        <v>219</v>
       </c>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
@@ -2144,16 +2169,16 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>8</v>
@@ -2162,7 +2187,7 @@
         <v>31</v>
       </c>
       <c r="L23" s="5">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="M23" s="28" t="s">
         <v>66</v>
@@ -2173,19 +2198,19 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>233</v>
+      <c r="C24" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>31</v>
@@ -2193,8 +2218,8 @@
       <c r="L24" s="5">
         <v>70</v>
       </c>
-      <c r="M24" s="31" t="s">
-        <v>257</v>
+      <c r="M24" s="28" t="s">
+        <v>64</v>
       </c>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
@@ -2202,28 +2227,28 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>8</v>
+        <v>231</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>31</v>
       </c>
       <c r="L25" s="5">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2231,16 +2256,16 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>11</v>
@@ -2249,10 +2274,10 @@
         <v>31</v>
       </c>
       <c r="L26" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -2260,16 +2285,16 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
       </c>
-      <c r="C27" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>11</v>
+      <c r="C27" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="G27" s="28" t="s">
         <v>11</v>
@@ -2278,39 +2303,39 @@
         <v>31</v>
       </c>
       <c r="L27" s="5">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
       <c r="P27" s="23"/>
     </row>
-    <row r="28" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="L28" s="5">
-        <v>40</v>
-      </c>
-      <c r="M28" s="28" t="s">
-        <v>60</v>
+        <v>100</v>
+      </c>
+      <c r="M28" s="31" t="s">
+        <v>159</v>
       </c>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
@@ -2318,95 +2343,87 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>24</v>
+        <v>41</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="L29" s="5">
-        <v>10</v>
-      </c>
-      <c r="M29" s="31" t="s">
-        <v>212</v>
+        <v>40</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
       <c r="P29" s="23"/>
     </row>
-    <row r="30" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B30" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>271</v>
+        <v>96</v>
       </c>
       <c r="L30" s="5">
-        <v>40</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>63</v>
+        <v>10</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>210</v>
       </c>
       <c r="N30" s="30"/>
       <c r="O30" s="30"/>
       <c r="P30" s="23"/>
     </row>
-    <row r="31" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B31" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="K31" s="31" t="s">
-        <v>271</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="K31" s="31"/>
       <c r="L31" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
@@ -2414,25 +2431,29 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="D32" s="31" t="s">
         <v>167</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="31" t="s">
-        <v>192</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="K32" s="31"/>
       <c r="L32" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2440,25 +2461,37 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B33" s="29">
-        <v>2</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>168</v>
+        <v>1</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>167</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>280</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>192</v>
+        <v>279</v>
       </c>
       <c r="L33" s="5">
-        <v>20</v>
-      </c>
-      <c r="M33" s="31" t="s">
-        <v>222</v>
+        <v>50</v>
+      </c>
+      <c r="M33" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
@@ -2466,25 +2499,25 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L34" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -2492,25 +2525,25 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B35" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L35" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -2518,23 +2551,25 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="K36" s="31" t="s">
-        <v>192</v>
-      </c>
       <c r="L36" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2542,26 +2577,25 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>250</v>
+        <v>174</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37" s="31"/>
+        <v>11</v>
+      </c>
+      <c r="K37" s="31" t="s">
+        <v>190</v>
+      </c>
       <c r="L37" s="5">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2569,26 +2603,23 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="31"/>
+        <v>188</v>
+      </c>
+      <c r="F38" s="31"/>
+      <c r="K38" s="31" t="s">
+        <v>190</v>
+      </c>
       <c r="L38" s="5">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2596,26 +2627,26 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>203</v>
+        <v>247</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="5">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2623,25 +2654,26 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
       </c>
-      <c r="C40" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>177</v>
-      </c>
+      <c r="C40" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="31"/>
       <c r="L40" s="5">
-        <v>-30</v>
+        <v>70</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -2649,157 +2681,163 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="H41" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>205</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="31"/>
       <c r="L41" s="5">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
       <c r="P41" s="23"/>
     </row>
-    <row r="42" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>197</v>
+    <row r="42" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>195</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>242</v>
+        <v>30</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>15</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="L42" s="29">
-        <v>30</v>
-      </c>
-      <c r="M42" s="28" t="s">
-        <v>110</v>
+        <v>175</v>
+      </c>
+      <c r="L42" s="5">
+        <v>-30</v>
+      </c>
+      <c r="M42" s="31" t="s">
+        <v>211</v>
       </c>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
-      <c r="P42" s="29"/>
-    </row>
-    <row r="43" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P42" s="23"/>
+    </row>
+    <row r="43" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B43" s="29">
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="F43" s="31" t="s">
-        <v>25</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="I43" s="31"/>
       <c r="J43" s="31" t="s">
-        <v>7</v>
+        <v>269</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="L43" s="29">
-        <v>40</v>
+        <v>203</v>
+      </c>
+      <c r="L43" s="5">
+        <v>20</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
-      <c r="P43" s="29"/>
+      <c r="P43" s="23"/>
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>20</v>
+        <v>109</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>239</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="L44" s="29" t="s">
-        <v>207</v>
+        <v>260</v>
+      </c>
+      <c r="L44" s="29">
+        <v>30</v>
       </c>
       <c r="M44" s="28" t="s">
-        <v>106</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="N44" s="30"/>
       <c r="O44" s="30"/>
       <c r="P44" s="29"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="29">
+        <v>1</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>252</v>
-      </c>
-      <c r="K45" t="s">
-        <v>259</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="M45" t="s">
-        <v>99</v>
-      </c>
-      <c r="N45"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K46" t="s">
-        <v>262</v>
-      </c>
-      <c r="L46" s="5">
-        <v>100</v>
-      </c>
-      <c r="M46" t="s">
-        <v>23</v>
-      </c>
-      <c r="N46"/>
+      <c r="K45" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="L45" s="29">
+        <v>40</v>
+      </c>
+      <c r="M45" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="29"/>
+    </row>
+    <row r="46" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" s="29">
+        <v>1</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="L46" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="M46" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="O46" s="30"/>
+      <c r="P46" s="29"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2809,16 +2847,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>103</v>
+        <v>249</v>
       </c>
       <c r="K47" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M47" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="N47"/>
     </row>
@@ -2830,16 +2868,22 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="K48" t="s">
-        <v>260</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>207</v>
+        <v>259</v>
+      </c>
+      <c r="L48" s="5">
+        <v>100</v>
       </c>
       <c r="M48" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="N48"/>
     </row>
@@ -2851,16 +2895,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M49" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="N49"/>
     </row>
@@ -2872,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="K50" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M50" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="N50"/>
     </row>
@@ -2893,19 +2937,16 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
       <c r="K51" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M51" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="N51"/>
     </row>
@@ -2917,19 +2958,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K52" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M52" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="N52"/>
     </row>
@@ -2941,16 +2979,19 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>204</v>
+        <v>32</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="K53" t="s">
-        <v>261</v>
+        <v>179</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M53" t="s">
-        <v>206</v>
+        <v>274</v>
       </c>
       <c r="N53"/>
     </row>
@@ -2962,39 +3003,84 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>231</v>
+        <v>42</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="K54" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M54" t="s">
-        <v>265</v>
+        <v>51</v>
       </c>
       <c r="N54"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>7</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="K55" t="s">
-        <v>178</v>
-      </c>
-      <c r="L55" s="5">
+        <v>258</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="M55" t="s">
+        <v>204</v>
+      </c>
+      <c r="N55"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>229</v>
+      </c>
+      <c r="K56" t="s">
+        <v>230</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="M56" t="s">
+        <v>262</v>
+      </c>
+      <c r="N56"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="K57" t="s">
+        <v>176</v>
+      </c>
+      <c r="L57" s="5">
         <v>0</v>
       </c>
-      <c r="M55" t="s">
-        <v>162</v>
-      </c>
-      <c r="N55"/>
+      <c r="M57" t="s">
+        <v>160</v>
+      </c>
+      <c r="N57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3033,10 +3119,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3056,7 +3142,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3068,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3079,7 +3165,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3091,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3102,7 +3188,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>11</v>
@@ -3111,7 +3197,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3122,7 +3208,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>14</v>
@@ -3134,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3145,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>25</v>
@@ -3154,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3165,7 +3251,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>12</v>
@@ -3174,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3185,7 +3271,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>13</v>
@@ -3194,7 +3280,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3205,7 +3291,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>26</v>
@@ -3214,13 +3300,13 @@
         <v>26</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3317,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>22</v>
@@ -3240,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3251,7 +3337,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
@@ -3263,7 +3349,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,19 +3360,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3297,7 +3383,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>15</v>
@@ -3306,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3317,19 +3403,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3340,7 +3426,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>24</v>
@@ -3349,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3363,7 +3449,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,25 +3468,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3545,15 +3631,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A6)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A6)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" si="3"/>
-        <v>0.7</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="E6" s="17">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="F6" s="17">
         <f t="shared" si="1"/>
@@ -3603,7 +3689,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -3837,75 +3923,75 @@
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>133</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>133</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I2" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>133</v>
-      </c>
       <c r="L2" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M2" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="N2" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>133</v>
-      </c>
       <c r="P2" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
@@ -3933,7 +4019,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -3959,10 +4045,10 @@
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
@@ -3973,7 +4059,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -3998,7 +4084,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
@@ -4009,7 +4095,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="17">
         <v>2</v>
@@ -4019,7 +4105,7 @@
         <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4043,7 +4129,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4053,10 +4139,10 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4066,7 +4152,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4091,7 +4177,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4101,10 +4187,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4114,7 +4200,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4138,7 +4224,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4148,10 +4234,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
@@ -4162,7 +4248,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4186,7 +4272,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
@@ -4196,10 +4282,10 @@
         <v>#N/A</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="17">
         <v>2</v>
@@ -4209,7 +4295,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4234,7 +4320,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4244,10 +4330,10 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="17">
         <v>1</v>
@@ -4257,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4282,7 +4368,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4292,10 +4378,10 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4305,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -4329,7 +4415,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
@@ -4338,7 +4424,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
@@ -4377,7 +4463,7 @@
         <v/>
       </c>
       <c r="E13" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
@@ -4388,7 +4474,7 @@
         <v/>
       </c>
       <c r="H13" s="50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="17">
@@ -4416,7 +4502,7 @@
         <v/>
       </c>
       <c r="E14" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,12,FALSE)),"",VLOOKUP(E14,Specials!C:P,12,FALSE))</f>
@@ -4456,7 +4542,7 @@
         <v/>
       </c>
       <c r="E15" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
@@ -4598,7 +4684,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -4608,7 +4694,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -4639,7 +4725,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -4648,7 +4734,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -4676,7 +4762,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -4686,7 +4772,7 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>32</v>
@@ -4712,7 +4798,7 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" s="49">
         <f>SUM(B3:B21)</f>
@@ -4724,7 +4810,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -4736,7 +4822,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -4750,21 +4836,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -4788,7 +4874,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Specials!$C$3:$C$55</xm:f>
+            <xm:f>Specials!$C$3:$C$57</xm:f>
           </x14:formula1>
           <xm:sqref>E14:E21</xm:sqref>
         </x14:dataValidation>
@@ -4800,10 +4886,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4814,37 +4900,47 @@
     <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4856,7 +4952,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4868,8 +4964,14 @@
         <f>SUM(F$3:F3) / A3</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4881,7 +4983,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -4893,8 +4995,14 @@
         <f>SUM(F$3:F4) / A4</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4906,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -4918,8 +5026,14 @@
         <f>SUM(F$3:F5) / A5</f>
         <v>18.333333333333332</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4931,7 +5045,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -4943,8 +5057,11 @@
         <f>SUM(F$3:F6) / A6</f>
         <v>21.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4956,7 +5073,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>
@@ -4968,6 +5085,9 @@
         <f>SUM(F$3:F7) / A7</f>
         <v>24</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
creating bundles and bw conversion
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -680,9 +680,6 @@
     <t>Grain Breed!</t>
   </si>
   <si>
-    <t>Setup</t>
-  </si>
-  <si>
     <t>The Red Material</t>
   </si>
   <si>
@@ -870,6 +867,9 @@
   </si>
   <si>
     <t>Resource Hog</t>
+  </si>
+  <si>
+    <t>Starting Player</t>
   </si>
 </sst>
 </file>
@@ -1490,13 +1490,13 @@
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.140625" bestFit="1" customWidth="1"/>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1575,7 +1575,7 @@
         <v>185</v>
       </c>
       <c r="K2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
@@ -1610,7 +1610,7 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
@@ -1630,10 +1630,10 @@
         <v>167</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
@@ -1659,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K5" t="s">
         <v>113</v>
@@ -1711,13 +1711,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="K7" t="s">
         <v>250</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="K7" t="s">
-        <v>251</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
@@ -1763,7 +1763,7 @@
         <v>48</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
@@ -1995,20 +1995,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D17" s="54" t="s">
         <v>167</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J17" s="54"/>
       <c r="L17" s="5">
         <v>10</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -2061,11 +2061,11 @@
         <v>31</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J19" s="54"/>
       <c r="K19" s="54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
@@ -2161,7 +2161,7 @@
         <v>30</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
@@ -2233,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F25" s="28" t="s">
         <v>14</v>
@@ -2248,7 +2248,7 @@
         <v>70</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>8</v>
@@ -2277,7 +2277,7 @@
         <v>80</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>14</v>
@@ -2306,7 +2306,7 @@
         <v>90</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
@@ -2416,7 +2416,7 @@
         <v>8</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="5">
@@ -2437,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D32" s="31" t="s">
         <v>167</v>
@@ -2446,14 +2446,14 @@
         <v>14</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="5">
         <v>50</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2479,13 +2479,13 @@
         <v>11</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L33" s="5">
         <v>50</v>
@@ -2517,7 +2517,7 @@
         <v>20</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -2543,7 +2543,7 @@
         <v>20</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>8</v>
@@ -2673,7 +2673,7 @@
         <v>70</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -2700,7 +2700,7 @@
         <v>80</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
@@ -2740,14 +2740,14 @@
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I43" s="31"/>
       <c r="J43" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K43" s="31" t="s">
         <v>203</v>
@@ -2756,7 +2756,7 @@
         <v>20</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -2773,10 +2773,10 @@
         <v>109</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L44" s="29">
         <v>30</v>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>25</v>
@@ -2805,13 +2805,13 @@
         <v>7</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L45" s="29">
         <v>40</v>
       </c>
       <c r="M45" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
@@ -2828,7 +2828,7 @@
         <v>20</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L46" s="29" t="s">
         <v>205</v>
@@ -2847,10 +2847,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>205</v>
@@ -2877,7 +2877,7 @@
         <v>96</v>
       </c>
       <c r="K48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L48" s="5">
         <v>100</v>
@@ -2898,7 +2898,7 @@
         <v>101</v>
       </c>
       <c r="K49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>205</v>
@@ -2919,7 +2919,7 @@
         <v>67</v>
       </c>
       <c r="K50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L50" s="5" t="s">
         <v>205</v>
@@ -2940,7 +2940,7 @@
         <v>100</v>
       </c>
       <c r="K51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L51" s="5" t="s">
         <v>205</v>
@@ -2961,13 +2961,13 @@
         <v>29</v>
       </c>
       <c r="K52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L52" s="5" t="s">
         <v>205</v>
       </c>
       <c r="M52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N52"/>
     </row>
@@ -2991,7 +2991,7 @@
         <v>205</v>
       </c>
       <c r="M53" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N53"/>
     </row>
@@ -3030,7 +3030,7 @@
         <v>202</v>
       </c>
       <c r="K55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>205</v>
@@ -3048,16 +3048,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
+        <v>228</v>
+      </c>
+      <c r="K56" t="s">
         <v>229</v>
-      </c>
-      <c r="K56" t="s">
-        <v>230</v>
       </c>
       <c r="L56" s="5" t="s">
         <v>205</v>
       </c>
       <c r="M56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N56"/>
     </row>
@@ -3165,7 +3165,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>14</v>
@@ -3240,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3317,7 +3317,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>22</v>
@@ -3326,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>164</v>
       </c>
       <c r="H1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -4928,10 +4928,10 @@
         <v>170</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>170</v>
@@ -4952,7 +4952,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4983,7 +4983,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -5014,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5027,7 +5027,7 @@
         <v>18.333333333333332</v>
       </c>
       <c r="H5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -5045,7 +5045,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5073,7 +5073,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
more bw conversion, more bundling
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -56,9 +56,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
     <t>Not to be confused with wood grain. Also, shouldn't wood be a plant? No. No it's not. Ever.</t>
   </si>
   <si>
-    <t>Cheap. Abundant. Necessary. Ubiquitous both in games and throughout games.</t>
-  </si>
-  <si>
     <t>Or is it brick? Pottery? Ok fine, let's just call it the red one.</t>
   </si>
   <si>
@@ -870,6 +864,12 @@
   </si>
   <si>
     <t>Starting Player</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>Cheap. Abundant. Literally the stuff games are made of.</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1491,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1529,19 +1529,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="H1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="J1" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1558,13 +1558,13 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="12"/>
@@ -1572,16 +1572,16 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1589,28 +1589,28 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
@@ -1618,28 +1618,28 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
@@ -1647,28 +1647,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
@@ -1676,28 +1676,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34"/>
@@ -1705,25 +1705,25 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
@@ -1731,45 +1731,45 @@
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
       </c>
       <c r="M8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
@@ -1777,31 +1777,31 @@
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L10" s="5">
         <v>20</v>
       </c>
       <c r="M10" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N10" s="24"/>
       <c r="O10" s="24"/>
@@ -1809,28 +1809,28 @@
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
@@ -1838,28 +1838,28 @@
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L12" s="5">
         <v>30</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
@@ -1867,25 +1867,25 @@
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1893,31 +1893,31 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L14" s="5">
         <v>20</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
@@ -1925,31 +1925,31 @@
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L15" s="5">
         <v>10</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
@@ -1957,31 +1957,31 @@
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L16" s="5">
         <v>10</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
@@ -1989,26 +1989,26 @@
     </row>
     <row r="17" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J17" s="54"/>
       <c r="L17" s="5">
         <v>10</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -2016,26 +2016,26 @@
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="25"/>
       <c r="J18" s="54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L18" s="5">
         <v>30</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
@@ -2043,35 +2043,35 @@
     </row>
     <row r="19" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="23">
         <v>1</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J19" s="54"/>
       <c r="K19" s="54" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
@@ -2079,28 +2079,28 @@
     </row>
     <row r="20" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B20" s="29">
         <v>1</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>8</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K20" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L20" s="5">
         <v>40</v>
       </c>
       <c r="M20" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
@@ -2108,28 +2108,28 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B21" s="29">
         <v>1</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L21" s="5">
         <v>30</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
@@ -2137,31 +2137,31 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B22" s="29">
         <v>2</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L22" s="5">
         <v>30</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
@@ -2169,13 +2169,13 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>8</v>
@@ -2184,13 +2184,13 @@
         <v>8</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L23" s="5">
         <v>60</v>
       </c>
       <c r="M23" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -2198,28 +2198,28 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B24" s="29">
         <v>1</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L24" s="5">
         <v>70</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
@@ -2227,28 +2227,28 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25" s="5">
         <v>70</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2256,28 +2256,28 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L26" s="5">
         <v>80</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -2285,28 +2285,28 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B27" s="29">
         <v>1</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L27" s="5">
         <v>90</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
@@ -2314,28 +2314,28 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L28" s="5">
         <v>100</v>
       </c>
       <c r="M28" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
@@ -2343,28 +2343,28 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L29" s="5">
         <v>40</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
@@ -2372,28 +2372,28 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B30" s="29">
         <v>1</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L30" s="5">
         <v>10</v>
       </c>
       <c r="M30" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N30" s="30"/>
       <c r="O30" s="30"/>
@@ -2401,29 +2401,29 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B31" s="29">
         <v>2</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="5">
         <v>40</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
@@ -2431,29 +2431,29 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="5">
         <v>50</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2461,37 +2461,37 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B33" s="29">
         <v>1</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="K33" s="31" t="s">
         <v>276</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="K33" s="31" t="s">
-        <v>278</v>
       </c>
       <c r="L33" s="5">
         <v>50</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
@@ -2499,25 +2499,25 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L34" s="5">
         <v>20</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -2525,25 +2525,25 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B35" s="29">
         <v>2</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L35" s="5">
         <v>20</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -2551,25 +2551,25 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K36" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L36" s="5">
         <v>30</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2577,25 +2577,25 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L37" s="5">
         <v>30</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2603,23 +2603,23 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F38" s="31"/>
       <c r="K38" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L38" s="5">
         <v>10</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2627,26 +2627,26 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>8</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="5">
         <v>60</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2654,26 +2654,26 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K40" s="31"/>
       <c r="L40" s="5">
         <v>70</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -2681,26 +2681,26 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F41" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K41" s="31"/>
       <c r="L41" s="5">
         <v>80</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
@@ -2708,25 +2708,25 @@
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L42" s="5">
         <v>-30</v>
       </c>
       <c r="M42" s="31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
@@ -2734,29 +2734,29 @@
     </row>
     <row r="43" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B43" s="29">
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I43" s="31"/>
       <c r="J43" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L43" s="5">
         <v>20</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -2764,25 +2764,25 @@
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L44" s="29">
         <v>30</v>
       </c>
       <c r="M44" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
@@ -2790,28 +2790,28 @@
     </row>
     <row r="45" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B45" s="29">
         <v>1</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F45" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J45" s="31" t="s">
         <v>7</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L45" s="29">
         <v>40</v>
       </c>
       <c r="M45" s="31" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
@@ -2819,22 +2819,22 @@
     </row>
     <row r="46" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B46" s="29">
         <v>1</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L46" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M46" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O46" s="30"/>
       <c r="P46" s="29"/>
@@ -2847,16 +2847,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N47"/>
     </row>
@@ -2868,22 +2868,22 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K48" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L48" s="5">
         <v>100</v>
       </c>
       <c r="M48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N48"/>
     </row>
@@ -2895,16 +2895,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N49"/>
     </row>
@@ -2916,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N50"/>
     </row>
@@ -2937,16 +2937,16 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K51" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N51"/>
     </row>
@@ -2958,16 +2958,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K52" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="N52"/>
     </row>
@@ -2979,19 +2979,19 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K53" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M53" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N53"/>
     </row>
@@ -3003,19 +3003,19 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K54" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N54"/>
     </row>
@@ -3027,16 +3027,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
+        <v>200</v>
+      </c>
+      <c r="K55" t="s">
+        <v>255</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="M55" t="s">
         <v>202</v>
-      </c>
-      <c r="K55" t="s">
-        <v>257</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="M55" t="s">
-        <v>204</v>
       </c>
       <c r="N55"/>
     </row>
@@ -3048,37 +3048,37 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K56" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M56" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N56"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K57" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L57" s="5">
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N57"/>
     </row>
@@ -3094,7 +3094,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,16 +3113,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3142,7 +3142,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3154,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>154</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3165,19 +3165,19 @@
         <v>4</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3188,16 +3188,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3208,10 +3208,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>8</v>
@@ -3220,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3231,16 +3231,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3251,16 +3251,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3271,16 +3271,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3291,22 +3291,22 @@
         <v>2</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3317,16 +3317,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3337,19 +3337,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3360,19 +3360,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3383,16 +3383,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3403,19 +3403,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" s="5">
         <v>20</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3426,16 +3426,16 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3468,25 +3468,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A3)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A3)</f>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A4)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A4)</f>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A5)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A5)</f>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A6)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A6)</f>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A7)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A7)</f>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A9)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A9)</f>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A10)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A10)</f>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A11)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A11)</f>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A12)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A12)</f>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A13)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A13)</f>
@@ -3923,75 +3923,75 @@
   <sheetData>
     <row r="1" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="60"/>
       <c r="E1" s="55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="47" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>131</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="38" t="s">
-        <v>131</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K2" s="38" t="s">
-        <v>131</v>
-      </c>
       <c r="L2" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="38" t="s">
-        <v>131</v>
-      </c>
       <c r="P2" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
@@ -4019,7 +4019,7 @@
         <v/>
       </c>
       <c r="L3" s="50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M3" s="37"/>
       <c r="N3" s="17" t="str">
@@ -4034,7 +4034,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="17">
         <f>IF(ISNA(VLOOKUP(A4,Specials!C:P,12,FALSE)),"",VLOOKUP(A4,Specials!C:P,12,FALSE))</f>
@@ -4045,10 +4045,10 @@
         <v>You may now build buildings.</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
@@ -4059,7 +4059,7 @@
         <v/>
       </c>
       <c r="H4" s="50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="17" t="str">
@@ -4084,7 +4084,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
@@ -4095,7 +4095,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="17">
         <v>2</v>
@@ -4105,7 +4105,7 @@
         <v/>
       </c>
       <c r="H5" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="17">
@@ -4129,7 +4129,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
@@ -4139,10 +4139,10 @@
         <v>You do not need to pay any required Stone for Buildings.</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -4152,7 +4152,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="17" t="str">
@@ -4177,7 +4177,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
@@ -4187,10 +4187,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -4200,7 +4200,7 @@
         <v>You may trash this card for 1 Food</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="17">
@@ -4224,7 +4224,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -4234,10 +4234,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
@@ -4248,7 +4248,7 @@
         <v/>
       </c>
       <c r="H8" s="50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I8" s="37"/>
       <c r="J8" s="17">
@@ -4272,7 +4272,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
@@ -4282,10 +4282,10 @@
         <v>#N/A</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="17">
         <v>2</v>
@@ -4295,7 +4295,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I9" s="37"/>
       <c r="J9" s="17" t="str">
@@ -4320,7 +4320,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -4330,10 +4330,10 @@
         <v>#N/A</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="17">
         <v>1</v>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="17" t="str">
@@ -4368,7 +4368,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
@@ -4378,10 +4378,10 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -4391,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="17">
@@ -4415,7 +4415,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
@@ -4424,7 +4424,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
@@ -4435,7 +4435,7 @@
         <v/>
       </c>
       <c r="H12" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="37"/>
       <c r="J12" s="17">
@@ -4463,7 +4463,7 @@
         <v/>
       </c>
       <c r="E13" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
@@ -4474,7 +4474,7 @@
         <v/>
       </c>
       <c r="H13" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="17">
@@ -4502,7 +4502,7 @@
         <v/>
       </c>
       <c r="E14" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,12,FALSE)),"",VLOOKUP(E14,Specials!C:P,12,FALSE))</f>
@@ -4513,7 +4513,7 @@
         <v/>
       </c>
       <c r="H14" s="50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="17" t="str">
@@ -4542,7 +4542,7 @@
         <v/>
       </c>
       <c r="E15" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="17" t="str">
         <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
@@ -4553,7 +4553,7 @@
         <v/>
       </c>
       <c r="H15" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="37"/>
       <c r="J15" s="17" t="str">
@@ -4684,7 +4684,7 @@
         <v/>
       </c>
       <c r="E19" s="37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F19" s="17">
         <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
@@ -4694,7 +4694,7 @@
         <v>90</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I19" s="37"/>
       <c r="J19" s="17" t="str">
@@ -4725,7 +4725,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
@@ -4734,7 +4734,7 @@
         <v>250</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I20" s="37"/>
       <c r="J20" s="17" t="str">
@@ -4762,7 +4762,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="17">
         <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
@@ -4772,10 +4772,10 @@
         <v>240</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J21" s="17">
         <f>IF(ISNA(VLOOKUP(I21,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I21,Specials!$C:$P,12,FALSE))</f>
@@ -4798,7 +4798,7 @@
     </row>
     <row r="22" spans="1:16" s="42" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="49">
         <f>SUM(B3:B21)</f>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" s="45">
         <f>SUM(F3:F21)</f>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J22" s="45">
         <f>SUM(J3:J21)</f>
@@ -4836,21 +4836,21 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" s="17" t="e">
         <f>C22/B22</f>
         <v>#N/A</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F23" s="46">
         <f>G22/F22</f>
         <v>58</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J23" s="46">
         <f>K22/J22</f>
@@ -4905,13 +4905,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -4919,22 +4919,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4952,7 +4952,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4965,7 +4965,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -4983,7 +4983,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -4996,7 +4996,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -5014,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5027,7 +5027,7 @@
         <v>18.333333333333332</v>
       </c>
       <c r="H5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -5045,7 +5045,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5073,7 +5073,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
printed out this version
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="4755" windowHeight="1875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Specials" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Ladders" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$15</definedName>
+    <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$16</definedName>
     <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="283">
   <si>
     <t>Type</t>
   </si>
@@ -779,9 +779,6 @@
     <t>Or is it wheat? Reeds? Seeds? Corn? Did you know that corn is a type of grain? Be sure to bring up this fact in your next Euro game. Everyone will appreciate the rules ambiguity it creates.</t>
   </si>
   <si>
-    <t>Cue the sexual innuendo jokes.</t>
-  </si>
-  <si>
     <t>Good move. Not Great. What else are you going to do to get points? No pressure. But you should think of something. Now.</t>
   </si>
   <si>
@@ -870,6 +867,15 @@
   </si>
   <si>
     <t>Cheap. Abundant. Literally the stuff games are made of.</t>
+  </si>
+  <si>
+    <t>What, exactly, are we making out of these?</t>
+  </si>
+  <si>
+    <t>The Expensive Materials</t>
+  </si>
+  <si>
+    <t>There's only one card like this. See? You don't need to memorize deck distributions to be good at this.</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
@@ -1517,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -1558,7 +1564,7 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1610,7 +1616,7 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
@@ -1630,10 +1636,10 @@
         <v>165</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
@@ -1995,20 +2001,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D17" s="54" t="s">
         <v>165</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J17" s="54"/>
       <c r="L17" s="5">
         <v>10</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -2061,11 +2067,11 @@
         <v>30</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J19" s="54"/>
       <c r="K19" s="54" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L19" s="5">
         <v>40</v>
@@ -2248,7 +2254,7 @@
         <v>70</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2416,7 +2422,7 @@
         <v>8</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="5">
@@ -2437,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D32" s="31" t="s">
         <v>165</v>
@@ -2446,14 +2452,14 @@
         <v>13</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="5">
         <v>50</v>
       </c>
       <c r="M32" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2479,13 +2485,13 @@
         <v>10</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L33" s="5">
         <v>50</v>
@@ -2517,7 +2523,7 @@
         <v>20</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -2740,14 +2746,14 @@
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I43" s="31"/>
       <c r="J43" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K43" s="31" t="s">
         <v>201</v>
@@ -2776,7 +2782,7 @@
         <v>236</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L44" s="29">
         <v>30</v>
@@ -2850,7 +2856,7 @@
         <v>246</v>
       </c>
       <c r="K47" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>203</v>
@@ -2877,7 +2883,7 @@
         <v>95</v>
       </c>
       <c r="K48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L48" s="5">
         <v>100</v>
@@ -2919,7 +2925,7 @@
         <v>66</v>
       </c>
       <c r="K50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L50" s="5" t="s">
         <v>203</v>
@@ -2991,7 +2997,7 @@
         <v>203</v>
       </c>
       <c r="M53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N53"/>
     </row>
@@ -3030,7 +3036,7 @@
         <v>200</v>
       </c>
       <c r="K55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>203</v>
@@ -3057,7 +3063,7 @@
         <v>203</v>
       </c>
       <c r="M56" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N56"/>
     </row>
@@ -3090,11 +3096,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -3154,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3201,26 +3207,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="27">
-        <v>4</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>155</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3228,19 +3234,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="27">
-        <v>3</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>51</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3251,16 +3260,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="26" t="s">
-        <v>48</v>
+      <c r="H7" s="53" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3271,16 +3280,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="53" t="s">
-        <v>45</v>
+      <c r="H8" s="26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3288,25 +3297,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
-      <c r="H9" s="26" t="s">
-        <v>52</v>
+      <c r="H9" s="53" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3314,65 +3317,68 @@
         <v>6</v>
       </c>
       <c r="B10" s="27">
+        <v>2</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C11" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="53" t="s">
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="53" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+    <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="27">
-        <v>1</v>
-      </c>
-      <c r="C11" s="53" t="s">
+      <c r="B12" s="27">
+        <v>1</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D12" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E12" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="53" t="s">
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="53" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="27">
-        <v>2</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3380,19 +3386,22 @@
         <v>6</v>
       </c>
       <c r="B13" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>14</v>
+        <v>95</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>84</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
       </c>
-      <c r="H13" s="26" t="s">
-        <v>61</v>
+      <c r="H13" s="53" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3403,22 +3412,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>6</v>
       </c>
@@ -3426,15 +3432,38 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="5">
+        <v>20</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="27">
+        <v>3</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="H15" s="53" t="s">
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="53" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3511,15 +3540,15 @@
       </c>
       <c r="F2" s="16">
         <f t="shared" ref="F2:F13" si="1">SUM(B:B)/B2</f>
-        <v>3.7647058823529411</v>
+        <v>3.8823529411764706</v>
       </c>
       <c r="G2" s="16">
         <f t="shared" ref="G2:G13" si="2">1-POWER(B2/SUM(B:B),0.5)</f>
-        <v>0.48461179679779243</v>
+        <v>0.49248078107744775</v>
       </c>
       <c r="H2" s="16">
         <f>1+G2</f>
-        <v>1.4846117967977923</v>
+        <v>1.4924807810774476</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3528,7 +3557,7 @@
       </c>
       <c r="B3" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A3)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A3)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A3)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A3)</f>
@@ -3536,23 +3565,23 @@
       </c>
       <c r="D3" s="17">
         <f t="shared" ref="D3:D13" si="3">IF(ISNUMBER(B3/C3),B3/C3,"")</f>
-        <v>1.3333333333333333</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="E3" s="17">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.69230769230769229</v>
       </c>
       <c r="F3" s="17">
         <f t="shared" si="1"/>
-        <v>5.333333333333333</v>
+        <v>5.0769230769230766</v>
       </c>
       <c r="G3" s="21">
         <f t="shared" si="2"/>
-        <v>0.5669872981077807</v>
+        <v>0.55618731770070273</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H13" si="4">1+G3</f>
-        <v>1.5669872981077808</v>
+        <v>1.5561873177007026</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3577,15 +3606,15 @@
       </c>
       <c r="F4" s="17">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="G4" s="21">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0.7538170180413345</v>
       </c>
       <c r="H4" s="17">
         <f t="shared" si="4"/>
-        <v>1.75</v>
+        <v>1.7538170180413344</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3610,15 +3639,15 @@
       </c>
       <c r="F5" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3627,7 +3656,7 @@
       </c>
       <c r="B6" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A6)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A6)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <f>SUMIFS(Specials!B:B,Specials!F:F,Economy!A6)+SUMIFS(Specials!B:B,Specials!G:G,Economy!A6)</f>
@@ -3635,23 +3664,23 @@
       </c>
       <c r="D6" s="17">
         <f t="shared" si="3"/>
-        <v>0.63636363636363635</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="E6" s="17">
         <f t="shared" si="0"/>
-        <v>1.5714285714285714</v>
+        <v>1.375</v>
       </c>
       <c r="F6" s="17">
         <f t="shared" si="1"/>
-        <v>9.1428571428571423</v>
+        <v>8.25</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="2"/>
-        <v>0.66928108611692616</v>
+        <v>0.6518446880886043</v>
       </c>
       <c r="H6" s="17">
         <f t="shared" si="4"/>
-        <v>1.6692810861169263</v>
+        <v>1.6518446880886044</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3676,15 +3705,15 @@
       </c>
       <c r="F7" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H7" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3709,15 +3738,15 @@
       </c>
       <c r="F8" s="17">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="21">
         <f t="shared" si="2"/>
-        <v>0.82322330470336313</v>
+        <v>0.8259223440443022</v>
       </c>
       <c r="H8" s="17">
         <f t="shared" si="4"/>
-        <v>1.823223304703363</v>
+        <v>1.8259223440443022</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,15 +3771,15 @@
       </c>
       <c r="F9" s="17">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="G9" s="21">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0.7538170180413345</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="4"/>
-        <v>1.75</v>
+        <v>1.7538170180413344</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3775,15 +3804,15 @@
       </c>
       <c r="F10" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G10" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H10" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3808,15 +3837,15 @@
       </c>
       <c r="F11" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G11" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H11" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3841,15 +3870,15 @@
       </c>
       <c r="F12" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G12" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H12" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3874,15 +3903,15 @@
       </c>
       <c r="F13" s="17">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="G13" s="21">
         <f t="shared" si="2"/>
-        <v>0.78349364905389041</v>
+        <v>0.78679928364438956</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" si="4"/>
-        <v>1.7834936490538904</v>
+        <v>1.7867992836443896</v>
       </c>
     </row>
   </sheetData>
@@ -4911,7 +4940,7 @@
         <v>162</v>
       </c>
       <c r="H1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -4952,7 +4981,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4983,7 +5012,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -5014,7 +5043,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5027,7 +5056,7 @@
         <v>18.333333333333332</v>
       </c>
       <c r="H5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -5045,7 +5074,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5073,7 +5102,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
ladder engine: make it cheaper
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -16,8 +16,7 @@
     <sheet name="Resources" sheetId="6" r:id="rId2"/>
     <sheet name="Economy" sheetId="2" r:id="rId3"/>
     <sheet name="Actions per Game" sheetId="7" r:id="rId4"/>
-    <sheet name="Scenarios" sheetId="3" r:id="rId5"/>
-    <sheet name="Ladders" sheetId="4" r:id="rId6"/>
+    <sheet name="Ladders" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$16</definedName>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="282">
   <si>
     <t>Type</t>
   </si>
@@ -195,9 +194,6 @@
     <t>Free Food!</t>
   </si>
   <si>
-    <t>More Grain!</t>
-  </si>
-  <si>
     <t>Moo.</t>
   </si>
   <si>
@@ -324,36 +320,18 @@
     <t>The Expensive Animal</t>
   </si>
   <si>
-    <t>The Multiplying Plant</t>
-  </si>
-  <si>
     <t>The Expensive Plant</t>
   </si>
   <si>
     <t>The Rare Resource</t>
   </si>
   <si>
-    <t>The Good Material</t>
-  </si>
-  <si>
-    <t>The Good Building</t>
-  </si>
-  <si>
     <t>Carrot</t>
   </si>
   <si>
     <t>Trash</t>
   </si>
   <si>
-    <t>The Amazing Building</t>
-  </si>
-  <si>
-    <t>The Unused Resources Payoff</t>
-  </si>
-  <si>
-    <t>The Diversified Strategy Payoff</t>
-  </si>
-  <si>
     <t>The Military Commitment</t>
   </si>
   <si>
@@ -429,75 +407,12 @@
     <t>The Combo Materials</t>
   </si>
   <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Action Cost</t>
-  </si>
-  <si>
     <t>VPs</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>VPs/Action Overall</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>No cost with the chain run</t>
-  </si>
-  <si>
-    <t>Take it and play it.</t>
-  </si>
-  <si>
-    <t>Take the resource</t>
-  </si>
-  <si>
-    <t>Also no play cost. Have four grain at this point.</t>
-  </si>
-  <si>
-    <t>No cost play on the chain run</t>
-  </si>
-  <si>
-    <t>4xGrain, 4xSheep</t>
-  </si>
-  <si>
-    <t>Pay the stone</t>
-  </si>
-  <si>
-    <t>Military Strategy</t>
-  </si>
-  <si>
-    <t>Resource Collection Strategy, Lots of Chaining</t>
-  </si>
-  <si>
-    <t>No need to pay</t>
-  </si>
-  <si>
-    <t>Building Strategy, Not much chaining</t>
-  </si>
-  <si>
-    <t>The Payoff with Math</t>
-  </si>
-  <si>
-    <t>Grain, Sheep,Glass, Carrot,Silk</t>
-  </si>
-  <si>
-    <t>(2xGlass + 1xSilk)^2</t>
-  </si>
-  <si>
-    <t>Get 2xClay</t>
-  </si>
-  <si>
-    <t>Pay 2xClay</t>
-  </si>
-  <si>
-    <t>Pay 1xClay, no stone</t>
-  </si>
-  <si>
     <t>The Strange Combo</t>
   </si>
   <si>
@@ -579,12 +494,6 @@
     <t>30 VP for each Soldier, +30 additional VP if you end the game with the most soldiers.</t>
   </si>
   <si>
-    <t>Ladder Strategy</t>
-  </si>
-  <si>
-    <t>Figure this out with the new rule</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -771,9 +680,6 @@
     <t>The Ladder Engine</t>
   </si>
   <si>
-    <t>As an action, once per turn, you may trash 1 Special in your hand or 1 Resource card on your tableau to Climb a Ladder 1 space.</t>
-  </si>
-  <si>
     <t>Or is it wheat? Reeds? Seeds? Corn? Did you know that corn is a type of grain? Be sure to bring up this fact in your next Euro game. Everyone will appreciate the rules ambiguity it creates.</t>
   </si>
   <si>
@@ -1000,6 +906,9 @@
   </si>
   <si>
     <t>Est. Take Actions/Player Max</t>
+  </si>
+  <si>
+    <t>Once per turn, you may trash 1 Special in your hand or 1 Resource card on your tableau to Climb a Ladder 1 space.</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +993,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1130,79 +1039,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1211,7 +1047,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1282,29 +1118,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1333,24 +1146,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1665,7 +1460,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -1703,10 +1498,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>17</v>
@@ -1715,7 +1510,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1732,13 +1527,13 @@
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="12"/>
@@ -1746,16 +1541,16 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="K2" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
       <c r="L2" s="5">
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="32"/>
@@ -1763,7 +1558,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1778,23 +1573,23 @@
         <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="L3" s="5">
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>257</v>
-      </c>
-      <c r="N3" s="55" t="s">
-        <v>305</v>
-      </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="56"/>
+        <v>226</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="O3" s="38"/>
+      <c r="P3" s="39"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1803,27 +1598,27 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="K4" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="L4" s="5">
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="56"/>
+        <v>62</v>
+      </c>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1835,117 +1630,117 @@
         <v>8</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="56"/>
+        <v>75</v>
+      </c>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="39"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="L6" s="5">
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="56"/>
+        <v>74</v>
+      </c>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="39"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="K7" t="s">
-        <v>235</v>
+        <v>281</v>
       </c>
       <c r="L7" s="5">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>168</v>
-      </c>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="56"/>
+        <v>140</v>
+      </c>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="39"/>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="L8" s="5">
         <v>-100</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="52" t="s">
-        <v>227</v>
+        <v>70</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="L9" s="5">
         <v>30</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
@@ -1953,13 +1748,13 @@
     </row>
     <row r="10" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="23">
         <v>2</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>205</v>
+      <c r="C10" s="35" t="s">
+        <v>175</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>21</v>
@@ -1971,13 +1766,13 @@
         <v>21</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L10" s="5">
         <v>20</v>
       </c>
-      <c r="M10" s="52" t="s">
-        <v>163</v>
+      <c r="M10" s="35" t="s">
+        <v>135</v>
       </c>
       <c r="N10" s="24"/>
       <c r="O10" s="24"/>
@@ -1985,28 +1780,28 @@
     </row>
     <row r="11" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="52" t="s">
-        <v>203</v>
+      <c r="J11" s="35" t="s">
+        <v>173</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L11" s="5">
         <v>50</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
@@ -2014,7 +1809,7 @@
     </row>
     <row r="12" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
@@ -2035,33 +1830,33 @@
         <v>30</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
-        <v>72</v>
+      <c r="A13" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
-      <c r="C13" s="52" t="s">
-        <v>177</v>
+      <c r="C13" s="35" t="s">
+        <v>147</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L13" s="5">
         <v>10</v>
       </c>
-      <c r="M13" s="52" t="s">
-        <v>178</v>
+      <c r="M13" s="35" t="s">
+        <v>148</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -2069,13 +1864,13 @@
     </row>
     <row r="14" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>10</v>
@@ -2083,8 +1878,8 @@
       <c r="H14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="52" t="s">
-        <v>198</v>
+      <c r="J14" s="35" t="s">
+        <v>168</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>32</v>
@@ -2092,8 +1887,8 @@
       <c r="L14" s="5">
         <v>20</v>
       </c>
-      <c r="M14" s="52" t="s">
-        <v>153</v>
+      <c r="M14" s="35" t="s">
+        <v>125</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
@@ -2101,13 +1896,13 @@
     </row>
     <row r="15" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>8</v>
@@ -2115,8 +1910,8 @@
       <c r="H15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="52" t="s">
-        <v>199</v>
+      <c r="J15" s="35" t="s">
+        <v>169</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>33</v>
@@ -2124,8 +1919,8 @@
       <c r="L15" s="5">
         <v>10</v>
       </c>
-      <c r="M15" s="52" t="s">
-        <v>152</v>
+      <c r="M15" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
@@ -2133,13 +1928,13 @@
     </row>
     <row r="16" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>13</v>
@@ -2147,8 +1942,8 @@
       <c r="H16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="52" t="s">
-        <v>197</v>
+      <c r="J16" s="35" t="s">
+        <v>167</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>34</v>
@@ -2156,8 +1951,8 @@
       <c r="L16" s="5">
         <v>10</v>
       </c>
-      <c r="M16" s="52" t="s">
-        <v>200</v>
+      <c r="M16" s="35" t="s">
+        <v>170</v>
       </c>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
@@ -2165,26 +1960,26 @@
     </row>
     <row r="17" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
       </c>
-      <c r="C17" s="52" t="s">
-        <v>251</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="H17" s="52" t="s">
-        <v>264</v>
-      </c>
-      <c r="J17" s="52"/>
+      <c r="C17" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="J17" s="35"/>
       <c r="L17" s="5">
         <v>10</v>
       </c>
-      <c r="M17" s="52" t="s">
-        <v>252</v>
+      <c r="M17" s="35" t="s">
+        <v>221</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -2192,20 +1987,20 @@
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D18" s="25"/>
-      <c r="J18" s="52" t="s">
-        <v>204</v>
+      <c r="J18" s="35" t="s">
+        <v>174</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="L18" s="5">
         <v>30</v>
@@ -2218,33 +2013,33 @@
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
-        <v>72</v>
+      <c r="A19" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="B19" s="23">
         <v>2</v>
       </c>
-      <c r="C19" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="D19" s="53" t="s">
+      <c r="C19" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="52"/>
+      <c r="J19" s="35"/>
       <c r="L19" s="5">
         <v>20</v>
       </c>
-      <c r="M19" s="52" t="s">
-        <v>278</v>
+      <c r="M19" s="35" t="s">
+        <v>247</v>
       </c>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
@@ -2252,7 +2047,7 @@
     </row>
     <row r="20" spans="1:16" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="23">
         <v>1</v>
@@ -2260,25 +2055,25 @@
       <c r="C20" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="E20" s="52" t="s">
-        <v>158</v>
+      <c r="D20" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>130</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="52" t="s">
-        <v>264</v>
-      </c>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
+      <c r="I20" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="5">
         <v>40</v>
       </c>
-      <c r="M20" s="52" t="s">
-        <v>265</v>
+      <c r="M20" s="35" t="s">
+        <v>234</v>
       </c>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
@@ -2286,28 +2081,28 @@
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B21" s="29">
         <v>1</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>21</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="L21" s="5">
         <v>40</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
@@ -2315,13 +2110,13 @@
     </row>
     <row r="22" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B22" s="29">
         <v>1</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>11</v>
@@ -2340,7 +2135,7 @@
         <v>30</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
@@ -2348,13 +2143,13 @@
     </row>
     <row r="23" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B23" s="29">
         <v>1</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>11</v>
@@ -2369,7 +2164,7 @@
         <v>30</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -2377,13 +2172,13 @@
     </row>
     <row r="24" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B24" s="29">
         <v>2</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>21</v>
@@ -2395,13 +2190,13 @@
         <v>21</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="L24" s="5">
         <v>30</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
@@ -2409,13 +2204,13 @@
     </row>
     <row r="25" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" s="28" t="s">
         <v>8</v>
@@ -2430,7 +2225,7 @@
         <v>60</v>
       </c>
       <c r="M25" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -2438,13 +2233,13 @@
     </row>
     <row r="26" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B26" s="29">
         <v>1</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F26" s="28" t="s">
         <v>13</v>
@@ -2459,7 +2254,7 @@
         <v>70</v>
       </c>
       <c r="M26" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
@@ -2467,13 +2262,13 @@
     </row>
     <row r="27" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>186</v>
-      </c>
-      <c r="B27" s="29">
-        <v>1</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>216</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>13</v>
@@ -2488,7 +2283,7 @@
         <v>70</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
@@ -2496,13 +2291,13 @@
     </row>
     <row r="28" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B28" s="29">
         <v>1</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>8</v>
@@ -2517,7 +2312,7 @@
         <v>80</v>
       </c>
       <c r="M28" s="31" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
@@ -2525,13 +2320,13 @@
     </row>
     <row r="29" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B29" s="29">
         <v>1</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>13</v>
@@ -2546,7 +2341,7 @@
         <v>90</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
@@ -2554,13 +2349,13 @@
     </row>
     <row r="30" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B30" s="29">
         <v>1</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>10</v>
@@ -2575,7 +2370,7 @@
         <v>100</v>
       </c>
       <c r="M30" s="31" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="N30" s="30"/>
       <c r="O30" s="30"/>
@@ -2583,13 +2378,13 @@
     </row>
     <row r="31" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B31" s="29">
         <v>1</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>10</v>
@@ -2601,13 +2396,13 @@
         <v>30</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="L31" s="5">
         <v>110</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
@@ -2615,7 +2410,7 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B32" s="29">
         <v>1</v>
@@ -2636,7 +2431,7 @@
         <v>40</v>
       </c>
       <c r="M32" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
@@ -2644,13 +2439,13 @@
     </row>
     <row r="33" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B33" s="29">
         <v>1</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>23</v>
@@ -2659,13 +2454,13 @@
         <v>23</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L33" s="5">
         <v>10</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
@@ -2673,29 +2468,29 @@
     </row>
     <row r="34" spans="1:16" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B34" s="29">
         <v>1</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="F34" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H34" s="31" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="K34" s="31"/>
       <c r="L34" s="5">
         <v>40</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -2703,29 +2498,29 @@
     </row>
     <row r="35" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B35" s="29">
         <v>1</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="K35" s="31"/>
       <c r="L35" s="5">
         <v>50</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -2733,25 +2528,25 @@
     </row>
     <row r="36" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="F36" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H36" s="31" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="J36" s="31"/>
       <c r="K36" s="31"/>
@@ -2759,7 +2554,7 @@
         <v>50</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -2767,13 +2562,13 @@
     </row>
     <row r="37" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
@@ -2790,7 +2585,7 @@
         <v>80</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -2798,25 +2593,25 @@
     </row>
     <row r="38" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K38" s="31" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L38" s="5">
         <v>20</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -2824,25 +2619,25 @@
     </row>
     <row r="39" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B39" s="29">
         <v>2</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>21</v>
       </c>
       <c r="K39" s="31" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L39" s="5">
         <v>20</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -2850,25 +2645,25 @@
     </row>
     <row r="40" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="F40" s="31" t="s">
         <v>13</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L40" s="5">
         <v>30</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -2876,25 +2671,25 @@
     </row>
     <row r="41" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L41" s="5">
         <v>30</v>
       </c>
       <c r="M41" s="31" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
@@ -2902,23 +2697,23 @@
     </row>
     <row r="42" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B42" s="29">
         <v>1</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="F42" s="31"/>
       <c r="K42" s="31" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="L42" s="5">
         <v>10</v>
       </c>
       <c r="M42" s="31" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
@@ -2926,26 +2721,26 @@
     </row>
     <row r="43" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B43" s="29">
         <v>1</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="F43" s="31"/>
       <c r="J43" s="31" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="L43" s="5">
         <v>10</v>
       </c>
       <c r="M43" s="31" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
@@ -2953,26 +2748,26 @@
     </row>
     <row r="44" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B44" s="29">
         <v>1</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="F44" s="31"/>
       <c r="J44" s="31" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="L44" s="5">
         <v>10</v>
       </c>
       <c r="M44" s="31" t="s">
-        <v>269</v>
+        <v>238</v>
       </c>
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
@@ -2980,13 +2775,13 @@
     </row>
     <row r="45" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B45" s="29">
         <v>1</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>8</v>
@@ -2999,7 +2794,7 @@
         <v>60</v>
       </c>
       <c r="M45" s="31" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
@@ -3007,13 +2802,13 @@
     </row>
     <row r="46" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B46" s="29">
         <v>1</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>25</v>
@@ -3026,7 +2821,7 @@
         <v>70</v>
       </c>
       <c r="M46" s="31" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="N46" s="30"/>
       <c r="O46" s="30"/>
@@ -3034,13 +2829,13 @@
     </row>
     <row r="47" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B47" s="29">
         <v>1</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>10</v>
@@ -3053,7 +2848,7 @@
         <v>80</v>
       </c>
       <c r="M47" s="31" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="N47" s="30"/>
       <c r="O47" s="30"/>
@@ -3061,7 +2856,7 @@
     </row>
     <row r="48" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B48" s="29">
         <v>1</v>
@@ -3073,13 +2868,13 @@
         <v>14</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="L48" s="5">
         <v>-30</v>
       </c>
       <c r="M48" s="31" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="N48" s="30"/>
       <c r="O48" s="30"/>
@@ -3087,25 +2882,25 @@
     </row>
     <row r="49" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B49" s="29">
         <v>1</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="F49" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5">
         <v>50</v>
       </c>
       <c r="M49" s="31" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="N49" s="30"/>
       <c r="O49" s="30"/>
@@ -3113,29 +2908,29 @@
     </row>
     <row r="50" spans="1:16" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B50" s="29">
         <v>1</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="I50" s="31"/>
       <c r="J50" s="31" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="L50" s="5">
         <v>20</v>
       </c>
       <c r="M50" s="31" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="N50" s="30"/>
       <c r="O50" s="30"/>
@@ -3143,25 +2938,25 @@
     </row>
     <row r="51" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B51" s="29">
         <v>1</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J51" s="31" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="L51" s="29">
         <v>30</v>
       </c>
       <c r="M51" s="28" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="N51" s="30"/>
       <c r="O51" s="30"/>
@@ -3169,13 +2964,13 @@
     </row>
     <row r="52" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B52" s="29">
         <v>1</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>24</v>
@@ -3184,13 +2979,13 @@
         <v>7</v>
       </c>
       <c r="K52" s="31" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="L52" s="29">
         <v>40</v>
       </c>
       <c r="M52" s="31" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="N52" s="30"/>
       <c r="O52" s="30"/>
@@ -3198,7 +2993,7 @@
     </row>
     <row r="53" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B53" s="29">
         <v>1</v>
@@ -3207,13 +3002,13 @@
         <v>19</v>
       </c>
       <c r="K53" s="31" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="L53" s="29" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M53" s="28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="O53" s="30"/>
       <c r="P53" s="29"/>
@@ -3232,10 +3027,10 @@
         <v>14</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K54" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="L54" s="5">
         <v>100</v>
@@ -3253,13 +3048,13 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K55" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M55" t="s">
         <v>36</v>
@@ -3274,13 +3069,13 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="K56" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M56" t="s">
         <v>26</v>
@@ -3298,13 +3093,13 @@
         <v>28</v>
       </c>
       <c r="K57" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M57" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="N57"/>
     </row>
@@ -3319,16 +3114,16 @@
         <v>31</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="K58" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M58" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="N58"/>
     </row>
@@ -3346,13 +3141,13 @@
         <v>30</v>
       </c>
       <c r="K59" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N59"/>
     </row>
@@ -3364,16 +3159,16 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="K60" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M60" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="N60"/>
     </row>
@@ -3385,16 +3180,16 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="K61" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M61" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="N61"/>
     </row>
@@ -3406,37 +3201,37 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="K62" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="M62" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="N62"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="B63" s="3">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K63" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="L63" s="5">
         <v>0</v>
       </c>
       <c r="M63" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="N63"/>
     </row>
@@ -3471,16 +3266,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3500,7 +3295,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>8</v>
@@ -3511,8 +3306,8 @@
       <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="51" t="s">
-        <v>260</v>
+      <c r="H2" s="34" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3522,8 +3317,8 @@
       <c r="B3" s="27">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
-        <v>206</v>
+      <c r="C3" s="34" t="s">
+        <v>176</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>13</v>
@@ -3534,8 +3329,8 @@
       <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="51" t="s">
-        <v>146</v>
+      <c r="H3" s="34" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3341,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>10</v>
@@ -3554,31 +3349,31 @@
       <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="51" t="s">
-        <v>147</v>
+      <c r="H4" s="34" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="27">
         <v>1</v>
       </c>
-      <c r="C5" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D5" s="51" t="s">
+      <c r="C5" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="H5" s="51" t="s">
-        <v>263</v>
+      <c r="H5" s="34" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3589,7 +3384,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>13</v>
@@ -3600,8 +3395,8 @@
       <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="51" t="s">
-        <v>148</v>
+      <c r="H6" s="34" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3612,7 +3407,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>24</v>
@@ -3620,8 +3415,8 @@
       <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="51" t="s">
-        <v>261</v>
+      <c r="H7" s="34" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3632,7 +3427,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>11</v>
@@ -3641,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3652,7 +3447,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>12</v>
@@ -3660,8 +3455,8 @@
       <c r="G9" s="5">
         <v>1</v>
       </c>
-      <c r="H9" s="51" t="s">
-        <v>44</v>
+      <c r="H9" s="34" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3672,7 +3467,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>25</v>
@@ -3681,13 +3476,13 @@
         <v>25</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3697,8 +3492,8 @@
       <c r="B11" s="27">
         <v>3</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>209</v>
+      <c r="C11" s="34" t="s">
+        <v>179</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>21</v>
@@ -3706,31 +3501,31 @@
       <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="51" t="s">
-        <v>236</v>
+      <c r="H11" s="34" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12" s="51" t="s">
+      <c r="C12" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="34" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
-      <c r="H12" s="51" t="s">
-        <v>145</v>
+      <c r="H12" s="34" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3741,19 +3536,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>91</v>
-      </c>
       <c r="F13" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
       </c>
-      <c r="H13" s="51" t="s">
-        <v>210</v>
+      <c r="H13" s="34" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3764,7 +3559,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>14</v>
@@ -3773,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3784,19 +3579,19 @@
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G15" s="5">
         <v>20</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3815,8 +3610,8 @@
       <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H16" s="51" t="s">
-        <v>149</v>
+      <c r="H16" s="34" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3849,25 +3644,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4070,7 +3865,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B8" s="9">
         <f>SUMIFS(Resources!B:B,Resources!D:D,Economy!A8)+SUMIFS(Resources!B:B,Resources!E:E,Economy!A8)</f>
@@ -4280,7 +4075,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,46 +4086,46 @@
     <col min="4" max="4" width="8.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="57" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="57" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="62" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="98.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="40" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="40" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="98.7109375" style="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="58" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>299</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>304</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>301</v>
-      </c>
-      <c r="E1" s="58" t="s">
-        <v>302</v>
-      </c>
-      <c r="F1" s="58" t="s">
-        <v>306</v>
-      </c>
-      <c r="G1" s="59" t="s">
-        <v>308</v>
-      </c>
-      <c r="H1" s="59" t="s">
-        <v>309</v>
-      </c>
-      <c r="I1" s="61" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="K1" s="60" t="s">
-        <v>126</v>
+    <row r="1" spans="1:11" s="41" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4356,24 +4151,24 @@
         <f>D2+E2*D2</f>
         <v>94</v>
       </c>
-      <c r="G2" s="57">
+      <c r="G2" s="40">
         <f>1-(2*(A2+1)-2)/(2*(A2+1))</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="40">
         <f>1-(2*(A2+1)-4)/(2*(A2+1))</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="I2" s="62">
+      <c r="I2" s="45">
         <f>F2*G2</f>
         <v>31.333333333333336</v>
       </c>
       <c r="J2" s="3">
-        <f>F2*G3</f>
-        <v>23.5</v>
-      </c>
-      <c r="K2" s="54" t="s">
-        <v>307</v>
+        <f>F2*H2</f>
+        <v>62.666666666666671</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4399,15 +4194,15 @@
         <f t="shared" ref="F3:F5" si="1">D3+E3*D3</f>
         <v>90</v>
       </c>
-      <c r="G3" s="57">
+      <c r="G3" s="40">
         <f t="shared" ref="G3:G5" si="2">1-(2*(A3+1)-2)/(2*(A3+1))</f>
         <v>0.25</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="40">
         <f t="shared" ref="H3:H5" si="3">1-(2*(A3+1)-4)/(2*(A3+1))</f>
         <v>0.5</v>
       </c>
-      <c r="I3" s="62">
+      <c r="I3" s="45">
         <f t="shared" ref="I3:I5" si="4">F3*G3</f>
         <v>22.5</v>
       </c>
@@ -4439,15 +4234,15 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="G4" s="57">
+      <c r="G4" s="40">
         <f t="shared" si="2"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="40">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="I4" s="62">
+      <c r="I4" s="45">
         <f t="shared" si="4"/>
         <v>17.199999999999996</v>
       </c>
@@ -4479,15 +4274,15 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="40">
         <f t="shared" si="2"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="H5" s="57">
+      <c r="H5" s="40">
         <f t="shared" si="3"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="I5" s="62">
+      <c r="I5" s="45">
         <f t="shared" si="4"/>
         <v>13.666666666666664</v>
       </c>
@@ -4495,8 +4290,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K5" s="54" t="s">
-        <v>300</v>
+      <c r="K5" s="37" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -4507,997 +4302,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="O2" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="P2" s="36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A3,Specials!C:P,12,FALSE)),"",VLOOKUP(A3,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="C3" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A3,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A3,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E3,Specials!$C:$P,12,FALSE)),"",VLOOKUP(E3,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G3" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E3,Specials!$C:$P,9,FALSE)),"",VLOOKUP(E3,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I3,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I3,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K3" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I3,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I3,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L3" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M3,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M3,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O3" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M3,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M3,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P3" s="48"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A4,Specials!C:P,12,FALSE)),"",VLOOKUP(A4,Specials!C:P,12,FALSE))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C4" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A4,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A4,Specials!C:P,9,FALSE))</f>
-        <v>You may now build buildings.</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,12,FALSE)),"",VLOOKUP(E4,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G4" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E4,Specials!C:P,9,FALSE)),"",VLOOKUP(E4,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I4,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I4,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K4" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I4,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I4,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L4" s="48"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M4,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M4,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O4" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M4,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M4,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P4" s="48"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A5,Specials!C:P,12,FALSE)),"",VLOOKUP(A5,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="C5" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A5,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A5,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="17">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E5,Specials!C:P,9,FALSE)),"",VLOOKUP(E5,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="17">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I5,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I5,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L5" s="48"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M5,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M5,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O5" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M5,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M5,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P5" s="48"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="17">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(A6,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A6,Specials!C:P,9,FALSE))</f>
-        <v>You do not need to pay any required Stone for Buildings.</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="17">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E6,Specials!C:P,9,FALSE)),"",VLOOKUP(E6,Specials!C:P,9,FALSE))</f>
-        <v>You may trash this card for 1 Food</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I6,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I6,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K6" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I6,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I6,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L6" s="48"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M6,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M6,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O6" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M6,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M6,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P6" s="48"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="17">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <f>IF(ISNA(VLOOKUP(A7,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A7,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="17">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E7,Specials!C:P,9,FALSE)),"",VLOOKUP(E7,Specials!C:P,9,FALSE))</f>
-        <v>You may trash this card for 1 Food</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="17">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I7,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I7,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L7" s="48"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M7,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M7,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O7" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M7,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M7,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P7" s="48"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="17">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A8,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A8,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,12,FALSE)),"",VLOOKUP(E8,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G8" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E8,Specials!C:P,9,FALSE)),"",VLOOKUP(E8,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="17">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I8,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I8,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M8,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M8,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O8" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M8,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M8,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P8" s="48"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="17">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A9,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A9,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="17">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3">
-        <f>IF(ISNA(VLOOKUP(E9,Specials!C:P,9,FALSE)),"",VLOOKUP(E9,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" s="35"/>
-      <c r="J9" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I9,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I9,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K9" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I9,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I9,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M9,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M9,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O9" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M9,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M9,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P9" s="48"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="17">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A10,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A10,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="17">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <f>IF(ISNA(VLOOKUP(E10,Specials!C:P,9,FALSE)),"",VLOOKUP(E10,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I10,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I10,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K10" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I10,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I10,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M10,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M10,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O10" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M10,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M10,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P10" s="48"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="17">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="e">
-        <f>IF(ISNA(VLOOKUP(A11,Specials!'C':Economy!O,8,FALSE)),"",VLOOKUP(A11,Specials!C:P,9,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="17">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <f>IF(ISNA(VLOOKUP(E11,Specials!C:P,9,FALSE)),"",VLOOKUP(E11,Specials!C:P,9,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="17">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I11,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I11,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L11" s="48"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M11,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M11,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O11" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M11,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M11,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P11" s="48"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="17">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>40</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,12,FALSE)),"",VLOOKUP(E12,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G12" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E12,Specials!C:P,9,FALSE)),"",VLOOKUP(E12,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H12" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="35"/>
-      <c r="J12" s="17">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I12,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I12,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M12,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M12,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O12" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M12,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M12,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P12" s="48"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A14,Specials!C:P,12,FALSE)),"",VLOOKUP(A14,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,12,FALSE)),"",VLOOKUP(E13,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G13" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E13,Specials!C:P,9,FALSE)),"",VLOOKUP(E13,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H13" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="17">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I13,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I13,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M13,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M13,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O13" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M13,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M13,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P13" s="48"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A15,Specials!C:P,12,FALSE)),"",VLOOKUP(A15,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,12,FALSE)),"",VLOOKUP(E14,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G14" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E14,Specials!C:P,9,FALSE)),"",VLOOKUP(E14,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I14,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I14,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K14" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I14,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I14,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M14,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M14,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O14" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M14,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M14,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P14" s="48"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A16,Specials!C:P,12,FALSE)),"",VLOOKUP(A16,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,12,FALSE)),"",VLOOKUP(E15,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G15" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E15,Specials!C:P,9,FALSE)),"",VLOOKUP(E15,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I15,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I15,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K15" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I15,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I15,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M15,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M15,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O15" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M15,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M15,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P15" s="48"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A17,Specials!C:P,12,FALSE)),"",VLOOKUP(A17,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="F16" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E16,Specials!C:P,12,FALSE)),"",VLOOKUP(E16,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G16" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E16,Specials!C:P,9,FALSE)),"",VLOOKUP(E16,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I16,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I16,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K16" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I16,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I16,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M16,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M16,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O16" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M16,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M16,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P16" s="48"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A18,Specials!C:P,12,FALSE)),"",VLOOKUP(A18,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="F17" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E17,Specials!C:P,12,FALSE)),"",VLOOKUP(E17,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G17" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E17,Specials!C:P,9,FALSE)),"",VLOOKUP(E17,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I17,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I17,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K17" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I17,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I17,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M17,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M17,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O17" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M17,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M17,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P17" s="48"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A19,Specials!C:P,12,FALSE)),"",VLOOKUP(A19,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="F18" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E18,Specials!C:P,12,FALSE)),"",VLOOKUP(E18,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G18" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(E18,Specials!C:P,9,FALSE)),"",VLOOKUP(E18,Specials!C:P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I18,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I18,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K18" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I18,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I18,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M18,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M18,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O18" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M18,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M18,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P18" s="48"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A19,Specials!C:P,12,FALSE)),"",VLOOKUP(A19,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="17">
-        <f>IF(ISNA(VLOOKUP(E19,Specials!C:P,12,FALSE)),"",VLOOKUP(E19,Specials!C:P,12,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>90</v>
-      </c>
-      <c r="H19" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I19,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I19,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K19" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I19,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I19,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M19,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M19,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O19" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M19,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M19,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P19" s="48"/>
-    </row>
-    <row r="20" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(A20,Specials!C:P,12,FALSE)),"",VLOOKUP(A20,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="17">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3">
-        <v>250</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(I20,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I20,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="K20" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(I20,Specials!$C:$P,9,FALSE)),"",VLOOKUP(I20,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L20" s="48"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M20,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M20,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O20" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M20,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M20,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P20" s="48"/>
-    </row>
-    <row r="21" spans="1:16" s="39" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(E21,Specials!C:P,12,FALSE)),"",VLOOKUP(E21,Specials!C:P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G21" s="3">
-        <v>240</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="I21" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="17">
-        <f>IF(ISNA(VLOOKUP(I21,Specials!$C:$P,12,FALSE)),"",VLOOKUP(I21,Specials!$C:$P,12,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <v>240</v>
-      </c>
-      <c r="L21" s="48"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="17" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,Specials!$C:$P,12,FALSE)),"",VLOOKUP(M21,Specials!$C:$P,12,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O21" s="3" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,Specials!$C:$P,9,FALSE)),"",VLOOKUP(M21,Specials!$C:$P,9,FALSE))</f>
-        <v/>
-      </c>
-      <c r="P21" s="48"/>
-    </row>
-    <row r="22" spans="1:16" s="40" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="47">
-        <f>SUM(B3:B21)</f>
-        <v>12</v>
-      </c>
-      <c r="C22" s="46" t="e">
-        <f>SUM(C3:C21)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="43">
-        <f>SUM(F3:F21)</f>
-        <v>10</v>
-      </c>
-      <c r="G22" s="40">
-        <f>SUM(G3:G21)</f>
-        <v>580</v>
-      </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="J22" s="43">
-        <f>SUM(J3:J21)</f>
-        <v>12</v>
-      </c>
-      <c r="K22" s="40">
-        <f>SUM(K3:K21)</f>
-        <v>240</v>
-      </c>
-      <c r="L22" s="49"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="17" t="e">
-        <f>C22/B22</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="44">
-        <f>G22/F22</f>
-        <v>58</v>
-      </c>
-      <c r="I23" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="J23" s="44">
-        <f>K22/J22</f>
-        <v>20</v>
-      </c>
-      <c r="L23" s="48"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12 A12 A16:A20 I3:I9 I11:I21 A3:A10 M3:M9 M11:M21">
-      <formula1>$C$3:$C$55</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Specials!$C$3:$C$63</xm:f>
-          </x14:formula1>
-          <xm:sqref>E14:E21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -5518,13 +4322,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -5532,22 +4336,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -5565,7 +4369,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -5578,7 +4382,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -5596,7 +4400,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -5609,7 +4413,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -5627,7 +4431,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -5640,7 +4444,7 @@
         <v>18.333333333333332</v>
       </c>
       <c r="H5" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -5658,7 +4462,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -5686,7 +4490,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
ladder backs, and other tweaks
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1459,8 +1459,8 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
preparing for TGC buy
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\victory-point-salad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C07A65-6EB7-491E-911B-D1FD35A52662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E00E67-7B56-4FBE-B8D8-5353B9645347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="Cards" localSheetId="1">Resources!$C$2:$C$17</definedName>
-    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$63</definedName>
+    <definedName name="Cards" localSheetId="0">Specials!$C$2:$C$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="316">
   <si>
     <t>Type</t>
   </si>
@@ -847,9 +847,6 @@
     <t>Take That!</t>
   </si>
   <si>
-    <t>There's Always a Golem</t>
-  </si>
-  <si>
     <t>The "Free" Soldier</t>
   </si>
   <si>
@@ -862,9 +859,6 @@
     <t>Aggression does have benefits.</t>
   </si>
   <si>
-    <t>Tank and spank always works.</t>
-  </si>
-  <si>
     <t>Trash an opponent's card with exactly one soldier.</t>
   </si>
   <si>
@@ -943,9 +937,6 @@
     <t>50 VP if you have 4 Sheep. 50 VP if you have 3 Cattle.</t>
   </si>
   <si>
-    <t>The Milk Engine</t>
-  </si>
-  <si>
     <t>Teets!</t>
   </si>
   <si>
@@ -1123,24 +1114,15 @@
     <t>Milk</t>
   </si>
   <si>
-    <t>Once per turn, you may use an action to get a resource card with Milk from the discard pile.</t>
-  </si>
-  <si>
     <t>Huh… I guess that cattle was female.</t>
   </si>
   <si>
-    <t>You may trash this card for 1 Food. Must be trashed at the end of this turn.</t>
-  </si>
-  <si>
     <t>To trash this card, place 3 Food or equivalent on this card in a single turn before Endgame. Trash the food. This does not cost an action, and cannot be part of a chain.</t>
   </si>
   <si>
     <t>Veggie Soup</t>
   </si>
   <si>
-    <t>At each round start before Endgame, player with the most soldiers places Largest Army token on any card in a purchase row. Anyone who takes that card must pay this person 1 Resource Card. In a tie, nobody places the token.</t>
-  </si>
-  <si>
     <t>Chain 3x Climb</t>
   </si>
   <si>
@@ -1148,6 +1130,42 @@
   </si>
   <si>
     <t>AntiReq</t>
+  </si>
+  <si>
+    <t>Milk Mastery</t>
+  </si>
+  <si>
+    <t>Once per turn, you may use an action to gain a resource card with Milk from the Trash pile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Play immediately. When you gain a Milk resource card from the Trash pile, you may gain an extra one. </t>
+  </si>
+  <si>
+    <t>Double Teets!</t>
+  </si>
+  <si>
+    <t>Gotta milk this joke as long as we can.</t>
+  </si>
+  <si>
+    <t>Milk Climb!</t>
+  </si>
+  <si>
+    <t>At each round start before Endgame, player with the most soldiers places the Army token on any card in a purchase row. Anyone who takes that card must pay this person 1 Resource Card. In a tie, nobody places the token.</t>
+  </si>
+  <si>
+    <t>You may trash this card for 1 Food. Must be trashed at the end of your turn.</t>
+  </si>
+  <si>
+    <t>Spoiler: use it or lose it.</t>
+  </si>
+  <si>
+    <t>The Milk Strategy</t>
+  </si>
+  <si>
+    <t>Clay Soldier</t>
+  </si>
+  <si>
+    <t>Kiln recommended.</t>
   </si>
 </sst>
 </file>
@@ -1720,11 +1738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1756,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>9</v>
@@ -1780,7 +1798,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="K1" s="28" t="s">
         <v>140</v>
@@ -1792,19 +1810,19 @@
         <v>5</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="O1" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="P1" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="P1" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="Q1" s="29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>1</v>
@@ -1853,10 +1871,10 @@
         <v/>
       </c>
       <c r="S2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="T2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
@@ -1873,10 +1891,10 @@
         <v>127</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L3" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="M3" s="3">
         <v>20</v>
@@ -1894,18 +1912,18 @@
         <v>2</v>
       </c>
       <c r="Q3" s="12">
-        <f t="shared" ref="Q3:Q52" si="0">N3/P3</f>
+        <f t="shared" ref="Q3:Q54" si="0">N3/P3</f>
         <v>10</v>
       </c>
       <c r="R3" s="12" t="str">
-        <f t="shared" ref="R3:R52" si="1">IF(O3&lt;&gt;P3,N3/O3,"")</f>
+        <f t="shared" ref="R3:R54" si="1">IF(O3&lt;&gt;P3,N3/O3,"")</f>
         <v/>
       </c>
       <c r="S3" t="s">
         <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -1954,7 +1972,7 @@
         <v>75</v>
       </c>
       <c r="T4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
@@ -2003,7 +2021,7 @@
         <v>74</v>
       </c>
       <c r="T5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
@@ -2020,7 +2038,7 @@
         <v>190</v>
       </c>
       <c r="L6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M6" s="3">
         <v>20</v>
@@ -2049,7 +2067,7 @@
         <v>137</v>
       </c>
       <c r="T6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2066,7 +2084,7 @@
         <v>45</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M7" s="8">
         <v>30</v>
@@ -2095,7 +2113,7 @@
         <v>55</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2147,7 +2165,7 @@
         <v>132</v>
       </c>
       <c r="T8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2196,7 +2214,7 @@
         <v>58</v>
       </c>
       <c r="T9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2245,7 +2263,7 @@
         <v>53</v>
       </c>
       <c r="T10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2291,7 +2309,7 @@
         <v>144</v>
       </c>
       <c r="T11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -2343,7 +2361,7 @@
         <v>122</v>
       </c>
       <c r="T12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
@@ -2395,7 +2413,7 @@
         <v>121</v>
       </c>
       <c r="T13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
@@ -2447,7 +2465,7 @@
         <v>163</v>
       </c>
       <c r="T14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -2458,13 +2476,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
         <v>127</v>
       </c>
       <c r="H15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M15" s="3">
         <v>10</v>
@@ -2490,10 +2508,10 @@
         <v>5</v>
       </c>
       <c r="S15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2539,7 +2557,7 @@
         <v>27</v>
       </c>
       <c r="T16" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2550,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -2588,10 +2606,10 @@
         <v/>
       </c>
       <c r="S17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T17" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -2602,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
@@ -2611,7 +2629,7 @@
         <v>11</v>
       </c>
       <c r="L18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="M18" s="3">
         <v>40</v>
@@ -2637,10 +2655,10 @@
         <v/>
       </c>
       <c r="S18" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="T18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2663,7 +2681,7 @@
         <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M19" s="3">
         <v>60</v>
@@ -2689,10 +2707,10 @@
         <v>30</v>
       </c>
       <c r="S19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="T19" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -2703,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -2712,7 +2730,7 @@
         <v>30</v>
       </c>
       <c r="L20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="M20" s="3">
         <v>30</v>
@@ -2738,10 +2756,10 @@
         <v>18.888888888888889</v>
       </c>
       <c r="S20" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="T20" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2752,16 +2770,16 @@
         <v>1</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>241</v>
+        <v>313</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>12</v>
       </c>
       <c r="K21" s="32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="M21" s="32">
         <v>40</v>
@@ -2787,10 +2805,10 @@
         <v/>
       </c>
       <c r="S21" s="26" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="T21" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2801,7 +2819,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2839,10 +2857,10 @@
         <v/>
       </c>
       <c r="S22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="T22" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2891,7 +2909,7 @@
         <v>133</v>
       </c>
       <c r="T23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2943,7 +2961,7 @@
         <v>170</v>
       </c>
       <c r="T24" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
@@ -2992,7 +3010,7 @@
         <v>60</v>
       </c>
       <c r="T25" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
@@ -3041,7 +3059,7 @@
         <v>59</v>
       </c>
       <c r="T26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -3090,7 +3108,7 @@
         <v>197</v>
       </c>
       <c r="T27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
@@ -3139,7 +3157,7 @@
         <v>182</v>
       </c>
       <c r="T28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
@@ -3188,7 +3206,7 @@
         <v>183</v>
       </c>
       <c r="T29" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
@@ -3237,7 +3255,7 @@
         <v>119</v>
       </c>
       <c r="T30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
@@ -3248,7 +3266,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -3260,7 +3278,7 @@
         <v>30</v>
       </c>
       <c r="L31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M31" s="3">
         <v>110</v>
@@ -3286,10 +3304,10 @@
         <v>27.5</v>
       </c>
       <c r="S31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3338,7 +3356,7 @@
         <v>54</v>
       </c>
       <c r="T32" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3349,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
@@ -3387,10 +3405,10 @@
         <v/>
       </c>
       <c r="S33" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="T33" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3410,7 +3428,7 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M34" s="3">
         <v>40</v>
@@ -3439,7 +3457,7 @@
         <v>56</v>
       </c>
       <c r="T34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3450,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
       <c r="D35" t="s">
         <v>127</v>
@@ -3459,7 +3477,7 @@
         <v>13</v>
       </c>
       <c r="H35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M35" s="3">
         <v>40</v>
@@ -3485,10 +3503,10 @@
         <v>14.857142857142856</v>
       </c>
       <c r="S35" t="s">
-        <v>214</v>
+        <v>315</v>
       </c>
       <c r="T35" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3511,7 +3529,7 @@
         <v>10</v>
       </c>
       <c r="H36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M36" s="3">
         <v>40</v>
@@ -3540,7 +3558,7 @@
         <v>90</v>
       </c>
       <c r="T36" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3551,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F37" t="s">
         <v>23</v>
@@ -3560,7 +3578,7 @@
         <v>23</v>
       </c>
       <c r="L37" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M37" s="3">
         <v>80</v>
@@ -3582,10 +3600,10 @@
         <v>25</v>
       </c>
       <c r="S37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="T37" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3602,7 +3620,7 @@
         <v>11</v>
       </c>
       <c r="L38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M38" s="3">
         <v>10</v>
@@ -3627,7 +3645,7 @@
         <v>198</v>
       </c>
       <c r="T38" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3644,7 +3662,7 @@
         <v>21</v>
       </c>
       <c r="L39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M39" s="3">
         <v>10</v>
@@ -3669,7 +3687,7 @@
         <v>171</v>
       </c>
       <c r="T39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3686,7 +3704,7 @@
         <v>13</v>
       </c>
       <c r="L40" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M40" s="3">
         <v>10</v>
@@ -3711,7 +3729,7 @@
         <v>131</v>
       </c>
       <c r="T40" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3728,7 +3746,7 @@
         <v>10</v>
       </c>
       <c r="L41" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M41" s="3">
         <v>20</v>
@@ -3753,7 +3771,7 @@
         <v>165</v>
       </c>
       <c r="T41" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3767,7 +3785,7 @@
         <v>145</v>
       </c>
       <c r="L42" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M42" s="3">
         <v>10</v>
@@ -3792,7 +3810,7 @@
         <v>146</v>
       </c>
       <c r="T42" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3803,42 +3821,32 @@
         <v>1</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>226</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
+      </c>
+      <c r="F43" t="s">
+        <v>297</v>
       </c>
       <c r="L43" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="M43" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N43" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L43)),AVERAGE(Ladders!C$3:C$7)+M43,M43)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="O43" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F43,Economy!I:I) + SUMIF(Economy!A:A,Specials!G43,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L43)),1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P43" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F43,Economy!I:I) + SUMIF(Economy!A:A,Specials!G43,Economy!I:I) + SUMIF(Specials!K:K,Specials!H43,Specials!P:P) + SUMIF(Specials!K:K,Specials!I43,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L43)),1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q43" s="12">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="R43" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="S43" t="s">
-        <v>245</v>
-      </c>
-      <c r="T43" t="s">
-        <v>254</v>
+        <f t="shared" ref="Q43" si="2">N43/P43</f>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3849,20 +3857,20 @@
         <v>1</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="L44" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="M44" s="3">
         <v>10</v>
       </c>
       <c r="N44" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L44)),AVERAGE(Ladders!C$3:C$7)+M44,M44)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O44" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F44,Economy!I:I) + SUMIF(Economy!A:A,Specials!G44,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L44)),1,0)</f>
@@ -3874,17 +3882,17 @@
       </c>
       <c r="Q44" s="12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="R44" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S44" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="T44" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3895,42 +3903,42 @@
         <v>1</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" t="s">
-        <v>21</v>
+        <v>226</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L45" t="s">
+        <v>269</v>
       </c>
       <c r="M45" s="3">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="N45" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L45)),AVERAGE(Ladders!C$3:C$7)+M45,M45)</f>
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="O45" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F45,Economy!I:I) + SUMIF(Economy!A:A,Specials!G45,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L45)),1,0)</f>
-        <v>3.6470588235294117</v>
+        <v>1</v>
       </c>
       <c r="P45" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F45,Economy!I:I) + SUMIF(Economy!A:A,Specials!G45,Economy!I:I) + SUMIF(Specials!K:K,Specials!H45,Specials!P:P) + SUMIF(Specials!K:K,Specials!I45,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L45)),1,0)</f>
-        <v>3.6470588235294117</v>
+        <v>1</v>
       </c>
       <c r="Q45" s="12">
         <f t="shared" si="0"/>
-        <v>16.451612903225808</v>
+        <v>10</v>
       </c>
       <c r="R45" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S45" t="s">
-        <v>273</v>
+        <v>225</v>
       </c>
       <c r="T45" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3941,42 +3949,41 @@
         <v>1</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>155</v>
+        <v>304</v>
       </c>
       <c r="F46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" t="s">
-        <v>12</v>
+        <v>297</v>
+      </c>
+      <c r="H46" t="s">
+        <v>239</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="L46" t="s">
+        <v>306</v>
       </c>
       <c r="M46" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="N46" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L46)),AVERAGE(Ladders!C$3:C$7)+M46,M46)</f>
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O46" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F46,Economy!I:I) + SUMIF(Economy!A:A,Specials!G46,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L46)),1,0)</f>
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="P46" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F46,Economy!I:I) + SUMIF(Economy!A:A,Specials!G46,Economy!I:I) + SUMIF(Specials!K:K,Specials!H46,Specials!P:P) + SUMIF(Specials!K:K,Specials!I46,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L46)),1,0)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="Q46" s="12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="R46" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" ref="Q46" si="3">N46/P46</f>
+        <v>2.5</v>
       </c>
       <c r="S46" t="s">
-        <v>184</v>
-      </c>
-      <c r="T46" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3987,42 +3994,42 @@
         <v>1</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M47" s="3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="N47" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L47)),AVERAGE(Ladders!C$3:C$7)+M47,M47)</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="O47" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F47,Economy!I:I) + SUMIF(Economy!A:A,Specials!G47,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L47)),1,0)</f>
-        <v>4</v>
+        <v>3.6470588235294117</v>
       </c>
       <c r="P47" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F47,Economy!I:I) + SUMIF(Economy!A:A,Specials!G47,Economy!I:I) + SUMIF(Specials!K:K,Specials!H47,Specials!P:P) + SUMIF(Specials!K:K,Specials!I47,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L47)),1,0)</f>
-        <v>4</v>
+        <v>3.6470588235294117</v>
       </c>
       <c r="Q47" s="12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16.451612903225808</v>
       </c>
       <c r="R47" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S47" t="s">
-        <v>185</v>
+        <v>270</v>
       </c>
       <c r="T47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4033,42 +4040,42 @@
         <v>1</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
-      </c>
-      <c r="L48" t="s">
-        <v>135</v>
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
       </c>
       <c r="M48" s="3">
-        <v>-30</v>
+        <v>70</v>
       </c>
       <c r="N48" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L48)),AVERAGE(Ladders!C$3:C$7)+M48,M48)</f>
-        <v>-30</v>
+        <v>70</v>
       </c>
       <c r="O48" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F48,Economy!I:I) + SUMIF(Economy!A:A,Specials!G48,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L48)),1,0)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="P48" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F48,Economy!I:I) + SUMIF(Economy!A:A,Specials!G48,Economy!I:I) + SUMIF(Specials!K:K,Specials!H48,Specials!P:P) + SUMIF(Specials!K:K,Specials!I48,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L48)),1,0)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="Q48" s="12">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>20</v>
       </c>
       <c r="R48" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S48" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="T48" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4079,42 +4086,42 @@
         <v>1</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="J49" t="s">
-        <v>223</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L49" t="s">
-        <v>292</v>
+        <v>156</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>24</v>
       </c>
       <c r="M49" s="3">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="N49" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L49)),AVERAGE(Ladders!C$3:C$7)+M49,M49)</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="O49" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F49,Economy!I:I) + SUMIF(Economy!A:A,Specials!G49,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L49)),1,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P49" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F49,Economy!I:I) + SUMIF(Economy!A:A,Specials!G49,Economy!I:I) + SUMIF(Specials!K:K,Specials!H49,Specials!P:P) + SUMIF(Specials!K:K,Specials!I49,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L49)),1,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q49" s="12">
-        <f t="shared" ref="Q49" si="2">N49/P49</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="R49" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S49" t="s">
-        <v>293</v>
+        <v>185</v>
+      </c>
+      <c r="T49" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4125,48 +4132,45 @@
         <v>1</v>
       </c>
       <c r="C50" s="39" t="s">
-        <v>296</v>
-      </c>
-      <c r="H50" t="s">
-        <v>223</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>295</v>
+        <v>29</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
       </c>
       <c r="L50" t="s">
-        <v>294</v>
+        <v>135</v>
       </c>
       <c r="M50" s="3">
-        <v>20</v>
+        <v>-30</v>
       </c>
       <c r="N50" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L50)),AVERAGE(Ladders!C$3:C$7)+M50,M50)</f>
-        <v>20</v>
+        <v>-30</v>
       </c>
       <c r="O50" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F50,Economy!I:I) + SUMIF(Economy!A:A,Specials!G50,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L50)),1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P50" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F50,Economy!I:I) + SUMIF(Economy!A:A,Specials!G50,Economy!I:I) + SUMIF(Specials!K:K,Specials!H50,Specials!P:P) + SUMIF(Specials!K:K,Specials!I50,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L50)),1,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q50" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R50" s="12">
+        <v>-10</v>
+      </c>
+      <c r="R50" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="S50" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="T50" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>152</v>
       </c>
@@ -4174,45 +4178,45 @@
         <v>1</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>95</v>
+        <v>201</v>
+      </c>
+      <c r="J51" t="s">
+        <v>221</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="L51" t="s">
-        <v>200</v>
+        <v>289</v>
       </c>
       <c r="M51" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="N51" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L51)),AVERAGE(Ladders!C$3:C$7)+M51,M51)</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="O51" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F51,Economy!I:I) + SUMIF(Economy!A:A,Specials!G51,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L51)),1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P51" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F51,Economy!I:I) + SUMIF(Economy!A:A,Specials!G51,Economy!I:I) + SUMIF(Specials!K:K,Specials!H51,Specials!P:P) + SUMIF(Specials!K:K,Specials!I51,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L51)),1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q51" s="12">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" ref="Q51" si="4">N51/P51</f>
+        <v>10</v>
       </c>
       <c r="R51" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S51" t="s">
-        <v>94</v>
-      </c>
-      <c r="T51" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>152</v>
       </c>
@@ -4220,45 +4224,45 @@
         <v>1</v>
       </c>
       <c r="C52" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="F52" t="s">
-        <v>24</v>
+        <v>293</v>
+      </c>
+      <c r="H52" t="s">
+        <v>221</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="L52" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="M52" s="3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N52" s="34">
         <f>IF(ISNUMBER(SEARCH("climb",L52)),AVERAGE(Ladders!C$3:C$7)+M52,M52)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="O52" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F52,Economy!I:I) + SUMIF(Economy!A:A,Specials!G52,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L52)),1,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P52" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F52,Economy!I:I) + SUMIF(Economy!A:A,Specials!G52,Economy!I:I) + SUMIF(Specials!K:K,Specials!H52,Specials!P:P) + SUMIF(Specials!K:K,Specials!I52,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L52)),1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q52" s="12">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="R52" s="12" t="str">
+        <v>5</v>
+      </c>
+      <c r="R52" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S52" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="T52" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.35">
@@ -4269,17 +4273,20 @@
         <v>1</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>19</v>
+        <v>95</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="L53" t="s">
-        <v>177</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="N53" s="34" t="str">
-        <f>IF(ISNUMBER(SEARCH("climb",L53)),AVERAGE(Ladders!C$3:C$7)+M53,"")</f>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="M53" s="3">
+        <v>30</v>
+      </c>
+      <c r="N53" s="34">
+        <f>IF(ISNUMBER(SEARCH("climb",L53)),AVERAGE(Ladders!C$3:C$7)+M53,M53)</f>
+        <v>30</v>
       </c>
       <c r="O53" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F53,Economy!I:I) + SUMIF(Economy!A:A,Specials!G53,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L53)),1,0)</f>
@@ -4289,75 +4296,82 @@
         <f>2 + SUMIF(Economy!A:A,Specials!F53,Economy!I:I) + SUMIF(Economy!A:A,Specials!G53,Economy!I:I) + SUMIF(Specials!K:K,Specials!H53,Specials!P:P) + SUMIF(Specials!K:K,Specials!I53,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L53)),1,0)</f>
         <v>2</v>
       </c>
+      <c r="Q53" s="12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R53" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="S53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="T53" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K54" s="8"/>
-      <c r="L54" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="M54" s="8">
-        <v>100</v>
-      </c>
-      <c r="N54" s="35" t="str">
-        <f>IF(ISNUMBER(SEARCH("climb",L54)),AVERAGE(Ladders!C$3:C$7)+M54,"")</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L54" t="s">
+        <v>280</v>
+      </c>
+      <c r="M54" s="3">
+        <v>40</v>
+      </c>
+      <c r="N54" s="34">
+        <f>IF(ISNUMBER(SEARCH("climb",L54)),AVERAGE(Ladders!C$3:C$7)+M54,M54)</f>
+        <v>40</v>
+      </c>
+      <c r="O54" s="12">
+        <f>2 + SUMIF(Economy!A:A,Specials!F54,Economy!I:I) + SUMIF(Economy!A:A,Specials!G54,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L54)),1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="P54" s="12">
+        <f>2 + SUMIF(Economy!A:A,Specials!F54,Economy!I:I) + SUMIF(Economy!A:A,Specials!G54,Economy!I:I) + SUMIF(Specials!K:K,Specials!H54,Specials!P:P) + SUMIF(Specials!K:K,Specials!I54,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L54)),1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="Q54" s="12">
+        <f t="shared" si="0"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="R54" s="12" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O54" s="11">
-        <f>2 + SUMIF(Economy!A:A,Specials!F54,Economy!I:I) + SUMIF(Economy!A:A,Specials!G54,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L54)),1,0)</f>
-        <v>4</v>
-      </c>
-      <c r="P54" s="11">
-        <f>2 + SUMIF(Economy!A:A,Specials!F54,Economy!I:I) + SUMIF(Economy!A:A,Specials!G54,Economy!I:I) + SUMIF(Specials!K:K,Specials!H54,Specials!P:P) + SUMIF(Specials!K:K,Specials!I54,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L54)),1,0)</f>
-        <v>4</v>
-      </c>
-      <c r="Q54" s="11">
-        <f>M54/P54</f>
-        <v>25</v>
-      </c>
-      <c r="R54" s="11">
-        <f>M54/P54</f>
-        <v>25</v>
-      </c>
-      <c r="S54" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T54" s="4" t="s">
-        <v>254</v>
+      <c r="S54" t="s">
+        <v>188</v>
+      </c>
+      <c r="T54" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" s="39" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="L55" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="M55" s="3" t="s">
         <v>159</v>
@@ -4375,45 +4389,60 @@
         <v>2</v>
       </c>
       <c r="S55" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="T55" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="3">
-        <v>1</v>
-      </c>
-      <c r="C56" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="L56" t="s">
-        <v>176</v>
-      </c>
-      <c r="M56" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="N56" s="34" t="str">
+      <c r="B56" s="8">
+        <v>1</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K56" s="8"/>
+      <c r="L56" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="M56" s="8">
+        <v>100</v>
+      </c>
+      <c r="N56" s="35" t="str">
         <f>IF(ISNUMBER(SEARCH("climb",L56)),AVERAGE(Ladders!C$3:C$7)+M56,"")</f>
         <v/>
       </c>
-      <c r="O56" s="12">
+      <c r="O56" s="11">
         <f>2 + SUMIF(Economy!A:A,Specials!F56,Economy!I:I) + SUMIF(Economy!A:A,Specials!G56,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L56)),1,0)</f>
-        <v>2</v>
-      </c>
-      <c r="P56" s="12">
+        <v>4</v>
+      </c>
+      <c r="P56" s="11">
         <f>2 + SUMIF(Economy!A:A,Specials!F56,Economy!I:I) + SUMIF(Economy!A:A,Specials!G56,Economy!I:I) + SUMIF(Specials!K:K,Specials!H56,Specials!P:P) + SUMIF(Specials!K:K,Specials!I56,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L56)),1,0)</f>
-        <v>2</v>
-      </c>
-      <c r="S56" t="s">
-        <v>26</v>
-      </c>
-      <c r="T56" t="s">
-        <v>254</v>
+        <v>4</v>
+      </c>
+      <c r="Q56" s="11">
+        <f>M56/P56</f>
+        <v>25</v>
+      </c>
+      <c r="R56" s="11">
+        <f>M56/P56</f>
+        <v>25</v>
+      </c>
+      <c r="S56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T56" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.35">
@@ -4424,10 +4453,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="39" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="L57" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>159</v>
@@ -4445,10 +4474,10 @@
         <v>2</v>
       </c>
       <c r="S57" t="s">
-        <v>175</v>
+        <v>36</v>
       </c>
       <c r="T57" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.35">
@@ -4459,13 +4488,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H58" t="s">
-        <v>141</v>
+        <v>228</v>
       </c>
       <c r="L58" t="s">
-        <v>278</v>
+        <v>176</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>159</v>
@@ -4483,10 +4509,10 @@
         <v>2</v>
       </c>
       <c r="S58" t="s">
-        <v>213</v>
+        <v>26</v>
       </c>
       <c r="T58" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.35">
@@ -4497,13 +4523,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="H59" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L59" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>159</v>
@@ -4518,13 +4541,13 @@
       </c>
       <c r="P59" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F59,Economy!I:I) + SUMIF(Economy!A:A,Specials!G59,Economy!I:I) + SUMIF(Specials!K:K,Specials!H59,Specials!P:P) + SUMIF(Specials!K:K,Specials!I59,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L59)),1,0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S59" t="s">
-        <v>48</v>
+        <v>175</v>
       </c>
       <c r="T59" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.35">
@@ -4535,10 +4558,13 @@
         <v>1</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>157</v>
+        <v>31</v>
+      </c>
+      <c r="H60" t="s">
+        <v>141</v>
       </c>
       <c r="L60" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>159</v>
@@ -4556,10 +4582,10 @@
         <v>2</v>
       </c>
       <c r="S60" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="T60" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.35">
@@ -4570,10 +4596,13 @@
         <v>1</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>178</v>
+        <v>40</v>
+      </c>
+      <c r="H61" t="s">
+        <v>30</v>
       </c>
       <c r="L61" t="s">
-        <v>268</v>
+        <v>138</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>159</v>
@@ -4588,161 +4617,231 @@
       </c>
       <c r="P61" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F61,Economy!I:I) + SUMIF(Economy!A:A,Specials!G61,Economy!I:I) + SUMIF(Specials!K:K,Specials!H61,Specials!P:P) + SUMIF(Specials!K:K,Specials!I61,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L61)),1,0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S61" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="T61" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="32">
-        <v>1</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>269</v>
-      </c>
-      <c r="K62" s="32"/>
-      <c r="L62" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="M62" s="32" t="s">
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="L62" t="s">
+        <v>264</v>
+      </c>
+      <c r="M62" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="N62" s="36" t="str">
+      <c r="N62" s="34" t="str">
         <f>IF(ISNUMBER(SEARCH("climb",L62)),AVERAGE(Ladders!C$3:C$7)+M62,"")</f>
         <v/>
       </c>
-      <c r="O62" s="31">
+      <c r="O62" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F62,Economy!I:I) + SUMIF(Economy!A:A,Specials!G62,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L62)),1,0)</f>
         <v>2</v>
       </c>
-      <c r="P62" s="31">
+      <c r="P62" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F62,Economy!I:I) + SUMIF(Economy!A:A,Specials!G62,Economy!I:I) + SUMIF(Specials!K:K,Specials!H62,Specials!P:P) + SUMIF(Specials!K:K,Specials!I62,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L62)),1,0)</f>
         <v>2</v>
       </c>
-      <c r="Q62" s="31"/>
-      <c r="R62" s="31"/>
-      <c r="S62" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="T62" s="26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B63" s="8">
-        <v>1</v>
-      </c>
-      <c r="C63" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="K63" s="8"/>
-      <c r="L63" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="M63" s="8">
-        <v>0</v>
-      </c>
-      <c r="N63" s="35" t="str">
+      <c r="S62" t="s">
+        <v>158</v>
+      </c>
+      <c r="T62" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="L63" t="s">
+        <v>265</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N63" s="34" t="str">
         <f>IF(ISNUMBER(SEARCH("climb",L63)),AVERAGE(Ladders!C$3:C$7)+M63,"")</f>
         <v/>
       </c>
-      <c r="O63" s="11">
+      <c r="O63" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F63,Economy!I:I) + SUMIF(Economy!A:A,Specials!G63,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L63)),1,0)</f>
         <v>2</v>
       </c>
-      <c r="P63" s="11">
+      <c r="P63" s="12">
         <f>2 + SUMIF(Economy!A:A,Specials!F63,Economy!I:I) + SUMIF(Economy!A:A,Specials!G63,Economy!I:I) + SUMIF(Specials!K:K,Specials!H63,Specials!P:P) + SUMIF(Specials!K:K,Specials!I63,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L63)),1,0)</f>
         <v>2</v>
       </c>
-      <c r="Q63" s="11">
-        <f>M63/P63</f>
-        <v>0</v>
-      </c>
-      <c r="R63" s="11">
-        <f>M63/P63</f>
-        <v>0</v>
-      </c>
-      <c r="S63" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="T63" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="B64" s="33">
-        <v>1</v>
-      </c>
-      <c r="C64" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="K64" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="L64" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="M64" s="33">
-        <v>40</v>
-      </c>
-      <c r="N64" s="37" t="str">
+      <c r="S63" t="s">
+        <v>202</v>
+      </c>
+      <c r="T63" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="32">
+        <v>1</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="K64" s="32"/>
+      <c r="L64" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="M64" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="N64" s="36" t="str">
         <f>IF(ISNUMBER(SEARCH("climb",L64)),AVERAGE(Ladders!C$3:C$7)+M64,"")</f>
         <v/>
       </c>
-      <c r="O64" s="30"/>
-      <c r="P64" s="30"/>
-      <c r="Q64" s="30"/>
-      <c r="R64" s="30"/>
-      <c r="S64" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="T64" s="27" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="32">
-        <v>4</v>
-      </c>
-      <c r="C65" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="K65" s="32"/>
-      <c r="L65" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="M65" s="32">
-        <v>-100</v>
-      </c>
-      <c r="N65" s="36" t="str">
+      <c r="O64" s="31">
+        <f>2 + SUMIF(Economy!A:A,Specials!F64,Economy!I:I) + SUMIF(Economy!A:A,Specials!G64,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L64)),1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="P64" s="31">
+        <f>2 + SUMIF(Economy!A:A,Specials!F64,Economy!I:I) + SUMIF(Economy!A:A,Specials!G64,Economy!I:I) + SUMIF(Specials!K:K,Specials!H64,Specials!P:P) + SUMIF(Specials!K:K,Specials!I64,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L64)),1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q64" s="31"/>
+      <c r="R64" s="31"/>
+      <c r="S64" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="T64" s="26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="8">
+        <v>1</v>
+      </c>
+      <c r="C65" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="K65" s="8"/>
+      <c r="L65" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M65" s="8">
+        <v>0</v>
+      </c>
+      <c r="N65" s="35" t="str">
         <f>IF(ISNUMBER(SEARCH("climb",L65)),AVERAGE(Ladders!C$3:C$7)+M65,"")</f>
         <v/>
       </c>
-      <c r="O65" s="31"/>
-      <c r="P65" s="31"/>
-      <c r="Q65" s="31"/>
-      <c r="R65" s="31"/>
-      <c r="S65" s="26" t="s">
+      <c r="O65" s="11">
+        <f>2 + SUMIF(Economy!A:A,Specials!F65,Economy!I:I) + SUMIF(Economy!A:A,Specials!G65,Economy!I:I)-IF(ISNUMBER(SEARCH("Play immediately",L65)),1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="P65" s="11">
+        <f>2 + SUMIF(Economy!A:A,Specials!F65,Economy!I:I) + SUMIF(Economy!A:A,Specials!G65,Economy!I:I) + SUMIF(Specials!K:K,Specials!H65,Specials!P:P) + SUMIF(Specials!K:K,Specials!I65,Specials!P:P)-IF(ISNUMBER(SEARCH("Play immediately",L65)),1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q65" s="11">
+        <f>M65/P65</f>
+        <v>0</v>
+      </c>
+      <c r="R65" s="11">
+        <f>M65/P65</f>
+        <v>0</v>
+      </c>
+      <c r="S65" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="T65" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B66" s="33">
+        <v>1</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K66" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="L66" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="M66" s="33">
+        <v>40</v>
+      </c>
+      <c r="N66" s="37" t="str">
+        <f>IF(ISNUMBER(SEARCH("climb",L66)),AVERAGE(Ladders!C$3:C$7)+M66,"")</f>
+        <v/>
+      </c>
+      <c r="O66" s="30"/>
+      <c r="P66" s="30"/>
+      <c r="Q66" s="30"/>
+      <c r="R66" s="30"/>
+      <c r="S66" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="T66" s="27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="32">
+        <v>4</v>
+      </c>
+      <c r="C67" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="K67" s="32"/>
+      <c r="L67" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="M67" s="32">
+        <v>-100</v>
+      </c>
+      <c r="N67" s="36" t="str">
+        <f>IF(ISNUMBER(SEARCH("climb",L67)),AVERAGE(Ladders!C$3:C$7)+M67,"")</f>
+        <v/>
+      </c>
+      <c r="O67" s="31"/>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="31"/>
+      <c r="S67" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="T65" s="26" t="s">
-        <v>254</v>
+      <c r="T67" s="26" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4758,7 +4857,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4777,7 +4876,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -4818,7 +4917,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4872,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -4884,7 +4983,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4927,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -5004,7 +5103,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -5016,7 +5115,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -5047,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -5156,16 +5255,19 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D18" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F18" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="G18">
         <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -5206,7 +5308,7 @@
         <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>106</v>
@@ -5221,10 +5323,10 @@
         <v>108</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -5755,34 +5857,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>257</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>260</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>113</v>
@@ -5798,18 +5900,18 @@
       </c>
       <c r="C2" s="3">
         <f>SUMIF(Specials!A:A,"Midgame",Specials!B:B)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3">
         <f>B2+C2</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3">
         <f>D2+E2*D2</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G2" s="17">
         <f>1-(2*(A2+1)-2)/(2*(A2+1))</f>
@@ -5821,14 +5923,14 @@
       </c>
       <c r="I2" s="22">
         <f>F2*G2</f>
-        <v>32.666666666666671</v>
+        <v>34.000000000000007</v>
       </c>
       <c r="J2" s="3">
         <f>F2*H2</f>
-        <v>65.333333333333343</v>
+        <v>68.000000000000014</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -5841,18 +5943,18 @@
       </c>
       <c r="C3" s="3">
         <f>SUMIF(Specials!A:A,"Midgame",Specials!B:B)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D5" si="0">B3+C3</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F5" si="1">D3+E3*D3</f>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G3" s="17">
         <f t="shared" ref="G3:G5" si="2">1-(2*(A3+1)-2)/(2*(A3+1))</f>
@@ -5864,11 +5966,11 @@
       </c>
       <c r="I3" s="22">
         <f t="shared" ref="I3:I5" si="4">F3*G3</f>
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ref="J3:J5" si="5">F3*G4</f>
-        <v>18.799999999999997</v>
+        <v>19.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -5881,18 +5983,18 @@
       </c>
       <c r="C4" s="3">
         <f>SUMIF(Specials!A:A,"Midgame",Specials!B:B)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" si="2"/>
@@ -5904,11 +6006,11 @@
       </c>
       <c r="I4" s="22">
         <f t="shared" si="4"/>
-        <v>17.999999999999996</v>
+        <v>18.799999999999997</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="5"/>
-        <v>14.999999999999996</v>
+        <v>15.666666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -5921,18 +6023,18 @@
       </c>
       <c r="C5" s="3">
         <f>SUMIF(Specials!A:A,"Midgame",Specials!B:B)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" si="2"/>
@@ -5944,14 +6046,14 @@
       </c>
       <c r="I5" s="22">
         <f t="shared" si="4"/>
-        <v>14.33333333333333</v>
+        <v>14.999999999999996</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -5990,7 +6092,7 @@
         <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -6106,7 +6208,7 @@
         <v>18.333333333333332</v>
       </c>
       <c r="J5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -6204,7 +6306,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -6240,7 +6342,7 @@
         <v>1</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="O1" s="9"/>
       <c r="P1" s="2"/>
@@ -6253,25 +6355,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="L2">
         <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>